<commit_message>
Hydroflask EMEA Testcase TEST_DGLD_HF_EMEA_RT_009 Changes and Testdata Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F20D8B5-8672-45D8-BE95-882BD7CA155E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFADCC4-661A-4E73-A256-BD4CEB268FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23040" windowHeight="11292" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="512">
   <si>
     <t>UserName</t>
   </si>
@@ -1590,14 +1590,20 @@
   <si>
     <t>Exclusives,New Arrivals,Best Sellers</t>
   </si>
+  <si>
+    <t>HFEMEA20OFF</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1771,7 +1777,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1804,7 +1810,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2113,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU49"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4711,7 +4717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAA7450-0FE7-4C50-95DC-266117BAF81B}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -8330,8 +8336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8570,7 +8576,7 @@
         <v>156</v>
       </c>
       <c r="J9" t="s">
-        <v>229</v>
+        <v>511</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
@@ -8636,7 +8642,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="Y14" t="s">
-        <v>260</v>
+        <v>510</v>
       </c>
       <c r="Z14" t="s">
         <v>266</v>

</xml_diff>

<commit_message>
Hydroflask EMEA TEST_DGLD_HF_EMEA_RT_009 Changes and Testdata Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFADCC4-661A-4E73-A256-BD4CEB268FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CD0717-512A-41C4-8AEA-EFBB4859A3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="520">
   <si>
     <t>UserName</t>
   </si>
@@ -1595,6 +1595,30 @@
   </si>
   <si>
     <t>Delivery</t>
+  </si>
+  <si>
+    <t>93 York House</t>
+  </si>
+  <si>
+    <t>Bradford</t>
+  </si>
+  <si>
+    <t>West Yorkshire</t>
+  </si>
+  <si>
+    <t>BD109ET</t>
+  </si>
+  <si>
+    <t>71 Worthy Street</t>
+  </si>
+  <si>
+    <t>Chorley</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>PR60NH</t>
   </si>
 </sst>
 </file>
@@ -2119,7 +2143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -8336,8 +8360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8474,16 +8498,16 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
-        <v>152</v>
+        <v>512</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>513</v>
       </c>
       <c r="M2" t="s">
-        <v>19</v>
+        <v>514</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>18</v>
+        <v>515</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>59</v>
@@ -8659,16 +8683,16 @@
         <v>15</v>
       </c>
       <c r="K15" t="s">
-        <v>62</v>
+        <v>516</v>
       </c>
       <c r="L15" t="s">
-        <v>63</v>
+        <v>517</v>
       </c>
       <c r="M15" t="s">
-        <v>64</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>65</v>
+        <v>518</v>
+      </c>
+      <c r="N15" t="s">
+        <v>519</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Hydroflask EMEA TEST_DGLD_HF_EMEA_BCT_007 Changes and Testdata Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CD0717-512A-41C4-8AEA-EFBB4859A3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE4F6A2-975D-4BE7-81F0-D31C01CC7214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="522">
   <si>
     <t>UserName</t>
   </si>
@@ -1619,6 +1619,12 @@
   </si>
   <si>
     <t>PR60NH</t>
+  </si>
+  <si>
+    <t>oxobuyer@oxo.com</t>
+  </si>
+  <si>
+    <t>oxobuyer123</t>
   </si>
 </sst>
 </file>
@@ -2144,7 +2150,7 @@
   <dimension ref="A1:AU49"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2351,16 +2357,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" t="s">
-        <v>152</v>
+        <v>512</v>
       </c>
       <c r="T2" t="s">
-        <v>17</v>
+        <v>513</v>
       </c>
       <c r="V2" t="s">
-        <v>19</v>
+        <v>514</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>18</v>
+        <v>515</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>59</v>
@@ -2576,8 +2582,8 @@
       <c r="A10" t="s">
         <v>156</v>
       </c>
-      <c r="J10" t="s">
-        <v>229</v>
+      <c r="J10" s="23" t="s">
+        <v>511</v>
       </c>
       <c r="W10" s="3"/>
       <c r="X10" s="4"/>
@@ -2749,7 +2755,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="AI20" t="s">
-        <v>260</v>
+        <v>510</v>
       </c>
       <c r="AJ20" t="s">
         <v>266</v>
@@ -8360,8 +8366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8646,11 +8652,11 @@
         <v>77</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>79</v>
+        <v>521</v>
       </c>
       <c r="E13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>78</v>
+        <v>520</v>
       </c>
       <c r="I13" s="2"/>
       <c r="O13" s="5"/>

</xml_diff>

<commit_message>
HF_EMEA : TEST_DGLD_HF_EMEA_BCT_002_Footer_Links_Validation and also updated the testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE4F6A2-975D-4BE7-81F0-D31C01CC7214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F49BD9-ECE2-47F4-8AC6-23AFA6D4EC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23040" windowHeight="11292" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1397,9 +1397,6 @@
     <t>CustomizeLinks</t>
   </si>
   <si>
-    <t>Track Your Order,Refer A Friend,Loyalty Program Terms and Conditions</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -1558,15 +1555,9 @@
     <t>gaddamramyasree0809+automation@gmail.com</t>
   </si>
   <si>
-    <t>Contact Us,Find a Store,FAQs,Track Your Order,Shipping &amp; Returns,Warranty</t>
-  </si>
-  <si>
     <t>Refill For Good,Corporate Responsibility</t>
   </si>
   <si>
-    <t>Our Story,Careersl,Group Customization,Pro Deal</t>
-  </si>
-  <si>
     <t>24 oz,32 oz</t>
   </si>
   <si>
@@ -1625,6 +1616,15 @@
   </si>
   <si>
     <t>oxobuyer123</t>
+  </si>
+  <si>
+    <t>Contact Us,Find a Store,Track Your Order</t>
+  </si>
+  <si>
+    <t>Our Story,Group Customization,Pro Deal</t>
+  </si>
+  <si>
+    <t>Track Your Order</t>
   </si>
 </sst>
 </file>
@@ -1632,8 +1632,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1807,7 +1807,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1840,7 +1840,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2313,7 +2313,7 @@
         <v>209</v>
       </c>
       <c r="AT1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AU1" t="s">
         <v>367</v>
@@ -2357,16 +2357,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" t="s">
+        <v>509</v>
+      </c>
+      <c r="T2" t="s">
+        <v>510</v>
+      </c>
+      <c r="V2" t="s">
+        <v>511</v>
+      </c>
+      <c r="W2" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="T2" t="s">
-        <v>513</v>
-      </c>
-      <c r="V2" t="s">
-        <v>514</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>515</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>59</v>
@@ -2379,10 +2379,10 @@
         <v>301</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2397,7 +2397,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -2469,13 +2469,13 @@
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>451</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>453</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -2490,10 +2490,10 @@
         <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2532,7 +2532,7 @@
         <v>23</v>
       </c>
       <c r="AA6" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AB6">
         <v>123</v>
@@ -2583,7 +2583,7 @@
         <v>156</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="W10" s="3"/>
       <c r="X10" s="4"/>
@@ -2653,16 +2653,16 @@
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="AC14" s="39" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="AD14" s="37"/>
       <c r="AE14" s="39" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.3">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="I18" s="2"/>
       <c r="AL18" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.3">
@@ -2755,7 +2755,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="AI20" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="AJ20" t="s">
         <v>266</v>
@@ -2769,7 +2769,7 @@
         <v>45</v>
       </c>
       <c r="AA21" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AB21">
         <v>123</v>
@@ -2806,7 +2806,7 @@
         <v>47</v>
       </c>
       <c r="AA22" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AB22">
         <v>1234</v>
@@ -2820,7 +2820,7 @@
         <v>49</v>
       </c>
       <c r="AA23" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AB23">
         <v>123</v>
@@ -2859,7 +2859,7 @@
         <v>23</v>
       </c>
       <c r="AA24" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AB24">
         <v>123</v>
@@ -2919,10 +2919,10 @@
         <v>337</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.3">
@@ -2973,7 +2973,7 @@
         <v>153</v>
       </c>
       <c r="AL30" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.3">
@@ -3269,10 +3269,10 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>461</v>
+      </c>
+      <c r="P49" s="31" t="s">
         <v>462</v>
-      </c>
-      <c r="P49" s="31" t="s">
-        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -3437,10 +3437,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -3455,10 +3455,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -3484,10 +3484,10 @@
         <v>194</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>29</v>
@@ -3502,10 +3502,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s">
@@ -3534,10 +3534,10 @@
         <v>196</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -3552,10 +3552,10 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" t="s">
@@ -3718,7 +3718,7 @@
         <v>50</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I14" s="2"/>
       <c r="K14" t="s">
@@ -3943,10 +3943,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -3961,10 +3961,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -4006,10 +4006,10 @@
         <v>189</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -4180,10 +4180,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -4198,10 +4198,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -4653,10 +4653,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -4730,7 +4730,7 @@
         <v>154</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>263</v>
@@ -4835,7 +4835,7 @@
         <v>230</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -4865,7 +4865,7 @@
         <v>267</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>278</v>
@@ -4896,7 +4896,7 @@
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
       <c r="I4" s="25" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -4924,7 +4924,7 @@
       <c r="H5" s="25"/>
       <c r="I5" s="35"/>
       <c r="J5" s="25" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
@@ -4985,7 +4985,7 @@
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
       <c r="M7" s="33" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
@@ -5014,7 +5014,7 @@
       <c r="O8" s="25"/>
       <c r="P8" s="25"/>
       <c r="Q8" s="24" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="R8" s="25"/>
       <c r="S8" s="25"/>
@@ -5027,7 +5027,7 @@
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
       <c r="E9" s="25" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
@@ -5068,7 +5068,7 @@
         <v>290</v>
       </c>
       <c r="S10" s="25" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -5106,10 +5106,10 @@
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
       <c r="G12" s="40" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
@@ -5179,7 +5179,7 @@
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="25" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
@@ -5225,26 +5225,26 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C18" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q19" t="s">
         <v>467</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -5509,10 +5509,10 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>276</v>
@@ -5541,7 +5541,7 @@
         <v>437</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>276</v>
@@ -5579,10 +5579,10 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>276</v>
@@ -5611,7 +5611,7 @@
         <v>437</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>276</v>
@@ -5649,10 +5649,10 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>276</v>
@@ -5681,7 +5681,7 @@
         <v>437</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>276</v>
@@ -5719,10 +5719,10 @@
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>276</v>
@@ -5751,7 +5751,7 @@
         <v>437</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>276</v>
@@ -5789,10 +5789,10 @@
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>276</v>
@@ -5821,7 +5821,7 @@
         <v>437</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>276</v>
@@ -5859,10 +5859,10 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -5900,10 +5900,10 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
@@ -5941,10 +5941,10 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>276</v>
@@ -5973,7 +5973,7 @@
         <v>437</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>276</v>
@@ -6824,7 +6824,7 @@
         <v>47</v>
       </c>
       <c r="AG53" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AH53">
         <v>1234</v>
@@ -7797,7 +7797,7 @@
         <v>105</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AK11" s="5" t="s">
         <v>286</v>
@@ -7806,7 +7806,7 @@
         <v>67</v>
       </c>
       <c r="AM11" s="15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.3">
@@ -8366,7 +8366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -8504,16 +8504,16 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
+        <v>509</v>
+      </c>
+      <c r="L2" t="s">
+        <v>510</v>
+      </c>
+      <c r="M2" t="s">
+        <v>511</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="L2" t="s">
-        <v>513</v>
-      </c>
-      <c r="M2" t="s">
-        <v>514</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>515</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>59</v>
@@ -8606,7 +8606,7 @@
         <v>156</v>
       </c>
       <c r="J9" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
@@ -8652,11 +8652,11 @@
         <v>77</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="I13" s="2"/>
       <c r="O13" s="5"/>
@@ -8672,7 +8672,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="Y14" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="Z14" t="s">
         <v>266</v>
@@ -8689,16 +8689,16 @@
         <v>15</v>
       </c>
       <c r="K15" t="s">
+        <v>513</v>
+      </c>
+      <c r="L15" t="s">
+        <v>514</v>
+      </c>
+      <c r="M15" t="s">
+        <v>515</v>
+      </c>
+      <c r="N15" t="s">
         <v>516</v>
-      </c>
-      <c r="L15" t="s">
-        <v>517</v>
-      </c>
-      <c r="M15" t="s">
-        <v>518</v>
-      </c>
-      <c r="N15" t="s">
-        <v>519</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>59</v>
@@ -8856,8 +8856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF53EDC-31F8-48E9-83B2-56073048BB22}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8910,7 +8910,7 @@
         <v>245</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>499</v>
+        <v>519</v>
       </c>
       <c r="C2" s="25"/>
     </row>
@@ -8920,7 +8920,7 @@
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25" t="s">
-        <v>501</v>
+        <v>520</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
@@ -8929,7 +8929,7 @@
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25" t="s">
-        <v>449</v>
+        <v>521</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="25" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -9271,7 +9271,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>29</v>
@@ -9286,7 +9286,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" t="s">

</xml_diff>

<commit_message>
Hydroflask EMEA TEST_DGLD_HF_EMEA_BCT_010 Changes with Testdata Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F49BD9-ECE2-47F4-8AC6-23AFA6D4EC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15066802-68FC-4171-80C7-A8D59BC6D60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23040" windowHeight="11292" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1632,8 +1632,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1807,7 +1807,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1840,7 +1840,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2149,8 +2149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU49"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2636,10 +2636,10 @@
         <v>1</v>
       </c>
       <c r="AE13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AF13" t="s">
-        <v>39</v>
+        <v>398</v>
       </c>
       <c r="AG13" t="s">
         <v>192</v>
@@ -8856,7 +8856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF53EDC-31F8-48E9-83B2-56073048BB22}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Hydroflask EMEA New Reg Testcases Added 008,012,016 Changes with Testdata Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15066802-68FC-4171-80C7-A8D59BC6D60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F643B334-645D-48E2-8190-A1C720A3B16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="520">
   <si>
     <t>UserName</t>
   </si>
@@ -1511,12 +1511,6 @@
 https://mcloud-na-preprod.hydroflask.com/26-l-day-escape-tote?color=Peppercorn
 https://mcloud-na-preprod.hydroflask.com/contact-us
 https://mcloud-na-preprod.hydroflask.com/prodeal/application/index/</t>
-  </si>
-  <si>
-    <t>rgaddam+APITEST@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>4001152559</t>
   </si>
   <si>
     <t>AccountDetails_TC6</t>
@@ -2149,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2357,16 +2351,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" t="s">
+        <v>507</v>
+      </c>
+      <c r="T2" t="s">
+        <v>508</v>
+      </c>
+      <c r="V2" t="s">
         <v>509</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" s="5" t="s">
         <v>510</v>
-      </c>
-      <c r="V2" t="s">
-        <v>511</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>512</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>59</v>
@@ -2379,10 +2373,10 @@
         <v>301</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2397,7 +2391,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -2583,7 +2577,7 @@
         <v>156</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W10" s="3"/>
       <c r="X10" s="4"/>
@@ -2755,7 +2749,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="AI20" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="AJ20" t="s">
         <v>266</v>
@@ -2930,11 +2924,11 @@
         <v>77</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>79</v>
+        <v>516</v>
       </c>
       <c r="E28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>78</v>
+        <v>515</v>
       </c>
       <c r="I28" s="2"/>
       <c r="W28" s="5"/>
@@ -3437,10 +3431,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -3455,10 +3449,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -3484,10 +3478,10 @@
         <v>194</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>29</v>
@@ -3502,10 +3496,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s">
@@ -3534,10 +3528,10 @@
         <v>196</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -3552,10 +3546,10 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" t="s">
@@ -3718,7 +3712,7 @@
         <v>50</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I14" s="2"/>
       <c r="K14" t="s">
@@ -3943,10 +3937,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -3961,10 +3955,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -4006,10 +4000,10 @@
         <v>189</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -4180,10 +4174,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -4198,10 +4192,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -4653,10 +4647,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -4835,7 +4829,7 @@
         <v>230</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -4865,7 +4859,7 @@
         <v>267</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>278</v>
@@ -4896,7 +4890,7 @@
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
       <c r="I4" s="25" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -4924,7 +4918,7 @@
       <c r="H5" s="25"/>
       <c r="I5" s="35"/>
       <c r="J5" s="25" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
@@ -4985,7 +4979,7 @@
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
       <c r="M7" s="33" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
@@ -5027,7 +5021,7 @@
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
       <c r="E9" s="25" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
@@ -5106,7 +5100,7 @@
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
       <c r="G12" s="40" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H12" s="33" t="s">
         <v>481</v>
@@ -5179,7 +5173,7 @@
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="25" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
@@ -5512,7 +5506,7 @@
         <v>469</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>276</v>
@@ -5582,7 +5576,7 @@
         <v>471</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>276</v>
@@ -5652,7 +5646,7 @@
         <v>472</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>276</v>
@@ -5722,7 +5716,7 @@
         <v>475</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>276</v>
@@ -5792,7 +5786,7 @@
         <v>479</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>276</v>
@@ -5859,10 +5853,10 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -5900,10 +5894,10 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
@@ -5944,7 +5938,7 @@
         <v>477</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>276</v>
@@ -7268,8 +7262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AS18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AM11" sqref="AM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7294,6 +7288,7 @@
     <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -7796,17 +7791,17 @@
       <c r="A11" t="s">
         <v>105</v>
       </c>
-      <c r="AJ11" s="5" t="s">
-        <v>485</v>
+      <c r="AJ11" s="5">
+        <v>43000000229</v>
       </c>
       <c r="AK11" s="5" t="s">
         <v>286</v>
       </c>
       <c r="AL11" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="AM11" s="15" t="s">
-        <v>484</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.3">
@@ -8366,8 +8361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8504,16 +8499,16 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
+        <v>507</v>
+      </c>
+      <c r="L2" t="s">
+        <v>508</v>
+      </c>
+      <c r="M2" t="s">
         <v>509</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" s="5" t="s">
         <v>510</v>
-      </c>
-      <c r="M2" t="s">
-        <v>511</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>512</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>59</v>
@@ -8606,7 +8601,7 @@
         <v>156</v>
       </c>
       <c r="J9" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
@@ -8652,11 +8647,11 @@
         <v>77</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="I13" s="2"/>
       <c r="O13" s="5"/>
@@ -8672,7 +8667,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="Y14" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="Z14" t="s">
         <v>266</v>
@@ -8689,16 +8684,16 @@
         <v>15</v>
       </c>
       <c r="K15" t="s">
+        <v>511</v>
+      </c>
+      <c r="L15" t="s">
+        <v>512</v>
+      </c>
+      <c r="M15" t="s">
         <v>513</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>514</v>
-      </c>
-      <c r="M15" t="s">
-        <v>515</v>
-      </c>
-      <c r="N15" t="s">
-        <v>516</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>59</v>
@@ -8910,7 +8905,7 @@
         <v>245</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C2" s="25"/>
     </row>
@@ -8920,7 +8915,7 @@
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
@@ -8929,7 +8924,7 @@
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
@@ -8938,7 +8933,7 @@
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="25" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -9271,7 +9266,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>29</v>
@@ -9286,7 +9281,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" t="s">

</xml_diff>

<commit_message>
HYF_EMEA : TEST_DGLD_HF_EMEA_RT_020_changeAddressIn_AddressBook(New testcase added)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6AD944-37A3-4739-A73D-E9E6BFA27514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5BC852-7CB1-4CEA-BEF8-09FEFF64182F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1700" uniqueCount="525">
   <si>
     <t>UserName</t>
   </si>
@@ -1623,14 +1623,26 @@
   <si>
     <t>hfemealotus@gmail.com</t>
   </si>
+  <si>
+    <t>93/5 Morrison Street</t>
+  </si>
+  <si>
+    <t>Edinburgh</t>
+  </si>
+  <si>
+    <t>Midlothian</t>
+  </si>
+  <si>
+    <t>EH3 8BX</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1811,7 +1823,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1844,7 +1856,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2156,34 +2168,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU49"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5:X5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="21" width="22.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="18" width="30.5546875" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="21" width="22.33203125" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.28515625" customWidth="1"/>
+    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2326,7 +2338,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2381,7 +2393,7 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="7"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>299</v>
       </c>
@@ -2417,16 +2429,16 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" t="s">
-        <v>152</v>
+        <v>505</v>
       </c>
       <c r="T3" t="s">
-        <v>17</v>
+        <v>506</v>
       </c>
       <c r="V3" t="s">
-        <v>19</v>
+        <v>507</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>18</v>
+        <v>508</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>59</v>
@@ -2434,7 +2446,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>368</v>
       </c>
@@ -2474,7 +2486,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>449</v>
       </c>
@@ -2512,16 +2524,16 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" t="s">
-        <v>152</v>
+        <v>505</v>
       </c>
       <c r="T5" t="s">
-        <v>17</v>
+        <v>506</v>
       </c>
       <c r="V5" t="s">
-        <v>19</v>
+        <v>507</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>18</v>
+        <v>508</v>
       </c>
       <c r="X5" s="5" t="s">
         <v>59</v>
@@ -2529,7 +2541,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2545,7 +2557,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>201</v>
       </c>
@@ -2557,7 +2569,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>302</v>
       </c>
@@ -2573,7 +2585,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>157</v>
       </c>
@@ -2585,7 +2597,7 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>156</v>
       </c>
@@ -2598,7 +2610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>174</v>
       </c>
@@ -2617,7 +2629,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>172</v>
       </c>
@@ -2630,7 +2642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2658,7 +2670,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>455</v>
       </c>
@@ -2672,7 +2684,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>178</v>
       </c>
@@ -2691,7 +2703,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>177</v>
       </c>
@@ -2704,7 +2716,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>191</v>
       </c>
@@ -2715,7 +2727,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2739,7 +2751,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -2752,7 +2764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2768,7 +2780,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -2782,7 +2794,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -2819,7 +2831,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2833,7 +2845,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -2875,7 +2887,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -2889,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2900,22 +2912,25 @@
         <v>15</v>
       </c>
       <c r="S26" t="s">
-        <v>62</v>
+        <v>521</v>
       </c>
       <c r="T26" t="s">
-        <v>63</v>
+        <v>523</v>
+      </c>
+      <c r="U26" t="s">
+        <v>511</v>
       </c>
       <c r="V26" t="s">
-        <v>64</v>
+        <v>522</v>
       </c>
       <c r="W26" s="5" t="s">
-        <v>65</v>
+        <v>524</v>
       </c>
       <c r="X26" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -2932,7 +2947,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -2949,7 +2964,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -2960,22 +2975,25 @@
         <v>15</v>
       </c>
       <c r="S29" t="s">
-        <v>62</v>
+        <v>521</v>
       </c>
       <c r="T29" t="s">
-        <v>63</v>
+        <v>523</v>
+      </c>
+      <c r="U29" t="s">
+        <v>511</v>
       </c>
       <c r="V29" t="s">
-        <v>64</v>
+        <v>522</v>
       </c>
       <c r="W29" s="5" t="s">
-        <v>65</v>
+        <v>524</v>
       </c>
       <c r="X29" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>153</v>
       </c>
@@ -2983,7 +3001,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>166</v>
       </c>
@@ -2994,7 +3012,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>168</v>
       </c>
@@ -3015,19 +3033,25 @@
       <c r="Q32" s="15"/>
       <c r="R32" s="15"/>
       <c r="S32" t="s">
-        <v>62</v>
+        <v>521</v>
       </c>
       <c r="T32" t="s">
-        <v>63</v>
-      </c>
-      <c r="U32" s="5" t="s">
-        <v>110</v>
+        <v>523</v>
+      </c>
+      <c r="U32" t="s">
+        <v>511</v>
       </c>
       <c r="V32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+      <c r="W32" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="X32" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -3042,7 +3066,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>281</v>
       </c>
@@ -3050,7 +3074,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>287</v>
       </c>
@@ -3064,7 +3088,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>217</v>
       </c>
@@ -3081,7 +3105,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>211</v>
       </c>
@@ -3098,7 +3122,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>347</v>
       </c>
@@ -3121,7 +3145,7 @@
       </c>
       <c r="R38" s="5"/>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>351</v>
       </c>
@@ -3129,7 +3153,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>354</v>
       </c>
@@ -3143,7 +3167,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>356</v>
       </c>
@@ -3160,7 +3184,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>361</v>
       </c>
@@ -3168,7 +3192,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>203</v>
       </c>
@@ -3203,7 +3227,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>372</v>
       </c>
@@ -3211,7 +3235,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>442</v>
       </c>
@@ -3219,7 +3243,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>443</v>
       </c>
@@ -3227,7 +3251,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>234</v>
       </c>
@@ -3235,7 +3259,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A48" s="38" t="s">
         <v>155</v>
       </c>
@@ -3274,7 +3298,7 @@
       </c>
       <c r="AE48" s="38"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>459</v>
       </c>
@@ -3330,18 +3354,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3439,7 +3463,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3486,7 +3510,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>194</v>
       </c>
@@ -3536,7 +3560,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>196</v>
       </c>
@@ -3583,7 +3607,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3599,7 +3623,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>157</v>
       </c>
@@ -3611,7 +3635,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>156</v>
       </c>
@@ -3622,7 +3646,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3644,7 +3668,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3657,7 +3681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -3673,7 +3697,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3687,7 +3711,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -3703,7 +3727,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3717,7 +3741,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -3759,7 +3783,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -3785,7 +3809,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3796,7 +3820,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -3811,7 +3835,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -3869,12 +3893,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3945,7 +3969,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3992,7 +4016,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4008,7 +4032,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>189</v>
       </c>
@@ -4039,7 +4063,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -4047,7 +4071,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -4080,20 +4104,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.28515625" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4182,7 +4206,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4230,7 +4254,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4246,7 +4270,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>217</v>
       </c>
@@ -4266,7 +4290,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>223</v>
       </c>
@@ -4285,7 +4309,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>224</v>
       </c>
@@ -4304,7 +4328,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -4312,7 +4336,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -4320,7 +4344,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>226</v>
       </c>
@@ -4337,7 +4361,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>211</v>
       </c>
@@ -4354,7 +4378,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>212</v>
       </c>
@@ -4371,7 +4395,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>228</v>
       </c>
@@ -4388,7 +4412,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>219</v>
       </c>
@@ -4399,7 +4423,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>155</v>
       </c>
@@ -4410,7 +4434,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4427,7 +4451,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>189</v>
       </c>
@@ -4456,7 +4480,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4467,7 +4491,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4481,7 +4505,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -4495,7 +4519,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -4509,7 +4533,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>170</v>
       </c>
@@ -4517,7 +4541,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>168</v>
       </c>
@@ -4547,7 +4571,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -4617,19 +4641,19 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4655,7 +4679,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4678,7 +4702,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>201</v>
       </c>
@@ -4709,16 +4733,16 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4732,7 +4756,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>154</v>
       </c>
@@ -4758,27 +4782,27 @@
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5703125" customWidth="1"/>
-    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5546875" customWidth="1"/>
+    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.140625" customWidth="1"/>
+    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.109375" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>2</v>
       </c>
@@ -4837,7 +4861,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>230</v>
       </c>
@@ -4862,7 +4886,7 @@
       <c r="R2" s="25"/>
       <c r="S2" s="25"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>232</v>
       </c>
@@ -4891,7 +4915,7 @@
       <c r="R3" s="25"/>
       <c r="S3" s="25"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>234</v>
       </c>
@@ -4916,7 +4940,7 @@
       <c r="R4" s="25"/>
       <c r="S4" s="25"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>235</v>
       </c>
@@ -4943,7 +4967,7 @@
       <c r="R5" s="25"/>
       <c r="S5" s="25"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>238</v>
       </c>
@@ -4976,7 +5000,7 @@
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>240</v>
       </c>
@@ -5001,7 +5025,7 @@
       <c r="R7" s="25"/>
       <c r="S7" s="25"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>264</v>
       </c>
@@ -5026,7 +5050,7 @@
       <c r="R8" s="25"/>
       <c r="S8" s="25"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>283</v>
       </c>
@@ -5051,7 +5075,7 @@
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>289</v>
       </c>
@@ -5078,7 +5102,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>323</v>
       </c>
@@ -5103,7 +5127,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>325</v>
       </c>
@@ -5130,7 +5154,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>326</v>
       </c>
@@ -5155,7 +5179,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>328</v>
       </c>
@@ -5180,7 +5204,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
         <v>341</v>
       </c>
@@ -5205,7 +5229,7 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>344</v>
       </c>
@@ -5230,7 +5254,7 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>462</v>
       </c>
@@ -5238,7 +5262,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>463</v>
       </c>
@@ -5246,7 +5270,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>464</v>
       </c>
@@ -5268,31 +5292,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.7109375" customWidth="1"/>
-    <col min="17" max="24" width="30.5703125" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" customWidth="1"/>
-    <col min="26" max="27" width="22.28515625" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.6640625" customWidth="1"/>
+    <col min="17" max="24" width="30.5546875" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" customWidth="1"/>
+    <col min="26" max="27" width="22.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.28515625" customWidth="1"/>
+    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5444,7 +5468,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5514,7 +5538,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>467</v>
       </c>
@@ -5584,7 +5608,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>469</v>
       </c>
@@ -5654,7 +5678,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>470</v>
       </c>
@@ -5724,7 +5748,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>473</v>
       </c>
@@ -5794,7 +5818,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>477</v>
       </c>
@@ -5864,7 +5888,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>482</v>
       </c>
@@ -5905,7 +5929,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>483</v>
       </c>
@@ -5946,7 +5970,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>475</v>
       </c>
@@ -6016,7 +6040,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>415</v>
       </c>
@@ -6077,7 +6101,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>299</v>
       </c>
@@ -6136,7 +6160,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>368</v>
       </c>
@@ -6182,7 +6206,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6205,7 +6229,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>302</v>
       </c>
@@ -6228,7 +6252,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>157</v>
       </c>
@@ -6247,7 +6271,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>156</v>
       </c>
@@ -6258,7 +6282,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6280,7 +6304,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>375</v>
       </c>
@@ -6293,7 +6317,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>377</v>
       </c>
@@ -6306,7 +6330,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>379</v>
       </c>
@@ -6319,7 +6343,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>384</v>
       </c>
@@ -6332,7 +6356,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>406</v>
       </c>
@@ -6345,7 +6369,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>385</v>
       </c>
@@ -6358,7 +6382,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>387</v>
       </c>
@@ -6374,7 +6398,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>389</v>
       </c>
@@ -6390,7 +6414,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>410</v>
       </c>
@@ -6409,7 +6433,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>414</v>
       </c>
@@ -6428,7 +6452,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>391</v>
       </c>
@@ -6444,7 +6468,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>394</v>
       </c>
@@ -6460,7 +6484,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>420</v>
       </c>
@@ -6476,7 +6500,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>421</v>
       </c>
@@ -6492,7 +6516,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>395</v>
       </c>
@@ -6508,7 +6532,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>398</v>
       </c>
@@ -6521,7 +6545,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>412</v>
       </c>
@@ -6534,7 +6558,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>399</v>
       </c>
@@ -6547,7 +6571,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>433</v>
       </c>
@@ -6560,7 +6584,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>407</v>
       </c>
@@ -6573,7 +6597,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>403</v>
       </c>
@@ -6589,7 +6613,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>432</v>
       </c>
@@ -6605,7 +6629,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>404</v>
       </c>
@@ -6621,7 +6645,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>411</v>
       </c>
@@ -6634,7 +6658,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>424</v>
       </c>
@@ -6656,7 +6680,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>226</v>
       </c>
@@ -6674,7 +6698,7 @@
       <c r="AI44" s="30"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>423</v>
       </c>
@@ -6687,7 +6711,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>219</v>
       </c>
@@ -6707,7 +6731,7 @@
       <c r="AI46" s="30"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>178</v>
       </c>
@@ -6726,7 +6750,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>177</v>
       </c>
@@ -6739,7 +6763,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>191</v>
       </c>
@@ -6750,7 +6774,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -6763,7 +6787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -6786,7 +6810,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -6800,7 +6824,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -6837,7 +6861,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -6851,7 +6875,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -6893,7 +6917,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -6919,7 +6943,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -6943,7 +6967,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -6967,7 +6991,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>120</v>
       </c>
@@ -6993,7 +7017,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>168</v>
       </c>
@@ -7025,7 +7049,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>287</v>
       </c>
@@ -7039,7 +7063,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>382</v>
       </c>
@@ -7053,7 +7077,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>217</v>
       </c>
@@ -7070,7 +7094,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>211</v>
       </c>
@@ -7087,7 +7111,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>347</v>
       </c>
@@ -7109,7 +7133,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>351</v>
       </c>
@@ -7117,7 +7141,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>354</v>
       </c>
@@ -7128,7 +7152,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>356</v>
       </c>
@@ -7145,7 +7169,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>361</v>
       </c>
@@ -7153,7 +7177,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>203</v>
       </c>
@@ -7188,7 +7212,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>372</v>
       </c>
@@ -7279,36 +7303,36 @@
       <selection activeCell="AQ3" sqref="AQ3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7445,7 +7469,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7496,7 +7520,7 @@
       <c r="AB2" s="11"/>
       <c r="AC2" s="12"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -7515,7 +7539,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>250</v>
       </c>
@@ -7528,7 +7552,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -7557,7 +7581,7 @@
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -7606,7 +7630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -7673,7 +7697,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -7731,7 +7755,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -7792,7 +7816,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -7800,7 +7824,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -7817,7 +7841,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -7862,7 +7886,7 @@
       </c>
       <c r="AK12" s="5"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>114</v>
       </c>
@@ -7889,7 +7913,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>251</v>
       </c>
@@ -7906,7 +7930,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -7925,7 +7949,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -7939,7 +7963,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>221</v>
       </c>
@@ -7954,7 +7978,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>156</v>
       </c>
@@ -8003,13 +8027,13 @@
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8086,7 +8110,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -8116,25 +8140,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8235,7 +8259,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -8321,7 +8345,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -8353,7 +8377,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -8379,25 +8403,25 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8483,7 +8507,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -8530,7 +8554,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -8546,7 +8570,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -8565,7 +8589,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>180</v>
       </c>
@@ -8578,7 +8602,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>181</v>
       </c>
@@ -8591,7 +8615,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -8602,7 +8626,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>157</v>
       </c>
@@ -8610,7 +8634,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>156</v>
       </c>
@@ -8618,7 +8642,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>170</v>
       </c>
@@ -8626,7 +8650,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>174</v>
       </c>
@@ -8645,7 +8669,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>172</v>
       </c>
@@ -8656,7 +8680,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -8671,7 +8695,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -8687,7 +8711,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -8714,7 +8738,7 @@
       </c>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -8728,7 +8752,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -8744,7 +8768,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>203</v>
       </c>
@@ -8781,7 +8805,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>243</v>
       </c>
@@ -8789,7 +8813,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>189</v>
       </c>
@@ -8812,7 +8836,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -8869,17 +8893,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>2</v>
       </c>
@@ -8914,7 +8938,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>245</v>
       </c>
@@ -8923,7 +8947,7 @@
       </c>
       <c r="C2" s="25"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>247</v>
       </c>
@@ -8932,7 +8956,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>249</v>
       </c>
@@ -8941,7 +8965,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>317</v>
       </c>
@@ -8959,24 +8983,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ACADB97-3AA8-40BF-AE7E-787123A27C76}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9044,7 +9068,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9088,7 +9112,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9104,7 +9128,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>184</v>
       </c>
@@ -9122,7 +9146,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -9130,7 +9154,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -9138,7 +9162,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>208</v>
       </c>
@@ -9177,37 +9201,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9290,7 +9314,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9331,7 +9355,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9347,7 +9371,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>157</v>
       </c>
@@ -9359,7 +9383,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -9377,7 +9401,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -9386,7 +9410,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -9398,7 +9422,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -9424,7 +9448,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -9435,7 +9459,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -9449,7 +9473,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
HYF_EMEA : TEST_DGLD_HF_EMEA_RT_024_WebPageLinkValidation(updated testdata and added new tetscase for hydroflask emea)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E9EF60-D768-48E4-B00F-91AC1282F455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC60778-F708-48A5-A976-57D469A8E943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1472,147 +1472,148 @@
     <t>rgaddam@helenoftroy.com</t>
   </si>
   <si>
-    <t>https://mcloud-na-preprod.hydroflask.com/customer/account/login/referer/aHR0cHM6Ly9tY2xvdWQtbmEtcHJlcHJvZC5oeWRyb2ZsYXNrLmNvbS9jdXN0b21lci9hY2NvdW50L2luZGV4Lw~~/
+    <t>AccountDetails_TC6</t>
+  </si>
+  <si>
+    <t>AccountDetails_TC12</t>
+  </si>
+  <si>
+    <t>hydroflaskqa+E2E1@gmail.com</t>
+  </si>
+  <si>
+    <t>hydroflaskqa+E2E2@gmail.com</t>
+  </si>
+  <si>
+    <t>hydroflaskqa+E2E4@gmail.com</t>
+  </si>
+  <si>
+    <t>hydroflaskqa+E2E7@gmail.com</t>
+  </si>
+  <si>
+    <t>hydroflaskqa+E2E9@gmail.com</t>
+  </si>
+  <si>
+    <t>hydroflaskqa+E2E6@gmail.com</t>
+  </si>
+  <si>
+    <t>hydroflaskqa+E2E12@gmail.com</t>
+  </si>
+  <si>
+    <t>hydroflaskqa+E2E16@gmail.com</t>
+  </si>
+  <si>
+    <t>qatester+Automation@gmail.com</t>
+  </si>
+  <si>
+    <t>gaddamramyasree0809+automation@gmail.com</t>
+  </si>
+  <si>
+    <t>Refill For Good,Corporate Responsibility</t>
+  </si>
+  <si>
+    <t>24 oz,32 oz</t>
+  </si>
+  <si>
+    <t>Bottles,Cups &amp; Tumblers,Coffee &amp; Tea,Accessories</t>
+  </si>
+  <si>
+    <t>Insulated Totes,Soft Coolers</t>
+  </si>
+  <si>
+    <t>Food Jars</t>
+  </si>
+  <si>
+    <t>Bottle Boots,Caps and Lids,Cleaning</t>
+  </si>
+  <si>
+    <t>Our Story,Contact,Refill For Good,Every Bottle Tells A Story</t>
+  </si>
+  <si>
+    <t>Micro Hydro,Spring Style Guide,Fitness Collection</t>
+  </si>
+  <si>
+    <t>Exclusives,New Arrivals,Best Sellers</t>
+  </si>
+  <si>
+    <t>HFEMEA20OFF</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>93 York House</t>
+  </si>
+  <si>
+    <t>Bradford</t>
+  </si>
+  <si>
+    <t>West Yorkshire</t>
+  </si>
+  <si>
+    <t>BD109ET</t>
+  </si>
+  <si>
+    <t>71 Worthy Street</t>
+  </si>
+  <si>
+    <t>Chorley</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>PR60NH</t>
+  </si>
+  <si>
+    <t>oxobuyer@oxo.com</t>
+  </si>
+  <si>
+    <t>oxobuyer123</t>
+  </si>
+  <si>
+    <t>Contact Us,Find a Store,Track Your Order</t>
+  </si>
+  <si>
+    <t>Our Story,Group Customization,Pro Deal</t>
+  </si>
+  <si>
+    <t>Track Your Order</t>
+  </si>
+  <si>
+    <t>Micro Hydro Mini Bottle</t>
+  </si>
+  <si>
+    <t>£</t>
+  </si>
+  <si>
+    <t>hfemealotus@gmail.com</t>
+  </si>
+  <si>
+    <t>93/5 Morrison Street</t>
+  </si>
+  <si>
+    <t>Edinburgh</t>
+  </si>
+  <si>
+    <t>Midlothian</t>
+  </si>
+  <si>
+    <t>EH3 8BX</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage4.hydroflask.com/gb/customer/account/login/referer/aHR0cHM6Ly9tY2xvdWQtbmEtc3RhZ2U0Lmh5ZHJvZmxhc2suY29tL2diL2N1c3RvbWVyL2FjY291bnQvaW5kZXgv/
 https://mcloud-na-preprod.hydroflask.com/customer/account/create/
-https://mcloud-na-preprod.hydroflask.com/shop/bottles-drinkware/bottles
-https://mcloud-na-preprod.hydroflask.com/corporate-responsibility
-https://mcloud-na-preprod.hydroflask.com/parks-for-all
-https://mcloud-na-preprod.hydroflask.com/shop/customize
-https://mcloud-na-preprod.hydroflask.com/our-story
-https://mcloud-na-preprod.hydroflask.com/house-of-hydro-rewards
-https://mcloud-na-preprod.hydroflask.com/32-oz-wide-mouth?color=Fir
-https://mcloud-na-preprod.hydroflask.com/26-l-day-escape-tote?color=Peppercorn
-https://mcloud-na-preprod.hydroflask.com/contact-us
-https://mcloud-na-preprod.hydroflask.com/prodeal/application/index/</t>
-  </si>
-  <si>
-    <t>AccountDetails_TC6</t>
-  </si>
-  <si>
-    <t>AccountDetails_TC12</t>
-  </si>
-  <si>
-    <t>hydroflaskqa+E2E1@gmail.com</t>
-  </si>
-  <si>
-    <t>hydroflaskqa+E2E2@gmail.com</t>
-  </si>
-  <si>
-    <t>hydroflaskqa+E2E4@gmail.com</t>
-  </si>
-  <si>
-    <t>hydroflaskqa+E2E7@gmail.com</t>
-  </si>
-  <si>
-    <t>hydroflaskqa+E2E9@gmail.com</t>
-  </si>
-  <si>
-    <t>hydroflaskqa+E2E6@gmail.com</t>
-  </si>
-  <si>
-    <t>hydroflaskqa+E2E12@gmail.com</t>
-  </si>
-  <si>
-    <t>hydroflaskqa+E2E16@gmail.com</t>
-  </si>
-  <si>
-    <t>qatester+Automation@gmail.com</t>
-  </si>
-  <si>
-    <t>gaddamramyasree0809+automation@gmail.com</t>
-  </si>
-  <si>
-    <t>Refill For Good,Corporate Responsibility</t>
-  </si>
-  <si>
-    <t>24 oz,32 oz</t>
-  </si>
-  <si>
-    <t>Bottles,Cups &amp; Tumblers,Coffee &amp; Tea,Accessories</t>
-  </si>
-  <si>
-    <t>Insulated Totes,Soft Coolers</t>
-  </si>
-  <si>
-    <t>Food Jars</t>
-  </si>
-  <si>
-    <t>Bottle Boots,Caps and Lids,Cleaning</t>
-  </si>
-  <si>
-    <t>Our Story,Contact,Refill For Good,Every Bottle Tells A Story</t>
-  </si>
-  <si>
-    <t>Micro Hydro,Spring Style Guide,Fitness Collection</t>
-  </si>
-  <si>
-    <t>Exclusives,New Arrivals,Best Sellers</t>
-  </si>
-  <si>
-    <t>HFEMEA20OFF</t>
-  </si>
-  <si>
-    <t>Delivery</t>
-  </si>
-  <si>
-    <t>93 York House</t>
-  </si>
-  <si>
-    <t>Bradford</t>
-  </si>
-  <si>
-    <t>West Yorkshire</t>
-  </si>
-  <si>
-    <t>BD109ET</t>
-  </si>
-  <si>
-    <t>71 Worthy Street</t>
-  </si>
-  <si>
-    <t>Chorley</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>PR60NH</t>
-  </si>
-  <si>
-    <t>oxobuyer@oxo.com</t>
-  </si>
-  <si>
-    <t>oxobuyer123</t>
-  </si>
-  <si>
-    <t>Contact Us,Find a Store,Track Your Order</t>
-  </si>
-  <si>
-    <t>Our Story,Group Customization,Pro Deal</t>
-  </si>
-  <si>
-    <t>Track Your Order</t>
-  </si>
-  <si>
-    <t>Micro Hydro Mini Bottle</t>
-  </si>
-  <si>
-    <t>£</t>
-  </si>
-  <si>
-    <t>hfemealotus@gmail.com</t>
-  </si>
-  <si>
-    <t>93/5 Morrison Street</t>
-  </si>
-  <si>
-    <t>Edinburgh</t>
-  </si>
-  <si>
-    <t>Midlothian</t>
-  </si>
-  <si>
-    <t>EH3 8BX</t>
+https://mcloud-na-stage4.hydroflask.com/gb/shop/bottles-drinkware/bottles?page=1
+https://mcloud-na-stage4.hydroflask.com/gb/corporate-responsibility
+https://mcloud-na-stage4.hydroflask.com/parks-for-all
+https://mcloud-na-stage4.hydroflask.com/shop/customize
+https://mcloud-na-stage4.hydroflask.com/our-story
+https://mcloud-na-stage4.hydroflask.com/house-of-hydro-rewards
+https://mcloud-na-stage4.hydroflask.com/32-oz-wide-mouth?color=Fir
+https://mcloud-na-stage4.hydroflask.com/26-l-day-escape-tote?color=Peppercorn
+https://mcloud-na-stage4.hydroflask.com/contact-us
+https://mcloud-na-stage4.hydroflask.com/prodeal/application/index/
+HYF_EMEA : TEST_DGLD_HF_EMEA_RT_021_Create_and_Edit_Gift_Registery_For_Register_User(testcase added and updated the testdata)</t>
   </si>
 </sst>
 </file>
@@ -2321,10 +2322,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -2339,10 +2340,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -2354,16 +2355,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" t="s">
+        <v>497</v>
+      </c>
+      <c r="T2" t="s">
         <v>498</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>499</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" s="5" t="s">
         <v>500</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>501</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>59</v>
@@ -2376,10 +2377,10 @@
         <v>295</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2394,7 +2395,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -2407,16 +2408,16 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" t="s">
+        <v>497</v>
+      </c>
+      <c r="T3" t="s">
         <v>498</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>499</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" s="5" t="s">
         <v>500</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>501</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>59</v>
@@ -2502,16 +2503,16 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" t="s">
+        <v>497</v>
+      </c>
+      <c r="T5" t="s">
         <v>498</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
         <v>499</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" s="5" t="s">
         <v>500</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>501</v>
       </c>
       <c r="X5" s="5" t="s">
         <v>59</v>
@@ -2580,7 +2581,7 @@
         <v>154</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="W10" s="3"/>
       <c r="X10" s="4"/>
@@ -2752,7 +2753,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="AI20" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="AJ20" t="s">
         <v>264</v>
@@ -2890,19 +2891,19 @@
         <v>15</v>
       </c>
       <c r="S26" t="s">
+        <v>513</v>
+      </c>
+      <c r="T26" t="s">
+        <v>515</v>
+      </c>
+      <c r="U26" t="s">
+        <v>503</v>
+      </c>
+      <c r="V26" t="s">
         <v>514</v>
       </c>
-      <c r="T26" t="s">
+      <c r="W26" s="5" t="s">
         <v>516</v>
-      </c>
-      <c r="U26" t="s">
-        <v>504</v>
-      </c>
-      <c r="V26" t="s">
-        <v>515</v>
-      </c>
-      <c r="W26" s="5" t="s">
-        <v>517</v>
       </c>
       <c r="X26" s="5" t="s">
         <v>59</v>
@@ -2930,11 +2931,11 @@
         <v>77</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I28" s="2"/>
       <c r="W28" s="5"/>
@@ -2953,19 +2954,19 @@
         <v>15</v>
       </c>
       <c r="S29" t="s">
+        <v>513</v>
+      </c>
+      <c r="T29" t="s">
+        <v>515</v>
+      </c>
+      <c r="U29" t="s">
+        <v>503</v>
+      </c>
+      <c r="V29" t="s">
         <v>514</v>
       </c>
-      <c r="T29" t="s">
+      <c r="W29" s="5" t="s">
         <v>516</v>
-      </c>
-      <c r="U29" t="s">
-        <v>504</v>
-      </c>
-      <c r="V29" t="s">
-        <v>515</v>
-      </c>
-      <c r="W29" s="5" t="s">
-        <v>517</v>
       </c>
       <c r="X29" s="5" t="s">
         <v>59</v>
@@ -3011,19 +3012,19 @@
       <c r="Q32" s="12"/>
       <c r="R32" s="12"/>
       <c r="S32" t="s">
+        <v>513</v>
+      </c>
+      <c r="T32" t="s">
+        <v>515</v>
+      </c>
+      <c r="U32" t="s">
+        <v>503</v>
+      </c>
+      <c r="V32" t="s">
         <v>514</v>
       </c>
-      <c r="T32" t="s">
+      <c r="W32" s="5" t="s">
         <v>516</v>
-      </c>
-      <c r="U32" t="s">
-        <v>504</v>
-      </c>
-      <c r="V32" t="s">
-        <v>515</v>
-      </c>
-      <c r="W32" s="5" t="s">
-        <v>517</v>
       </c>
       <c r="X32" s="5" t="s">
         <v>59</v>
@@ -3446,10 +3447,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -3464,10 +3465,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -3493,10 +3494,10 @@
         <v>192</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>29</v>
@@ -3511,10 +3512,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s">
@@ -3543,10 +3544,10 @@
         <v>194</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -3561,10 +3562,10 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" t="s">
@@ -3727,7 +3728,7 @@
         <v>50</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I14" s="2"/>
       <c r="K14" t="s">
@@ -3952,10 +3953,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -3970,10 +3971,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -4015,10 +4016,10 @@
         <v>187</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -4189,10 +4190,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -4207,10 +4208,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -4662,10 +4663,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -4707,8 +4708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F808DC-2462-40F4-8FE6-41754E94FF50}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4739,7 +4740,7 @@
         <v>152</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>474</v>
+        <v>517</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>261</v>
@@ -4844,7 +4845,7 @@
         <v>228</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -4874,7 +4875,7 @@
         <v>265</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>276</v>
@@ -4905,7 +4906,7 @@
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
@@ -4933,7 +4934,7 @@
       <c r="H5" s="22"/>
       <c r="I5" s="32"/>
       <c r="J5" s="22" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
@@ -4994,7 +4995,7 @@
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
       <c r="M7" s="30" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="N7" s="22"/>
       <c r="O7" s="22"/>
@@ -5036,7 +5037,7 @@
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
@@ -5115,7 +5116,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
       <c r="G12" s="37" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H12" s="30" t="s">
         <v>472</v>
@@ -5188,7 +5189,7 @@
       </c>
       <c r="B15" s="22"/>
       <c r="C15" s="22" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -5521,7 +5522,7 @@
         <v>460</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>274</v>
@@ -5591,7 +5592,7 @@
         <v>462</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>274</v>
@@ -5661,7 +5662,7 @@
         <v>463</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>274</v>
@@ -5731,7 +5732,7 @@
         <v>466</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>274</v>
@@ -5801,7 +5802,7 @@
         <v>470</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>274</v>
@@ -5868,10 +5869,10 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -5909,10 +5910,10 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
@@ -5953,7 +5954,7 @@
         <v>468</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>274</v>
@@ -7277,7 +7278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AS18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -7479,16 +7480,16 @@
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="O2" s="22" t="s">
         <v>514</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="P2" s="22" t="s">
         <v>516</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>517</v>
       </c>
       <c r="Q2" s="22">
         <v>9898989898</v>
@@ -7649,7 +7650,7 @@
         <v>333</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K5" s="31"/>
       <c r="L5" s="22"/>
@@ -7720,21 +7721,21 @@
         <v>67</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K6" s="31"/>
       <c r="L6" s="22"/>
       <c r="M6" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="O6" s="22" t="s">
         <v>514</v>
       </c>
-      <c r="N6" s="22" t="s">
+      <c r="P6" s="22" t="s">
         <v>516</v>
-      </c>
-      <c r="O6" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>517</v>
       </c>
       <c r="Q6" s="22">
         <v>9898989898</v>
@@ -7779,7 +7780,7 @@
         <v>81</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="22"/>
@@ -7793,23 +7794,23 @@
         <v>96</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K7" s="31"/>
       <c r="L7" s="22" t="s">
         <v>81</v>
       </c>
       <c r="M7" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="O7" s="22" t="s">
         <v>514</v>
       </c>
-      <c r="N7" s="22" t="s">
+      <c r="P7" s="22" t="s">
         <v>516</v>
-      </c>
-      <c r="O7" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="P7" s="22" t="s">
-        <v>517</v>
       </c>
       <c r="Q7" s="22">
         <v>9898989898</v>
@@ -7868,7 +7869,7 @@
         <v>100</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="22"/>
@@ -7882,23 +7883,23 @@
         <v>96</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K8" s="31"/>
       <c r="L8" s="22" t="s">
         <v>100</v>
       </c>
       <c r="M8" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="O8" s="22" t="s">
         <v>514</v>
       </c>
-      <c r="N8" s="22" t="s">
+      <c r="P8" s="22" t="s">
         <v>516</v>
-      </c>
-      <c r="O8" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="P8" s="22" t="s">
-        <v>517</v>
       </c>
       <c r="Q8" s="22">
         <v>9898989898</v>
@@ -7951,7 +7952,7 @@
         <v>95</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="22"/>
@@ -7965,23 +7966,23 @@
         <v>96</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K9" s="31"/>
       <c r="L9" s="22" t="s">
         <v>95</v>
       </c>
       <c r="M9" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="O9" s="22" t="s">
         <v>514</v>
       </c>
-      <c r="N9" s="22" t="s">
+      <c r="P9" s="22" t="s">
         <v>516</v>
-      </c>
-      <c r="O9" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="P9" s="22" t="s">
-        <v>517</v>
       </c>
       <c r="Q9" s="22">
         <v>9898989898</v>
@@ -8156,23 +8157,23 @@
         <v>67</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="O12" s="22" t="s">
         <v>514</v>
       </c>
-      <c r="N12" s="22" t="s">
+      <c r="P12" s="22" t="s">
         <v>516</v>
-      </c>
-      <c r="O12" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="P12" s="22" t="s">
-        <v>517</v>
       </c>
       <c r="Q12" s="22">
         <v>9898989898</v>
@@ -8231,7 +8232,7 @@
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K13" s="31"/>
       <c r="L13" s="22"/>
@@ -8459,7 +8460,7 @@
       </c>
       <c r="I17" s="22"/>
       <c r="J17" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K17" s="31"/>
       <c r="L17" s="22"/>
@@ -9101,16 +9102,16 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
+        <v>497</v>
+      </c>
+      <c r="L2" t="s">
         <v>498</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>499</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" s="5" t="s">
         <v>500</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>501</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>59</v>
@@ -9203,7 +9204,7 @@
         <v>154</v>
       </c>
       <c r="J9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
@@ -9249,11 +9250,11 @@
         <v>77</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I13" s="2"/>
       <c r="O13" s="5"/>
@@ -9269,7 +9270,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="Y14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Z14" t="s">
         <v>264</v>
@@ -9286,16 +9287,16 @@
         <v>15</v>
       </c>
       <c r="K15" t="s">
+        <v>501</v>
+      </c>
+      <c r="L15" t="s">
         <v>502</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>503</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>504</v>
-      </c>
-      <c r="N15" t="s">
-        <v>505</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>59</v>
@@ -9507,7 +9508,7 @@
         <v>243</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C2" s="22"/>
     </row>
@@ -9517,7 +9518,7 @@
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
@@ -9526,7 +9527,7 @@
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
@@ -9535,7 +9536,7 @@
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="22" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -9637,10 +9638,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -9655,7 +9656,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" t="s">
@@ -9698,16 +9699,16 @@
       </c>
       <c r="H4" s="2"/>
       <c r="S4" t="s">
+        <v>510</v>
+      </c>
+      <c r="T4" t="s">
+        <v>510</v>
+      </c>
+      <c r="U4" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="T4" t="s">
-        <v>511</v>
-      </c>
-      <c r="U4" s="5" t="s">
+      <c r="V4" s="12" t="s">
         <v>512</v>
-      </c>
-      <c r="V4" s="12" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -9731,16 +9732,16 @@
         <v>206</v>
       </c>
       <c r="S7" t="s">
+        <v>510</v>
+      </c>
+      <c r="T7" t="s">
+        <v>510</v>
+      </c>
+      <c r="U7" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="T7" t="s">
-        <v>511</v>
-      </c>
-      <c r="U7" s="5" t="s">
+      <c r="V7" s="12" t="s">
         <v>512</v>
-      </c>
-      <c r="V7" s="12" t="s">
-        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -9881,7 +9882,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>29</v>
@@ -9896,7 +9897,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" t="s">

</xml_diff>

<commit_message>
HYF_EMEA : TEST_DGLD_HF_EMEA_RT_028,Test_DGLD_HF_EMEA_RT_031(added and updated new testcases & testdata for hydro emea)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC60778-F708-48A5-A976-57D469A8E943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E139A9-6DFA-417F-A2B1-2AA08BDFC67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1612,8 +1612,7 @@
 https://mcloud-na-stage4.hydroflask.com/32-oz-wide-mouth?color=Fir
 https://mcloud-na-stage4.hydroflask.com/26-l-day-escape-tote?color=Peppercorn
 https://mcloud-na-stage4.hydroflask.com/contact-us
-https://mcloud-na-stage4.hydroflask.com/prodeal/application/index/
-HYF_EMEA : TEST_DGLD_HF_EMEA_RT_021_Create_and_Edit_Gift_Registery_For_Register_User(testcase added and updated the testdata)</t>
+https://mcloud-na-stage4.hydroflask.com/prodeal/application/index/</t>
   </si>
 </sst>
 </file>
@@ -1621,8 +1620,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1803,7 +1802,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1833,7 +1832,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>

</xml_diff>

<commit_message>
HF_EMEA testcases 46 Changes with testdata Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E139A9-6DFA-417F-A2B1-2AA08BDFC67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF917B49-164D-4A82-8DF5-39F5B72F040B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1115,9 +1115,6 @@
     <t>Full_RedeemGiftcard</t>
   </si>
   <si>
-    <t>8ZZ85J64V9773K56R72Z</t>
-  </si>
-  <si>
     <t>GiftCard2</t>
   </si>
   <si>
@@ -1350,9 +1347,6 @@
   </si>
   <si>
     <t>QaLotus</t>
-  </si>
-  <si>
-    <t>3BR58M97G4985P29A74E</t>
   </si>
   <si>
     <t>Giftcard_Partial_1</t>
@@ -1614,14 +1608,20 @@
 https://mcloud-na-stage4.hydroflask.com/contact-us
 https://mcloud-na-stage4.hydroflask.com/prodeal/application/index/</t>
   </si>
+  <si>
+    <t>8DZ67T85R4856M74K23D</t>
+  </si>
+  <si>
+    <t>4SX89R79W7673P94T66S</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1802,7 +1802,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1832,7 +1832,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2146,8 +2146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU49"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D13"/>
+    <sheetView tabSelected="1" topLeftCell="N29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2205,13 +2205,13 @@
         <v>24</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>348</v>
@@ -2223,7 +2223,7 @@
         <v>343</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>345</v>
@@ -2310,10 +2310,10 @@
         <v>207</v>
       </c>
       <c r="AT1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="AU1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.3">
@@ -2321,10 +2321,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -2339,10 +2339,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -2354,16 +2354,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" t="s">
+        <v>495</v>
+      </c>
+      <c r="T2" t="s">
+        <v>496</v>
+      </c>
+      <c r="V2" t="s">
         <v>497</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" s="5" t="s">
         <v>498</v>
-      </c>
-      <c r="V2" t="s">
-        <v>499</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>500</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>59</v>
@@ -2376,10 +2376,10 @@
         <v>295</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2394,7 +2394,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -2407,16 +2407,16 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" t="s">
+        <v>495</v>
+      </c>
+      <c r="T3" t="s">
+        <v>496</v>
+      </c>
+      <c r="V3" t="s">
         <v>497</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3" s="5" t="s">
         <v>498</v>
-      </c>
-      <c r="V3" t="s">
-        <v>499</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>500</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>59</v>
@@ -2426,7 +2426,7 @@
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>296</v>
@@ -2466,13 +2466,13 @@
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -2487,10 +2487,10 @@
         <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2502,16 +2502,16 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" t="s">
+        <v>495</v>
+      </c>
+      <c r="T5" t="s">
+        <v>496</v>
+      </c>
+      <c r="V5" t="s">
         <v>497</v>
       </c>
-      <c r="T5" t="s">
+      <c r="W5" s="5" t="s">
         <v>498</v>
-      </c>
-      <c r="V5" t="s">
-        <v>499</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>500</v>
       </c>
       <c r="X5" s="5" t="s">
         <v>59</v>
@@ -2529,7 +2529,7 @@
         <v>23</v>
       </c>
       <c r="AA6" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AB6">
         <v>123</v>
@@ -2580,7 +2580,7 @@
         <v>154</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="W10" s="3"/>
       <c r="X10" s="4"/>
@@ -2636,7 +2636,7 @@
         <v>327</v>
       </c>
       <c r="AF13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AG13" t="s">
         <v>190</v>
@@ -2645,21 +2645,21 @@
         <v>1</v>
       </c>
       <c r="AU13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="AC14" s="36" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="AD14" s="34"/>
       <c r="AE14" s="36" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.3">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="I18" s="2"/>
       <c r="AL18" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.3">
@@ -2752,7 +2752,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="AI20" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="AJ20" t="s">
         <v>264</v>
@@ -2766,7 +2766,7 @@
         <v>45</v>
       </c>
       <c r="AA21" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AB21">
         <v>123</v>
@@ -2803,7 +2803,7 @@
         <v>47</v>
       </c>
       <c r="AA22" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AB22">
         <v>1234</v>
@@ -2817,7 +2817,7 @@
         <v>49</v>
       </c>
       <c r="AA23" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AB23">
         <v>123</v>
@@ -2856,7 +2856,7 @@
         <v>23</v>
       </c>
       <c r="AA24" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AB24">
         <v>123</v>
@@ -2890,19 +2890,19 @@
         <v>15</v>
       </c>
       <c r="S26" t="s">
+        <v>511</v>
+      </c>
+      <c r="T26" t="s">
         <v>513</v>
       </c>
-      <c r="T26" t="s">
-        <v>515</v>
-      </c>
       <c r="U26" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="V26" t="s">
+        <v>512</v>
+      </c>
+      <c r="W26" s="5" t="s">
         <v>514</v>
-      </c>
-      <c r="W26" s="5" t="s">
-        <v>516</v>
       </c>
       <c r="X26" s="5" t="s">
         <v>59</v>
@@ -2919,10 +2919,10 @@
         <v>331</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.3">
@@ -2930,11 +2930,11 @@
         <v>77</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I28" s="2"/>
       <c r="W28" s="5"/>
@@ -2953,19 +2953,19 @@
         <v>15</v>
       </c>
       <c r="S29" t="s">
+        <v>511</v>
+      </c>
+      <c r="T29" t="s">
         <v>513</v>
       </c>
-      <c r="T29" t="s">
-        <v>515</v>
-      </c>
       <c r="U29" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="V29" t="s">
+        <v>512</v>
+      </c>
+      <c r="W29" s="5" t="s">
         <v>514</v>
-      </c>
-      <c r="W29" s="5" t="s">
-        <v>516</v>
       </c>
       <c r="X29" s="5" t="s">
         <v>59</v>
@@ -2976,7 +2976,7 @@
         <v>151</v>
       </c>
       <c r="AL30" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.3">
@@ -3011,19 +3011,19 @@
       <c r="Q32" s="12"/>
       <c r="R32" s="12"/>
       <c r="S32" t="s">
+        <v>511</v>
+      </c>
+      <c r="T32" t="s">
         <v>513</v>
       </c>
-      <c r="T32" t="s">
-        <v>515</v>
-      </c>
       <c r="U32" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="V32" t="s">
+        <v>512</v>
+      </c>
+      <c r="W32" s="5" t="s">
         <v>514</v>
-      </c>
-      <c r="W32" s="5" t="s">
-        <v>516</v>
       </c>
       <c r="X32" s="5" t="s">
         <v>59</v>
@@ -3105,10 +3105,10 @@
         <v>340</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
@@ -3116,10 +3116,10 @@
         <v>342</v>
       </c>
       <c r="P38" s="28" t="s">
-        <v>434</v>
+        <v>516</v>
       </c>
       <c r="Q38" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="R38" s="5"/>
     </row>
@@ -3136,10 +3136,10 @@
         <v>347</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="N40" s="26" t="s">
         <v>353</v>
@@ -3167,7 +3167,7 @@
         <v>354</v>
       </c>
       <c r="P42" t="s">
-        <v>355</v>
+        <v>517</v>
       </c>
     </row>
     <row r="43" spans="1:46" x14ac:dyDescent="0.3">
@@ -3207,26 +3207,26 @@
     </row>
     <row r="44" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>364</v>
+      </c>
+      <c r="P44" s="5" t="s">
         <v>365</v>
-      </c>
-      <c r="P44" s="5" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="45" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>433</v>
+      </c>
+      <c r="P45" s="29" t="s">
         <v>435</v>
-      </c>
-      <c r="P45" s="29" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="46" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>434</v>
+      </c>
+      <c r="P46" s="28" t="s">
         <v>436</v>
-      </c>
-      <c r="P46" s="28" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="47" spans="1:46" x14ac:dyDescent="0.3">
@@ -3278,10 +3278,10 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="P49" s="28" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -3446,10 +3446,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -3464,10 +3464,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -3493,10 +3493,10 @@
         <v>192</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>29</v>
@@ -3511,10 +3511,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s">
@@ -3543,10 +3543,10 @@
         <v>194</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -3561,10 +3561,10 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" t="s">
@@ -3727,7 +3727,7 @@
         <v>50</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I14" s="2"/>
       <c r="K14" t="s">
@@ -3952,10 +3952,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -3970,10 +3970,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -4015,10 +4015,10 @@
         <v>187</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -4189,10 +4189,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -4207,10 +4207,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -4524,7 +4524,7 @@
         <v>166</v>
       </c>
       <c r="F22" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>277</v>
@@ -4662,10 +4662,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -4707,7 +4707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F808DC-2462-40F4-8FE6-41754E94FF50}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4739,7 +4739,7 @@
         <v>152</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>261</v>
@@ -4803,7 +4803,7 @@
         <v>317</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I1" s="21" t="s">
         <v>232</v>
@@ -4824,7 +4824,7 @@
         <v>253</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P1" s="21" t="s">
         <v>254</v>
@@ -4836,7 +4836,7 @@
         <v>286</v>
       </c>
       <c r="S1" s="39" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -4844,7 +4844,7 @@
         <v>228</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -4874,7 +4874,7 @@
         <v>265</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>276</v>
@@ -4905,7 +4905,7 @@
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
@@ -4933,7 +4933,7 @@
       <c r="H5" s="22"/>
       <c r="I5" s="32"/>
       <c r="J5" s="22" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
@@ -4960,7 +4960,7 @@
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
       <c r="L6" s="21" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="M6" s="22"/>
       <c r="N6" s="21" t="s">
@@ -4994,7 +4994,7 @@
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
       <c r="M7" s="30" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="N7" s="22"/>
       <c r="O7" s="22"/>
@@ -5023,7 +5023,7 @@
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
       <c r="Q8" s="21" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
@@ -5036,7 +5036,7 @@
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
@@ -5077,7 +5077,7 @@
         <v>287</v>
       </c>
       <c r="S10" s="22" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -5115,10 +5115,10 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
       <c r="G12" s="37" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="B15" s="22"/>
       <c r="C15" s="22" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -5221,7 +5221,7 @@
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
       <c r="K16" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
@@ -5234,26 +5234,26 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C17" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C18" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="Q19" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -5314,13 +5314,13 @@
         <v>218</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>144</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>188</v>
@@ -5347,10 +5347,10 @@
         <v>24</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>348</v>
@@ -5362,7 +5362,7 @@
         <v>343</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>345</v>
@@ -5464,20 +5464,20 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" t="s">
+        <v>418</v>
+      </c>
+      <c r="H2" t="s">
         <v>419</v>
-      </c>
-      <c r="H2" t="s">
-        <v>420</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" t="s">
+        <v>426</v>
+      </c>
+      <c r="N2" t="s">
         <v>427</v>
-      </c>
-      <c r="N2" t="s">
-        <v>428</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>270</v>
@@ -5486,7 +5486,7 @@
         <v>274</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -5518,10 +5518,10 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>274</v>
@@ -5534,29 +5534,29 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" t="s">
+        <v>418</v>
+      </c>
+      <c r="H3" t="s">
         <v>419</v>
-      </c>
-      <c r="H3" t="s">
-        <v>420</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" t="s">
+        <v>426</v>
+      </c>
+      <c r="N3" t="s">
         <v>427</v>
       </c>
-      <c r="N3" t="s">
-        <v>428</v>
-      </c>
       <c r="O3" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>274</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -5588,10 +5588,10 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>274</v>
@@ -5604,29 +5604,29 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" t="s">
+        <v>418</v>
+      </c>
+      <c r="H4" t="s">
         <v>419</v>
-      </c>
-      <c r="H4" t="s">
-        <v>420</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" t="s">
+        <v>426</v>
+      </c>
+      <c r="N4" t="s">
         <v>427</v>
       </c>
-      <c r="N4" t="s">
-        <v>428</v>
-      </c>
       <c r="O4" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>274</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -5658,10 +5658,10 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>274</v>
@@ -5674,29 +5674,29 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" t="s">
+        <v>418</v>
+      </c>
+      <c r="H5" t="s">
         <v>419</v>
-      </c>
-      <c r="H5" t="s">
-        <v>420</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" t="s">
+        <v>426</v>
+      </c>
+      <c r="N5" t="s">
         <v>427</v>
       </c>
-      <c r="N5" t="s">
-        <v>428</v>
-      </c>
       <c r="O5" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>274</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -5728,10 +5728,10 @@
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>274</v>
@@ -5744,29 +5744,29 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" t="s">
+        <v>418</v>
+      </c>
+      <c r="H6" t="s">
         <v>419</v>
-      </c>
-      <c r="H6" t="s">
-        <v>420</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" t="s">
+        <v>426</v>
+      </c>
+      <c r="N6" t="s">
         <v>427</v>
       </c>
-      <c r="N6" t="s">
-        <v>428</v>
-      </c>
       <c r="O6" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>274</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -5798,10 +5798,10 @@
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>274</v>
@@ -5814,29 +5814,29 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" t="s">
+        <v>418</v>
+      </c>
+      <c r="H7" t="s">
         <v>419</v>
-      </c>
-      <c r="H7" t="s">
-        <v>420</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" t="s">
+        <v>426</v>
+      </c>
+      <c r="N7" t="s">
         <v>427</v>
       </c>
-      <c r="N7" t="s">
-        <v>428</v>
-      </c>
       <c r="O7" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>274</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -5868,10 +5868,10 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -5886,10 +5886,10 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" t="s">
+        <v>426</v>
+      </c>
+      <c r="N8" t="s">
         <v>427</v>
-      </c>
-      <c r="N8" t="s">
-        <v>428</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
@@ -5909,10 +5909,10 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
@@ -5927,10 +5927,10 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" t="s">
+        <v>426</v>
+      </c>
+      <c r="N9" t="s">
         <v>427</v>
-      </c>
-      <c r="N9" t="s">
-        <v>428</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
@@ -5950,10 +5950,10 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>274</v>
@@ -5966,29 +5966,29 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" t="s">
+        <v>418</v>
+      </c>
+      <c r="H10" t="s">
         <v>419</v>
-      </c>
-      <c r="H10" t="s">
-        <v>420</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" t="s">
+        <v>426</v>
+      </c>
+      <c r="N10" t="s">
         <v>427</v>
       </c>
-      <c r="N10" t="s">
-        <v>428</v>
-      </c>
       <c r="O10" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>274</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>270</v>
@@ -6042,10 +6042,10 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" t="s">
+        <v>426</v>
+      </c>
+      <c r="N11" t="s">
         <v>427</v>
-      </c>
-      <c r="N11" t="s">
-        <v>428</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>270</v>
@@ -6062,16 +6062,16 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" t="s">
+        <v>408</v>
+      </c>
+      <c r="Z11" t="s">
         <v>409</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AB11" t="s">
         <v>410</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" s="5" t="s">
         <v>411</v>
-      </c>
-      <c r="AC11" s="5" t="s">
-        <v>412</v>
       </c>
       <c r="AD11" s="5" t="s">
         <v>59</v>
@@ -6140,7 +6140,7 @@
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>296</v>
@@ -6284,12 +6284,12 @@
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="AI19" s="27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AJ19" s="5" t="s">
         <v>113</v>
@@ -6297,12 +6297,12 @@
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="AI20" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AJ20" s="5" t="s">
         <v>113</v>
@@ -6310,12 +6310,12 @@
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="AI21" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AJ21" s="5" t="s">
         <v>113</v>
@@ -6323,12 +6323,12 @@
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="AI22" s="27" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AJ22" s="5" t="s">
         <v>113</v>
@@ -6336,12 +6336,12 @@
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="AI23" s="27" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AJ23" s="5" t="s">
         <v>120</v>
@@ -6349,12 +6349,12 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="AI24" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AJ24" s="5" t="s">
         <v>120</v>
@@ -6362,12 +6362,12 @@
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="AI25" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AJ25" s="5" t="s">
         <v>120</v>
@@ -6378,26 +6378,26 @@
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="AI26" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AJ26" s="5" t="s">
         <v>120</v>
       </c>
       <c r="AL26" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J27" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -6413,10 +6413,10 @@
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J28" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -6432,44 +6432,44 @@
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="AI29" s="27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AJ29" s="5" t="s">
         <v>120</v>
       </c>
       <c r="AL29" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="AI30" s="27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AJ30" s="5" t="s">
         <v>113</v>
       </c>
       <c r="AL30" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="AI31" s="27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AJ31" s="5" t="s">
         <v>113</v>
@@ -6480,44 +6480,44 @@
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="AI32" s="27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AJ32" s="5" t="s">
         <v>113</v>
       </c>
       <c r="AL32" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
       <c r="AI33" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AJ33" s="5" t="s">
         <v>113</v>
       </c>
       <c r="AL33" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
       <c r="AI34" s="27" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AJ34" s="5" t="s">
         <v>113</v>
@@ -6525,12 +6525,12 @@
     </row>
     <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
       <c r="AI35" s="27" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AJ35" s="5" t="s">
         <v>120</v>
@@ -6538,25 +6538,25 @@
     </row>
     <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
       <c r="AI36" s="27" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AJ36" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="AI37" s="27" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AJ37" s="5" t="s">
         <v>113</v>
@@ -6564,12 +6564,12 @@
     </row>
     <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="AI38" s="27" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AJ38" s="5" t="s">
         <v>120</v>
@@ -6577,31 +6577,31 @@
     </row>
     <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="AI39" s="27" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AJ39" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AL39" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
       <c r="AI40" s="27" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AJ40" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AL40" t="s">
         <v>39</v>
@@ -6609,7 +6609,7 @@
     </row>
     <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
@@ -6617,15 +6617,15 @@
         <v>177</v>
       </c>
       <c r="AJ41" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AL41" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
@@ -6638,24 +6638,24 @@
     </row>
     <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G43" t="s">
+        <v>418</v>
+      </c>
+      <c r="H43" t="s">
         <v>419</v>
       </c>
-      <c r="H43" t="s">
-        <v>420</v>
-      </c>
       <c r="I43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P43" s="2"/>
       <c r="AI43" s="27"/>
       <c r="AJ43" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
@@ -6678,7 +6678,7 @@
     </row>
     <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J45" s="15"/>
       <c r="O45" s="2"/>
@@ -6833,7 +6833,7 @@
         <v>47</v>
       </c>
       <c r="AG53" s="7" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="AH53">
         <v>1234</v>
@@ -7043,7 +7043,7 @@
     </row>
     <row r="62" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="M62" t="s">
         <v>35</v>
@@ -7052,7 +7052,7 @@
         <v>67</v>
       </c>
       <c r="AU62" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="63" spans="1:50" x14ac:dyDescent="0.3">
@@ -7094,20 +7094,20 @@
         <v>340</v>
       </c>
       <c r="Q65" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="R65" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S65" s="5"/>
       <c r="U65" t="s">
         <v>342</v>
       </c>
       <c r="V65" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="W65" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="X65" s="5"/>
     </row>
@@ -7124,7 +7124,7 @@
         <v>347</v>
       </c>
       <c r="S67" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="T67" s="26" t="s">
         <v>353</v>
@@ -7152,7 +7152,7 @@
         <v>354</v>
       </c>
       <c r="V69" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="70" spans="1:47" x14ac:dyDescent="0.3">
@@ -7192,10 +7192,10 @@
     </row>
     <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>364</v>
+      </c>
+      <c r="V71" s="5" t="s">
         <v>365</v>
-      </c>
-      <c r="V71" s="5" t="s">
-        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -7479,16 +7479,16 @@
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="N2" s="22" t="s">
         <v>513</v>
       </c>
-      <c r="N2" s="22" t="s">
-        <v>515</v>
-      </c>
       <c r="O2" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="P2" s="22" t="s">
         <v>514</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>516</v>
       </c>
       <c r="Q2" s="22">
         <v>9898989898</v>
@@ -7649,7 +7649,7 @@
         <v>333</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="K5" s="31"/>
       <c r="L5" s="22"/>
@@ -7720,21 +7720,21 @@
         <v>67</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="K6" s="31"/>
       <c r="L6" s="22"/>
       <c r="M6" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="N6" s="22" t="s">
         <v>513</v>
       </c>
-      <c r="N6" s="22" t="s">
-        <v>515</v>
-      </c>
       <c r="O6" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="P6" s="22" t="s">
         <v>514</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>516</v>
       </c>
       <c r="Q6" s="22">
         <v>9898989898</v>
@@ -7779,7 +7779,7 @@
         <v>81</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="22"/>
@@ -7793,23 +7793,23 @@
         <v>96</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="K7" s="31"/>
       <c r="L7" s="22" t="s">
         <v>81</v>
       </c>
       <c r="M7" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="N7" s="22" t="s">
         <v>513</v>
       </c>
-      <c r="N7" s="22" t="s">
-        <v>515</v>
-      </c>
       <c r="O7" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="P7" s="22" t="s">
         <v>514</v>
-      </c>
-      <c r="P7" s="22" t="s">
-        <v>516</v>
       </c>
       <c r="Q7" s="22">
         <v>9898989898</v>
@@ -7868,7 +7868,7 @@
         <v>100</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="22"/>
@@ -7882,23 +7882,23 @@
         <v>96</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="K8" s="31"/>
       <c r="L8" s="22" t="s">
         <v>100</v>
       </c>
       <c r="M8" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="N8" s="22" t="s">
         <v>513</v>
       </c>
-      <c r="N8" s="22" t="s">
-        <v>515</v>
-      </c>
       <c r="O8" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="P8" s="22" t="s">
         <v>514</v>
-      </c>
-      <c r="P8" s="22" t="s">
-        <v>516</v>
       </c>
       <c r="Q8" s="22">
         <v>9898989898</v>
@@ -7951,7 +7951,7 @@
         <v>95</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="22"/>
@@ -7965,23 +7965,23 @@
         <v>96</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="K9" s="31"/>
       <c r="L9" s="22" t="s">
         <v>95</v>
       </c>
       <c r="M9" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="N9" s="22" t="s">
         <v>513</v>
       </c>
-      <c r="N9" s="22" t="s">
-        <v>515</v>
-      </c>
       <c r="O9" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="P9" s="22" t="s">
         <v>514</v>
-      </c>
-      <c r="P9" s="22" t="s">
-        <v>516</v>
       </c>
       <c r="Q9" s="22">
         <v>9898989898</v>
@@ -8156,23 +8156,23 @@
         <v>67</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="N12" s="22" t="s">
         <v>513</v>
       </c>
-      <c r="N12" s="22" t="s">
-        <v>515</v>
-      </c>
       <c r="O12" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="P12" s="22" t="s">
         <v>514</v>
-      </c>
-      <c r="P12" s="22" t="s">
-        <v>516</v>
       </c>
       <c r="Q12" s="22">
         <v>9898989898</v>
@@ -8231,7 +8231,7 @@
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="K13" s="31"/>
       <c r="L13" s="22"/>
@@ -8459,7 +8459,7 @@
       </c>
       <c r="I17" s="22"/>
       <c r="J17" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="K17" s="31"/>
       <c r="L17" s="22"/>
@@ -8679,7 +8679,7 @@
         <v>25</v>
       </c>
       <c r="R2" s="40" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S2" t="s">
         <v>260</v>
@@ -9101,16 +9101,16 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
+        <v>495</v>
+      </c>
+      <c r="L2" t="s">
+        <v>496</v>
+      </c>
+      <c r="M2" t="s">
         <v>497</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" s="5" t="s">
         <v>498</v>
-      </c>
-      <c r="M2" t="s">
-        <v>499</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>500</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>59</v>
@@ -9203,7 +9203,7 @@
         <v>154</v>
       </c>
       <c r="J9" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
@@ -9249,11 +9249,11 @@
         <v>77</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I13" s="2"/>
       <c r="O13" s="5"/>
@@ -9269,7 +9269,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="Y14" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="Z14" t="s">
         <v>264</v>
@@ -9286,16 +9286,16 @@
         <v>15</v>
       </c>
       <c r="K15" t="s">
+        <v>499</v>
+      </c>
+      <c r="L15" t="s">
+        <v>500</v>
+      </c>
+      <c r="M15" t="s">
         <v>501</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>502</v>
-      </c>
-      <c r="M15" t="s">
-        <v>503</v>
-      </c>
-      <c r="N15" t="s">
-        <v>504</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>59</v>
@@ -9507,7 +9507,7 @@
         <v>243</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C2" s="22"/>
     </row>
@@ -9517,7 +9517,7 @@
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
@@ -9526,7 +9526,7 @@
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
@@ -9535,7 +9535,7 @@
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="22" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -9626,7 +9626,7 @@
         <v>205</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>183</v>
@@ -9637,10 +9637,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -9655,7 +9655,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" t="s">
@@ -9698,16 +9698,16 @@
       </c>
       <c r="H4" s="2"/>
       <c r="S4" t="s">
+        <v>508</v>
+      </c>
+      <c r="T4" t="s">
+        <v>508</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="V4" s="12" t="s">
         <v>510</v>
-      </c>
-      <c r="T4" t="s">
-        <v>510</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>511</v>
-      </c>
-      <c r="V4" s="12" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -9731,16 +9731,16 @@
         <v>206</v>
       </c>
       <c r="S7" t="s">
+        <v>508</v>
+      </c>
+      <c r="T7" t="s">
+        <v>508</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="V7" s="12" t="s">
         <v>510</v>
-      </c>
-      <c r="T7" t="s">
-        <v>510</v>
-      </c>
-      <c r="U7" s="5" t="s">
-        <v>511</v>
-      </c>
-      <c r="V7" s="12" t="s">
-        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -9881,7 +9881,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>29</v>
@@ -9896,7 +9896,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" t="s">

</xml_diff>

<commit_message>
HF_EMEA Testcases TEST_DGLD_HF_EMEA_RT_051,53 & 55 Added New and Changes with Testdata Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0513CB50-EB5F-470E-946B-01B5117038B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A61AE7-4574-4ACA-A7CE-B3EAED06389E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="520">
   <si>
     <t>UserName</t>
   </si>
@@ -1614,14 +1614,20 @@
   <si>
     <t>Hfemeanewaccount@gmail.com</t>
   </si>
+  <si>
+    <t>£25.00</t>
+  </si>
+  <si>
+    <t>£79.00</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1802,7 +1808,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1832,7 +1838,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2146,34 +2152,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="21" width="22.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="18" width="30.5546875" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="21" width="22.33203125" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.28515625" customWidth="1"/>
+    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2316,7 +2322,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2371,7 +2377,7 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="7"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>295</v>
       </c>
@@ -2426,7 +2432,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>360</v>
       </c>
@@ -2466,7 +2472,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>440</v>
       </c>
@@ -2521,7 +2527,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2537,7 +2543,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>199</v>
       </c>
@@ -2549,7 +2555,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>298</v>
       </c>
@@ -2565,7 +2571,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -2577,7 +2583,7 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -2590,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -2609,7 +2615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -2622,7 +2628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2650,7 +2656,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>446</v>
       </c>
@@ -2664,7 +2670,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>176</v>
       </c>
@@ -2683,7 +2689,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>175</v>
       </c>
@@ -2696,7 +2702,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>189</v>
       </c>
@@ -2707,7 +2713,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2731,7 +2737,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -2744,7 +2750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2760,7 +2766,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -2774,7 +2780,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -2811,7 +2817,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2825,7 +2831,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -2867,7 +2873,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -2881,7 +2887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2910,7 +2916,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -2927,7 +2933,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -2944,7 +2950,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>118</v>
       </c>
@@ -2973,7 +2979,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>151</v>
       </c>
@@ -2981,7 +2987,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -2992,7 +2998,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>166</v>
       </c>
@@ -3031,7 +3037,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>184</v>
       </c>
@@ -3046,7 +3052,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>279</v>
       </c>
@@ -3054,7 +3060,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>284</v>
       </c>
@@ -3068,7 +3074,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>215</v>
       </c>
@@ -3085,7 +3091,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>209</v>
       </c>
@@ -3102,7 +3108,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>340</v>
       </c>
@@ -3125,7 +3131,7 @@
       </c>
       <c r="R38" s="5"/>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>344</v>
       </c>
@@ -3133,7 +3139,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>347</v>
       </c>
@@ -3141,13 +3147,13 @@
         <v>431</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>362</v>
+        <v>519</v>
       </c>
       <c r="N40" s="26" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>349</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>354</v>
       </c>
@@ -3172,7 +3178,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>201</v>
       </c>
@@ -3207,7 +3213,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>364</v>
       </c>
@@ -3215,7 +3221,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>433</v>
       </c>
@@ -3223,7 +3229,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>434</v>
       </c>
@@ -3231,7 +3237,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>232</v>
       </c>
@@ -3239,7 +3245,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A48" s="35" t="s">
         <v>153</v>
       </c>
@@ -3278,7 +3284,7 @@
       </c>
       <c r="AE48" s="35"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>450</v>
       </c>
@@ -3335,18 +3341,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3444,7 +3450,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3491,7 +3497,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3541,7 +3547,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3588,7 +3594,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -3616,7 +3622,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -3627,7 +3633,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3649,7 +3655,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3662,7 +3668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -3678,7 +3684,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3692,7 +3698,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -3708,7 +3714,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3722,7 +3728,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -3764,7 +3770,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -3790,7 +3796,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3801,7 +3807,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -3816,7 +3822,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -3874,12 +3880,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3950,7 +3956,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3997,7 +4003,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4013,7 +4019,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -4044,7 +4050,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4052,7 +4058,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -4085,20 +4091,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.28515625" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4187,7 +4193,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4235,7 +4241,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4251,7 +4257,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -4271,7 +4277,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -4290,7 +4296,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -4309,7 +4315,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -4317,7 +4323,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -4325,7 +4331,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -4342,7 +4348,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -4359,7 +4365,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -4376,7 +4382,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -4393,7 +4399,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -4404,7 +4410,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -4415,7 +4421,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4432,7 +4438,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -4461,7 +4467,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4472,7 +4478,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4486,7 +4492,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -4500,7 +4506,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -4514,7 +4520,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -4522,7 +4528,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -4552,7 +4558,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -4622,19 +4628,19 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4660,7 +4666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4683,7 +4689,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -4714,16 +4720,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4737,7 +4743,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -4763,27 +4769,27 @@
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5703125" customWidth="1"/>
-    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5546875" customWidth="1"/>
+    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.140625" customWidth="1"/>
+    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.109375" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -4842,7 +4848,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>228</v>
       </c>
@@ -4867,7 +4873,7 @@
       <c r="R2" s="22"/>
       <c r="S2" s="22"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>230</v>
       </c>
@@ -4896,7 +4902,7 @@
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>232</v>
       </c>
@@ -4921,7 +4927,7 @@
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>233</v>
       </c>
@@ -4948,7 +4954,7 @@
       <c r="R5" s="22"/>
       <c r="S5" s="22"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>236</v>
       </c>
@@ -4981,7 +4987,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>238</v>
       </c>
@@ -5006,7 +5012,7 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>262</v>
       </c>
@@ -5031,7 +5037,7 @@
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>281</v>
       </c>
@@ -5056,7 +5062,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>286</v>
       </c>
@@ -5083,7 +5089,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>319</v>
       </c>
@@ -5108,7 +5114,7 @@
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>321</v>
       </c>
@@ -5135,7 +5141,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>322</v>
       </c>
@@ -5160,7 +5166,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>324</v>
       </c>
@@ -5185,7 +5191,7 @@
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>335</v>
       </c>
@@ -5210,7 +5216,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>338</v>
       </c>
@@ -5235,7 +5241,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>453</v>
       </c>
@@ -5243,7 +5249,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>454</v>
       </c>
@@ -5251,7 +5257,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>455</v>
       </c>
@@ -5273,31 +5279,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.7109375" customWidth="1"/>
-    <col min="17" max="24" width="30.5703125" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" customWidth="1"/>
-    <col min="26" max="27" width="22.28515625" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.6640625" customWidth="1"/>
+    <col min="17" max="24" width="30.5546875" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" customWidth="1"/>
+    <col min="26" max="27" width="22.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.28515625" customWidth="1"/>
+    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5449,7 +5455,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5519,7 +5525,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>458</v>
       </c>
@@ -5589,7 +5595,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>460</v>
       </c>
@@ -5659,7 +5665,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>461</v>
       </c>
@@ -5729,7 +5735,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>464</v>
       </c>
@@ -5799,7 +5805,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>468</v>
       </c>
@@ -5869,7 +5875,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>472</v>
       </c>
@@ -5910,7 +5916,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>473</v>
       </c>
@@ -5951,7 +5957,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>466</v>
       </c>
@@ -6021,7 +6027,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>407</v>
       </c>
@@ -6082,7 +6088,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>295</v>
       </c>
@@ -6141,7 +6147,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>360</v>
       </c>
@@ -6187,7 +6193,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6210,7 +6216,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>298</v>
       </c>
@@ -6233,7 +6239,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -6252,7 +6258,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6263,7 +6269,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6285,7 +6291,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>367</v>
       </c>
@@ -6298,7 +6304,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>369</v>
       </c>
@@ -6311,7 +6317,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>371</v>
       </c>
@@ -6324,7 +6330,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>376</v>
       </c>
@@ -6337,7 +6343,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>398</v>
       </c>
@@ -6350,7 +6356,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>377</v>
       </c>
@@ -6363,7 +6369,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>379</v>
       </c>
@@ -6379,7 +6385,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>381</v>
       </c>
@@ -6395,7 +6401,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>402</v>
       </c>
@@ -6414,7 +6420,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>406</v>
       </c>
@@ -6433,7 +6439,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>383</v>
       </c>
@@ -6449,7 +6455,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>386</v>
       </c>
@@ -6465,7 +6471,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>412</v>
       </c>
@@ -6481,7 +6487,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>413</v>
       </c>
@@ -6497,7 +6503,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>387</v>
       </c>
@@ -6513,7 +6519,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>390</v>
       </c>
@@ -6526,7 +6532,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>404</v>
       </c>
@@ -6539,7 +6545,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>391</v>
       </c>
@@ -6552,7 +6558,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>425</v>
       </c>
@@ -6565,7 +6571,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>399</v>
       </c>
@@ -6578,7 +6584,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>395</v>
       </c>
@@ -6594,7 +6600,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>424</v>
       </c>
@@ -6610,7 +6616,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>396</v>
       </c>
@@ -6626,7 +6632,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>403</v>
       </c>
@@ -6639,7 +6645,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>416</v>
       </c>
@@ -6661,7 +6667,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -6679,7 +6685,7 @@
       <c r="AI44" s="27"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>415</v>
       </c>
@@ -6692,7 +6698,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -6712,7 +6718,7 @@
       <c r="AI46" s="27"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -6731,7 +6737,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -6744,7 +6750,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -6755,7 +6761,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -6768,7 +6774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -6791,7 +6797,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -6805,7 +6811,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -6842,7 +6848,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -6856,7 +6862,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -6898,7 +6904,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -6924,7 +6930,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -6948,7 +6954,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -6972,7 +6978,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -6998,7 +7004,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -7030,7 +7036,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -7044,7 +7050,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>374</v>
       </c>
@@ -7058,7 +7064,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -7075,7 +7081,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -7092,7 +7098,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>340</v>
       </c>
@@ -7114,7 +7120,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>344</v>
       </c>
@@ -7122,7 +7128,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>347</v>
       </c>
@@ -7133,7 +7139,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>349</v>
       </c>
@@ -7150,7 +7156,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>354</v>
       </c>
@@ -7158,7 +7164,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -7193,7 +7199,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>364</v>
       </c>
@@ -7284,36 +7290,36 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -7450,7 +7456,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
@@ -7525,7 +7531,7 @@
       <c r="AR2" s="22"/>
       <c r="AS2" s="22"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
@@ -7582,7 +7588,7 @@
       <c r="AR3" s="22"/>
       <c r="AS3" s="22"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>248</v>
       </c>
@@ -7635,7 +7641,7 @@
       <c r="AR4" s="22"/>
       <c r="AS4" s="22"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>68</v>
       </c>
@@ -7698,7 +7704,7 @@
       <c r="AR5" s="22"/>
       <c r="AS5" s="22"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>75</v>
       </c>
@@ -7777,7 +7783,7 @@
       <c r="AR6" s="22"/>
       <c r="AS6" s="22"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>81</v>
       </c>
@@ -7866,7 +7872,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>100</v>
       </c>
@@ -7949,7 +7955,7 @@
       <c r="AR8" s="22"/>
       <c r="AS8" s="22"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>95</v>
       </c>
@@ -8034,7 +8040,7 @@
       <c r="AR9" s="22"/>
       <c r="AS9" s="22"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>40</v>
       </c>
@@ -8085,7 +8091,7 @@
       <c r="AR10" s="22"/>
       <c r="AS10" s="22"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>103</v>
       </c>
@@ -8142,7 +8148,7 @@
       <c r="AR11" s="22"/>
       <c r="AS11" s="22"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>107</v>
       </c>
@@ -8217,7 +8223,7 @@
       <c r="AR12" s="22"/>
       <c r="AS12" s="22"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>112</v>
       </c>
@@ -8280,7 +8286,7 @@
       <c r="AR13" s="22"/>
       <c r="AS13" s="22"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>249</v>
       </c>
@@ -8335,7 +8341,7 @@
       <c r="AR14" s="22"/>
       <c r="AS14" s="22"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>119</v>
       </c>
@@ -8392,7 +8398,7 @@
       <c r="AR15" s="22"/>
       <c r="AS15" s="22"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>121</v>
       </c>
@@ -8447,7 +8453,7 @@
       <c r="AR16" s="22"/>
       <c r="AS16" s="22"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>219</v>
       </c>
@@ -8502,7 +8508,7 @@
       <c r="AR17" s="22"/>
       <c r="AS17" s="22"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>154</v>
       </c>
@@ -8594,13 +8600,13 @@
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8677,7 +8683,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -8707,25 +8713,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8826,7 +8832,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -8912,7 +8918,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -8944,7 +8950,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -8970,25 +8976,25 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9074,7 +9080,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9121,7 +9127,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9137,7 +9143,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -9156,7 +9162,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>178</v>
       </c>
@@ -9169,7 +9175,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>179</v>
       </c>
@@ -9182,7 +9188,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>153</v>
       </c>
@@ -9193,7 +9199,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -9201,7 +9207,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -9209,7 +9215,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>168</v>
       </c>
@@ -9217,7 +9223,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -9236,7 +9242,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -9247,7 +9253,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -9262,7 +9268,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -9278,7 +9284,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -9305,7 +9311,7 @@
       </c>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -9319,7 +9325,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -9335,7 +9341,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>201</v>
       </c>
@@ -9372,7 +9378,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>241</v>
       </c>
@@ -9380,7 +9386,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -9403,7 +9409,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>166</v>
       </c>
@@ -9460,17 +9466,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -9505,7 +9511,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>243</v>
       </c>
@@ -9514,7 +9520,7 @@
       </c>
       <c r="C2" s="22"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>245</v>
       </c>
@@ -9523,7 +9529,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>247</v>
       </c>
@@ -9532,7 +9538,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>313</v>
       </c>
@@ -9554,20 +9560,20 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9635,7 +9641,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9679,7 +9685,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9695,7 +9701,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -9713,7 +9719,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -9721,7 +9727,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -9729,7 +9735,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -9766,37 +9772,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9879,7 +9885,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9920,7 +9926,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9936,7 +9942,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -9948,7 +9954,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -9966,7 +9972,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -9975,7 +9981,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -9987,7 +9993,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -10013,7 +10019,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -10024,7 +10030,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -10038,7 +10044,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
HF_EMEA Testcases TEST_DGLD_HF_EMEA_RT_46,51 & 53 giftcard Changes with testdata Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A61AE7-4574-4ACA-A7CE-B3EAED06389E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915B98A4-8238-4083-A74A-EEA9AF7009D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="523">
   <si>
     <t>UserName</t>
   </si>
@@ -1358,9 +1358,6 @@
     <t>5TB65S29F7534E44Y74A</t>
   </si>
   <si>
-    <t>9GX98U37V2332J98P68B</t>
-  </si>
-  <si>
     <t>CustomizeLinks</t>
   </si>
   <si>
@@ -1401,9 +1398,6 @@
   </si>
   <si>
     <t>Giftcard_Partial_3</t>
-  </si>
-  <si>
-    <t>2SL47R28J5473J54N28Z</t>
   </si>
   <si>
     <t>24 oz,32 oz,40 oz</t>
@@ -1619,6 +1613,21 @@
   </si>
   <si>
     <t>£79.00</t>
+  </si>
+  <si>
+    <t>9TS89X86V4385U48N45L</t>
+  </si>
+  <si>
+    <t>Giftcard_Partial_4</t>
+  </si>
+  <si>
+    <t>6HE74S92G8455H93B64J</t>
+  </si>
+  <si>
+    <t>6NA45V72N5876V96X45U</t>
+  </si>
+  <si>
+    <t>anbogi@helenoftroy.com</t>
   </si>
 </sst>
 </file>
@@ -2150,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU49"/>
+  <dimension ref="A1:AU50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2316,7 +2325,7 @@
         <v>207</v>
       </c>
       <c r="AT1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AU1" t="s">
         <v>357</v>
@@ -2327,10 +2336,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -2345,10 +2354,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -2360,16 +2369,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" t="s">
+        <v>492</v>
+      </c>
+      <c r="T2" t="s">
+        <v>493</v>
+      </c>
+      <c r="V2" t="s">
         <v>494</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" s="5" t="s">
         <v>495</v>
-      </c>
-      <c r="V2" t="s">
-        <v>496</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>497</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>59</v>
@@ -2382,10 +2391,10 @@
         <v>295</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2400,10 +2409,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -2415,16 +2424,16 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" t="s">
+        <v>492</v>
+      </c>
+      <c r="T3" t="s">
+        <v>493</v>
+      </c>
+      <c r="V3" t="s">
         <v>494</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3" s="5" t="s">
         <v>495</v>
-      </c>
-      <c r="V3" t="s">
-        <v>496</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>497</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>59</v>
@@ -2474,13 +2483,13 @@
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>439</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>441</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -2495,10 +2504,10 @@
         <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2510,16 +2519,16 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" t="s">
+        <v>492</v>
+      </c>
+      <c r="T5" t="s">
+        <v>493</v>
+      </c>
+      <c r="V5" t="s">
         <v>494</v>
       </c>
-      <c r="T5" t="s">
+      <c r="W5" s="5" t="s">
         <v>495</v>
-      </c>
-      <c r="V5" t="s">
-        <v>496</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>497</v>
       </c>
       <c r="X5" s="5" t="s">
         <v>59</v>
@@ -2537,7 +2546,7 @@
         <v>23</v>
       </c>
       <c r="AA6" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AB6">
         <v>123</v>
@@ -2588,7 +2597,7 @@
         <v>154</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="W10" s="3"/>
       <c r="X10" s="4"/>
@@ -2658,16 +2667,16 @@
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="AC14" s="36" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AD14" s="34"/>
       <c r="AE14" s="36" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.3">
@@ -2734,7 +2743,7 @@
       </c>
       <c r="I18" s="2"/>
       <c r="AL18" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.3">
@@ -2760,7 +2769,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="AI20" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="AJ20" t="s">
         <v>264</v>
@@ -2774,7 +2783,7 @@
         <v>45</v>
       </c>
       <c r="AA21" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AB21">
         <v>123</v>
@@ -2811,7 +2820,7 @@
         <v>47</v>
       </c>
       <c r="AA22" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AB22">
         <v>1234</v>
@@ -2825,7 +2834,7 @@
         <v>49</v>
       </c>
       <c r="AA23" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AB23">
         <v>123</v>
@@ -2864,7 +2873,7 @@
         <v>23</v>
       </c>
       <c r="AA24" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AB24">
         <v>123</v>
@@ -2898,19 +2907,19 @@
         <v>15</v>
       </c>
       <c r="S26" t="s">
+        <v>508</v>
+      </c>
+      <c r="T26" t="s">
         <v>510</v>
       </c>
-      <c r="T26" t="s">
-        <v>512</v>
-      </c>
       <c r="U26" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="V26" t="s">
+        <v>509</v>
+      </c>
+      <c r="W26" s="5" t="s">
         <v>511</v>
-      </c>
-      <c r="W26" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="X26" s="5" t="s">
         <v>59</v>
@@ -2927,10 +2936,10 @@
         <v>331</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.3">
@@ -2938,11 +2947,11 @@
         <v>77</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I28" s="2"/>
       <c r="W28" s="5"/>
@@ -2961,19 +2970,19 @@
         <v>15</v>
       </c>
       <c r="S29" t="s">
+        <v>508</v>
+      </c>
+      <c r="T29" t="s">
         <v>510</v>
       </c>
-      <c r="T29" t="s">
-        <v>512</v>
-      </c>
       <c r="U29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="V29" t="s">
+        <v>509</v>
+      </c>
+      <c r="W29" s="5" t="s">
         <v>511</v>
-      </c>
-      <c r="W29" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="X29" s="5" t="s">
         <v>59</v>
@@ -2984,7 +2993,7 @@
         <v>151</v>
       </c>
       <c r="AL30" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.3">
@@ -3019,19 +3028,19 @@
       <c r="Q32" s="12"/>
       <c r="R32" s="12"/>
       <c r="S32" t="s">
+        <v>508</v>
+      </c>
+      <c r="T32" t="s">
         <v>510</v>
       </c>
-      <c r="T32" t="s">
-        <v>512</v>
-      </c>
       <c r="U32" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="V32" t="s">
+        <v>509</v>
+      </c>
+      <c r="W32" s="5" t="s">
         <v>511</v>
-      </c>
-      <c r="W32" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="X32" s="5" t="s">
         <v>59</v>
@@ -3124,7 +3133,7 @@
         <v>342</v>
       </c>
       <c r="P38" s="28" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="Q38" s="5" t="s">
         <v>356</v>
@@ -3147,10 +3156,10 @@
         <v>431</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="N40" s="26" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="41" spans="1:46" x14ac:dyDescent="0.3">
@@ -3164,7 +3173,7 @@
         <v>350</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>351</v>
+        <v>522</v>
       </c>
       <c r="AO41" t="s">
         <v>352</v>
@@ -3175,7 +3184,7 @@
         <v>354</v>
       </c>
       <c r="P42" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="43" spans="1:46" x14ac:dyDescent="0.3">
@@ -3234,7 +3243,7 @@
         <v>434</v>
       </c>
       <c r="P46" s="28" t="s">
-        <v>436</v>
+        <v>521</v>
       </c>
     </row>
     <row r="47" spans="1:46" x14ac:dyDescent="0.3">
@@ -3286,10 +3295,18 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="P49" s="28" t="s">
-        <v>451</v>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>519</v>
+      </c>
+      <c r="P50" t="s">
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -3455,10 +3472,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -3473,10 +3490,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -3502,10 +3519,10 @@
         <v>192</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>29</v>
@@ -3520,10 +3537,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s">
@@ -3552,10 +3569,10 @@
         <v>194</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -3570,10 +3587,10 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" t="s">
@@ -3736,7 +3753,7 @@
         <v>50</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I14" s="2"/>
       <c r="K14" t="s">
@@ -3961,10 +3978,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -3979,10 +3996,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -4024,10 +4041,10 @@
         <v>187</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -4198,10 +4215,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -4216,10 +4233,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -4671,10 +4688,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -4748,7 +4765,7 @@
         <v>152</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>261</v>
@@ -4845,7 +4862,7 @@
         <v>286</v>
       </c>
       <c r="S1" s="39" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -4853,7 +4870,7 @@
         <v>228</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -4883,7 +4900,7 @@
         <v>265</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>276</v>
@@ -4914,7 +4931,7 @@
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
@@ -4942,7 +4959,7 @@
       <c r="H5" s="22"/>
       <c r="I5" s="32"/>
       <c r="J5" s="22" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
@@ -5003,7 +5020,7 @@
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
       <c r="M7" s="30" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="N7" s="22"/>
       <c r="O7" s="22"/>
@@ -5032,7 +5049,7 @@
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
       <c r="Q8" s="21" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
@@ -5045,7 +5062,7 @@
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
@@ -5086,7 +5103,7 @@
         <v>287</v>
       </c>
       <c r="S10" s="22" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -5124,10 +5141,10 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
       <c r="G12" s="37" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
@@ -5197,7 +5214,7 @@
       </c>
       <c r="B15" s="22"/>
       <c r="C15" s="22" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -5243,26 +5260,26 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C18" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Q19" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -5527,10 +5544,10 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>274</v>
@@ -5559,7 +5576,7 @@
         <v>427</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>274</v>
@@ -5597,10 +5614,10 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>274</v>
@@ -5629,7 +5646,7 @@
         <v>427</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>274</v>
@@ -5667,10 +5684,10 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>274</v>
@@ -5699,7 +5716,7 @@
         <v>427</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>274</v>
@@ -5737,10 +5754,10 @@
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>274</v>
@@ -5769,7 +5786,7 @@
         <v>427</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>274</v>
@@ -5807,10 +5824,10 @@
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>274</v>
@@ -5839,7 +5856,7 @@
         <v>427</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>274</v>
@@ -5877,10 +5894,10 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -5918,10 +5935,10 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
@@ -5959,10 +5976,10 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>274</v>
@@ -5991,7 +6008,7 @@
         <v>427</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>274</v>
@@ -6842,7 +6859,7 @@
         <v>47</v>
       </c>
       <c r="AG53" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AH53">
         <v>1234</v>
@@ -7488,16 +7505,16 @@
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="N2" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="N2" s="22" t="s">
-        <v>512</v>
-      </c>
       <c r="O2" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="P2" s="22" t="s">
         <v>511</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>513</v>
       </c>
       <c r="Q2" s="22">
         <v>9898989898</v>
@@ -7658,7 +7675,7 @@
         <v>333</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K5" s="31"/>
       <c r="L5" s="22"/>
@@ -7729,21 +7746,21 @@
         <v>67</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K6" s="31"/>
       <c r="L6" s="22"/>
       <c r="M6" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="N6" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="N6" s="22" t="s">
-        <v>512</v>
-      </c>
       <c r="O6" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="P6" s="22" t="s">
         <v>511</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>513</v>
       </c>
       <c r="Q6" s="22">
         <v>9898989898</v>
@@ -7788,7 +7805,7 @@
         <v>81</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="22"/>
@@ -7802,23 +7819,23 @@
         <v>96</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K7" s="31"/>
       <c r="L7" s="22" t="s">
         <v>81</v>
       </c>
       <c r="M7" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="N7" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="N7" s="22" t="s">
-        <v>512</v>
-      </c>
       <c r="O7" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="P7" s="22" t="s">
         <v>511</v>
-      </c>
-      <c r="P7" s="22" t="s">
-        <v>513</v>
       </c>
       <c r="Q7" s="22">
         <v>9898989898</v>
@@ -7877,7 +7894,7 @@
         <v>100</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="22"/>
@@ -7891,23 +7908,23 @@
         <v>96</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K8" s="31"/>
       <c r="L8" s="22" t="s">
         <v>100</v>
       </c>
       <c r="M8" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="N8" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="N8" s="22" t="s">
-        <v>512</v>
-      </c>
       <c r="O8" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="P8" s="22" t="s">
         <v>511</v>
-      </c>
-      <c r="P8" s="22" t="s">
-        <v>513</v>
       </c>
       <c r="Q8" s="22">
         <v>9898989898</v>
@@ -7960,7 +7977,7 @@
         <v>95</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="22"/>
@@ -7974,23 +7991,23 @@
         <v>96</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K9" s="31"/>
       <c r="L9" s="22" t="s">
         <v>95</v>
       </c>
       <c r="M9" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="N9" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="N9" s="22" t="s">
-        <v>512</v>
-      </c>
       <c r="O9" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="P9" s="22" t="s">
         <v>511</v>
-      </c>
-      <c r="P9" s="22" t="s">
-        <v>513</v>
       </c>
       <c r="Q9" s="22">
         <v>9898989898</v>
@@ -8165,23 +8182,23 @@
         <v>67</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="N12" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="N12" s="22" t="s">
-        <v>512</v>
-      </c>
       <c r="O12" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="P12" s="22" t="s">
         <v>511</v>
-      </c>
-      <c r="P12" s="22" t="s">
-        <v>513</v>
       </c>
       <c r="Q12" s="22">
         <v>9898989898</v>
@@ -8240,7 +8257,7 @@
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K13" s="31"/>
       <c r="L13" s="22"/>
@@ -8468,7 +8485,7 @@
       </c>
       <c r="I17" s="22"/>
       <c r="J17" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K17" s="31"/>
       <c r="L17" s="22"/>
@@ -8688,7 +8705,7 @@
         <v>25</v>
       </c>
       <c r="R2" s="40" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S2" t="s">
         <v>260</v>
@@ -9110,16 +9127,16 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
+        <v>492</v>
+      </c>
+      <c r="L2" t="s">
+        <v>493</v>
+      </c>
+      <c r="M2" t="s">
         <v>494</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" s="5" t="s">
         <v>495</v>
-      </c>
-      <c r="M2" t="s">
-        <v>496</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>497</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>59</v>
@@ -9212,7 +9229,7 @@
         <v>154</v>
       </c>
       <c r="J9" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
@@ -9258,11 +9275,11 @@
         <v>77</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I13" s="2"/>
       <c r="O13" s="5"/>
@@ -9278,7 +9295,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="Y14" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="Z14" t="s">
         <v>264</v>
@@ -9295,16 +9312,16 @@
         <v>15</v>
       </c>
       <c r="K15" t="s">
+        <v>496</v>
+      </c>
+      <c r="L15" t="s">
+        <v>497</v>
+      </c>
+      <c r="M15" t="s">
         <v>498</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>499</v>
-      </c>
-      <c r="M15" t="s">
-        <v>500</v>
-      </c>
-      <c r="N15" t="s">
-        <v>501</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>59</v>
@@ -9516,7 +9533,7 @@
         <v>243</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C2" s="22"/>
     </row>
@@ -9526,7 +9543,7 @@
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
@@ -9535,7 +9552,7 @@
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
@@ -9544,7 +9561,7 @@
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="22" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -9646,10 +9663,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -9664,7 +9681,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" t="s">
@@ -9707,16 +9724,16 @@
       </c>
       <c r="H4" s="2"/>
       <c r="S4" t="s">
+        <v>505</v>
+      </c>
+      <c r="T4" t="s">
+        <v>505</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="V4" s="12" t="s">
         <v>507</v>
-      </c>
-      <c r="T4" t="s">
-        <v>507</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="V4" s="12" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -9740,16 +9757,16 @@
         <v>206</v>
       </c>
       <c r="S7" t="s">
+        <v>505</v>
+      </c>
+      <c r="T7" t="s">
+        <v>505</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="V7" s="12" t="s">
         <v>507</v>
-      </c>
-      <c r="T7" t="s">
-        <v>507</v>
-      </c>
-      <c r="U7" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="V7" s="12" t="s">
-        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -9890,7 +9907,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>29</v>
@@ -9905,7 +9922,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" t="s">

</xml_diff>

<commit_message>
HF-EMEA: 066,56 Testcases and testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915B98A4-8238-4083-A74A-EEA9AF7009D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E1EA54-6E1E-45AC-B20E-D6B52A2E295F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="527">
   <si>
     <t>UserName</t>
   </si>
@@ -1629,14 +1629,26 @@
   <si>
     <t>anbogi@helenoftroy.com</t>
   </si>
+  <si>
+    <t>Gift_CardAccountDetails</t>
+  </si>
+  <si>
+    <t>Flat 93 Cleveland Tower</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>B1 1UD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1817,7 +1829,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1847,7 +1859,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2159,36 +2171,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU50"/>
+  <dimension ref="A1:AU51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="18" width="30.5546875" customWidth="1"/>
-    <col min="19" max="19" width="19.6640625" customWidth="1"/>
-    <col min="20" max="21" width="22.33203125" customWidth="1"/>
-    <col min="22" max="22" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="18" width="30.5703125" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1"/>
+    <col min="20" max="21" width="22.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.33203125" customWidth="1"/>
+    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2331,7 +2343,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2386,7 +2398,7 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="7"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>295</v>
       </c>
@@ -2441,15 +2453,15 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>360</v>
+        <v>523</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>296</v>
+        <v>507</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>296</v>
+        <v>507</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>29</v>
@@ -2464,9 +2476,11 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="I4" s="2"/>
+        <v>507</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>507</v>
+      </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -2476,20 +2490,33 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
+      <c r="S4" s="15" t="s">
+        <v>524</v>
+      </c>
+      <c r="T4" t="s">
+        <v>525</v>
+      </c>
+      <c r="V4" t="s">
+        <v>494</v>
+      </c>
+      <c r="W4" t="s">
+        <v>526</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>439</v>
+        <v>360</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>440</v>
+        <v>296</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>448</v>
+        <v>296</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -2504,11 +2531,9 @@
         <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>448</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -2518,359 +2543,362 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" t="s">
-        <v>492</v>
-      </c>
-      <c r="T5" t="s">
-        <v>493</v>
-      </c>
-      <c r="V5" t="s">
-        <v>494</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>495</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>439</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" t="s">
+        <v>492</v>
+      </c>
+      <c r="T6" t="s">
+        <v>493</v>
+      </c>
+      <c r="V6" t="s">
+        <v>494</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="7"/>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="Z6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA6" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="AB6">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>199</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="7"/>
-      <c r="AS7" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="Z7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="AB7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>298</v>
+        <v>199</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="Z8" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="AA8" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="AB8">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="7"/>
+      <c r="AS8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>298</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="J9" t="s">
+      <c r="Z9" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="AA9" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="AB9">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="J10" t="s">
         <v>203</v>
       </c>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="7"/>
-    </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="7"/>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>154</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J11" s="20" t="s">
         <v>491</v>
-      </c>
-      <c r="W10" s="3"/>
-      <c r="X10" s="4"/>
-      <c r="AD10" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>172</v>
       </c>
       <c r="W11" s="3"/>
       <c r="X11" s="4"/>
-      <c r="AC11" t="s">
-        <v>173</v>
-      </c>
-      <c r="AD11" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>173</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AD11" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="W12" s="3"/>
       <c r="X12" s="4"/>
       <c r="AC12" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>173</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>170</v>
+      </c>
+      <c r="W13" s="3"/>
+      <c r="X13" s="4"/>
+      <c r="AC13" t="s">
         <v>171</v>
-      </c>
-      <c r="AD12" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="AC13" s="12" t="s">
-        <v>312</v>
       </c>
       <c r="AD13" s="34">
         <v>1</v>
       </c>
-      <c r="AE13" t="s">
-        <v>327</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>388</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>190</v>
-      </c>
-      <c r="AH13">
-        <v>1</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>445</v>
+        <v>25</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="AC14" s="36" t="s">
-        <v>446</v>
-      </c>
-      <c r="AD14" s="34"/>
-      <c r="AE14" s="36" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AC14" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="AD14" s="34">
+        <v>1</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>388</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>190</v>
+      </c>
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>445</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="AC15" t="s">
-        <v>177</v>
-      </c>
-      <c r="AD15" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AC15" s="36" t="s">
+        <v>446</v>
+      </c>
+      <c r="AD15" s="34"/>
+      <c r="AE15" s="36" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="AC16" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AD16" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AE16" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="AD17" s="5"/>
-      <c r="AF17" t="s">
+      <c r="AC17" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD17" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>189</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="AD18" s="5"/>
+      <c r="AF18" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>34</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>31</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="2"/>
-      <c r="AL18" s="12" t="s">
+      <c r="I19" s="2"/>
+      <c r="AL19" s="12" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="AD19" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AH19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="G20" s="6"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="AI20" t="s">
+      <c r="AD20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="AI21" t="s">
         <v>490</v>
       </c>
-      <c r="AJ20" t="s">
+      <c r="AJ21" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="Z21" s="5" t="s">
+      <c r="Z22" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="AA21" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="AB21">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="S22" t="s">
-        <v>150</v>
-      </c>
-      <c r="T22" t="s">
-        <v>17</v>
-      </c>
-      <c r="V22" t="s">
-        <v>19</v>
-      </c>
-      <c r="W22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="X22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z22" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="AA22" s="7" t="s">
         <v>444</v>
       </c>
       <c r="AB22">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="S23" t="s">
+        <v>150</v>
+      </c>
+      <c r="T23" t="s">
+        <v>17</v>
+      </c>
+      <c r="V23" t="s">
+        <v>19</v>
+      </c>
+      <c r="W23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="X23" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="Z23" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA23" s="7" t="s">
         <v>444</v>
       </c>
       <c r="AB23">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="2"/>
-      <c r="S24" t="s">
-        <v>150</v>
-      </c>
-      <c r="T24" t="s">
-        <v>17</v>
-      </c>
-      <c r="V24" t="s">
-        <v>19</v>
-      </c>
-      <c r="W24" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="X24" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y24" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="Z24" s="5" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="AA24" s="7" t="s">
         <v>444</v>
@@ -2878,231 +2906,259 @@
       <c r="AB24">
         <v>123</v>
       </c>
-      <c r="AK24" s="5" t="s">
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="S25" t="s">
+        <v>150</v>
+      </c>
+      <c r="T25" t="s">
+        <v>17</v>
+      </c>
+      <c r="V25" t="s">
+        <v>19</v>
+      </c>
+      <c r="W25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="X25" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA25" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="AB25">
+        <v>123</v>
+      </c>
+      <c r="AK25" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>55</v>
       </c>
-      <c r="Z25" s="5" t="s">
+      <c r="Z26" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AA25" s="7" t="s">
+      <c r="AA26" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="AB25" s="5">
+      <c r="AB26" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>61</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>14</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>15</v>
       </c>
-      <c r="S26" t="s">
+      <c r="S27" t="s">
         <v>508</v>
       </c>
-      <c r="T26" t="s">
+      <c r="T27" t="s">
         <v>510</v>
       </c>
-      <c r="U26" t="s">
+      <c r="U27" t="s">
         <v>498</v>
       </c>
-      <c r="V26" t="s">
+      <c r="V27" t="s">
         <v>509</v>
       </c>
-      <c r="W26" s="5" t="s">
+      <c r="W27" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="X26" s="5" t="s">
+      <c r="X27" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D28" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H28" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="I27" s="12" t="s">
+      <c r="I28" s="12" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>501</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="H28" s="2" t="s">
+      <c r="E29" s="2"/>
+      <c r="H29" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="I28" s="2"/>
-      <c r="W28" s="5"/>
-      <c r="X28" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>118</v>
-      </c>
-      <c r="F29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" t="s">
-        <v>15</v>
-      </c>
-      <c r="S29" t="s">
-        <v>508</v>
-      </c>
-      <c r="T29" t="s">
-        <v>510</v>
-      </c>
-      <c r="U29" t="s">
-        <v>498</v>
-      </c>
-      <c r="V29" t="s">
-        <v>509</v>
-      </c>
-      <c r="W29" s="5" t="s">
-        <v>511</v>
-      </c>
+      <c r="I29" s="2"/>
+      <c r="W29" s="5"/>
       <c r="X29" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S30" t="s">
+        <v>508</v>
+      </c>
+      <c r="T30" t="s">
+        <v>510</v>
+      </c>
+      <c r="U30" t="s">
+        <v>498</v>
+      </c>
+      <c r="V30" t="s">
+        <v>509</v>
+      </c>
+      <c r="W30" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="X30" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>151</v>
       </c>
-      <c r="AL30" t="s">
+      <c r="AL31" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>164</v>
       </c>
-      <c r="AM31" t="s">
+      <c r="AM32" t="s">
         <v>297</v>
       </c>
-      <c r="AN31" t="s">
+      <c r="AN32" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>166</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>167</v>
       </c>
-      <c r="H32" s="12" t="s">
+      <c r="H33" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="12"/>
-      <c r="R32" s="12"/>
-      <c r="S32" t="s">
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" t="s">
         <v>508</v>
       </c>
-      <c r="T32" t="s">
+      <c r="T33" t="s">
         <v>510</v>
       </c>
-      <c r="U32" t="s">
+      <c r="U33" t="s">
         <v>498</v>
       </c>
-      <c r="V32" t="s">
+      <c r="V33" t="s">
         <v>509</v>
       </c>
-      <c r="W32" s="5" t="s">
+      <c r="W33" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="X32" s="5" t="s">
+      <c r="X33" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>184</v>
       </c>
-      <c r="H33" s="25" t="s">
+      <c r="H34" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="I33" s="12"/>
-      <c r="AC33" t="s">
+      <c r="I34" s="12"/>
+      <c r="AC34" t="s">
         <v>257</v>
       </c>
-      <c r="AO33" t="s">
+      <c r="AO34" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>279</v>
       </c>
-      <c r="AO34" t="s">
+      <c r="AO35" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>284</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" t="s">
         <v>15</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G36" t="s">
         <v>14</v>
       </c>
-      <c r="AO35" t="s">
+      <c r="AO36" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>215</v>
       </c>
-      <c r="AC36" t="s">
+      <c r="AC37" t="s">
         <v>255</v>
       </c>
-      <c r="AD36" s="5" t="s">
+      <c r="AD37" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="AF36" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>209</v>
       </c>
       <c r="AF37" t="s">
         <v>39</v>
@@ -3110,243 +3166,260 @@
       <c r="AP37" t="s">
         <v>83</v>
       </c>
-      <c r="AQ37" t="s">
+    </row>
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>209</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP38" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ38" t="s">
         <v>216</v>
       </c>
-      <c r="AR37" t="s">
+      <c r="AR38" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>340</v>
       </c>
-      <c r="J38" s="5" t="s">
+      <c r="J39" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="K39" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="O38" t="s">
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="O39" t="s">
         <v>342</v>
       </c>
-      <c r="P38" s="28" t="s">
+      <c r="P39" s="28" t="s">
         <v>513</v>
       </c>
-      <c r="Q38" s="5" t="s">
+      <c r="Q39" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="R38" s="5"/>
-    </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="R39" s="5"/>
+    </row>
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>344</v>
       </c>
-      <c r="R39" t="s">
+      <c r="R40" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>347</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="L41" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="M40" s="5" t="s">
+      <c r="M41" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="N40" s="26" t="s">
+      <c r="N41" s="26" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>349</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F42" t="s">
         <v>14</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G42" t="s">
         <v>350</v>
       </c>
-      <c r="H41" s="12" t="s">
+      <c r="H42" s="12" t="s">
         <v>522</v>
       </c>
-      <c r="AO41" t="s">
+      <c r="AO42" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>354</v>
       </c>
-      <c r="P42" t="s">
+      <c r="P43" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>201</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B44" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D44" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F44" t="s">
         <v>14</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G44" t="s">
         <v>350</v>
       </c>
-      <c r="H43" s="12" t="s">
+      <c r="H44" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="S43" t="s">
+      <c r="S44" t="s">
         <v>62</v>
       </c>
-      <c r="T43" t="s">
+      <c r="T44" t="s">
         <v>63</v>
       </c>
-      <c r="V43" t="s">
+      <c r="V44" t="s">
         <v>64</v>
       </c>
-      <c r="W43" s="5" t="s">
+      <c r="W44" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="X43" s="5" t="s">
+      <c r="X44" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>364</v>
       </c>
-      <c r="P44" s="5" t="s">
+      <c r="P45" s="5" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>433</v>
       </c>
-      <c r="P45" s="29" t="s">
+      <c r="P46" s="29" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>434</v>
       </c>
-      <c r="P46" s="28" t="s">
+      <c r="P47" s="28" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>232</v>
       </c>
-      <c r="AT47" s="33" t="s">
+      <c r="AT48" s="33" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A48" s="35" t="s">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A49" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="35"/>
-      <c r="J48" s="35"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="35"/>
-      <c r="N48" s="35"/>
-      <c r="O48" s="35"/>
-      <c r="P48" s="35"/>
-      <c r="Q48" s="35"/>
-      <c r="R48" s="35"/>
-      <c r="S48" s="35"/>
-      <c r="T48" s="35"/>
-      <c r="U48" s="35"/>
-      <c r="V48" s="35"/>
-      <c r="W48" s="35"/>
-      <c r="X48" s="35"/>
-      <c r="Y48" s="35"/>
-      <c r="Z48" s="35"/>
-      <c r="AA48" s="35"/>
-      <c r="AB48" s="35"/>
-      <c r="AC48" s="35" t="s">
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+      <c r="M49" s="35"/>
+      <c r="N49" s="35"/>
+      <c r="O49" s="35"/>
+      <c r="P49" s="35"/>
+      <c r="Q49" s="35"/>
+      <c r="R49" s="35"/>
+      <c r="S49" s="35"/>
+      <c r="T49" s="35"/>
+      <c r="U49" s="35"/>
+      <c r="V49" s="35"/>
+      <c r="W49" s="35"/>
+      <c r="X49" s="35"/>
+      <c r="Y49" s="35"/>
+      <c r="Z49" s="35"/>
+      <c r="AA49" s="35"/>
+      <c r="AB49" s="35"/>
+      <c r="AC49" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="AD48" s="35">
+      <c r="AD49" s="35">
         <v>1</v>
       </c>
-      <c r="AE48" s="35"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="AE49" s="35"/>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>449</v>
       </c>
-      <c r="P49" s="28" t="s">
+      <c r="P50" s="28" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>519</v>
       </c>
-      <c r="P50" t="s">
+      <c r="P51" t="s">
         <v>518</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D18" r:id="rId2" display="Lotuswave@123" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D19" r:id="rId2" display="Lotuswave@123" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H24" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E27" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H28" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="AL18" r:id="rId7" xr:uid="{081C5E6B-B750-4DF9-A406-8CFA5CF35321}"/>
-    <hyperlink ref="H32" r:id="rId8" xr:uid="{E7117AFE-BF51-4362-86E8-EC31CD714F35}"/>
+    <hyperlink ref="H25" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E28" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H29" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="AL19" r:id="rId7" xr:uid="{081C5E6B-B750-4DF9-A406-8CFA5CF35321}"/>
+    <hyperlink ref="H33" r:id="rId8" xr:uid="{E7117AFE-BF51-4362-86E8-EC31CD714F35}"/>
     <hyperlink ref="D2" r:id="rId9" xr:uid="{2D39057E-A748-4174-BA59-49433F76661C}"/>
-    <hyperlink ref="H33" r:id="rId10" xr:uid="{7ECA06F7-0F76-44C2-9FB9-4179E4310E54}"/>
+    <hyperlink ref="H34" r:id="rId10" xr:uid="{7ECA06F7-0F76-44C2-9FB9-4179E4310E54}"/>
     <hyperlink ref="B2" r:id="rId11" xr:uid="{B14C1544-364C-4E03-A43F-D19E66177301}"/>
     <hyperlink ref="I2" r:id="rId12" xr:uid="{AA16F981-3056-4646-A2C1-ECE17E4E92D7}"/>
     <hyperlink ref="C2" r:id="rId13" xr:uid="{6B47FB1F-967B-4003-9184-BEF0C984D5EA}"/>
-    <hyperlink ref="H27" r:id="rId14" xr:uid="{64862719-EAD4-4268-AF34-CDC0319543E7}"/>
-    <hyperlink ref="I27" r:id="rId15" xr:uid="{8EE57DBF-CF86-4B54-B5B4-2B9596DA7CE9}"/>
+    <hyperlink ref="H28" r:id="rId14" xr:uid="{64862719-EAD4-4268-AF34-CDC0319543E7}"/>
+    <hyperlink ref="I28" r:id="rId15" xr:uid="{8EE57DBF-CF86-4B54-B5B4-2B9596DA7CE9}"/>
     <hyperlink ref="D3" r:id="rId16" xr:uid="{43D25ADB-4E4D-4766-8BDD-9478BEC1A271}"/>
     <hyperlink ref="E3" r:id="rId17" xr:uid="{26E68202-5CE3-42C9-9DA5-1788DD83F3DD}"/>
-    <hyperlink ref="AC13" r:id="rId18" display="https://mcloud-na-preprod.hydroflask.com/wide-mouth-flex-cap?color=Black" xr:uid="{29EA729C-67AB-4332-AD2E-87301AAE2E8C}"/>
-    <hyperlink ref="H41" r:id="rId19" xr:uid="{7950AECF-C1F8-4C97-8F40-50E8B8819E85}"/>
-    <hyperlink ref="B43" r:id="rId20" xr:uid="{F8F2B0AD-86F8-4E80-8B1A-138B21EB05DB}"/>
-    <hyperlink ref="D43" r:id="rId21" xr:uid="{F252BFF6-7553-465C-B03F-0EDCA58E86DD}"/>
-    <hyperlink ref="H43" r:id="rId22" xr:uid="{819E02F2-2ED2-485D-85EB-576F27665CFC}"/>
-    <hyperlink ref="E5" r:id="rId23" xr:uid="{1D5FD444-4596-442E-BAE6-C911BFAC6718}"/>
-    <hyperlink ref="D5" r:id="rId24" xr:uid="{193852EB-47AA-454A-91E5-A4E8624ADA13}"/>
-    <hyperlink ref="B5" r:id="rId25" xr:uid="{450F9719-F0D6-46E4-A813-0721F12125A4}"/>
-    <hyperlink ref="I5" r:id="rId26" display="LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{4B3C7CD9-EB98-4907-833E-9C41C9ADEE76}"/>
-    <hyperlink ref="C5" r:id="rId27" display="LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{72A898E1-E814-40B9-9CCE-853A961F2109}"/>
-    <hyperlink ref="H5" r:id="rId28" xr:uid="{4A93039F-9FB8-42CB-9ACE-C0BE7F576AAE}"/>
-    <hyperlink ref="D27" r:id="rId29" xr:uid="{ADDAE6FC-BD5F-4B77-8488-C7AA571E5B74}"/>
+    <hyperlink ref="AC14" r:id="rId18" display="https://mcloud-na-preprod.hydroflask.com/wide-mouth-flex-cap?color=Black" xr:uid="{29EA729C-67AB-4332-AD2E-87301AAE2E8C}"/>
+    <hyperlink ref="H42" r:id="rId19" xr:uid="{7950AECF-C1F8-4C97-8F40-50E8B8819E85}"/>
+    <hyperlink ref="B44" r:id="rId20" xr:uid="{F8F2B0AD-86F8-4E80-8B1A-138B21EB05DB}"/>
+    <hyperlink ref="D44" r:id="rId21" xr:uid="{F252BFF6-7553-465C-B03F-0EDCA58E86DD}"/>
+    <hyperlink ref="H44" r:id="rId22" xr:uid="{819E02F2-2ED2-485D-85EB-576F27665CFC}"/>
+    <hyperlink ref="E6" r:id="rId23" xr:uid="{1D5FD444-4596-442E-BAE6-C911BFAC6718}"/>
+    <hyperlink ref="D6" r:id="rId24" xr:uid="{193852EB-47AA-454A-91E5-A4E8624ADA13}"/>
+    <hyperlink ref="B6" r:id="rId25" xr:uid="{450F9719-F0D6-46E4-A813-0721F12125A4}"/>
+    <hyperlink ref="I6" r:id="rId26" display="LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{4B3C7CD9-EB98-4907-833E-9C41C9ADEE76}"/>
+    <hyperlink ref="C6" r:id="rId27" display="LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{72A898E1-E814-40B9-9CCE-853A961F2109}"/>
+    <hyperlink ref="H6" r:id="rId28" xr:uid="{4A93039F-9FB8-42CB-9ACE-C0BE7F576AAE}"/>
+    <hyperlink ref="D28" r:id="rId29" xr:uid="{ADDAE6FC-BD5F-4B77-8488-C7AA571E5B74}"/>
     <hyperlink ref="B3" r:id="rId30" xr:uid="{4C8A5F37-6801-432A-83D9-87956E37DC33}"/>
     <hyperlink ref="C3" r:id="rId31" xr:uid="{98DA5743-5463-4C67-80BC-A5B72466CF09}"/>
     <hyperlink ref="H3" r:id="rId32" xr:uid="{8BB37601-C38B-45F2-8233-C6E902C59024}"/>
     <hyperlink ref="I3" r:id="rId33" xr:uid="{867E547C-77C0-4645-B477-E04A428B234D}"/>
+    <hyperlink ref="H4" r:id="rId34" xr:uid="{E7256B83-DC26-4708-AE9C-81FB186678F7}"/>
+    <hyperlink ref="E4" r:id="rId35" xr:uid="{D50736A5-4DBC-478E-9DE0-ABB9D0062209}"/>
+    <hyperlink ref="D4" r:id="rId36" xr:uid="{69779EF0-F236-481C-A058-70D6A46D05A2}"/>
+    <hyperlink ref="B4" r:id="rId37" xr:uid="{D3894DA7-9C12-4B05-8D36-237B29B85F74}"/>
+    <hyperlink ref="I4" r:id="rId38" xr:uid="{80743E67-671B-43D1-A4CD-D302F8246EAB}"/>
+    <hyperlink ref="C4" r:id="rId39" xr:uid="{A9B3E11E-DA4C-432B-9EA4-560C3B1DE7F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
 
@@ -3358,18 +3431,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3467,7 +3540,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3514,7 +3587,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3564,7 +3637,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3611,7 +3684,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3627,7 +3700,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -3639,7 +3712,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -3650,7 +3723,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3672,7 +3745,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3685,7 +3758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -3701,7 +3774,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3715,7 +3788,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -3731,7 +3804,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3745,7 +3818,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -3787,7 +3860,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -3813,7 +3886,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3824,7 +3897,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -3839,7 +3912,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -3897,12 +3970,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3973,7 +4046,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4020,7 +4093,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4036,7 +4109,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -4067,7 +4140,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4075,7 +4148,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -4108,20 +4181,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.33203125" customWidth="1"/>
-    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.28515625" customWidth="1"/>
+    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4210,7 +4283,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4258,7 +4331,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4274,7 +4347,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -4294,7 +4367,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -4313,7 +4386,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -4332,7 +4405,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -4340,7 +4413,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -4348,7 +4421,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -4365,7 +4438,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -4382,7 +4455,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -4399,7 +4472,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -4416,7 +4489,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -4427,7 +4500,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -4438,7 +4511,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4455,7 +4528,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -4484,7 +4557,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4495,7 +4568,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4509,7 +4582,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -4523,7 +4596,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -4537,7 +4610,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -4545,7 +4618,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -4575,7 +4648,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -4645,19 +4718,19 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.6640625" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4683,7 +4756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4706,7 +4779,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -4737,16 +4810,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4760,7 +4833,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -4786,27 +4859,27 @@
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5546875" customWidth="1"/>
-    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5703125" customWidth="1"/>
+    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.109375" customWidth="1"/>
+    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.140625" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -4865,7 +4938,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>228</v>
       </c>
@@ -4890,7 +4963,7 @@
       <c r="R2" s="22"/>
       <c r="S2" s="22"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>230</v>
       </c>
@@ -4919,7 +4992,7 @@
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>232</v>
       </c>
@@ -4944,7 +5017,7 @@
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>233</v>
       </c>
@@ -4971,7 +5044,7 @@
       <c r="R5" s="22"/>
       <c r="S5" s="22"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>236</v>
       </c>
@@ -5004,7 +5077,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>238</v>
       </c>
@@ -5029,7 +5102,7 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>262</v>
       </c>
@@ -5054,7 +5127,7 @@
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>281</v>
       </c>
@@ -5079,7 +5152,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>286</v>
       </c>
@@ -5106,7 +5179,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>319</v>
       </c>
@@ -5131,7 +5204,7 @@
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>321</v>
       </c>
@@ -5158,7 +5231,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>322</v>
       </c>
@@ -5183,7 +5256,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>324</v>
       </c>
@@ -5208,7 +5281,7 @@
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>335</v>
       </c>
@@ -5233,7 +5306,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>338</v>
       </c>
@@ -5258,7 +5331,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>451</v>
       </c>
@@ -5266,7 +5339,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>452</v>
       </c>
@@ -5274,7 +5347,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>453</v>
       </c>
@@ -5296,31 +5369,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.6640625" customWidth="1"/>
-    <col min="17" max="24" width="30.5546875" customWidth="1"/>
-    <col min="25" max="25" width="19.6640625" customWidth="1"/>
-    <col min="26" max="27" width="22.33203125" customWidth="1"/>
-    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.7109375" customWidth="1"/>
+    <col min="17" max="24" width="30.5703125" customWidth="1"/>
+    <col min="25" max="25" width="19.7109375" customWidth="1"/>
+    <col min="26" max="27" width="22.28515625" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.33203125" customWidth="1"/>
+    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5472,7 +5545,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5542,7 +5615,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>456</v>
       </c>
@@ -5612,7 +5685,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>458</v>
       </c>
@@ -5682,7 +5755,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>459</v>
       </c>
@@ -5752,7 +5825,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>462</v>
       </c>
@@ -5822,7 +5895,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>466</v>
       </c>
@@ -5892,7 +5965,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>470</v>
       </c>
@@ -5933,7 +6006,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>471</v>
       </c>
@@ -5974,7 +6047,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>464</v>
       </c>
@@ -6044,7 +6117,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>407</v>
       </c>
@@ -6105,7 +6178,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>295</v>
       </c>
@@ -6164,7 +6237,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>360</v>
       </c>
@@ -6210,7 +6283,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6233,7 +6306,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>298</v>
       </c>
@@ -6256,7 +6329,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -6275,7 +6348,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6286,7 +6359,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6308,7 +6381,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>367</v>
       </c>
@@ -6321,7 +6394,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>369</v>
       </c>
@@ -6334,7 +6407,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>371</v>
       </c>
@@ -6347,7 +6420,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>376</v>
       </c>
@@ -6360,7 +6433,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>398</v>
       </c>
@@ -6373,7 +6446,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>377</v>
       </c>
@@ -6386,7 +6459,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>379</v>
       </c>
@@ -6402,7 +6475,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>381</v>
       </c>
@@ -6418,7 +6491,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>402</v>
       </c>
@@ -6437,7 +6510,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>406</v>
       </c>
@@ -6456,7 +6529,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>383</v>
       </c>
@@ -6472,7 +6545,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>386</v>
       </c>
@@ -6488,7 +6561,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>412</v>
       </c>
@@ -6504,7 +6577,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>413</v>
       </c>
@@ -6520,7 +6593,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>387</v>
       </c>
@@ -6536,7 +6609,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>390</v>
       </c>
@@ -6549,7 +6622,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>404</v>
       </c>
@@ -6562,7 +6635,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>391</v>
       </c>
@@ -6575,7 +6648,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>425</v>
       </c>
@@ -6588,7 +6661,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>399</v>
       </c>
@@ -6601,7 +6674,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>395</v>
       </c>
@@ -6617,7 +6690,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>424</v>
       </c>
@@ -6633,7 +6706,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>396</v>
       </c>
@@ -6649,7 +6722,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>403</v>
       </c>
@@ -6662,7 +6735,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>416</v>
       </c>
@@ -6684,7 +6757,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -6702,7 +6775,7 @@
       <c r="AI44" s="27"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>415</v>
       </c>
@@ -6715,7 +6788,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -6735,7 +6808,7 @@
       <c r="AI46" s="27"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -6754,7 +6827,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -6767,7 +6840,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -6778,7 +6851,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -6791,7 +6864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -6814,7 +6887,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -6828,7 +6901,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -6865,7 +6938,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -6879,7 +6952,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -6921,7 +6994,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -6947,7 +7020,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -6971,7 +7044,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -6995,7 +7068,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -7021,7 +7094,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -7053,7 +7126,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -7067,7 +7140,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>374</v>
       </c>
@@ -7081,7 +7154,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -7098,7 +7171,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -7115,7 +7188,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>340</v>
       </c>
@@ -7137,7 +7210,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>344</v>
       </c>
@@ -7145,7 +7218,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>347</v>
       </c>
@@ -7156,7 +7229,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>349</v>
       </c>
@@ -7173,7 +7246,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>354</v>
       </c>
@@ -7181,7 +7254,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -7216,7 +7289,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>364</v>
       </c>
@@ -7307,36 +7380,36 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -7473,7 +7546,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
@@ -7548,7 +7621,7 @@
       <c r="AR2" s="22"/>
       <c r="AS2" s="22"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
@@ -7605,7 +7678,7 @@
       <c r="AR3" s="22"/>
       <c r="AS3" s="22"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>248</v>
       </c>
@@ -7658,7 +7731,7 @@
       <c r="AR4" s="22"/>
       <c r="AS4" s="22"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>68</v>
       </c>
@@ -7721,7 +7794,7 @@
       <c r="AR5" s="22"/>
       <c r="AS5" s="22"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>75</v>
       </c>
@@ -7800,7 +7873,7 @@
       <c r="AR6" s="22"/>
       <c r="AS6" s="22"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>81</v>
       </c>
@@ -7889,7 +7962,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>100</v>
       </c>
@@ -7972,7 +8045,7 @@
       <c r="AR8" s="22"/>
       <c r="AS8" s="22"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>95</v>
       </c>
@@ -8057,7 +8130,7 @@
       <c r="AR9" s="22"/>
       <c r="AS9" s="22"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>40</v>
       </c>
@@ -8108,7 +8181,7 @@
       <c r="AR10" s="22"/>
       <c r="AS10" s="22"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>103</v>
       </c>
@@ -8165,7 +8238,7 @@
       <c r="AR11" s="22"/>
       <c r="AS11" s="22"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>107</v>
       </c>
@@ -8240,7 +8313,7 @@
       <c r="AR12" s="22"/>
       <c r="AS12" s="22"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>112</v>
       </c>
@@ -8303,7 +8376,7 @@
       <c r="AR13" s="22"/>
       <c r="AS13" s="22"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>249</v>
       </c>
@@ -8358,7 +8431,7 @@
       <c r="AR14" s="22"/>
       <c r="AS14" s="22"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>119</v>
       </c>
@@ -8415,7 +8488,7 @@
       <c r="AR15" s="22"/>
       <c r="AS15" s="22"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>121</v>
       </c>
@@ -8470,7 +8543,7 @@
       <c r="AR16" s="22"/>
       <c r="AS16" s="22"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>219</v>
       </c>
@@ -8525,7 +8598,7 @@
       <c r="AR17" s="22"/>
       <c r="AS17" s="22"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>154</v>
       </c>
@@ -8617,13 +8690,13 @@
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8700,7 +8773,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -8730,25 +8803,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.44140625" customWidth="1"/>
-    <col min="32" max="32" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.42578125" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8849,7 +8922,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -8935,7 +9008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -8967,7 +9040,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -8993,25 +9066,25 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.44140625" customWidth="1"/>
-    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9097,7 +9170,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9144,7 +9217,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9160,7 +9233,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -9179,7 +9252,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>178</v>
       </c>
@@ -9192,7 +9265,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>179</v>
       </c>
@@ -9205,7 +9278,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>153</v>
       </c>
@@ -9216,7 +9289,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -9224,7 +9297,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -9232,7 +9305,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>168</v>
       </c>
@@ -9240,7 +9313,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -9259,7 +9332,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -9270,7 +9343,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -9285,7 +9358,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -9301,7 +9374,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -9328,7 +9401,7 @@
       </c>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -9342,7 +9415,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -9358,7 +9431,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>201</v>
       </c>
@@ -9395,7 +9468,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>241</v>
       </c>
@@ -9403,7 +9476,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -9426,7 +9499,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>166</v>
       </c>
@@ -9483,17 +9556,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -9528,7 +9601,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>243</v>
       </c>
@@ -9537,7 +9610,7 @@
       </c>
       <c r="C2" s="22"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>245</v>
       </c>
@@ -9546,7 +9619,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>247</v>
       </c>
@@ -9555,7 +9628,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>313</v>
       </c>
@@ -9577,20 +9650,20 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9658,7 +9731,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9702,7 +9775,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9718,7 +9791,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -9736,7 +9809,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -9744,7 +9817,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -9752,7 +9825,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -9789,37 +9862,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9902,7 +9975,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9943,7 +10016,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9959,7 +10032,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -9971,7 +10044,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -9989,7 +10062,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -9998,7 +10071,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -10010,7 +10083,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -10036,7 +10109,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -10047,7 +10120,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -10061,7 +10134,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
HF_EMEA TEST_DGLD_HF_EMEA_BCT_001 Changes with Testdata Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA872DC-CA8B-4E86-A5FF-2447AB368509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{ADA872DC-CA8B-4E86-A5FF-2447AB368509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69E6C548-07FB-4B82-A7BE-046737449FF7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="11952" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="534">
   <si>
     <t>UserName</t>
   </si>
@@ -1499,25 +1499,10 @@
     <t>24 oz,32 oz</t>
   </si>
   <si>
-    <t>Bottles,Cups &amp; Tumblers,Coffee &amp; Tea,Accessories</t>
-  </si>
-  <si>
-    <t>Insulated Totes,Soft Coolers</t>
-  </si>
-  <si>
     <t>Food Jars</t>
   </si>
   <si>
-    <t>Bottle Boots,Caps and Lids,Cleaning</t>
-  </si>
-  <si>
-    <t>Our Story,Contact,Refill For Good,Every Bottle Tells A Story</t>
-  </si>
-  <si>
     <t>Micro Hydro,Spring Style Guide,Fitness Collection</t>
-  </si>
-  <si>
-    <t>Exclusives,New Arrivals,Best Sellers</t>
   </si>
   <si>
     <t>HFEMEA20OFF</t>
@@ -1655,6 +1640,27 @@
   </si>
   <si>
     <t>Qa Test - 69 Aire Street, Knottingley, WEST YORKSHIRE, WF11 9AZ</t>
+  </si>
+  <si>
+    <t>Bottles,Travel Tumbler,Coffee &amp; Tea,Accessories</t>
+  </si>
+  <si>
+    <t>Bottle Boots,Caps &amp; Lids,Cleaning</t>
+  </si>
+  <si>
+    <t>New Arrivals,Best Sellers</t>
+  </si>
+  <si>
+    <t>Our Story,Contact,Refill For Good,Blog</t>
+  </si>
+  <si>
+    <t>Food Jars,Insulated Totes,Soft Coolers</t>
+  </si>
+  <si>
+    <t>Shopby Collections</t>
+  </si>
+  <si>
+    <t>Micro Hydro</t>
   </si>
 </sst>
 </file>
@@ -2188,34 +2194,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="M21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="S55" sqref="S55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="21" width="22.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="18" width="30.5546875" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="21" width="22.33203125" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.28515625" customWidth="1"/>
+    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2358,15 +2364,15 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -2381,10 +2387,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -2396,16 +2402,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="T2" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="V2" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>59</v>
@@ -2413,15 +2419,15 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="7"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>295</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2436,10 +2442,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -2451,16 +2457,16 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="T3" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="V3" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>59</v>
@@ -2468,15 +2474,15 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:47" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>29</v>
@@ -2491,10 +2497,10 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -2506,16 +2512,16 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="15" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="T4" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="V4" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="W4" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>59</v>
@@ -2523,7 +2529,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>360</v>
       </c>
@@ -2563,7 +2569,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>439</v>
       </c>
@@ -2601,16 +2607,16 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="T6" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="V6" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="X6" s="5" t="s">
         <v>59</v>
@@ -2618,7 +2624,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2634,7 +2640,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>199</v>
       </c>
@@ -2646,7 +2652,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>298</v>
       </c>
@@ -2662,7 +2668,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2674,12 +2680,12 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>154</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="W11" s="3"/>
       <c r="X11" s="4"/>
@@ -2687,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>172</v>
       </c>
@@ -2706,7 +2712,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>170</v>
       </c>
@@ -2719,7 +2725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2747,7 +2753,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>445</v>
       </c>
@@ -2761,7 +2767,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>176</v>
       </c>
@@ -2780,7 +2786,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>175</v>
       </c>
@@ -2793,7 +2799,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>189</v>
       </c>
@@ -2804,7 +2810,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -2828,7 +2834,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -2841,7 +2847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2851,13 +2857,13 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="AI21" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="AJ21" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2871,7 +2877,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -2908,7 +2914,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2922,7 +2928,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -2964,7 +2970,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2978,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -2989,25 +2995,25 @@
         <v>15</v>
       </c>
       <c r="S27" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="T27" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="U27" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="V27" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="W27" s="5" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="X27" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -3024,16 +3030,16 @@
         <v>469</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>77</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="E29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="I29" s="2"/>
       <c r="W29" s="5"/>
@@ -3041,7 +3047,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>118</v>
       </c>
@@ -3052,25 +3058,25 @@
         <v>15</v>
       </c>
       <c r="S30" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="T30" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="U30" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="V30" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="W30" s="5" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="X30" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -3078,7 +3084,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -3089,7 +3095,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>166</v>
       </c>
@@ -3110,25 +3116,25 @@
       <c r="Q33" s="12"/>
       <c r="R33" s="12"/>
       <c r="S33" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="T33" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="U33" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="V33" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="W33" s="5" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="X33" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>184</v>
       </c>
@@ -3143,7 +3149,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>279</v>
       </c>
@@ -3151,7 +3157,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>284</v>
       </c>
@@ -3165,7 +3171,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>215</v>
       </c>
@@ -3182,7 +3188,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>209</v>
       </c>
@@ -3199,7 +3205,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>340</v>
       </c>
@@ -3215,14 +3221,14 @@
         <v>342</v>
       </c>
       <c r="P39" s="28" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="Q39" s="5" t="s">
         <v>356</v>
       </c>
       <c r="R39" s="5"/>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>344</v>
       </c>
@@ -3230,7 +3236,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>347</v>
       </c>
@@ -3238,13 +3244,13 @@
         <v>431</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="N41" s="26" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>349</v>
       </c>
@@ -3255,21 +3261,21 @@
         <v>350</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="AO42" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>354</v>
       </c>
       <c r="P43" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>201</v>
       </c>
@@ -3304,7 +3310,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>364</v>
       </c>
@@ -3312,7 +3318,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>433</v>
       </c>
@@ -3320,15 +3326,15 @@
         <v>435</v>
       </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>434</v>
       </c>
       <c r="P47" s="28" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>232</v>
       </c>
@@ -3336,7 +3342,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" s="35" t="s">
         <v>153</v>
       </c>
@@ -3375,28 +3381,28 @@
       </c>
       <c r="AE49" s="35"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>449</v>
       </c>
       <c r="P50" s="28" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="P51" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="S52" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -3454,18 +3460,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3563,7 +3569,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3610,7 +3616,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3660,7 +3666,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3707,7 +3713,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3723,7 +3729,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -3735,7 +3741,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -3746,7 +3752,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3768,7 +3774,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3781,7 +3787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -3797,7 +3803,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3811,7 +3817,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -3827,7 +3833,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3841,7 +3847,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -3883,7 +3889,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -3909,7 +3915,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3920,7 +3926,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -3935,7 +3941,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -3993,12 +3999,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4069,7 +4075,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4116,7 +4122,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4132,7 +4138,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -4163,7 +4169,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4171,7 +4177,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -4204,20 +4210,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.28515625" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4306,7 +4312,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4354,7 +4360,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4370,7 +4376,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -4390,7 +4396,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -4409,7 +4415,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -4428,7 +4434,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -4436,7 +4442,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -4444,7 +4450,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -4461,7 +4467,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -4478,7 +4484,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -4495,7 +4501,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -4512,7 +4518,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -4523,7 +4529,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -4534,7 +4540,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4551,7 +4557,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -4580,7 +4586,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4591,7 +4597,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4605,7 +4611,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -4619,7 +4625,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -4633,7 +4639,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -4641,7 +4647,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -4671,7 +4677,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -4741,19 +4747,19 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4779,7 +4785,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4802,7 +4808,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -4833,16 +4839,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4856,12 +4862,12 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>152</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>261</v>
@@ -4876,33 +4882,33 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAA7450-0FE7-4C50-95DC-266117BAF81B}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I18" activeCellId="1" sqref="J20 I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5703125" customWidth="1"/>
-    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5546875" customWidth="1"/>
+    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.140625" customWidth="1"/>
+    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.109375" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -4961,12 +4967,12 @@
         <v>436</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>228</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>483</v>
+        <v>527</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -4986,7 +4992,7 @@
       <c r="R2" s="22"/>
       <c r="S2" s="22"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>230</v>
       </c>
@@ -4996,7 +5002,7 @@
         <v>265</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>276</v>
@@ -5015,7 +5021,7 @@
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>232</v>
       </c>
@@ -5027,7 +5033,7 @@
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22" t="s">
-        <v>486</v>
+        <v>528</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
@@ -5040,7 +5046,7 @@
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>233</v>
       </c>
@@ -5055,7 +5061,7 @@
       <c r="H5" s="22"/>
       <c r="I5" s="32"/>
       <c r="J5" s="22" t="s">
-        <v>489</v>
+        <v>529</v>
       </c>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
@@ -5067,7 +5073,7 @@
       <c r="R5" s="22"/>
       <c r="S5" s="22"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>236</v>
       </c>
@@ -5100,7 +5106,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>238</v>
       </c>
@@ -5116,7 +5122,7 @@
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
       <c r="M7" s="30" t="s">
-        <v>487</v>
+        <v>530</v>
       </c>
       <c r="N7" s="22"/>
       <c r="O7" s="22"/>
@@ -5125,7 +5131,7 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>262</v>
       </c>
@@ -5150,7 +5156,7 @@
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>281</v>
       </c>
@@ -5158,7 +5164,7 @@
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22" t="s">
-        <v>484</v>
+        <v>531</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
@@ -5175,7 +5181,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>286</v>
       </c>
@@ -5202,7 +5208,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>319</v>
       </c>
@@ -5227,7 +5233,7 @@
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>321</v>
       </c>
@@ -5237,7 +5243,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
       <c r="G12" s="37" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="H12" s="30" t="s">
         <v>468</v>
@@ -5254,7 +5260,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>322</v>
       </c>
@@ -5279,7 +5285,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>324</v>
       </c>
@@ -5304,7 +5310,7 @@
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>335</v>
       </c>
@@ -5329,7 +5335,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>338</v>
       </c>
@@ -5354,7 +5360,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>451</v>
       </c>
@@ -5362,7 +5368,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>452</v>
       </c>
@@ -5370,12 +5376,20 @@
         <v>455</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>453</v>
       </c>
       <c r="Q19" t="s">
         <v>454</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>532</v>
+      </c>
+      <c r="J20" t="s">
+        <v>533</v>
       </c>
     </row>
   </sheetData>
@@ -5392,31 +5406,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.7109375" customWidth="1"/>
-    <col min="17" max="24" width="30.5703125" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" customWidth="1"/>
-    <col min="26" max="27" width="22.28515625" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.6640625" customWidth="1"/>
+    <col min="17" max="24" width="30.5546875" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" customWidth="1"/>
+    <col min="26" max="27" width="22.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.28515625" customWidth="1"/>
+    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5568,7 +5582,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5638,7 +5652,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>456</v>
       </c>
@@ -5708,7 +5722,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>458</v>
       </c>
@@ -5778,7 +5792,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>459</v>
       </c>
@@ -5848,7 +5862,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>462</v>
       </c>
@@ -5918,7 +5932,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>466</v>
       </c>
@@ -5988,7 +6002,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>470</v>
       </c>
@@ -6029,7 +6043,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>471</v>
       </c>
@@ -6070,7 +6084,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>464</v>
       </c>
@@ -6140,7 +6154,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>407</v>
       </c>
@@ -6201,7 +6215,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>295</v>
       </c>
@@ -6260,7 +6274,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>360</v>
       </c>
@@ -6306,7 +6320,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6329,7 +6343,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>298</v>
       </c>
@@ -6352,7 +6366,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -6371,7 +6385,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6382,7 +6396,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6404,7 +6418,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>367</v>
       </c>
@@ -6417,7 +6431,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>369</v>
       </c>
@@ -6430,7 +6444,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>371</v>
       </c>
@@ -6443,7 +6457,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>376</v>
       </c>
@@ -6456,7 +6470,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>398</v>
       </c>
@@ -6469,7 +6483,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>377</v>
       </c>
@@ -6482,7 +6496,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>379</v>
       </c>
@@ -6498,7 +6512,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>381</v>
       </c>
@@ -6514,7 +6528,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>402</v>
       </c>
@@ -6533,7 +6547,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>406</v>
       </c>
@@ -6552,7 +6566,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>383</v>
       </c>
@@ -6568,7 +6582,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>386</v>
       </c>
@@ -6584,7 +6598,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>412</v>
       </c>
@@ -6600,7 +6614,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>413</v>
       </c>
@@ -6616,7 +6630,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>387</v>
       </c>
@@ -6632,7 +6646,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>390</v>
       </c>
@@ -6645,7 +6659,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>404</v>
       </c>
@@ -6658,7 +6672,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>391</v>
       </c>
@@ -6671,7 +6685,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>425</v>
       </c>
@@ -6684,7 +6698,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>399</v>
       </c>
@@ -6697,7 +6711,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>395</v>
       </c>
@@ -6713,7 +6727,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>424</v>
       </c>
@@ -6729,7 +6743,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>396</v>
       </c>
@@ -6745,7 +6759,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>403</v>
       </c>
@@ -6758,7 +6772,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>416</v>
       </c>
@@ -6780,7 +6794,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -6798,7 +6812,7 @@
       <c r="AI44" s="27"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>415</v>
       </c>
@@ -6811,7 +6825,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -6831,7 +6845,7 @@
       <c r="AI46" s="27"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -6850,7 +6864,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -6863,7 +6877,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -6874,7 +6888,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -6887,7 +6901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -6910,7 +6924,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -6924,7 +6938,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -6961,7 +6975,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -6975,7 +6989,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -7017,7 +7031,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -7043,7 +7057,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -7067,7 +7081,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -7091,7 +7105,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -7117,7 +7131,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -7149,7 +7163,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -7163,7 +7177,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>374</v>
       </c>
@@ -7177,7 +7191,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -7194,7 +7208,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -7211,7 +7225,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>340</v>
       </c>
@@ -7233,7 +7247,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>344</v>
       </c>
@@ -7241,7 +7255,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>347</v>
       </c>
@@ -7252,7 +7266,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>349</v>
       </c>
@@ -7269,7 +7283,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>354</v>
       </c>
@@ -7277,7 +7291,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -7312,7 +7326,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>364</v>
       </c>
@@ -7403,36 +7417,36 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -7569,7 +7583,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
@@ -7601,16 +7615,16 @@
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="22" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="O2" s="22" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="P2" s="22" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="Q2" s="22">
         <v>9898989898</v>
@@ -7644,7 +7658,7 @@
       <c r="AR2" s="22"/>
       <c r="AS2" s="22"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
@@ -7701,7 +7715,7 @@
       <c r="AR3" s="22"/>
       <c r="AS3" s="22"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>248</v>
       </c>
@@ -7754,7 +7768,7 @@
       <c r="AR4" s="22"/>
       <c r="AS4" s="22"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>68</v>
       </c>
@@ -7771,7 +7785,7 @@
         <v>333</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="K5" s="31"/>
       <c r="L5" s="22"/>
@@ -7817,7 +7831,7 @@
       <c r="AR5" s="22"/>
       <c r="AS5" s="22"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>75</v>
       </c>
@@ -7842,21 +7856,21 @@
         <v>67</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="K6" s="31"/>
       <c r="L6" s="22"/>
       <c r="M6" s="22" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="Q6" s="22">
         <v>9898989898</v>
@@ -7896,12 +7910,12 @@
       <c r="AR6" s="22"/>
       <c r="AS6" s="22"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>81</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="22"/>
@@ -7915,23 +7929,23 @@
         <v>96</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="K7" s="31"/>
       <c r="L7" s="22" t="s">
         <v>81</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="O7" s="22" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="Q7" s="22">
         <v>9898989898</v>
@@ -7985,12 +7999,12 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>100</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="22"/>
@@ -8004,23 +8018,23 @@
         <v>96</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="K8" s="31"/>
       <c r="L8" s="22" t="s">
         <v>100</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="N8" s="22" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="O8" s="22" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="P8" s="22" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="Q8" s="22">
         <v>9898989898</v>
@@ -8068,12 +8082,12 @@
       <c r="AR8" s="22"/>
       <c r="AS8" s="22"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>95</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="22"/>
@@ -8087,23 +8101,23 @@
         <v>96</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="K9" s="31"/>
       <c r="L9" s="22" t="s">
         <v>95</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="N9" s="22" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="P9" s="22" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="Q9" s="22">
         <v>9898989898</v>
@@ -8153,7 +8167,7 @@
       <c r="AR9" s="22"/>
       <c r="AS9" s="22"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>40</v>
       </c>
@@ -8204,7 +8218,7 @@
       <c r="AR10" s="22"/>
       <c r="AS10" s="22"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>103</v>
       </c>
@@ -8261,7 +8275,7 @@
       <c r="AR11" s="22"/>
       <c r="AS11" s="22"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>107</v>
       </c>
@@ -8278,23 +8292,23 @@
         <v>67</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="22" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="P12" s="22" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="Q12" s="22">
         <v>9898989898</v>
@@ -8336,7 +8350,7 @@
       <c r="AR12" s="22"/>
       <c r="AS12" s="22"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>112</v>
       </c>
@@ -8353,7 +8367,7 @@
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="K13" s="31"/>
       <c r="L13" s="22"/>
@@ -8399,7 +8413,7 @@
       <c r="AR13" s="22"/>
       <c r="AS13" s="22"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>249</v>
       </c>
@@ -8454,7 +8468,7 @@
       <c r="AR14" s="22"/>
       <c r="AS14" s="22"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>119</v>
       </c>
@@ -8511,7 +8525,7 @@
       <c r="AR15" s="22"/>
       <c r="AS15" s="22"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>121</v>
       </c>
@@ -8566,7 +8580,7 @@
       <c r="AR16" s="22"/>
       <c r="AS16" s="22"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>219</v>
       </c>
@@ -8581,7 +8595,7 @@
       </c>
       <c r="I17" s="22"/>
       <c r="J17" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="K17" s="31"/>
       <c r="L17" s="22"/>
@@ -8621,7 +8635,7 @@
       <c r="AR17" s="22"/>
       <c r="AS17" s="22"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>154</v>
       </c>
@@ -8713,13 +8727,13 @@
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8796,7 +8810,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -8826,25 +8840,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8945,7 +8959,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -9031,7 +9045,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -9063,7 +9077,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -9089,25 +9103,25 @@
       <selection activeCell="E28" sqref="E28:E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9193,7 +9207,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9223,16 +9237,16 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="L2" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="M2" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>59</v>
@@ -9240,7 +9254,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9256,7 +9270,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -9275,7 +9289,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>178</v>
       </c>
@@ -9288,7 +9302,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>179</v>
       </c>
@@ -9301,7 +9315,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>153</v>
       </c>
@@ -9312,7 +9326,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -9320,15 +9334,15 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>154</v>
       </c>
       <c r="J9" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>168</v>
       </c>
@@ -9336,7 +9350,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -9355,7 +9369,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -9366,22 +9380,22 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="E13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="I13" s="2"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -9391,13 +9405,13 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="Y14" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="Z14" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -9408,23 +9422,23 @@
         <v>15</v>
       </c>
       <c r="K15" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="L15" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="M15" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="N15" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>59</v>
       </c>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -9438,7 +9452,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -9454,7 +9468,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>201</v>
       </c>
@@ -9491,7 +9505,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>241</v>
       </c>
@@ -9499,7 +9513,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -9522,7 +9536,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>166</v>
       </c>
@@ -9579,17 +9593,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -9624,34 +9638,34 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>243</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="C2" s="22"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>245</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>247</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>313</v>
       </c>
@@ -9673,20 +9687,20 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9754,15 +9768,15 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -9777,7 +9791,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" t="s">
@@ -9798,7 +9812,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9814,25 +9828,25 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>182</v>
       </c>
       <c r="H4" s="2"/>
       <c r="S4" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="T4" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="V4" s="12" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -9840,7 +9854,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -9848,21 +9862,21 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>206</v>
       </c>
       <c r="S7" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="T7" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="V7" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -9885,37 +9899,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9998,7 +10012,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10039,7 +10053,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10055,7 +10069,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -10067,7 +10081,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -10085,7 +10099,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -10094,7 +10108,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -10106,7 +10120,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -10132,7 +10146,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -10143,7 +10157,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -10157,7 +10171,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
HF_EMEA TEST_DGLD_HF_EMEA_BCT_004 Changes with Testdata Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED940B8-D354-4BEC-8B40-F9EBDE1402FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FE2128-8FDC-4B87-A45D-63A62E37D959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="537">
   <si>
     <t>UserName</t>
   </si>
@@ -1659,16 +1659,28 @@
   <si>
     <t>Micro Hydro</t>
   </si>
+  <si>
+    <t>PLP Product</t>
+  </si>
+  <si>
+    <t>Sub Category</t>
+  </si>
+  <si>
+    <t>Caps &amp; Lids</t>
+  </si>
+  <si>
+    <t>24 oz Travel Tumbler - Black</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1802,6 +1814,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1842,12 +1860,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1877,7 +1895,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1908,6 +1926,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2189,36 +2208,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU52"/>
+  <dimension ref="A1:AV53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AC53" sqref="AC53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="21" width="22.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="18" width="30.5546875" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="21" width="22.33203125" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.28515625" customWidth="1"/>
+    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2354,14 +2373,17 @@
       <c r="AS1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AT1" s="43" t="s">
+        <v>534</v>
+      </c>
+      <c r="AU1" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2416,7 +2438,7 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="7"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>295</v>
       </c>
@@ -2471,7 +2493,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:47" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>517</v>
       </c>
@@ -2526,7 +2548,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>360</v>
       </c>
@@ -2568,7 +2590,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>439</v>
       </c>
@@ -2623,7 +2645,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2639,7 +2661,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>199</v>
       </c>
@@ -2651,7 +2673,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>298</v>
       </c>
@@ -2667,7 +2689,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2679,7 +2701,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>154</v>
       </c>
@@ -2692,7 +2714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>172</v>
       </c>
@@ -2711,7 +2733,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>170</v>
       </c>
@@ -2724,7 +2746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2748,11 +2770,11 @@
       <c r="AH14">
         <v>1</v>
       </c>
-      <c r="AU14" t="s">
+      <c r="AV14" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>445</v>
       </c>
@@ -2766,7 +2788,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>176</v>
       </c>
@@ -2785,7 +2807,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>175</v>
       </c>
@@ -2798,7 +2820,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>189</v>
       </c>
@@ -2809,7 +2831,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -2833,7 +2855,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -2846,7 +2868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2862,7 +2884,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2876,7 +2898,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -2913,7 +2935,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2927,7 +2949,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -2969,7 +2991,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2983,7 +3005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -3012,7 +3034,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -3029,7 +3051,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -3046,7 +3068,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>118</v>
       </c>
@@ -3075,7 +3097,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -3083,7 +3105,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -3094,7 +3116,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>166</v>
       </c>
@@ -3133,7 +3155,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>184</v>
       </c>
@@ -3148,7 +3170,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>279</v>
       </c>
@@ -3156,7 +3178,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>284</v>
       </c>
@@ -3170,7 +3192,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>215</v>
       </c>
@@ -3187,7 +3209,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>209</v>
       </c>
@@ -3204,7 +3226,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>340</v>
       </c>
@@ -3227,7 +3249,7 @@
       </c>
       <c r="R39" s="5"/>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>344</v>
       </c>
@@ -3235,7 +3257,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>347</v>
       </c>
@@ -3249,7 +3271,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>349</v>
       </c>
@@ -3266,7 +3288,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>354</v>
       </c>
@@ -3274,7 +3296,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>201</v>
       </c>
@@ -3309,7 +3331,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>364</v>
       </c>
@@ -3317,7 +3339,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>433</v>
       </c>
@@ -3325,7 +3347,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>434</v>
       </c>
@@ -3333,15 +3355,18 @@
         <v>515</v>
       </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>232</v>
       </c>
-      <c r="AT48" s="33" t="s">
+      <c r="AT48" t="s">
+        <v>535</v>
+      </c>
+      <c r="AU48" s="33" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" s="35" t="s">
         <v>153</v>
       </c>
@@ -3380,7 +3405,7 @@
       </c>
       <c r="AE49" s="35"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>449</v>
       </c>
@@ -3388,7 +3413,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>513</v>
       </c>
@@ -3396,12 +3421,20 @@
         <v>512</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>524</v>
       </c>
       <c r="S52" t="s">
         <v>525</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>533</v>
+      </c>
+      <c r="AC53" s="12" t="s">
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -3448,9 +3481,10 @@
     <hyperlink ref="I5" r:id="rId40" xr:uid="{92993A7C-001C-4FE6-9125-B4B00E04A753}"/>
     <hyperlink ref="H28" r:id="rId41" xr:uid="{22165C55-D8F7-4059-A2E1-F084718509FB}"/>
     <hyperlink ref="I28" r:id="rId42" xr:uid="{42C11063-5B1A-455C-98C2-65B906145796}"/>
+    <hyperlink ref="AC53" r:id="rId43" display="https://mcloud-na-stage4.hydroflask.com/gb/hydroflask-24-oz-travel-tumbler-black" xr:uid="{641B22C5-1E50-466C-8002-3D1A661FD7B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId43"/>
+  <pageSetup orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
 
@@ -3462,18 +3496,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3571,7 +3605,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3618,7 +3652,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3668,7 +3702,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3715,7 +3749,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3731,7 +3765,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -3743,7 +3777,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -3754,7 +3788,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3776,7 +3810,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3789,7 +3823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -3805,7 +3839,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3819,7 +3853,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -3835,7 +3869,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3849,7 +3883,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -3891,7 +3925,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -3917,7 +3951,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3928,7 +3962,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -3943,7 +3977,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -4001,12 +4035,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4077,7 +4111,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4124,7 +4158,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4140,7 +4174,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -4171,7 +4205,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4179,7 +4213,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -4212,20 +4246,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.28515625" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4314,7 +4348,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4362,7 +4396,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4378,7 +4412,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -4398,7 +4432,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -4417,7 +4451,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -4436,7 +4470,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -4444,7 +4478,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -4452,7 +4486,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -4469,7 +4503,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -4486,7 +4520,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -4503,7 +4537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -4520,7 +4554,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -4531,7 +4565,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -4542,7 +4576,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4559,7 +4593,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -4588,7 +4622,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4599,7 +4633,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4613,7 +4647,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -4627,7 +4661,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -4641,7 +4675,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -4649,7 +4683,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -4679,7 +4713,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -4749,19 +4783,19 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4787,7 +4821,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4810,7 +4844,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -4841,16 +4875,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4864,7 +4898,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -4890,27 +4924,27 @@
       <selection activeCell="I18" activeCellId="1" sqref="J20 I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5703125" customWidth="1"/>
-    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5546875" customWidth="1"/>
+    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.140625" customWidth="1"/>
+    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.109375" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -4969,7 +5003,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>228</v>
       </c>
@@ -4994,7 +5028,7 @@
       <c r="R2" s="22"/>
       <c r="S2" s="22"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>230</v>
       </c>
@@ -5023,7 +5057,7 @@
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>232</v>
       </c>
@@ -5048,7 +5082,7 @@
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>233</v>
       </c>
@@ -5075,7 +5109,7 @@
       <c r="R5" s="22"/>
       <c r="S5" s="22"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>236</v>
       </c>
@@ -5108,7 +5142,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>238</v>
       </c>
@@ -5133,7 +5167,7 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>262</v>
       </c>
@@ -5158,7 +5192,7 @@
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>281</v>
       </c>
@@ -5183,7 +5217,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>286</v>
       </c>
@@ -5210,7 +5244,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>319</v>
       </c>
@@ -5235,7 +5269,7 @@
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>321</v>
       </c>
@@ -5262,7 +5296,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>322</v>
       </c>
@@ -5287,7 +5321,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>324</v>
       </c>
@@ -5312,7 +5346,7 @@
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>335</v>
       </c>
@@ -5337,7 +5371,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>338</v>
       </c>
@@ -5362,7 +5396,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>451</v>
       </c>
@@ -5370,7 +5404,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>452</v>
       </c>
@@ -5378,7 +5412,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>453</v>
       </c>
@@ -5386,7 +5420,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>531</v>
       </c>
@@ -5408,31 +5442,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.7109375" customWidth="1"/>
-    <col min="17" max="24" width="30.5703125" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" customWidth="1"/>
-    <col min="26" max="27" width="22.28515625" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.6640625" customWidth="1"/>
+    <col min="17" max="24" width="30.5546875" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" customWidth="1"/>
+    <col min="26" max="27" width="22.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.28515625" customWidth="1"/>
+    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5584,7 +5618,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5654,7 +5688,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>456</v>
       </c>
@@ -5724,7 +5758,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>458</v>
       </c>
@@ -5794,7 +5828,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>459</v>
       </c>
@@ -5864,7 +5898,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>462</v>
       </c>
@@ -5934,7 +5968,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>466</v>
       </c>
@@ -6004,7 +6038,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>469</v>
       </c>
@@ -6045,7 +6079,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>470</v>
       </c>
@@ -6086,7 +6120,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>464</v>
       </c>
@@ -6156,7 +6190,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>407</v>
       </c>
@@ -6217,7 +6251,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>295</v>
       </c>
@@ -6276,7 +6310,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>360</v>
       </c>
@@ -6322,7 +6356,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6345,7 +6379,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>298</v>
       </c>
@@ -6368,7 +6402,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -6387,7 +6421,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6398,7 +6432,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6420,7 +6454,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>367</v>
       </c>
@@ -6433,7 +6467,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>369</v>
       </c>
@@ -6446,7 +6480,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>371</v>
       </c>
@@ -6459,7 +6493,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>376</v>
       </c>
@@ -6472,7 +6506,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>398</v>
       </c>
@@ -6485,7 +6519,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>377</v>
       </c>
@@ -6498,7 +6532,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>379</v>
       </c>
@@ -6514,7 +6548,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>381</v>
       </c>
@@ -6530,7 +6564,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>402</v>
       </c>
@@ -6549,7 +6583,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>406</v>
       </c>
@@ -6568,7 +6602,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>383</v>
       </c>
@@ -6584,7 +6618,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>386</v>
       </c>
@@ -6600,7 +6634,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>412</v>
       </c>
@@ -6616,7 +6650,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>413</v>
       </c>
@@ -6632,7 +6666,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>387</v>
       </c>
@@ -6648,7 +6682,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>390</v>
       </c>
@@ -6661,7 +6695,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>404</v>
       </c>
@@ -6674,7 +6708,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>391</v>
       </c>
@@ -6687,7 +6721,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>425</v>
       </c>
@@ -6700,7 +6734,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>399</v>
       </c>
@@ -6713,7 +6747,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>395</v>
       </c>
@@ -6729,7 +6763,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>424</v>
       </c>
@@ -6745,7 +6779,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>396</v>
       </c>
@@ -6761,7 +6795,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>403</v>
       </c>
@@ -6774,7 +6808,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>416</v>
       </c>
@@ -6796,7 +6830,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -6814,7 +6848,7 @@
       <c r="AI44" s="27"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>415</v>
       </c>
@@ -6827,7 +6861,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -6847,7 +6881,7 @@
       <c r="AI46" s="27"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -6866,7 +6900,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -6879,7 +6913,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -6890,7 +6924,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -6903,7 +6937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -6926,7 +6960,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -6940,7 +6974,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -6977,7 +7011,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -6991,7 +7025,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -7033,7 +7067,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -7059,7 +7093,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -7083,7 +7117,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -7107,7 +7141,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -7133,7 +7167,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -7165,7 +7199,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -7179,7 +7213,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>374</v>
       </c>
@@ -7193,7 +7227,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -7210,7 +7244,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -7227,7 +7261,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>340</v>
       </c>
@@ -7249,7 +7283,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>344</v>
       </c>
@@ -7257,7 +7291,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>347</v>
       </c>
@@ -7268,7 +7302,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>349</v>
       </c>
@@ -7285,7 +7319,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>354</v>
       </c>
@@ -7293,7 +7327,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -7328,7 +7362,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>364</v>
       </c>
@@ -7419,36 +7453,36 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -7585,7 +7619,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
@@ -7660,7 +7694,7 @@
       <c r="AR2" s="22"/>
       <c r="AS2" s="22"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
@@ -7717,7 +7751,7 @@
       <c r="AR3" s="22"/>
       <c r="AS3" s="22"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>248</v>
       </c>
@@ -7770,7 +7804,7 @@
       <c r="AR4" s="22"/>
       <c r="AS4" s="22"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>68</v>
       </c>
@@ -7833,7 +7867,7 @@
       <c r="AR5" s="22"/>
       <c r="AS5" s="22"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>75</v>
       </c>
@@ -7912,7 +7946,7 @@
       <c r="AR6" s="22"/>
       <c r="AS6" s="22"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>81</v>
       </c>
@@ -8001,7 +8035,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>100</v>
       </c>
@@ -8084,7 +8118,7 @@
       <c r="AR8" s="22"/>
       <c r="AS8" s="22"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>95</v>
       </c>
@@ -8169,7 +8203,7 @@
       <c r="AR9" s="22"/>
       <c r="AS9" s="22"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>40</v>
       </c>
@@ -8220,7 +8254,7 @@
       <c r="AR10" s="22"/>
       <c r="AS10" s="22"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>103</v>
       </c>
@@ -8277,7 +8311,7 @@
       <c r="AR11" s="22"/>
       <c r="AS11" s="22"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>107</v>
       </c>
@@ -8352,7 +8386,7 @@
       <c r="AR12" s="22"/>
       <c r="AS12" s="22"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>112</v>
       </c>
@@ -8415,7 +8449,7 @@
       <c r="AR13" s="22"/>
       <c r="AS13" s="22"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>249</v>
       </c>
@@ -8470,7 +8504,7 @@
       <c r="AR14" s="22"/>
       <c r="AS14" s="22"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>119</v>
       </c>
@@ -8527,7 +8561,7 @@
       <c r="AR15" s="22"/>
       <c r="AS15" s="22"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>121</v>
       </c>
@@ -8582,7 +8616,7 @@
       <c r="AR16" s="22"/>
       <c r="AS16" s="22"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>219</v>
       </c>
@@ -8637,7 +8671,7 @@
       <c r="AR17" s="22"/>
       <c r="AS17" s="22"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>154</v>
       </c>
@@ -8729,13 +8763,13 @@
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8812,7 +8846,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -8842,25 +8876,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8961,7 +8995,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -9047,7 +9081,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -9079,7 +9113,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -9105,25 +9139,25 @@
       <selection activeCell="E28" sqref="E28:E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9209,7 +9243,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9256,7 +9290,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9272,7 +9306,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -9291,7 +9325,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>178</v>
       </c>
@@ -9304,7 +9338,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>179</v>
       </c>
@@ -9317,7 +9351,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>153</v>
       </c>
@@ -9328,7 +9362,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -9336,7 +9370,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -9344,7 +9378,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>168</v>
       </c>
@@ -9352,7 +9386,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -9371,7 +9405,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -9382,7 +9416,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -9397,7 +9431,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -9413,7 +9447,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -9440,7 +9474,7 @@
       </c>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -9454,7 +9488,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -9470,7 +9504,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>201</v>
       </c>
@@ -9507,7 +9541,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>241</v>
       </c>
@@ -9515,7 +9549,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -9538,7 +9572,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>166</v>
       </c>
@@ -9595,17 +9629,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
@@ -9640,7 +9674,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>243</v>
       </c>
@@ -9649,7 +9683,7 @@
       </c>
       <c r="C2" s="22"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>245</v>
       </c>
@@ -9658,7 +9692,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>247</v>
       </c>
@@ -9667,7 +9701,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>313</v>
       </c>
@@ -9689,20 +9723,20 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9770,7 +9804,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9814,7 +9848,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9830,7 +9864,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -9848,7 +9882,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -9856,7 +9890,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -9864,7 +9898,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -9901,37 +9935,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10014,7 +10048,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10055,7 +10089,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10071,7 +10105,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -10083,7 +10117,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -10101,7 +10135,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -10110,7 +10144,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -10122,7 +10156,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -10148,7 +10182,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -10159,7 +10193,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -10173,7 +10207,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
HF-EMEA:- Added Assertion and changed the Product
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E5C223-B2D8-402A-A583-042CE71D3AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3510F04D-FDEB-4503-AFC2-C4F4D58862F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1666,13 +1666,13 @@
     <t>Caps &amp; Lids</t>
   </si>
   <si>
-    <t>24 oz Travel Tumbler - Black</t>
-  </si>
-  <si>
     <t>Account Information,Address Book,My Orders,Gift Cards,My Wishlist,My Out of Stock Subscriptions,Stored Payment Methods,My Newsletter Subscriptions</t>
   </si>
   <si>
     <t>Giftcard_Partial_5</t>
+  </si>
+  <si>
+    <t>Small Trail Series™ Boot</t>
   </si>
 </sst>
 </file>
@@ -1680,8 +1680,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1868,7 +1868,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1894,7 +1894,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2211,34 +2211,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV54"/>
   <sheetViews>
-    <sheetView topLeftCell="I40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="P40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AC53" sqref="AC53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="18" width="30.5546875" customWidth="1"/>
-    <col min="19" max="19" width="19.6640625" customWidth="1"/>
-    <col min="20" max="21" width="22.33203125" customWidth="1"/>
-    <col min="22" max="22" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="18" width="30.5703125" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1"/>
+    <col min="20" max="21" width="22.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.33203125" customWidth="1"/>
+    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2439,7 +2439,7 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="7"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -2494,7 +2494,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>516</v>
       </c>
@@ -2549,7 +2549,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -2591,7 +2591,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>438</v>
       </c>
@@ -2646,7 +2646,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>199</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>297</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2702,7 +2702,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>154</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>172</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>170</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>444</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>176</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>175</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>189</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>118</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>166</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>184</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>279</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>284</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>215</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>209</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>339</v>
       </c>
@@ -3250,7 +3250,7 @@
       </c>
       <c r="R39" s="5"/>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>343</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>346</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>348</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>353</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>201</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>363</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>432</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>433</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>232</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
         <v>153</v>
       </c>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="AE49" s="33"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>448</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>512</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>523</v>
       </c>
@@ -3430,17 +3430,17 @@
         <v>524</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>532</v>
       </c>
-      <c r="AC53" s="12" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC53" s="22" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="P54" t="s">
         <v>511</v>
@@ -3490,10 +3490,9 @@
     <hyperlink ref="I5" r:id="rId40" xr:uid="{92993A7C-001C-4FE6-9125-B4B00E04A753}"/>
     <hyperlink ref="H28" r:id="rId41" xr:uid="{22165C55-D8F7-4059-A2E1-F084718509FB}"/>
     <hyperlink ref="I28" r:id="rId42" xr:uid="{42C11063-5B1A-455C-98C2-65B906145796}"/>
-    <hyperlink ref="AC53" r:id="rId43" display="https://mcloud-na-stage4.hydroflask.com/gb/hydroflask-24-oz-travel-tumbler-black" xr:uid="{641B22C5-1E50-466C-8002-3D1A661FD7B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId44"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
 
@@ -3505,18 +3504,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3614,7 +3613,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3661,7 +3660,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3711,7 +3710,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3758,7 +3757,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3774,7 +3773,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -3786,7 +3785,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -3797,7 +3796,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3819,7 +3818,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3832,7 +3831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -3848,7 +3847,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3862,7 +3861,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -3878,7 +3877,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3892,7 +3891,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -3934,7 +3933,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -3960,7 +3959,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3971,7 +3970,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -3986,7 +3985,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -4044,12 +4043,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4120,7 +4119,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4167,7 +4166,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4183,7 +4182,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -4214,7 +4213,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4222,7 +4221,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -4255,20 +4254,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.33203125" customWidth="1"/>
-    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.28515625" customWidth="1"/>
+    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4357,7 +4356,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4405,7 +4404,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4421,7 +4420,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -4441,7 +4440,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -4460,7 +4459,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -4479,7 +4478,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -4487,7 +4486,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -4495,7 +4494,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -4512,7 +4511,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -4529,7 +4528,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -4546,7 +4545,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -4563,7 +4562,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -4574,7 +4573,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -4585,7 +4584,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4602,7 +4601,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -4631,7 +4630,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4642,7 +4641,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4656,7 +4655,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -4670,7 +4669,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -4684,7 +4683,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -4692,7 +4691,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -4722,7 +4721,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -4792,19 +4791,19 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.6640625" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4830,7 +4829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4853,12 +4852,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>199</v>
       </c>
       <c r="F3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G3" t="s">
         <v>327</v>
@@ -4884,16 +4883,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4907,7 +4906,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -4933,27 +4932,27 @@
       <selection activeCell="I18" activeCellId="1" sqref="J20 I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5546875" customWidth="1"/>
-    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5703125" customWidth="1"/>
+    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.109375" customWidth="1"/>
+    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.140625" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -5012,7 +5011,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>228</v>
       </c>
@@ -5037,7 +5036,7 @@
       <c r="R2" s="20"/>
       <c r="S2" s="20"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>230</v>
       </c>
@@ -5066,7 +5065,7 @@
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>232</v>
       </c>
@@ -5091,7 +5090,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>233</v>
       </c>
@@ -5118,7 +5117,7 @@
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>236</v>
       </c>
@@ -5151,7 +5150,7 @@
       <c r="R6" s="20"/>
       <c r="S6" s="20"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>238</v>
       </c>
@@ -5176,7 +5175,7 @@
       <c r="R7" s="20"/>
       <c r="S7" s="20"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>262</v>
       </c>
@@ -5201,7 +5200,7 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>281</v>
       </c>
@@ -5226,7 +5225,7 @@
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>286</v>
       </c>
@@ -5253,7 +5252,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>318</v>
       </c>
@@ -5278,7 +5277,7 @@
       <c r="R11" s="20"/>
       <c r="S11" s="20"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>320</v>
       </c>
@@ -5305,7 +5304,7 @@
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>321</v>
       </c>
@@ -5330,7 +5329,7 @@
       <c r="R13" s="20"/>
       <c r="S13" s="20"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>323</v>
       </c>
@@ -5355,7 +5354,7 @@
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>334</v>
       </c>
@@ -5380,7 +5379,7 @@
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>337</v>
       </c>
@@ -5405,7 +5404,7 @@
       <c r="R16" s="20"/>
       <c r="S16" s="20"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>450</v>
       </c>
@@ -5413,7 +5412,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>451</v>
       </c>
@@ -5421,7 +5420,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>452</v>
       </c>
@@ -5429,7 +5428,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>530</v>
       </c>
@@ -5451,31 +5450,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.6640625" customWidth="1"/>
-    <col min="17" max="24" width="30.5546875" customWidth="1"/>
-    <col min="25" max="25" width="19.6640625" customWidth="1"/>
-    <col min="26" max="27" width="22.33203125" customWidth="1"/>
-    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.7109375" customWidth="1"/>
+    <col min="17" max="24" width="30.5703125" customWidth="1"/>
+    <col min="25" max="25" width="19.7109375" customWidth="1"/>
+    <col min="26" max="27" width="22.28515625" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.33203125" customWidth="1"/>
+    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5627,7 +5626,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5697,7 +5696,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>455</v>
       </c>
@@ -5767,7 +5766,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>457</v>
       </c>
@@ -5837,7 +5836,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>458</v>
       </c>
@@ -5907,7 +5906,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>461</v>
       </c>
@@ -5977,7 +5976,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -6047,7 +6046,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>468</v>
       </c>
@@ -6088,7 +6087,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>469</v>
       </c>
@@ -6129,7 +6128,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>463</v>
       </c>
@@ -6199,7 +6198,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>406</v>
       </c>
@@ -6260,7 +6259,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -6319,7 +6318,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>359</v>
       </c>
@@ -6365,7 +6364,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6388,7 +6387,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>297</v>
       </c>
@@ -6411,7 +6410,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -6430,7 +6429,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6441,7 +6440,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6463,7 +6462,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>366</v>
       </c>
@@ -6476,7 +6475,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>368</v>
       </c>
@@ -6489,7 +6488,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -6502,7 +6501,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>375</v>
       </c>
@@ -6515,7 +6514,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>397</v>
       </c>
@@ -6528,7 +6527,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>376</v>
       </c>
@@ -6541,7 +6540,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -6557,7 +6556,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -6573,7 +6572,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>401</v>
       </c>
@@ -6592,7 +6591,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>405</v>
       </c>
@@ -6611,7 +6610,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>382</v>
       </c>
@@ -6627,7 +6626,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>385</v>
       </c>
@@ -6643,7 +6642,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>411</v>
       </c>
@@ -6659,7 +6658,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>412</v>
       </c>
@@ -6675,7 +6674,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>386</v>
       </c>
@@ -6691,7 +6690,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>389</v>
       </c>
@@ -6704,7 +6703,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>403</v>
       </c>
@@ -6717,7 +6716,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -6730,7 +6729,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>424</v>
       </c>
@@ -6743,7 +6742,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>398</v>
       </c>
@@ -6756,7 +6755,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>394</v>
       </c>
@@ -6772,7 +6771,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>423</v>
       </c>
@@ -6788,7 +6787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -6804,7 +6803,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>402</v>
       </c>
@@ -6817,7 +6816,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>415</v>
       </c>
@@ -6839,7 +6838,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -6857,7 +6856,7 @@
       <c r="AI44" s="25"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>414</v>
       </c>
@@ -6870,7 +6869,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -6890,7 +6889,7 @@
       <c r="AI46" s="25"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -6909,7 +6908,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -6922,7 +6921,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -6933,7 +6932,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -6946,7 +6945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -6969,7 +6968,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -6983,7 +6982,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -7020,7 +7019,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -7034,7 +7033,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -7076,7 +7075,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -7102,7 +7101,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -7126,7 +7125,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -7150,7 +7149,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -7176,7 +7175,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -7208,7 +7207,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -7222,7 +7221,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>373</v>
       </c>
@@ -7236,7 +7235,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -7253,7 +7252,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -7270,7 +7269,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>339</v>
       </c>
@@ -7292,7 +7291,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>343</v>
       </c>
@@ -7300,7 +7299,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>346</v>
       </c>
@@ -7311,7 +7310,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>348</v>
       </c>
@@ -7328,7 +7327,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>353</v>
       </c>
@@ -7336,7 +7335,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -7371,7 +7370,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>363</v>
       </c>
@@ -7462,36 +7461,36 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -7628,7 +7627,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -7703,7 +7702,7 @@
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
@@ -7760,7 +7759,7 @@
       <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>248</v>
       </c>
@@ -7813,7 +7812,7 @@
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>68</v>
       </c>
@@ -7876,7 +7875,7 @@
       <c r="AR5" s="20"/>
       <c r="AS5" s="20"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>75</v>
       </c>
@@ -7955,7 +7954,7 @@
       <c r="AR6" s="20"/>
       <c r="AS6" s="20"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>81</v>
       </c>
@@ -8044,7 +8043,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>100</v>
       </c>
@@ -8127,7 +8126,7 @@
       <c r="AR8" s="20"/>
       <c r="AS8" s="20"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>95</v>
       </c>
@@ -8212,7 +8211,7 @@
       <c r="AR9" s="20"/>
       <c r="AS9" s="20"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -8263,7 +8262,7 @@
       <c r="AR10" s="20"/>
       <c r="AS10" s="20"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>103</v>
       </c>
@@ -8320,7 +8319,7 @@
       <c r="AR11" s="20"/>
       <c r="AS11" s="20"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>107</v>
       </c>
@@ -8395,7 +8394,7 @@
       <c r="AR12" s="20"/>
       <c r="AS12" s="20"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>112</v>
       </c>
@@ -8458,7 +8457,7 @@
       <c r="AR13" s="20"/>
       <c r="AS13" s="20"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>249</v>
       </c>
@@ -8513,7 +8512,7 @@
       <c r="AR14" s="20"/>
       <c r="AS14" s="20"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>119</v>
       </c>
@@ -8570,7 +8569,7 @@
       <c r="AR15" s="20"/>
       <c r="AS15" s="20"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>121</v>
       </c>
@@ -8625,7 +8624,7 @@
       <c r="AR16" s="20"/>
       <c r="AS16" s="20"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>219</v>
       </c>
@@ -8680,7 +8679,7 @@
       <c r="AR17" s="20"/>
       <c r="AS17" s="20"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>154</v>
       </c>
@@ -8772,13 +8771,13 @@
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8855,7 +8854,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -8885,25 +8884,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.44140625" customWidth="1"/>
-    <col min="32" max="32" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.42578125" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9004,7 +9003,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -9090,7 +9089,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -9122,7 +9121,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -9144,29 +9143,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.44140625" customWidth="1"/>
-    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -9261,7 +9260,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -9322,7 +9321,7 @@
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>20</v>
       </c>
@@ -9363,7 +9362,7 @@
       <c r="AD3" s="20"/>
       <c r="AE3" s="20"/>
     </row>
-    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>25</v>
       </c>
@@ -9406,7 +9405,7 @@
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>178</v>
       </c>
@@ -9445,7 +9444,7 @@
       <c r="AD5" s="20"/>
       <c r="AE5" s="20"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>179</v>
       </c>
@@ -9484,7 +9483,7 @@
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>153</v>
       </c>
@@ -9523,7 +9522,7 @@
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>155</v>
       </c>
@@ -9560,7 +9559,7 @@
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>154</v>
       </c>
@@ -9597,7 +9596,7 @@
       <c r="AD9" s="20"/>
       <c r="AE9" s="20"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>168</v>
       </c>
@@ -9634,7 +9633,7 @@
       <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>172</v>
       </c>
@@ -9677,7 +9676,7 @@
       <c r="AD11" s="20"/>
       <c r="AE11" s="20"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>170</v>
       </c>
@@ -9716,7 +9715,7 @@
       <c r="AD12" s="20"/>
       <c r="AE12" s="20"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>77</v>
       </c>
@@ -9755,7 +9754,7 @@
       <c r="AD13" s="20"/>
       <c r="AE13" s="20"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>43</v>
       </c>
@@ -9794,7 +9793,7 @@
       <c r="AD14" s="20"/>
       <c r="AE14" s="20"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>118</v>
       </c>
@@ -9843,7 +9842,7 @@
       <c r="AD15" s="20"/>
       <c r="AE15" s="20"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
@@ -9884,7 +9883,7 @@
       <c r="AD16" s="20"/>
       <c r="AE16" s="20"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>46</v>
       </c>
@@ -9925,7 +9924,7 @@
       <c r="AD17" s="20"/>
       <c r="AE17" s="20"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>201</v>
       </c>
@@ -9980,7 +9979,7 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="20"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>241</v>
       </c>
@@ -10017,7 +10016,7 @@
       <c r="AD19" s="20"/>
       <c r="AE19" s="20"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>187</v>
       </c>
@@ -10064,7 +10063,7 @@
       <c r="AD20" s="20"/>
       <c r="AE20" s="20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>166</v>
       </c>
@@ -10111,7 +10110,7 @@
       <c r="AD21" s="20"/>
       <c r="AE21" s="20"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>343</v>
       </c>
@@ -10148,7 +10147,7 @@
       <c r="AD22" s="20"/>
       <c r="AE22" s="20"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>346</v>
       </c>
@@ -10185,7 +10184,7 @@
       <c r="AD23" s="20"/>
       <c r="AE23" s="20"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>348</v>
       </c>
@@ -10230,7 +10229,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
@@ -10298,17 +10297,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -10343,7 +10342,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>243</v>
       </c>
@@ -10352,7 +10351,7 @@
       </c>
       <c r="C2" s="20"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>245</v>
       </c>
@@ -10361,7 +10360,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>247</v>
       </c>
@@ -10370,7 +10369,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>312</v>
       </c>
@@ -10392,20 +10391,20 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10473,7 +10472,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10517,7 +10516,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10533,7 +10532,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -10551,7 +10550,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -10559,7 +10558,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -10567,7 +10566,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -10604,37 +10603,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10717,7 +10716,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10758,7 +10757,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10774,7 +10773,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -10786,7 +10785,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -10804,7 +10803,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -10813,7 +10812,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -10825,7 +10824,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -10851,7 +10850,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -10862,7 +10861,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -10876,7 +10875,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
HF_EMEA Payment details and product change in testdata updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3510F04D-FDEB-4503-AFC2-C4F4D58862F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0070F8F6-47AC-434D-A69B-5D3563DA770D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="540">
   <si>
     <t>UserName</t>
   </si>
@@ -1674,14 +1674,20 @@
   <si>
     <t>Small Trail Series™ Boot</t>
   </si>
+  <si>
+    <t>12 oz (355 ml) Mug</t>
+  </si>
+  <si>
+    <t>5555555555554440</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1863,12 +1869,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1894,7 +1900,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1926,8 +1932,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2211,34 +2216,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AC53" sqref="AC53"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="21" width="22.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="18" width="30.5546875" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="21" width="22.33203125" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.28515625" customWidth="1"/>
+    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2384,7 +2389,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2439,7 +2444,7 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="7"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -2494,7 +2499,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:48" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>516</v>
       </c>
@@ -2549,7 +2554,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -2591,7 +2596,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>438</v>
       </c>
@@ -2646,7 +2651,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2662,7 +2667,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>199</v>
       </c>
@@ -2674,7 +2679,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>297</v>
       </c>
@@ -2690,7 +2695,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2702,7 +2707,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>154</v>
       </c>
@@ -2715,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>172</v>
       </c>
@@ -2734,7 +2739,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>170</v>
       </c>
@@ -2747,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2760,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="AE14" t="s">
-        <v>326</v>
+        <v>538</v>
       </c>
       <c r="AF14" t="s">
         <v>387</v>
@@ -2775,7 +2780,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>444</v>
       </c>
@@ -2789,7 +2794,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>176</v>
       </c>
@@ -2808,7 +2813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>175</v>
       </c>
@@ -2821,7 +2826,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>189</v>
       </c>
@@ -2832,7 +2837,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -2856,7 +2861,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -2869,7 +2874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2885,7 +2890,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2899,7 +2904,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -2936,7 +2941,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2950,7 +2955,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -2992,7 +2997,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -3006,7 +3011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -3035,7 +3040,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -3052,7 +3057,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -3069,7 +3074,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>118</v>
       </c>
@@ -3098,7 +3103,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -3106,7 +3111,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -3117,7 +3122,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>166</v>
       </c>
@@ -3156,7 +3161,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>184</v>
       </c>
@@ -3171,7 +3176,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>279</v>
       </c>
@@ -3179,7 +3184,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>284</v>
       </c>
@@ -3193,7 +3198,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>215</v>
       </c>
@@ -3210,7 +3215,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>209</v>
       </c>
@@ -3227,7 +3232,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>339</v>
       </c>
@@ -3250,7 +3255,7 @@
       </c>
       <c r="R39" s="5"/>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>343</v>
       </c>
@@ -3258,7 +3263,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>346</v>
       </c>
@@ -3272,7 +3277,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>348</v>
       </c>
@@ -3289,7 +3294,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>353</v>
       </c>
@@ -3297,7 +3302,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>201</v>
       </c>
@@ -3332,7 +3337,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>363</v>
       </c>
@@ -3340,7 +3345,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>432</v>
       </c>
@@ -3348,7 +3353,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>433</v>
       </c>
@@ -3356,7 +3361,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>232</v>
       </c>
@@ -3367,7 +3372,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" s="33" t="s">
         <v>153</v>
       </c>
@@ -3406,7 +3411,7 @@
       </c>
       <c r="AE49" s="33"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>448</v>
       </c>
@@ -3414,7 +3419,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>512</v>
       </c>
@@ -3422,7 +3427,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>523</v>
       </c>
@@ -3430,7 +3435,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>532</v>
       </c>
@@ -3438,7 +3443,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>536</v>
       </c>
@@ -3504,18 +3509,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3613,7 +3618,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3660,7 +3665,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3710,7 +3715,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3757,7 +3762,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3773,7 +3778,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -3785,7 +3790,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -3796,7 +3801,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3818,7 +3823,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3831,7 +3836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -3847,7 +3852,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3861,7 +3866,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -3877,7 +3882,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3891,7 +3896,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -3933,7 +3938,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -3959,7 +3964,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3970,7 +3975,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -3985,7 +3990,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -4043,12 +4048,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4119,7 +4124,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4166,7 +4171,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4182,7 +4187,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -4213,7 +4218,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4221,7 +4226,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -4254,20 +4259,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.28515625" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4356,7 +4361,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4404,7 +4409,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4420,7 +4425,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -4440,7 +4445,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -4459,7 +4464,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -4478,7 +4483,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -4486,7 +4491,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -4494,7 +4499,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -4511,7 +4516,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -4528,7 +4533,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -4545,7 +4550,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -4562,7 +4567,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -4573,7 +4578,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -4584,7 +4589,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4601,7 +4606,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -4630,7 +4635,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4641,7 +4646,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4655,7 +4660,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -4669,7 +4674,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -4683,7 +4688,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -4691,7 +4696,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -4721,7 +4726,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -4791,19 +4796,19 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4829,7 +4834,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4852,7 +4857,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -4883,16 +4888,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4906,7 +4911,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -4932,27 +4937,27 @@
       <selection activeCell="I18" activeCellId="1" sqref="J20 I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5703125" customWidth="1"/>
-    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5546875" customWidth="1"/>
+    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.140625" customWidth="1"/>
+    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.109375" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -5011,7 +5016,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>228</v>
       </c>
@@ -5036,7 +5041,7 @@
       <c r="R2" s="20"/>
       <c r="S2" s="20"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>230</v>
       </c>
@@ -5065,7 +5070,7 @@
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>232</v>
       </c>
@@ -5090,7 +5095,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>233</v>
       </c>
@@ -5117,7 +5122,7 @@
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>236</v>
       </c>
@@ -5150,7 +5155,7 @@
       <c r="R6" s="20"/>
       <c r="S6" s="20"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>238</v>
       </c>
@@ -5175,7 +5180,7 @@
       <c r="R7" s="20"/>
       <c r="S7" s="20"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>262</v>
       </c>
@@ -5200,7 +5205,7 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>281</v>
       </c>
@@ -5225,7 +5230,7 @@
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>286</v>
       </c>
@@ -5252,7 +5257,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>318</v>
       </c>
@@ -5277,7 +5282,7 @@
       <c r="R11" s="20"/>
       <c r="S11" s="20"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>320</v>
       </c>
@@ -5304,7 +5309,7 @@
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>321</v>
       </c>
@@ -5329,7 +5334,7 @@
       <c r="R13" s="20"/>
       <c r="S13" s="20"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>323</v>
       </c>
@@ -5354,7 +5359,7 @@
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>334</v>
       </c>
@@ -5379,7 +5384,7 @@
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>337</v>
       </c>
@@ -5404,7 +5409,7 @@
       <c r="R16" s="20"/>
       <c r="S16" s="20"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>450</v>
       </c>
@@ -5412,7 +5417,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>451</v>
       </c>
@@ -5420,7 +5425,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>452</v>
       </c>
@@ -5428,7 +5433,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>530</v>
       </c>
@@ -5450,31 +5455,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.7109375" customWidth="1"/>
-    <col min="17" max="24" width="30.5703125" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" customWidth="1"/>
-    <col min="26" max="27" width="22.28515625" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.6640625" customWidth="1"/>
+    <col min="17" max="24" width="30.5546875" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" customWidth="1"/>
+    <col min="26" max="27" width="22.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.28515625" customWidth="1"/>
+    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5626,7 +5631,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5696,7 +5701,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>455</v>
       </c>
@@ -5766,7 +5771,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>457</v>
       </c>
@@ -5836,7 +5841,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>458</v>
       </c>
@@ -5906,7 +5911,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>461</v>
       </c>
@@ -5976,7 +5981,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -6046,7 +6051,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>468</v>
       </c>
@@ -6087,7 +6092,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>469</v>
       </c>
@@ -6128,7 +6133,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>463</v>
       </c>
@@ -6198,7 +6203,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>406</v>
       </c>
@@ -6259,7 +6264,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -6318,7 +6323,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>359</v>
       </c>
@@ -6364,7 +6369,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6387,7 +6392,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>297</v>
       </c>
@@ -6410,7 +6415,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -6429,7 +6434,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6440,7 +6445,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6462,7 +6467,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>366</v>
       </c>
@@ -6475,7 +6480,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>368</v>
       </c>
@@ -6488,7 +6493,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -6501,7 +6506,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>375</v>
       </c>
@@ -6514,7 +6519,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>397</v>
       </c>
@@ -6527,7 +6532,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>376</v>
       </c>
@@ -6540,7 +6545,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -6556,7 +6561,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -6572,7 +6577,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>401</v>
       </c>
@@ -6591,7 +6596,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>405</v>
       </c>
@@ -6610,7 +6615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>382</v>
       </c>
@@ -6626,7 +6631,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>385</v>
       </c>
@@ -6642,7 +6647,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>411</v>
       </c>
@@ -6658,7 +6663,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>412</v>
       </c>
@@ -6674,7 +6679,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>386</v>
       </c>
@@ -6690,7 +6695,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>389</v>
       </c>
@@ -6703,7 +6708,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>403</v>
       </c>
@@ -6716,7 +6721,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -6729,7 +6734,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>424</v>
       </c>
@@ -6742,7 +6747,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>398</v>
       </c>
@@ -6755,7 +6760,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>394</v>
       </c>
@@ -6771,7 +6776,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>423</v>
       </c>
@@ -6787,7 +6792,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -6803,7 +6808,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>402</v>
       </c>
@@ -6816,7 +6821,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>415</v>
       </c>
@@ -6838,7 +6843,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -6856,7 +6861,7 @@
       <c r="AI44" s="25"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>414</v>
       </c>
@@ -6869,7 +6874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -6889,7 +6894,7 @@
       <c r="AI46" s="25"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -6908,7 +6913,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -6921,7 +6926,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -6932,7 +6937,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -6945,7 +6950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -6968,7 +6973,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -6982,7 +6987,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -7019,7 +7024,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -7033,7 +7038,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -7075,7 +7080,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -7101,7 +7106,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -7125,7 +7130,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -7149,7 +7154,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -7175,7 +7180,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -7207,7 +7212,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -7221,7 +7226,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>373</v>
       </c>
@@ -7235,7 +7240,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -7252,7 +7257,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -7269,7 +7274,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>339</v>
       </c>
@@ -7291,7 +7296,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>343</v>
       </c>
@@ -7299,7 +7304,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>346</v>
       </c>
@@ -7310,7 +7315,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>348</v>
       </c>
@@ -7327,7 +7332,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>353</v>
       </c>
@@ -7335,7 +7340,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -7370,7 +7375,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>363</v>
       </c>
@@ -7461,36 +7466,36 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -7627,7 +7632,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -7702,7 +7707,7 @@
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
@@ -7759,7 +7764,7 @@
       <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>248</v>
       </c>
@@ -7812,7 +7817,7 @@
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>68</v>
       </c>
@@ -7875,7 +7880,7 @@
       <c r="AR5" s="20"/>
       <c r="AS5" s="20"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>75</v>
       </c>
@@ -7954,7 +7959,7 @@
       <c r="AR6" s="20"/>
       <c r="AS6" s="20"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>81</v>
       </c>
@@ -8043,7 +8048,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>100</v>
       </c>
@@ -8126,7 +8131,7 @@
       <c r="AR8" s="20"/>
       <c r="AS8" s="20"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>95</v>
       </c>
@@ -8211,7 +8216,7 @@
       <c r="AR9" s="20"/>
       <c r="AS9" s="20"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -8262,7 +8267,7 @@
       <c r="AR10" s="20"/>
       <c r="AS10" s="20"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>103</v>
       </c>
@@ -8319,7 +8324,7 @@
       <c r="AR11" s="20"/>
       <c r="AS11" s="20"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>107</v>
       </c>
@@ -8394,7 +8399,7 @@
       <c r="AR12" s="20"/>
       <c r="AS12" s="20"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>112</v>
       </c>
@@ -8457,7 +8462,7 @@
       <c r="AR13" s="20"/>
       <c r="AS13" s="20"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>249</v>
       </c>
@@ -8512,7 +8517,7 @@
       <c r="AR14" s="20"/>
       <c r="AS14" s="20"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>119</v>
       </c>
@@ -8569,7 +8574,7 @@
       <c r="AR15" s="20"/>
       <c r="AS15" s="20"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>121</v>
       </c>
@@ -8624,7 +8629,7 @@
       <c r="AR16" s="20"/>
       <c r="AS16" s="20"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>219</v>
       </c>
@@ -8679,7 +8684,7 @@
       <c r="AR17" s="20"/>
       <c r="AS17" s="20"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>154</v>
       </c>
@@ -8771,13 +8776,13 @@
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8854,7 +8859,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="150" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -8884,25 +8889,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9003,7 +9008,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -9089,7 +9094,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -9121,7 +9126,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -9143,29 +9148,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -9260,7 +9266,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -9321,7 +9327,7 @@
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>20</v>
       </c>
@@ -9340,13 +9346,13 @@
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
       <c r="P3" s="20"/>
-      <c r="Q3" s="20">
-        <v>4242424242424240</v>
-      </c>
-      <c r="R3" s="42">
-        <v>46113</v>
-      </c>
-      <c r="S3" s="20">
+      <c r="Q3" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="S3">
         <v>123</v>
       </c>
       <c r="T3" s="20"/>
@@ -9362,7 +9368,7 @@
       <c r="AD3" s="20"/>
       <c r="AE3" s="20"/>
     </row>
-    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>25</v>
       </c>
@@ -9393,7 +9399,7 @@
         <v>1</v>
       </c>
       <c r="X4" s="12" t="s">
-        <v>326</v>
+        <v>538</v>
       </c>
       <c r="Y4" s="21" t="s">
         <v>39</v>
@@ -9405,7 +9411,7 @@
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>178</v>
       </c>
@@ -9444,7 +9450,7 @@
       <c r="AD5" s="20"/>
       <c r="AE5" s="20"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>179</v>
       </c>
@@ -9483,7 +9489,7 @@
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>153</v>
       </c>
@@ -9522,7 +9528,7 @@
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>155</v>
       </c>
@@ -9559,7 +9565,7 @@
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>154</v>
       </c>
@@ -9596,7 +9602,7 @@
       <c r="AD9" s="20"/>
       <c r="AE9" s="20"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>168</v>
       </c>
@@ -9633,7 +9639,7 @@
       <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>172</v>
       </c>
@@ -9676,7 +9682,7 @@
       <c r="AD11" s="20"/>
       <c r="AE11" s="20"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>170</v>
       </c>
@@ -9715,7 +9721,7 @@
       <c r="AD12" s="20"/>
       <c r="AE12" s="20"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>77</v>
       </c>
@@ -9754,7 +9760,7 @@
       <c r="AD13" s="20"/>
       <c r="AE13" s="20"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>43</v>
       </c>
@@ -9793,7 +9799,7 @@
       <c r="AD14" s="20"/>
       <c r="AE14" s="20"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>118</v>
       </c>
@@ -9842,7 +9848,7 @@
       <c r="AD15" s="20"/>
       <c r="AE15" s="20"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
@@ -9861,13 +9867,13 @@
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
-      <c r="Q16" s="20">
-        <v>5555555555554440</v>
-      </c>
-      <c r="R16" s="43">
-        <v>45773</v>
-      </c>
-      <c r="S16" s="20">
+      <c r="Q16" s="42" t="s">
+        <v>539</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="S16">
         <v>123</v>
       </c>
       <c r="T16" s="20"/>
@@ -9883,7 +9889,7 @@
       <c r="AD16" s="20"/>
       <c r="AE16" s="20"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>46</v>
       </c>
@@ -9902,13 +9908,13 @@
       <c r="N17" s="20"/>
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
-      <c r="Q17" s="20">
-        <v>378282246310005</v>
-      </c>
-      <c r="R17" s="42">
-        <v>46113</v>
-      </c>
-      <c r="S17" s="20">
+      <c r="Q17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="S17">
         <v>1234</v>
       </c>
       <c r="T17" s="20"/>
@@ -9924,7 +9930,7 @@
       <c r="AD17" s="20"/>
       <c r="AE17" s="20"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>201</v>
       </c>
@@ -9979,7 +9985,7 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="20"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>241</v>
       </c>
@@ -10016,7 +10022,7 @@
       <c r="AD19" s="20"/>
       <c r="AE19" s="20"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>187</v>
       </c>
@@ -10063,7 +10069,7 @@
       <c r="AD20" s="20"/>
       <c r="AE20" s="20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>166</v>
       </c>
@@ -10110,7 +10116,7 @@
       <c r="AD21" s="20"/>
       <c r="AE21" s="20"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>343</v>
       </c>
@@ -10147,7 +10153,7 @@
       <c r="AD22" s="20"/>
       <c r="AE22" s="20"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>346</v>
       </c>
@@ -10184,7 +10190,7 @@
       <c r="AD23" s="20"/>
       <c r="AE23" s="20"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>348</v>
       </c>
@@ -10229,7 +10235,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
@@ -10297,17 +10303,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -10342,7 +10348,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>243</v>
       </c>
@@ -10351,7 +10357,7 @@
       </c>
       <c r="C2" s="20"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>245</v>
       </c>
@@ -10360,7 +10366,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>247</v>
       </c>
@@ -10369,7 +10375,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>312</v>
       </c>
@@ -10391,20 +10397,20 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10472,7 +10478,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10516,7 +10522,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10532,7 +10538,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -10550,7 +10556,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -10558,7 +10564,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -10566,7 +10572,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -10603,37 +10609,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10716,7 +10722,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10757,7 +10763,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10773,7 +10779,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -10785,7 +10791,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -10803,7 +10809,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -10812,7 +10818,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -10824,7 +10830,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -10850,7 +10856,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -10861,7 +10867,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -10875,7 +10881,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
HF_EMEA TEST_DGLD_HF_EMEA_RT_054 & 32 testcase Changes Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D1B08E-89A5-4DCA-9F9E-03A621AA6E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B169DC-F622-4D26-B476-D872C16C2A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1582,9 +1582,6 @@
     <t>8DZ67T85R4856M74K23D</t>
   </si>
   <si>
-    <t>4SX89R79W7673P94T66S</t>
-  </si>
-  <si>
     <t>Hfemeanewaccount@gmail.com</t>
   </si>
   <si>
@@ -1685,6 +1682,9 @@
   </si>
   <si>
     <t>Below5 Shipping method</t>
+  </si>
+  <si>
+    <t>9GT64Y68Y7425Z97J65X</t>
   </si>
 </sst>
 </file>
@@ -1692,8 +1692,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1873,7 +1873,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1899,7 +1899,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2212,34 +2212,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="21" width="22.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="18" width="30.5546875" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="21" width="22.33203125" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.28515625" customWidth="1"/>
+    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>207</v>
       </c>
       <c r="AT1" s="40" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>436</v>
@@ -2385,7 +2385,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2423,16 +2423,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" t="s">
+        <v>519</v>
+      </c>
+      <c r="T2" t="s">
+        <v>517</v>
+      </c>
+      <c r="V2" t="s">
         <v>520</v>
       </c>
-      <c r="T2" t="s">
-        <v>518</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="W2" s="5" t="s">
         <v>521</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>522</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>59</v>
@@ -2443,15 +2443,15 @@
         <v>499</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>294</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2466,10 +2466,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -2501,9 +2501,9 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:48" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>500</v>
@@ -2539,16 +2539,16 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="15" t="s">
+        <v>516</v>
+      </c>
+      <c r="T4" t="s">
         <v>517</v>
-      </c>
-      <c r="T4" t="s">
-        <v>518</v>
       </c>
       <c r="V4" t="s">
         <v>487</v>
       </c>
       <c r="W4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>59</v>
@@ -2556,15 +2556,15 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>359</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -2579,10 +2579,10 @@
         <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2598,7 +2598,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>438</v>
       </c>
@@ -2656,7 +2656,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>199</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>297</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2712,7 +2712,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>154</v>
       </c>
@@ -2725,9 +2725,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>484</v>
@@ -2736,7 +2736,7 @@
       <c r="X12" s="4"/>
       <c r="AD12" s="32"/>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>172</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>170</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>1</v>
       </c>
       <c r="AE15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AF15" t="s">
         <v>387</v>
@@ -2796,7 +2796,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>444</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>176</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>175</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>189</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -3067,13 +3067,13 @@
         <v>69</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>151</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>166</v>
       </c>
@@ -3177,12 +3177,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>184</v>
       </c>
       <c r="H35" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I35" s="12"/>
       <c r="AC35" t="s">
@@ -3192,7 +3192,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>279</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>284</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>215</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>209</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>339</v>
       </c>
@@ -3271,7 +3271,7 @@
       </c>
       <c r="R40" s="5"/>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>343</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>346</v>
       </c>
@@ -3287,13 +3287,13 @@
         <v>430</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="N42" s="24" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="43" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>348</v>
       </c>
@@ -3304,21 +3304,21 @@
         <v>349</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AO43" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>353</v>
       </c>
       <c r="P44" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="45" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>201</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>363</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>432</v>
       </c>
@@ -3369,26 +3369,26 @@
         <v>434</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>433</v>
       </c>
       <c r="P48" s="26" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="49" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>232</v>
       </c>
       <c r="AT49" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AU49" s="31" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A50" s="33" t="s">
         <v>153</v>
       </c>
@@ -3427,44 +3427,44 @@
       </c>
       <c r="AE50" s="33"/>
     </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>448</v>
       </c>
       <c r="P51" s="26" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="52" spans="1:47" x14ac:dyDescent="0.25">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="52" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="P52" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="53" spans="1:47" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="53" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>522</v>
+      </c>
+      <c r="S53" t="s">
         <v>523</v>
       </c>
-      <c r="S53" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="54" spans="1:47" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AC54" s="22" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="55" spans="1:47" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="55" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="P55" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -3525,18 +3525,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3681,7 +3681,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3731,7 +3731,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3778,7 +3778,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -3806,7 +3806,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -3817,7 +3817,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4006,7 +4006,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -4064,12 +4064,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4187,7 +4187,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -4275,20 +4275,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.28515625" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4425,7 +4425,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -4742,7 +4742,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -4812,19 +4812,19 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4873,12 +4873,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>199</v>
       </c>
       <c r="F3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G3" t="s">
         <v>327</v>
@@ -4904,16 +4904,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4927,7 +4927,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -4953,27 +4953,27 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5703125" customWidth="1"/>
-    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5546875" customWidth="1"/>
+    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.140625" customWidth="1"/>
+    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.109375" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -5032,12 +5032,12 @@
         <v>435</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>228</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -5057,7 +5057,7 @@
       <c r="R2" s="20"/>
       <c r="S2" s="20"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>230</v>
       </c>
@@ -5086,7 +5086,7 @@
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>232</v>
       </c>
@@ -5098,7 +5098,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
@@ -5111,7 +5111,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>233</v>
       </c>
@@ -5126,7 +5126,7 @@
       <c r="H5" s="20"/>
       <c r="I5" s="30"/>
       <c r="J5" s="20" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
@@ -5138,7 +5138,7 @@
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>236</v>
       </c>
@@ -5171,7 +5171,7 @@
       <c r="R6" s="20"/>
       <c r="S6" s="20"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>238</v>
       </c>
@@ -5187,7 +5187,7 @@
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
       <c r="M7" s="28" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
@@ -5196,7 +5196,7 @@
       <c r="R7" s="20"/>
       <c r="S7" s="20"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>262</v>
       </c>
@@ -5221,7 +5221,7 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>281</v>
       </c>
@@ -5229,7 +5229,7 @@
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -5246,7 +5246,7 @@
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>286</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>318</v>
       </c>
@@ -5298,7 +5298,7 @@
       <c r="R11" s="20"/>
       <c r="S11" s="20"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>320</v>
       </c>
@@ -5325,7 +5325,7 @@
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>321</v>
       </c>
@@ -5350,7 +5350,7 @@
       <c r="R13" s="20"/>
       <c r="S13" s="20"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>323</v>
       </c>
@@ -5375,7 +5375,7 @@
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>334</v>
       </c>
@@ -5400,7 +5400,7 @@
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>337</v>
       </c>
@@ -5425,7 +5425,7 @@
       <c r="R16" s="20"/>
       <c r="S16" s="20"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>450</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>451</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>452</v>
       </c>
@@ -5449,12 +5449,12 @@
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J20" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -5471,31 +5471,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.7109375" customWidth="1"/>
-    <col min="17" max="24" width="30.5703125" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" customWidth="1"/>
-    <col min="26" max="27" width="22.28515625" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.6640625" customWidth="1"/>
+    <col min="17" max="24" width="30.5546875" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" customWidth="1"/>
+    <col min="26" max="27" width="22.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.28515625" customWidth="1"/>
+    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5717,7 +5717,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>455</v>
       </c>
@@ -5787,7 +5787,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>457</v>
       </c>
@@ -5857,7 +5857,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>458</v>
       </c>
@@ -5927,7 +5927,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>461</v>
       </c>
@@ -5997,7 +5997,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -6067,7 +6067,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>468</v>
       </c>
@@ -6108,7 +6108,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>469</v>
       </c>
@@ -6149,7 +6149,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>463</v>
       </c>
@@ -6219,7 +6219,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>406</v>
       </c>
@@ -6280,7 +6280,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -6339,7 +6339,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>359</v>
       </c>
@@ -6385,7 +6385,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>297</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -6450,7 +6450,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6461,7 +6461,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>366</v>
       </c>
@@ -6496,7 +6496,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>368</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>375</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>397</v>
       </c>
@@ -6548,7 +6548,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>376</v>
       </c>
@@ -6561,7 +6561,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>401</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>405</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>382</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>385</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>411</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>412</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>386</v>
       </c>
@@ -6711,7 +6711,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>389</v>
       </c>
@@ -6724,7 +6724,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>403</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>424</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>398</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>394</v>
       </c>
@@ -6792,7 +6792,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>423</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>402</v>
       </c>
@@ -6837,7 +6837,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>415</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -6877,7 +6877,7 @@
       <c r="AI44" s="25"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>414</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -6910,7 +6910,7 @@
       <c r="AI46" s="25"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -6989,7 +6989,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -7003,7 +7003,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -7054,7 +7054,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>373</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -7273,7 +7273,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>339</v>
       </c>
@@ -7312,7 +7312,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>343</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>346</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>348</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>353</v>
       </c>
@@ -7356,7 +7356,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -7391,7 +7391,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>363</v>
       </c>
@@ -7482,36 +7482,36 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -7648,7 +7648,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -7723,7 +7723,7 @@
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
@@ -7780,7 +7780,7 @@
       <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>248</v>
       </c>
@@ -7833,7 +7833,7 @@
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>68</v>
       </c>
@@ -7896,7 +7896,7 @@
       <c r="AR5" s="20"/>
       <c r="AS5" s="20"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>75</v>
       </c>
@@ -7975,7 +7975,7 @@
       <c r="AR6" s="20"/>
       <c r="AS6" s="20"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>81</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>100</v>
       </c>
@@ -8147,7 +8147,7 @@
       <c r="AR8" s="20"/>
       <c r="AS8" s="20"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>95</v>
       </c>
@@ -8232,7 +8232,7 @@
       <c r="AR9" s="20"/>
       <c r="AS9" s="20"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -8283,7 +8283,7 @@
       <c r="AR10" s="20"/>
       <c r="AS10" s="20"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>103</v>
       </c>
@@ -8340,7 +8340,7 @@
       <c r="AR11" s="20"/>
       <c r="AS11" s="20"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>107</v>
       </c>
@@ -8415,7 +8415,7 @@
       <c r="AR12" s="20"/>
       <c r="AS12" s="20"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>112</v>
       </c>
@@ -8478,7 +8478,7 @@
       <c r="AR13" s="20"/>
       <c r="AS13" s="20"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>249</v>
       </c>
@@ -8533,7 +8533,7 @@
       <c r="AR14" s="20"/>
       <c r="AS14" s="20"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>119</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="AR15" s="20"/>
       <c r="AS15" s="20"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>121</v>
       </c>
@@ -8645,7 +8645,7 @@
       <c r="AR16" s="20"/>
       <c r="AS16" s="20"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>219</v>
       </c>
@@ -8700,7 +8700,7 @@
       <c r="AR17" s="20"/>
       <c r="AS17" s="20"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>154</v>
       </c>
@@ -8792,13 +8792,13 @@
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8875,12 +8875,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="R2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="S2" t="s">
         <v>260</v>
@@ -8905,25 +8905,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9024,7 +9024,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -9110,7 +9110,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -9142,7 +9142,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -9168,26 +9168,26 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -9282,7 +9282,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -9343,7 +9343,7 @@
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>20</v>
       </c>
@@ -9384,7 +9384,7 @@
       <c r="AD3" s="20"/>
       <c r="AE3" s="20"/>
     </row>
-    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>25</v>
       </c>
@@ -9415,7 +9415,7 @@
         <v>1</v>
       </c>
       <c r="X4" s="12" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="Y4" s="21" t="s">
         <v>39</v>
@@ -9427,7 +9427,7 @@
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>178</v>
       </c>
@@ -9466,7 +9466,7 @@
       <c r="AD5" s="20"/>
       <c r="AE5" s="20"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>179</v>
       </c>
@@ -9505,7 +9505,7 @@
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>153</v>
       </c>
@@ -9544,7 +9544,7 @@
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>155</v>
       </c>
@@ -9581,7 +9581,7 @@
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>154</v>
       </c>
@@ -9618,7 +9618,7 @@
       <c r="AD9" s="20"/>
       <c r="AE9" s="20"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>168</v>
       </c>
@@ -9655,7 +9655,7 @@
       <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>172</v>
       </c>
@@ -9698,7 +9698,7 @@
       <c r="AD11" s="20"/>
       <c r="AE11" s="20"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>170</v>
       </c>
@@ -9737,7 +9737,7 @@
       <c r="AD12" s="20"/>
       <c r="AE12" s="20"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>77</v>
       </c>
@@ -9776,7 +9776,7 @@
       <c r="AD13" s="20"/>
       <c r="AE13" s="20"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>43</v>
       </c>
@@ -9815,7 +9815,7 @@
       <c r="AD14" s="20"/>
       <c r="AE14" s="20"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>118</v>
       </c>
@@ -9864,7 +9864,7 @@
       <c r="AD15" s="20"/>
       <c r="AE15" s="20"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
@@ -9884,7 +9884,7 @@
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="41" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="R16" s="7" t="s">
         <v>443</v>
@@ -9905,7 +9905,7 @@
       <c r="AD16" s="20"/>
       <c r="AE16" s="20"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>46</v>
       </c>
@@ -9946,7 +9946,7 @@
       <c r="AD17" s="20"/>
       <c r="AE17" s="20"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>201</v>
       </c>
@@ -10001,7 +10001,7 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="20"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>241</v>
       </c>
@@ -10038,7 +10038,7 @@
       <c r="AD19" s="20"/>
       <c r="AE19" s="20"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>187</v>
       </c>
@@ -10085,7 +10085,7 @@
       <c r="AD20" s="20"/>
       <c r="AE20" s="20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>166</v>
       </c>
@@ -10132,7 +10132,7 @@
       <c r="AD21" s="20"/>
       <c r="AE21" s="20"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>343</v>
       </c>
@@ -10169,7 +10169,7 @@
       <c r="AD22" s="20"/>
       <c r="AE22" s="20"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>346</v>
       </c>
@@ -10194,7 +10194,7 @@
       <c r="T23" s="20"/>
       <c r="U23" s="20"/>
       <c r="V23" s="20" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="W23" s="20"/>
       <c r="X23" s="20"/>
@@ -10206,7 +10206,7 @@
       <c r="AD23" s="20"/>
       <c r="AE23" s="20"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>348</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>349</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
@@ -10251,7 +10251,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
@@ -10319,17 +10319,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -10364,7 +10364,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>243</v>
       </c>
@@ -10373,7 +10373,7 @@
       </c>
       <c r="C2" s="20"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>245</v>
       </c>
@@ -10382,7 +10382,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>247</v>
       </c>
@@ -10391,7 +10391,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>312</v>
       </c>
@@ -10413,20 +10413,20 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10494,7 +10494,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10538,7 +10538,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10554,7 +10554,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -10572,7 +10572,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -10580,7 +10580,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -10588,7 +10588,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -10625,37 +10625,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10738,7 +10738,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10779,7 +10779,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10795,7 +10795,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -10807,7 +10807,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -10825,7 +10825,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -10834,7 +10834,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -10846,7 +10846,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -10872,7 +10872,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -10883,7 +10883,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -10897,7 +10897,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
HYF_EMEA : TEST_DGLD_HF_EMEA_RT_054 changes and updated the OOS product in testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B169DC-F622-4D26-B476-D872C16C2A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E8C752-0081-45E8-BA11-BD85EB527D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="541">
   <si>
     <t>UserName</t>
   </si>
@@ -1542,9 +1542,6 @@
   </si>
   <si>
     <t>Track Your Order</t>
-  </si>
-  <si>
-    <t>Micro Hydro Mini Bottle</t>
   </si>
   <si>
     <t>£</t>
@@ -2212,7 +2209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
@@ -2376,7 +2373,7 @@
         <v>207</v>
       </c>
       <c r="AT1" s="40" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>436</v>
@@ -2390,10 +2387,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -2408,10 +2405,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -2423,16 +2420,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" t="s">
+        <v>518</v>
+      </c>
+      <c r="T2" t="s">
+        <v>516</v>
+      </c>
+      <c r="V2" t="s">
         <v>519</v>
       </c>
-      <c r="T2" t="s">
-        <v>517</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="W2" s="5" t="s">
         <v>520</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>521</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>59</v>
@@ -2440,7 +2437,7 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="7"/>
       <c r="AV2" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.3">
@@ -2448,10 +2445,10 @@
         <v>294</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2466,10 +2463,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -2481,19 +2478,19 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="U3" t="s">
         <v>491</v>
       </c>
       <c r="V3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>59</v>
@@ -2503,13 +2500,13 @@
     </row>
     <row r="4" spans="1:48" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>29</v>
@@ -2524,10 +2521,10 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -2539,16 +2536,16 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="15" t="s">
+        <v>515</v>
+      </c>
+      <c r="T4" t="s">
         <v>516</v>
-      </c>
-      <c r="T4" t="s">
-        <v>517</v>
       </c>
       <c r="V4" t="s">
         <v>487</v>
       </c>
       <c r="W4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>59</v>
@@ -2561,10 +2558,10 @@
         <v>359</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -2579,10 +2576,10 @@
         <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2636,19 +2633,19 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="U6" t="s">
         <v>491</v>
       </c>
       <c r="V6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="X6" s="5" t="s">
         <v>59</v>
@@ -2727,7 +2724,7 @@
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>484</v>
@@ -2781,7 +2778,7 @@
         <v>1</v>
       </c>
       <c r="AE15" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="AF15" t="s">
         <v>387</v>
@@ -3038,19 +3035,19 @@
         <v>15</v>
       </c>
       <c r="S28" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="U28" t="s">
         <v>491</v>
       </c>
       <c r="V28" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="W28" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="X28" s="5" t="s">
         <v>59</v>
@@ -3067,10 +3064,10 @@
         <v>69</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.3">
@@ -3101,19 +3098,19 @@
         <v>15</v>
       </c>
       <c r="S31" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T31" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="U31" t="s">
         <v>491</v>
       </c>
       <c r="V31" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="W31" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="X31" s="5" t="s">
         <v>59</v>
@@ -3159,19 +3156,19 @@
       <c r="Q34" s="12"/>
       <c r="R34" s="12"/>
       <c r="S34" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T34" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="U34" t="s">
         <v>491</v>
       </c>
       <c r="V34" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="W34" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="X34" s="5" t="s">
         <v>59</v>
@@ -3182,7 +3179,7 @@
         <v>184</v>
       </c>
       <c r="H35" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I35" s="12"/>
       <c r="AC35" t="s">
@@ -3264,7 +3261,7 @@
         <v>341</v>
       </c>
       <c r="P40" s="26" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="Q40" s="5" t="s">
         <v>355</v>
@@ -3287,10 +3284,10 @@
         <v>430</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="N42" s="24" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="43" spans="1:44" x14ac:dyDescent="0.3">
@@ -3304,7 +3301,7 @@
         <v>349</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="AO43" t="s">
         <v>351</v>
@@ -3315,7 +3312,7 @@
         <v>353</v>
       </c>
       <c r="P44" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="45" spans="1:44" x14ac:dyDescent="0.3">
@@ -3374,7 +3371,7 @@
         <v>433</v>
       </c>
       <c r="P48" s="26" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="49" spans="1:47" x14ac:dyDescent="0.3">
@@ -3382,7 +3379,7 @@
         <v>232</v>
       </c>
       <c r="AT49" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AU49" s="31" t="s">
         <v>232</v>
@@ -3432,39 +3429,39 @@
         <v>448</v>
       </c>
       <c r="P51" s="26" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="52" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="P52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="53" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>521</v>
+      </c>
+      <c r="S53" t="s">
         <v>522</v>
-      </c>
-      <c r="S53" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="54" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AC54" s="22" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="55" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="P55" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -4878,7 +4875,7 @@
         <v>199</v>
       </c>
       <c r="F3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G3" t="s">
         <v>327</v>
@@ -4932,7 +4929,7 @@
         <v>152</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>261</v>
@@ -5037,7 +5034,7 @@
         <v>228</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -5098,7 +5095,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
@@ -5126,7 +5123,7 @@
       <c r="H5" s="20"/>
       <c r="I5" s="30"/>
       <c r="J5" s="20" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
@@ -5187,7 +5184,7 @@
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
       <c r="M7" s="28" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
@@ -5229,7 +5226,7 @@
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -5451,10 +5448,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J20" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -7680,16 +7677,16 @@
       </c>
       <c r="L2" s="29"/>
       <c r="M2" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="O2" s="20" t="s">
         <v>501</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="P2" s="20" t="s">
         <v>503</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>502</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>504</v>
       </c>
       <c r="Q2" s="20">
         <v>9898989898</v>
@@ -7850,7 +7847,7 @@
         <v>332</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K5" s="29"/>
       <c r="L5" s="20"/>
@@ -7921,21 +7918,21 @@
         <v>67</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K6" s="29"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="O6" s="20" t="s">
         <v>501</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="P6" s="20" t="s">
         <v>503</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>502</v>
-      </c>
-      <c r="P6" s="20" t="s">
-        <v>504</v>
       </c>
       <c r="Q6" s="20">
         <v>9898989898</v>
@@ -7980,7 +7977,7 @@
         <v>81</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="20"/>
@@ -7994,23 +7991,23 @@
         <v>96</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K7" s="29"/>
       <c r="L7" s="20" t="s">
         <v>81</v>
       </c>
       <c r="M7" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="O7" s="20" t="s">
         <v>501</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="P7" s="20" t="s">
         <v>503</v>
-      </c>
-      <c r="O7" s="20" t="s">
-        <v>502</v>
-      </c>
-      <c r="P7" s="20" t="s">
-        <v>504</v>
       </c>
       <c r="Q7" s="20">
         <v>9898989898</v>
@@ -8069,7 +8066,7 @@
         <v>100</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="20"/>
@@ -8083,23 +8080,23 @@
         <v>96</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K8" s="29"/>
       <c r="L8" s="20" t="s">
         <v>100</v>
       </c>
       <c r="M8" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="O8" s="20" t="s">
         <v>501</v>
       </c>
-      <c r="N8" s="20" t="s">
+      <c r="P8" s="20" t="s">
         <v>503</v>
-      </c>
-      <c r="O8" s="20" t="s">
-        <v>502</v>
-      </c>
-      <c r="P8" s="20" t="s">
-        <v>504</v>
       </c>
       <c r="Q8" s="20">
         <v>9898989898</v>
@@ -8152,7 +8149,7 @@
         <v>95</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="20"/>
@@ -8166,23 +8163,23 @@
         <v>96</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K9" s="29"/>
       <c r="L9" s="20" t="s">
         <v>95</v>
       </c>
       <c r="M9" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="O9" s="20" t="s">
         <v>501</v>
       </c>
-      <c r="N9" s="20" t="s">
+      <c r="P9" s="20" t="s">
         <v>503</v>
-      </c>
-      <c r="O9" s="20" t="s">
-        <v>502</v>
-      </c>
-      <c r="P9" s="20" t="s">
-        <v>504</v>
       </c>
       <c r="Q9" s="20">
         <v>9898989898</v>
@@ -8357,23 +8354,23 @@
         <v>67</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="20"/>
       <c r="M12" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="N12" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="O12" s="20" t="s">
         <v>501</v>
       </c>
-      <c r="N12" s="20" t="s">
+      <c r="P12" s="20" t="s">
         <v>503</v>
-      </c>
-      <c r="O12" s="20" t="s">
-        <v>502</v>
-      </c>
-      <c r="P12" s="20" t="s">
-        <v>504</v>
       </c>
       <c r="Q12" s="20">
         <v>9898989898</v>
@@ -8432,7 +8429,7 @@
       </c>
       <c r="I13" s="20"/>
       <c r="J13" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K13" s="29"/>
       <c r="L13" s="20"/>
@@ -8660,7 +8657,7 @@
       </c>
       <c r="I17" s="20"/>
       <c r="J17" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K17" s="29"/>
       <c r="L17" s="20"/>
@@ -8880,7 +8877,7 @@
         <v>25</v>
       </c>
       <c r="R2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="S2" t="s">
         <v>260</v>
@@ -9415,7 +9412,7 @@
         <v>1</v>
       </c>
       <c r="X4" s="12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="Y4" s="21" t="s">
         <v>39</v>
@@ -9884,7 +9881,7 @@
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="41" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="R16" s="7" t="s">
         <v>443</v>
@@ -10194,7 +10191,7 @@
       <c r="T23" s="20"/>
       <c r="U23" s="20"/>
       <c r="V23" s="20" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="W23" s="20"/>
       <c r="X23" s="20"/>
@@ -10221,7 +10218,7 @@
         <v>349</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
@@ -10409,8 +10406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ACADB97-3AA8-40BF-AE7E-787123A27C76}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10499,10 +10496,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -10517,7 +10514,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" t="s">
@@ -10560,16 +10557,16 @@
       </c>
       <c r="H4" s="2"/>
       <c r="S4" t="s">
+        <v>445</v>
+      </c>
+      <c r="T4" t="s">
+        <v>445</v>
+      </c>
+      <c r="U4" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="T4" t="s">
-        <v>498</v>
-      </c>
-      <c r="U4" s="5" t="s">
+      <c r="V4" s="12" t="s">
         <v>499</v>
-      </c>
-      <c r="V4" s="12" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -10593,16 +10590,16 @@
         <v>206</v>
       </c>
       <c r="S7" t="s">
+        <v>445</v>
+      </c>
+      <c r="T7" t="s">
+        <v>445</v>
+      </c>
+      <c r="U7" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="T7" t="s">
-        <v>498</v>
-      </c>
-      <c r="U7" s="5" t="s">
+      <c r="V7" s="12" t="s">
         <v>499</v>
-      </c>
-      <c r="V7" s="12" t="s">
-        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HF_EMEA TEST_DGLD_HF_EMEA_EU_BCT_007 for stores changes updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E8C752-0081-45E8-BA11-BD85EB527D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9072DE61-5C36-4CDA-BADC-9C6E5BA5A901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="559">
   <si>
     <t>UserName</t>
   </si>
@@ -1682,6 +1682,60 @@
   </si>
   <si>
     <t>9GT64Y68Y7425Z97J65X</t>
+  </si>
+  <si>
+    <t>es_Address</t>
+  </si>
+  <si>
+    <t>Calle de la Virgen 47 BJ 1</t>
+  </si>
+  <si>
+    <t>Calasparra</t>
+  </si>
+  <si>
+    <t>Murcia</t>
+  </si>
+  <si>
+    <t>30420</t>
+  </si>
+  <si>
+    <t>eu_Address</t>
+  </si>
+  <si>
+    <t>Creuse</t>
+  </si>
+  <si>
+    <t>de_Address</t>
+  </si>
+  <si>
+    <t>Schaarsteinweg 2</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>20459</t>
+  </si>
+  <si>
+    <t>fr_Address</t>
+  </si>
+  <si>
+    <t>92 Rue Des Lacs</t>
+  </si>
+  <si>
+    <t>Lespinasse</t>
+  </si>
+  <si>
+    <t>Haute-Garonne</t>
+  </si>
+  <si>
+    <t>31150</t>
+  </si>
+  <si>
+    <t>Small Bottle Boot</t>
+  </si>
+  <si>
+    <t>Reef</t>
   </si>
 </sst>
 </file>
@@ -1865,7 +1919,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1926,6 +1980,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2207,10 +2264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV55"/>
+  <dimension ref="A1:AV59"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2226,7 +2283,7 @@
     <col min="10" max="18" width="30.5546875" customWidth="1"/>
     <col min="19" max="19" width="19.6640625" customWidth="1"/>
     <col min="20" max="21" width="22.33203125" customWidth="1"/>
-    <col min="22" max="22" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" customWidth="1"/>
     <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
@@ -2498,7 +2555,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:48" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>514</v>
       </c>
@@ -2655,862 +2712,1111 @@
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="Z7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA7" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="AB7">
-        <v>123</v>
-      </c>
+        <v>541</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" t="s">
+        <v>542</v>
+      </c>
+      <c r="T7" t="s">
+        <v>543</v>
+      </c>
+      <c r="V7" t="s">
+        <v>544</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="7"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>199</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+        <v>546</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="20" t="s">
+        <v>542</v>
+      </c>
+      <c r="T8" s="20" t="s">
+        <v>543</v>
+      </c>
+      <c r="U8" s="20"/>
+      <c r="V8" s="42" t="s">
+        <v>547</v>
+      </c>
+      <c r="W8" s="41" t="s">
+        <v>545</v>
+      </c>
+      <c r="X8" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y8" s="20"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="7"/>
-      <c r="AS8" t="s">
-        <v>327</v>
-      </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>297</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="Z9" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="AA9" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="AB9">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+        <v>548</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="20" t="s">
+        <v>549</v>
+      </c>
+      <c r="T9" s="41" t="s">
+        <v>550</v>
+      </c>
+      <c r="U9" s="20"/>
+      <c r="V9" s="42" t="s">
+        <v>550</v>
+      </c>
+      <c r="W9" s="41" t="s">
+        <v>551</v>
+      </c>
+      <c r="X9" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="7"/>
+    </row>
+    <row r="10" spans="1:48" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="J10" t="s">
-        <v>203</v>
-      </c>
+        <v>552</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="20" t="s">
+        <v>553</v>
+      </c>
+      <c r="T10" s="41" t="s">
+        <v>554</v>
+      </c>
+      <c r="U10" s="20"/>
+      <c r="V10" s="42" t="s">
+        <v>555</v>
+      </c>
+      <c r="W10" s="41" t="s">
+        <v>556</v>
+      </c>
+      <c r="X10" s="41">
+        <v>9898989898</v>
+      </c>
+      <c r="Y10" s="20"/>
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>154</v>
-      </c>
-      <c r="J11" s="18" t="s">
-        <v>484</v>
-      </c>
-      <c r="W11" s="3"/>
-      <c r="X11" s="4"/>
-      <c r="AD11" s="32">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="Z11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA11" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="AB11">
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>539</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>484</v>
-      </c>
-      <c r="W12" s="3"/>
-      <c r="X12" s="4"/>
-      <c r="AD12" s="32"/>
+        <v>199</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="7"/>
+      <c r="AS12" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>172</v>
-      </c>
-      <c r="W13" s="3"/>
-      <c r="X13" s="4"/>
-      <c r="AC13" t="s">
-        <v>173</v>
-      </c>
-      <c r="AD13" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>173</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>39</v>
+        <v>297</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="Z13" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA13" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="AB13">
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>170</v>
-      </c>
-      <c r="W14" s="3"/>
-      <c r="X14" s="4"/>
-      <c r="AC14" t="s">
-        <v>171</v>
-      </c>
-      <c r="AD14" s="32">
-        <v>1</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="J14" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="7"/>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="AC15" s="12" t="s">
-        <v>311</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>484</v>
+      </c>
+      <c r="W15" s="3"/>
+      <c r="X15" s="4"/>
       <c r="AD15" s="32">
         <v>1</v>
       </c>
-      <c r="AE15" t="s">
-        <v>535</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>387</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>190</v>
-      </c>
-      <c r="AH15">
-        <v>1</v>
-      </c>
-      <c r="AV15" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>444</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="AC16" s="34" t="s">
-        <v>445</v>
-      </c>
+        <v>539</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>484</v>
+      </c>
+      <c r="W16" s="3"/>
+      <c r="X16" s="4"/>
       <c r="AD16" s="32"/>
-      <c r="AE16" s="34" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="W17" s="3"/>
+      <c r="X17" s="4"/>
       <c r="AC17" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AD17" s="5" t="s">
         <v>120</v>
       </c>
       <c r="AE17" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AF17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>175</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+        <v>170</v>
+      </c>
+      <c r="W18" s="3"/>
+      <c r="X18" s="4"/>
       <c r="AC18" t="s">
-        <v>174</v>
-      </c>
-      <c r="AD18" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+      <c r="AD18" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>189</v>
+        <v>25</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="AD19" s="5"/>
+      <c r="AC19" s="12" t="s">
+        <v>557</v>
+      </c>
+      <c r="AD19" s="32">
+        <v>1</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>535</v>
+      </c>
       <c r="AF19" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+        <v>558</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>190</v>
+      </c>
+      <c r="AH19">
+        <v>1</v>
+      </c>
+      <c r="AV19" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>444</v>
+      </c>
+      <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="AL20" s="12" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AC20" s="34" t="s">
+        <v>445</v>
+      </c>
+      <c r="AD20" s="32"/>
+      <c r="AE20" s="34" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>176</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
+      <c r="AC21" t="s">
+        <v>177</v>
+      </c>
       <c r="AD21" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AH21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="G22" s="6"/>
+        <v>175</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="AI22" t="s">
+      <c r="AC22" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD22" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>189</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="AD23" s="5"/>
+      <c r="AF23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="AL24" s="12" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="AD25" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="AI26" t="s">
         <v>483</v>
       </c>
-      <c r="AJ22" t="s">
+      <c r="AJ26" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>44</v>
       </c>
-      <c r="Z23" s="5" t="s">
+      <c r="Z27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AA23" s="7" t="s">
+      <c r="AA27" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="AB23">
+      <c r="AB27">
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>46</v>
-      </c>
-      <c r="F24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="S24" t="s">
-        <v>150</v>
-      </c>
-      <c r="T24" t="s">
-        <v>17</v>
-      </c>
-      <c r="V24" t="s">
-        <v>19</v>
-      </c>
-      <c r="W24" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="X24" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z24" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA24" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="AB24">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z25" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA25" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="AB25">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="2"/>
-      <c r="S26" t="s">
-        <v>150</v>
-      </c>
-      <c r="T26" t="s">
-        <v>17</v>
-      </c>
-      <c r="V26" t="s">
-        <v>19</v>
-      </c>
-      <c r="W26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="X26" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y26" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA26" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="AB26">
-        <v>123</v>
-      </c>
-      <c r="AK26" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA27" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB27" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>61</v>
       </c>
       <c r="F28" t="s">
         <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
       <c r="S28" t="s">
-        <v>500</v>
+        <v>150</v>
       </c>
       <c r="T28" t="s">
-        <v>502</v>
-      </c>
-      <c r="U28" t="s">
-        <v>491</v>
+        <v>17</v>
       </c>
       <c r="V28" t="s">
-        <v>501</v>
+        <v>19</v>
       </c>
       <c r="W28" s="5" t="s">
-        <v>503</v>
+        <v>18</v>
       </c>
       <c r="X28" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="Z28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA28" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="AB28">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="Z29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA29" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="AB29">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="E30" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="F30" t="s">
+        <v>50</v>
+      </c>
       <c r="H30" s="2" t="s">
-        <v>493</v>
+        <v>28</v>
       </c>
       <c r="I30" s="2"/>
-      <c r="W30" s="5"/>
+      <c r="S30" t="s">
+        <v>150</v>
+      </c>
+      <c r="T30" t="s">
+        <v>17</v>
+      </c>
+      <c r="V30" t="s">
+        <v>19</v>
+      </c>
+      <c r="W30" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="X30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA30" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="AB30">
+        <v>123</v>
+      </c>
+      <c r="AK30" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA31" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="S32" t="s">
+        <v>500</v>
+      </c>
+      <c r="T32" t="s">
+        <v>502</v>
+      </c>
+      <c r="U32" t="s">
+        <v>491</v>
+      </c>
+      <c r="V32" t="s">
+        <v>501</v>
+      </c>
+      <c r="W32" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="X32" s="5" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>118</v>
-      </c>
-      <c r="F31" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" t="s">
-        <v>15</v>
-      </c>
-      <c r="S31" t="s">
-        <v>500</v>
-      </c>
-      <c r="T31" t="s">
-        <v>502</v>
-      </c>
-      <c r="U31" t="s">
-        <v>491</v>
-      </c>
-      <c r="V31" t="s">
-        <v>501</v>
-      </c>
-      <c r="W31" s="5" t="s">
-        <v>503</v>
-      </c>
-      <c r="X31" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL32" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="33" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>164</v>
-      </c>
-      <c r="AM33" t="s">
-        <v>296</v>
-      </c>
-      <c r="AN33" t="s">
-        <v>314</v>
+        <v>70</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="34" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>166</v>
-      </c>
-      <c r="F34" t="s">
-        <v>167</v>
-      </c>
-      <c r="H34" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="12"/>
-      <c r="R34" s="12"/>
-      <c r="S34" t="s">
-        <v>500</v>
-      </c>
-      <c r="T34" t="s">
-        <v>502</v>
-      </c>
-      <c r="U34" t="s">
-        <v>491</v>
-      </c>
-      <c r="V34" t="s">
-        <v>501</v>
-      </c>
-      <c r="W34" s="5" t="s">
-        <v>503</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="H34" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="W34" s="5"/>
       <c r="X34" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>184</v>
-      </c>
-      <c r="H35" s="23" t="s">
-        <v>506</v>
-      </c>
-      <c r="I35" s="12"/>
-      <c r="AC35" t="s">
-        <v>257</v>
-      </c>
-      <c r="AO35" t="s">
-        <v>186</v>
+        <v>118</v>
+      </c>
+      <c r="F35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
+        <v>15</v>
+      </c>
+      <c r="S35" t="s">
+        <v>500</v>
+      </c>
+      <c r="T35" t="s">
+        <v>502</v>
+      </c>
+      <c r="U35" t="s">
+        <v>491</v>
+      </c>
+      <c r="V35" t="s">
+        <v>501</v>
+      </c>
+      <c r="W35" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="X35" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>279</v>
-      </c>
-      <c r="AO36" t="s">
-        <v>280</v>
+        <v>151</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="37" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>284</v>
-      </c>
-      <c r="F37" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" t="s">
-        <v>14</v>
-      </c>
-      <c r="AO37" t="s">
-        <v>285</v>
+        <v>164</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>296</v>
+      </c>
+      <c r="AN37" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="38" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>215</v>
-      </c>
-      <c r="AC38" t="s">
-        <v>255</v>
-      </c>
-      <c r="AD38" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF38" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP38" t="s">
-        <v>83</v>
+        <v>166</v>
+      </c>
+      <c r="F38" t="s">
+        <v>167</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="12"/>
+      <c r="S38" t="s">
+        <v>500</v>
+      </c>
+      <c r="T38" t="s">
+        <v>502</v>
+      </c>
+      <c r="U38" t="s">
+        <v>491</v>
+      </c>
+      <c r="V38" t="s">
+        <v>501</v>
+      </c>
+      <c r="W38" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="X38" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>209</v>
-      </c>
-      <c r="AF39" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP39" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ39" t="s">
-        <v>216</v>
-      </c>
-      <c r="AR39" t="s">
-        <v>214</v>
+        <v>184</v>
+      </c>
+      <c r="H39" s="23" t="s">
+        <v>506</v>
+      </c>
+      <c r="I39" s="12"/>
+      <c r="AC39" t="s">
+        <v>257</v>
+      </c>
+      <c r="AO39" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>339</v>
-      </c>
-      <c r="J40" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="O40" t="s">
-        <v>341</v>
-      </c>
-      <c r="P40" s="26" t="s">
-        <v>505</v>
-      </c>
-      <c r="Q40" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="R40" s="5"/>
+        <v>279</v>
+      </c>
+      <c r="AO40" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>343</v>
-      </c>
-      <c r="R41" t="s">
-        <v>345</v>
+        <v>284</v>
+      </c>
+      <c r="F41" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO41" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>346</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="N42" s="24" t="s">
-        <v>507</v>
+        <v>215</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>255</v>
+      </c>
+      <c r="AD42" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP42" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>348</v>
-      </c>
-      <c r="F43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" t="s">
-        <v>349</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>513</v>
-      </c>
-      <c r="AO43" t="s">
-        <v>351</v>
+        <v>209</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP43" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ43" t="s">
+        <v>216</v>
+      </c>
+      <c r="AR43" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>353</v>
-      </c>
-      <c r="P44" t="s">
-        <v>540</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="O44" t="s">
+        <v>341</v>
+      </c>
+      <c r="P44" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="Q44" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="R44" s="5"/>
     </row>
     <row r="45" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>201</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="F45" t="s">
-        <v>14</v>
-      </c>
-      <c r="G45" t="s">
-        <v>349</v>
-      </c>
-      <c r="H45" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="S45" t="s">
-        <v>62</v>
-      </c>
-      <c r="T45" t="s">
-        <v>63</v>
-      </c>
-      <c r="V45" t="s">
-        <v>64</v>
-      </c>
-      <c r="W45" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="X45" s="5" t="s">
-        <v>66</v>
+        <v>343</v>
+      </c>
+      <c r="R45" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="46" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>363</v>
-      </c>
-      <c r="P46" s="5" t="s">
-        <v>364</v>
+        <v>346</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="M46" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="N46" s="24" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="47" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>432</v>
-      </c>
-      <c r="P47" s="27" t="s">
-        <v>434</v>
+        <v>348</v>
+      </c>
+      <c r="F47" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" t="s">
+        <v>349</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="AO47" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="48" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>433</v>
-      </c>
-      <c r="P48" s="26" t="s">
-        <v>512</v>
+        <v>353</v>
+      </c>
+      <c r="P48" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="49" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>232</v>
-      </c>
-      <c r="AT49" t="s">
-        <v>531</v>
-      </c>
-      <c r="AU49" s="31" t="s">
-        <v>232</v>
+        <v>201</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="F49" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" t="s">
+        <v>349</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="S49" t="s">
+        <v>62</v>
+      </c>
+      <c r="T49" t="s">
+        <v>63</v>
+      </c>
+      <c r="V49" t="s">
+        <v>64</v>
+      </c>
+      <c r="W49" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="X49" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A50" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="33"/>
-      <c r="L50" s="33"/>
-      <c r="M50" s="33"/>
-      <c r="N50" s="33"/>
-      <c r="O50" s="33"/>
-      <c r="P50" s="33"/>
-      <c r="Q50" s="33"/>
-      <c r="R50" s="33"/>
-      <c r="S50" s="33"/>
-      <c r="T50" s="33"/>
-      <c r="U50" s="33"/>
-      <c r="V50" s="33"/>
-      <c r="W50" s="33"/>
-      <c r="X50" s="33"/>
-      <c r="Y50" s="33"/>
-      <c r="Z50" s="33"/>
-      <c r="AA50" s="33"/>
-      <c r="AB50" s="33"/>
-      <c r="AC50" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="AD50" s="33">
-        <v>1</v>
-      </c>
-      <c r="AE50" s="33"/>
+      <c r="A50" t="s">
+        <v>363</v>
+      </c>
+      <c r="P50" s="5" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="51" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>448</v>
-      </c>
-      <c r="P51" s="26" t="s">
-        <v>511</v>
+        <v>432</v>
+      </c>
+      <c r="P51" s="27" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="52" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>510</v>
-      </c>
-      <c r="P52" t="s">
-        <v>509</v>
+        <v>433</v>
+      </c>
+      <c r="P52" s="26" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="53" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>521</v>
-      </c>
-      <c r="S53" t="s">
-        <v>522</v>
+        <v>232</v>
+      </c>
+      <c r="AT53" t="s">
+        <v>531</v>
+      </c>
+      <c r="AU53" s="31" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>529</v>
-      </c>
-      <c r="AC54" s="22" t="s">
-        <v>534</v>
-      </c>
+      <c r="A54" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B54" s="33"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="33"/>
+      <c r="L54" s="33"/>
+      <c r="M54" s="33"/>
+      <c r="N54" s="33"/>
+      <c r="O54" s="33"/>
+      <c r="P54" s="33"/>
+      <c r="Q54" s="33"/>
+      <c r="R54" s="33"/>
+      <c r="S54" s="33"/>
+      <c r="T54" s="33"/>
+      <c r="U54" s="33"/>
+      <c r="V54" s="33"/>
+      <c r="W54" s="33"/>
+      <c r="X54" s="33"/>
+      <c r="Y54" s="33"/>
+      <c r="Z54" s="33"/>
+      <c r="AA54" s="33"/>
+      <c r="AB54" s="33"/>
+      <c r="AC54" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="AD54" s="33">
+        <v>1</v>
+      </c>
+      <c r="AE54" s="33"/>
     </row>
     <row r="55" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>448</v>
+      </c>
+      <c r="P55" s="26" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="56" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>510</v>
+      </c>
+      <c r="P56" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="57" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>521</v>
+      </c>
+      <c r="S57" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="58" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>529</v>
+      </c>
+      <c r="AC58" s="22" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="59" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>533</v>
       </c>
-      <c r="P55" t="s">
+      <c r="P59" t="s">
         <v>509</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D20" r:id="rId2" display="Lotuswave@123" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H26" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H30" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="AL20" r:id="rId6" xr:uid="{081C5E6B-B750-4DF9-A406-8CFA5CF35321}"/>
-    <hyperlink ref="H34" r:id="rId7" xr:uid="{E7117AFE-BF51-4362-86E8-EC31CD714F35}"/>
-    <hyperlink ref="D2" r:id="rId8" xr:uid="{2D39057E-A748-4174-BA59-49433F76661C}"/>
-    <hyperlink ref="H35" r:id="rId9" xr:uid="{7ECA06F7-0F76-44C2-9FB9-4179E4310E54}"/>
-    <hyperlink ref="B2" r:id="rId10" xr:uid="{B14C1544-364C-4E03-A43F-D19E66177301}"/>
-    <hyperlink ref="I2" r:id="rId11" xr:uid="{AA16F981-3056-4646-A2C1-ECE17E4E92D7}"/>
-    <hyperlink ref="C2" r:id="rId12" xr:uid="{6B47FB1F-967B-4003-9184-BEF0C984D5EA}"/>
-    <hyperlink ref="D3" r:id="rId13" xr:uid="{43D25ADB-4E4D-4766-8BDD-9478BEC1A271}"/>
-    <hyperlink ref="E3" r:id="rId14" xr:uid="{26E68202-5CE3-42C9-9DA5-1788DD83F3DD}"/>
-    <hyperlink ref="AC15" r:id="rId15" display="https://mcloud-na-preprod.hydroflask.com/wide-mouth-flex-cap?color=Black" xr:uid="{29EA729C-67AB-4332-AD2E-87301AAE2E8C}"/>
-    <hyperlink ref="H43" r:id="rId16" xr:uid="{7950AECF-C1F8-4C97-8F40-50E8B8819E85}"/>
-    <hyperlink ref="B45" r:id="rId17" xr:uid="{F8F2B0AD-86F8-4E80-8B1A-138B21EB05DB}"/>
-    <hyperlink ref="D45" r:id="rId18" xr:uid="{F252BFF6-7553-465C-B03F-0EDCA58E86DD}"/>
-    <hyperlink ref="H45" r:id="rId19" xr:uid="{819E02F2-2ED2-485D-85EB-576F27665CFC}"/>
-    <hyperlink ref="E6" r:id="rId20" xr:uid="{1D5FD444-4596-442E-BAE6-C911BFAC6718}"/>
-    <hyperlink ref="D6" r:id="rId21" xr:uid="{193852EB-47AA-454A-91E5-A4E8624ADA13}"/>
-    <hyperlink ref="B6" r:id="rId22" xr:uid="{450F9719-F0D6-46E4-A813-0721F12125A4}"/>
-    <hyperlink ref="I6" r:id="rId23" display="LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{4B3C7CD9-EB98-4907-833E-9C41C9ADEE76}"/>
-    <hyperlink ref="C6" r:id="rId24" display="LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{72A898E1-E814-40B9-9CCE-853A961F2109}"/>
-    <hyperlink ref="H6" r:id="rId25" xr:uid="{4A93039F-9FB8-42CB-9ACE-C0BE7F576AAE}"/>
-    <hyperlink ref="D29" r:id="rId26" xr:uid="{ADDAE6FC-BD5F-4B77-8488-C7AA571E5B74}"/>
-    <hyperlink ref="B3" r:id="rId27" xr:uid="{4C8A5F37-6801-432A-83D9-87956E37DC33}"/>
-    <hyperlink ref="C3" r:id="rId28" xr:uid="{98DA5743-5463-4C67-80BC-A5B72466CF09}"/>
-    <hyperlink ref="H3" r:id="rId29" xr:uid="{8BB37601-C38B-45F2-8233-C6E902C59024}"/>
-    <hyperlink ref="I3" r:id="rId30" xr:uid="{867E547C-77C0-4645-B477-E04A428B234D}"/>
-    <hyperlink ref="H4" r:id="rId31" xr:uid="{E7256B83-DC26-4708-AE9C-81FB186678F7}"/>
-    <hyperlink ref="E4" r:id="rId32" xr:uid="{D50736A5-4DBC-478E-9DE0-ABB9D0062209}"/>
-    <hyperlink ref="D4" r:id="rId33" xr:uid="{69779EF0-F236-481C-A058-70D6A46D05A2}"/>
-    <hyperlink ref="B4" r:id="rId34" xr:uid="{D3894DA7-9C12-4B05-8D36-237B29B85F74}"/>
-    <hyperlink ref="I4" r:id="rId35" xr:uid="{80743E67-671B-43D1-A4CD-D302F8246EAB}"/>
-    <hyperlink ref="C4" r:id="rId36" xr:uid="{A9B3E11E-DA4C-432B-9EA4-560C3B1DE7F8}"/>
-    <hyperlink ref="B5" r:id="rId37" xr:uid="{1A2204FF-FA87-450C-B7A8-D6C45DF20846}"/>
-    <hyperlink ref="C5" r:id="rId38" xr:uid="{3B75E376-FC70-49B2-944E-50BA6A419594}"/>
-    <hyperlink ref="H5" r:id="rId39" xr:uid="{FE35CC26-D326-47B6-9D1E-B2E9811E21D2}"/>
-    <hyperlink ref="I5" r:id="rId40" xr:uid="{92993A7C-001C-4FE6-9125-B4B00E04A753}"/>
-    <hyperlink ref="H29" r:id="rId41" xr:uid="{22165C55-D8F7-4059-A2E1-F084718509FB}"/>
-    <hyperlink ref="I29" r:id="rId42" xr:uid="{42C11063-5B1A-455C-98C2-65B906145796}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{92F09EC2-FC6F-443B-965E-DCA7B56F1753}"/>
+    <hyperlink ref="D24" r:id="rId2" display="Lotuswave@123" xr:uid="{27A376CC-4E23-4441-B806-FE9FF359794E}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{5B310480-7344-4661-AB0F-D7D61F727B40}"/>
+    <hyperlink ref="H30" r:id="rId4" xr:uid="{D3AC8605-ACE0-4742-A275-CC55BA0B713E}"/>
+    <hyperlink ref="H34" r:id="rId5" xr:uid="{EBF04138-1F63-4113-A63D-68EC86409EAF}"/>
+    <hyperlink ref="AL24" r:id="rId6" xr:uid="{C3ED735C-0638-4013-B1A9-35D874D27CCD}"/>
+    <hyperlink ref="H38" r:id="rId7" xr:uid="{7B92FAF6-FC7B-4378-BAA5-F455D3557016}"/>
+    <hyperlink ref="D2" r:id="rId8" xr:uid="{6D9C84C2-080E-49A8-91A9-0C4040F17B99}"/>
+    <hyperlink ref="H39" r:id="rId9" xr:uid="{5EDA0D22-59C6-4E86-B1C8-F3DDADDA222C}"/>
+    <hyperlink ref="B2" r:id="rId10" xr:uid="{49EA4C67-65EF-4ECE-B592-DD27DDBFE9D8}"/>
+    <hyperlink ref="I2" r:id="rId11" xr:uid="{41758504-FDAA-49B8-A517-3CF2E58C91CC}"/>
+    <hyperlink ref="C2" r:id="rId12" xr:uid="{12FE48FE-6D5F-46FF-BB71-C2756AE73EE8}"/>
+    <hyperlink ref="D3" r:id="rId13" xr:uid="{62C3648F-7D52-4B9F-ADF3-7CB24D30FA17}"/>
+    <hyperlink ref="E3" r:id="rId14" xr:uid="{32229FD5-4AFA-45C3-BF60-2566B7569180}"/>
+    <hyperlink ref="AC19" r:id="rId15" display="https://mcloud-na-preprod.hydroflask.com/wide-mouth-flex-cap?color=Black" xr:uid="{618667E2-3380-4A1C-B34F-ABDD50D4EE61}"/>
+    <hyperlink ref="H47" r:id="rId16" xr:uid="{7BF19D0A-861B-44DA-ABCD-EB14EC4082CF}"/>
+    <hyperlink ref="B49" r:id="rId17" xr:uid="{44BE9CEE-1274-4416-B56D-993DF9A30DAD}"/>
+    <hyperlink ref="D49" r:id="rId18" xr:uid="{B31DCDCE-921F-4B4A-BEA7-7D9C21058AC8}"/>
+    <hyperlink ref="H49" r:id="rId19" xr:uid="{7332F9F7-6E5B-4009-8325-28D766EC646E}"/>
+    <hyperlink ref="E6" r:id="rId20" xr:uid="{2C317B8E-AF32-4D4C-AE44-1F2FC9B108BE}"/>
+    <hyperlink ref="D6" r:id="rId21" xr:uid="{E6081600-960B-4A22-B355-F1C4E40470AA}"/>
+    <hyperlink ref="B6" r:id="rId22" xr:uid="{7D100C12-0453-4673-AC35-2EA4A2603564}"/>
+    <hyperlink ref="I6" r:id="rId23" display="LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{4380A0E0-76DF-485C-8BEA-6C28F9B24971}"/>
+    <hyperlink ref="C6" r:id="rId24" display="LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{8F318BE4-05CB-41C2-8BFD-E5C42814E494}"/>
+    <hyperlink ref="H6" r:id="rId25" xr:uid="{407C8F4E-9B49-4856-B5B1-AADA1B530463}"/>
+    <hyperlink ref="D33" r:id="rId26" xr:uid="{CFA846D7-1044-49EA-A0C9-5358EDB0782D}"/>
+    <hyperlink ref="B3" r:id="rId27" xr:uid="{A4EF70F2-1E9D-4209-9990-D57B7B04D033}"/>
+    <hyperlink ref="C3" r:id="rId28" xr:uid="{A02552C8-A6E5-4D41-80F6-00B2ABF9087C}"/>
+    <hyperlink ref="H3" r:id="rId29" xr:uid="{475B0B91-5BB6-4DC1-8A14-637459A21F69}"/>
+    <hyperlink ref="I3" r:id="rId30" xr:uid="{31D5282C-3A0B-47FC-A07B-CC23BA4F574E}"/>
+    <hyperlink ref="H4" r:id="rId31" xr:uid="{D910C898-EA43-409E-B04E-9B9BFB5A3D9D}"/>
+    <hyperlink ref="E4" r:id="rId32" xr:uid="{B86A9B6C-A653-4B11-A92A-B12ECCF56B54}"/>
+    <hyperlink ref="D4" r:id="rId33" xr:uid="{5357CB07-F4C9-42F8-8AA6-82DE7438DA1F}"/>
+    <hyperlink ref="B4" r:id="rId34" xr:uid="{6B5AE7EC-0874-471E-8B2A-119BB6055DFF}"/>
+    <hyperlink ref="I4" r:id="rId35" xr:uid="{C425EF67-01D4-42EC-8E86-0A6DFDCBD4BA}"/>
+    <hyperlink ref="C4" r:id="rId36" xr:uid="{50F1E974-01BC-40BB-A015-3C5D601540DD}"/>
+    <hyperlink ref="B5" r:id="rId37" xr:uid="{0A429E56-7D42-4B18-B613-96996A8386C4}"/>
+    <hyperlink ref="C5" r:id="rId38" xr:uid="{817C7CDF-7723-4347-999A-B70D0C4C4C9F}"/>
+    <hyperlink ref="H5" r:id="rId39" xr:uid="{46997A70-4DF6-42DF-98DE-3A15FE00FF24}"/>
+    <hyperlink ref="I5" r:id="rId40" xr:uid="{323D0279-E435-4C6C-805F-A066B3FCDA92}"/>
+    <hyperlink ref="H33" r:id="rId41" xr:uid="{EDD9788C-AEBE-4F86-8A6C-8043A32B81A6}"/>
+    <hyperlink ref="I33" r:id="rId42" xr:uid="{68882096-6651-4D29-9355-6F1410B100AA}"/>
+    <hyperlink ref="H8" r:id="rId43" xr:uid="{867EC1A7-B881-422A-8354-C1C7FCE40AAE}"/>
+    <hyperlink ref="E8" r:id="rId44" xr:uid="{5ACEF6FA-BF68-4BBD-BE65-3578FCD63C44}"/>
+    <hyperlink ref="D8" r:id="rId45" xr:uid="{3607587D-2F3E-4312-8C6F-F1EF148F7A1A}"/>
+    <hyperlink ref="B8" r:id="rId46" xr:uid="{838DB807-8878-4727-B652-F09EAEE77C42}"/>
+    <hyperlink ref="I8" r:id="rId47" xr:uid="{C0E6A241-0765-4C32-84F5-3C36597F10B8}"/>
+    <hyperlink ref="C8" r:id="rId48" xr:uid="{93184341-165F-4978-8373-D4F8C53F1010}"/>
+    <hyperlink ref="B7" r:id="rId49" xr:uid="{8F43DB90-24E3-4846-8CAB-59E29F5C8F69}"/>
+    <hyperlink ref="C7" r:id="rId50" xr:uid="{8CDC1C5A-4BC4-487C-B68D-BB1736CC0DA3}"/>
+    <hyperlink ref="I7" r:id="rId51" xr:uid="{7EEA7DAF-6CEE-4D1C-8C7C-2398537E5F64}"/>
+    <hyperlink ref="H9" r:id="rId52" xr:uid="{20D94877-40D1-4499-BDB8-432C3EFF17CB}"/>
+    <hyperlink ref="E9" r:id="rId53" xr:uid="{1C0716E0-6BCD-4F2D-8B96-759D6C7BC81B}"/>
+    <hyperlink ref="D9" r:id="rId54" xr:uid="{CF4E4FEE-4C04-4CFB-BDD9-E9057E6D030B}"/>
+    <hyperlink ref="B9" r:id="rId55" xr:uid="{B77F0653-F665-442B-B15F-A91355FA4CB0}"/>
+    <hyperlink ref="I9" r:id="rId56" xr:uid="{5DAA662A-7326-4446-B116-E19C32060724}"/>
+    <hyperlink ref="C9" r:id="rId57" xr:uid="{A9717764-ED0E-45EE-9C90-0A9B4F50CACD}"/>
+    <hyperlink ref="H10" r:id="rId58" xr:uid="{A4A59B24-06B2-4E63-B3A2-5F0E79B1DBBA}"/>
+    <hyperlink ref="E10" r:id="rId59" xr:uid="{CA145D2C-147B-4D9D-A898-BAC9A2F14709}"/>
+    <hyperlink ref="D10" r:id="rId60" xr:uid="{F2DB5085-D4CD-48A5-9D5D-80C3365BFE48}"/>
+    <hyperlink ref="B10" r:id="rId61" xr:uid="{17E9DB6C-30D3-4F48-81EA-C35AF660B980}"/>
+    <hyperlink ref="I10" r:id="rId62" xr:uid="{797DAE89-D941-4743-B597-439A5C30AAF0}"/>
+    <hyperlink ref="C10" r:id="rId63" xr:uid="{34EC3537-EEF4-4D6F-923E-4AE4713BD831}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId43"/>
+  <pageSetup orientation="portrait" r:id="rId64"/>
 </worksheet>
 </file>
 
@@ -10406,7 +10712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ACADB97-3AA8-40BF-AE7E-787123A27C76}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
HF-EMEA: PLP product change and Price dragdrop changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9072DE61-5C36-4CDA-BADC-9C6E5BA5A901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBE5726-36E2-4F13-BEAE-1ED8493C0C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28800" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1663,9 +1663,6 @@
     <t>Giftcard_Partial_5</t>
   </si>
   <si>
-    <t>Small Trail Series™ Boot</t>
-  </si>
-  <si>
     <t>12 oz (355 ml) Mug</t>
   </si>
   <si>
@@ -1736,6 +1733,9 @@
   </si>
   <si>
     <t>Reef</t>
+  </si>
+  <si>
+    <t>Standard Mouth Flex Straw Cap</t>
   </si>
 </sst>
 </file>
@@ -1743,10 +1743,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1879,6 +1879,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1919,12 +1926,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1950,7 +1957,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1982,6 +1989,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2266,34 +2276,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="Q26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AC58" sqref="AC58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="18" width="30.5546875" customWidth="1"/>
-    <col min="19" max="19" width="19.6640625" customWidth="1"/>
-    <col min="20" max="21" width="22.33203125" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" customWidth="1"/>
-    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="18" width="30.5703125" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1"/>
+    <col min="20" max="21" width="22.28515625" customWidth="1"/>
+    <col min="22" max="22" width="14.7109375" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.33203125" customWidth="1"/>
+    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2439,7 +2449,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2497,7 +2507,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -2555,7 +2565,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:48" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>514</v>
       </c>
@@ -2610,7 +2620,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -2652,7 +2662,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>438</v>
       </c>
@@ -2710,9 +2720,9 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>499</v>
@@ -2748,16 +2758,16 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" t="s">
+        <v>541</v>
+      </c>
+      <c r="T7" t="s">
         <v>542</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>543</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" s="5" t="s">
         <v>544</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>545</v>
       </c>
       <c r="X7" s="5" t="s">
         <v>59</v>
@@ -2765,9 +2775,9 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="7"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>499</v>
@@ -2803,17 +2813,17 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="20" t="s">
+        <v>541</v>
+      </c>
+      <c r="T8" s="20" t="s">
         <v>542</v>
-      </c>
-      <c r="T8" s="20" t="s">
-        <v>543</v>
       </c>
       <c r="U8" s="20"/>
       <c r="V8" s="42" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="W8" s="41" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="X8" s="41" t="s">
         <v>59</v>
@@ -2822,9 +2832,9 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>499</v>
@@ -2860,17 +2870,17 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="20" t="s">
+        <v>548</v>
+      </c>
+      <c r="T9" s="41" t="s">
         <v>549</v>
-      </c>
-      <c r="T9" s="41" t="s">
-        <v>550</v>
       </c>
       <c r="U9" s="20"/>
       <c r="V9" s="42" t="s">
+        <v>549</v>
+      </c>
+      <c r="W9" s="41" t="s">
         <v>550</v>
-      </c>
-      <c r="W9" s="41" t="s">
-        <v>551</v>
       </c>
       <c r="X9" s="41" t="s">
         <v>59</v>
@@ -2879,9 +2889,9 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="1:48" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:48" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>499</v>
@@ -2917,17 +2927,17 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="20" t="s">
+        <v>552</v>
+      </c>
+      <c r="T10" s="41" t="s">
         <v>553</v>
-      </c>
-      <c r="T10" s="41" t="s">
-        <v>554</v>
       </c>
       <c r="U10" s="20"/>
       <c r="V10" s="42" t="s">
+        <v>554</v>
+      </c>
+      <c r="W10" s="41" t="s">
         <v>555</v>
-      </c>
-      <c r="W10" s="41" t="s">
-        <v>556</v>
       </c>
       <c r="X10" s="41">
         <v>9898989898</v>
@@ -2936,7 +2946,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2954,7 +2964,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>199</v>
       </c>
@@ -2966,7 +2976,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>297</v>
       </c>
@@ -2982,7 +2992,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>155</v>
       </c>
@@ -2994,7 +3004,7 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="7"/>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -3007,9 +3017,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="J16" s="18" t="s">
         <v>484</v>
@@ -3018,7 +3028,7 @@
       <c r="X16" s="4"/>
       <c r="AD16" s="32"/>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>172</v>
       </c>
@@ -3037,7 +3047,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>170</v>
       </c>
@@ -3050,23 +3060,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="AC19" s="12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="AD19" s="32">
         <v>1</v>
       </c>
       <c r="AE19" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="AF19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AG19" t="s">
         <v>190</v>
@@ -3078,7 +3088,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>444</v>
       </c>
@@ -3092,7 +3102,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>176</v>
       </c>
@@ -3111,7 +3121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>175</v>
       </c>
@@ -3124,7 +3134,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>189</v>
       </c>
@@ -3135,7 +3145,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -3159,7 +3169,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3172,7 +3182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -3188,7 +3198,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -3202,7 +3212,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -3239,7 +3249,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -3253,7 +3263,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -3295,7 +3305,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -3309,7 +3319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -3338,7 +3348,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -3355,7 +3365,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -3372,7 +3382,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>118</v>
       </c>
@@ -3401,7 +3411,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>151</v>
       </c>
@@ -3409,7 +3419,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>164</v>
       </c>
@@ -3420,7 +3430,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>166</v>
       </c>
@@ -3459,7 +3469,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>184</v>
       </c>
@@ -3474,7 +3484,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>279</v>
       </c>
@@ -3482,7 +3492,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>284</v>
       </c>
@@ -3496,7 +3506,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>215</v>
       </c>
@@ -3513,7 +3523,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>209</v>
       </c>
@@ -3530,7 +3540,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>339</v>
       </c>
@@ -3553,7 +3563,7 @@
       </c>
       <c r="R44" s="5"/>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>343</v>
       </c>
@@ -3561,7 +3571,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>346</v>
       </c>
@@ -3575,7 +3585,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>348</v>
       </c>
@@ -3592,15 +3602,15 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>353</v>
       </c>
       <c r="P48" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.3">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="49" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>201</v>
       </c>
@@ -3635,7 +3645,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>363</v>
       </c>
@@ -3643,7 +3653,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>432</v>
       </c>
@@ -3651,7 +3661,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="52" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>433</v>
       </c>
@@ -3659,7 +3669,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="53" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>232</v>
       </c>
@@ -3670,7 +3680,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="54" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
         <v>153</v>
       </c>
@@ -3709,7 +3719,7 @@
       </c>
       <c r="AE54" s="33"/>
     </row>
-    <row r="55" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>448</v>
       </c>
@@ -3717,7 +3727,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="56" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>510</v>
       </c>
@@ -3725,7 +3735,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="57" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>521</v>
       </c>
@@ -3733,15 +3743,15 @@
         <v>522</v>
       </c>
     </row>
-    <row r="58" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:47" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>529</v>
       </c>
-      <c r="AC58" s="22" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="59" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AC58" s="43" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="59" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>533</v>
       </c>
@@ -3828,18 +3838,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3937,7 +3947,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3984,7 +3994,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4034,7 +4044,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -4081,7 +4091,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4097,7 +4107,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -4109,7 +4119,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -4120,7 +4130,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4142,7 +4152,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -4155,7 +4165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -4171,7 +4181,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4185,7 +4195,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -4201,7 +4211,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -4215,7 +4225,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -4257,7 +4267,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -4283,7 +4293,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -4294,7 +4304,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4309,7 +4319,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -4367,12 +4377,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4443,7 +4453,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4490,7 +4500,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4506,7 +4516,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -4537,7 +4547,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4545,7 +4555,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -4578,20 +4588,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.33203125" customWidth="1"/>
-    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.28515625" customWidth="1"/>
+    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4680,7 +4690,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4728,7 +4738,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4744,7 +4754,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -4764,7 +4774,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -4783,7 +4793,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -4802,7 +4812,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -4810,7 +4820,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -4818,7 +4828,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -4835,7 +4845,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -4852,7 +4862,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -4869,7 +4879,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -4886,7 +4896,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -4897,7 +4907,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -4908,7 +4918,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4925,7 +4935,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -4954,7 +4964,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4965,7 +4975,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4979,7 +4989,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -4993,7 +5003,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -5007,7 +5017,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -5015,7 +5025,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -5045,7 +5055,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -5115,19 +5125,19 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.6640625" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5153,7 +5163,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5176,7 +5186,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -5207,16 +5217,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5230,7 +5240,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -5256,27 +5266,27 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5546875" customWidth="1"/>
-    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5703125" customWidth="1"/>
+    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.109375" customWidth="1"/>
+    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.140625" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -5335,7 +5345,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>228</v>
       </c>
@@ -5360,7 +5370,7 @@
       <c r="R2" s="20"/>
       <c r="S2" s="20"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>230</v>
       </c>
@@ -5389,7 +5399,7 @@
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>232</v>
       </c>
@@ -5414,7 +5424,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>233</v>
       </c>
@@ -5441,7 +5451,7 @@
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>236</v>
       </c>
@@ -5474,7 +5484,7 @@
       <c r="R6" s="20"/>
       <c r="S6" s="20"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>238</v>
       </c>
@@ -5499,7 +5509,7 @@
       <c r="R7" s="20"/>
       <c r="S7" s="20"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>262</v>
       </c>
@@ -5524,7 +5534,7 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>281</v>
       </c>
@@ -5549,7 +5559,7 @@
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>286</v>
       </c>
@@ -5576,7 +5586,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>318</v>
       </c>
@@ -5601,7 +5611,7 @@
       <c r="R11" s="20"/>
       <c r="S11" s="20"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>320</v>
       </c>
@@ -5628,7 +5638,7 @@
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>321</v>
       </c>
@@ -5653,7 +5663,7 @@
       <c r="R13" s="20"/>
       <c r="S13" s="20"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>323</v>
       </c>
@@ -5678,7 +5688,7 @@
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>334</v>
       </c>
@@ -5703,7 +5713,7 @@
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>337</v>
       </c>
@@ -5728,7 +5738,7 @@
       <c r="R16" s="20"/>
       <c r="S16" s="20"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>450</v>
       </c>
@@ -5736,7 +5746,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>451</v>
       </c>
@@ -5744,7 +5754,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>452</v>
       </c>
@@ -5752,12 +5762,12 @@
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>528</v>
       </c>
       <c r="J20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -5774,31 +5784,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.6640625" customWidth="1"/>
-    <col min="17" max="24" width="30.5546875" customWidth="1"/>
-    <col min="25" max="25" width="19.6640625" customWidth="1"/>
-    <col min="26" max="27" width="22.33203125" customWidth="1"/>
-    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.7109375" customWidth="1"/>
+    <col min="17" max="24" width="30.5703125" customWidth="1"/>
+    <col min="25" max="25" width="19.7109375" customWidth="1"/>
+    <col min="26" max="27" width="22.28515625" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.33203125" customWidth="1"/>
+    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5950,7 +5960,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6020,7 +6030,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>455</v>
       </c>
@@ -6090,7 +6100,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>457</v>
       </c>
@@ -6160,7 +6170,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>458</v>
       </c>
@@ -6230,7 +6240,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>461</v>
       </c>
@@ -6300,7 +6310,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -6370,7 +6380,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>468</v>
       </c>
@@ -6411,7 +6421,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>469</v>
       </c>
@@ -6452,7 +6462,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>463</v>
       </c>
@@ -6522,7 +6532,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>406</v>
       </c>
@@ -6583,7 +6593,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -6642,7 +6652,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>359</v>
       </c>
@@ -6688,7 +6698,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6711,7 +6721,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>297</v>
       </c>
@@ -6734,7 +6744,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -6753,7 +6763,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6764,7 +6774,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6786,7 +6796,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>366</v>
       </c>
@@ -6799,7 +6809,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>368</v>
       </c>
@@ -6812,7 +6822,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -6825,7 +6835,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>375</v>
       </c>
@@ -6838,7 +6848,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>397</v>
       </c>
@@ -6851,7 +6861,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>376</v>
       </c>
@@ -6864,7 +6874,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -6880,7 +6890,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -6896,7 +6906,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>401</v>
       </c>
@@ -6915,7 +6925,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>405</v>
       </c>
@@ -6934,7 +6944,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>382</v>
       </c>
@@ -6950,7 +6960,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>385</v>
       </c>
@@ -6966,7 +6976,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>411</v>
       </c>
@@ -6982,7 +6992,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>412</v>
       </c>
@@ -6998,7 +7008,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>386</v>
       </c>
@@ -7014,7 +7024,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>389</v>
       </c>
@@ -7027,7 +7037,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>403</v>
       </c>
@@ -7040,7 +7050,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -7053,7 +7063,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>424</v>
       </c>
@@ -7066,7 +7076,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>398</v>
       </c>
@@ -7079,7 +7089,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>394</v>
       </c>
@@ -7095,7 +7105,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>423</v>
       </c>
@@ -7111,7 +7121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -7127,7 +7137,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>402</v>
       </c>
@@ -7140,7 +7150,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>415</v>
       </c>
@@ -7162,7 +7172,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -7180,7 +7190,7 @@
       <c r="AI44" s="25"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>414</v>
       </c>
@@ -7193,7 +7203,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -7213,7 +7223,7 @@
       <c r="AI46" s="25"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -7232,7 +7242,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -7245,7 +7255,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -7256,7 +7266,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -7269,7 +7279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -7292,7 +7302,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -7306,7 +7316,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -7343,7 +7353,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -7357,7 +7367,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -7399,7 +7409,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -7425,7 +7435,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -7449,7 +7459,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -7473,7 +7483,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -7499,7 +7509,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -7531,7 +7541,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -7545,7 +7555,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>373</v>
       </c>
@@ -7559,7 +7569,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -7576,7 +7586,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -7593,7 +7603,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>339</v>
       </c>
@@ -7615,7 +7625,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>343</v>
       </c>
@@ -7623,7 +7633,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>346</v>
       </c>
@@ -7634,7 +7644,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>348</v>
       </c>
@@ -7651,7 +7661,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>353</v>
       </c>
@@ -7659,7 +7669,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -7694,7 +7704,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>363</v>
       </c>
@@ -7785,36 +7795,36 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -7951,7 +7961,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -8026,7 +8036,7 @@
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
@@ -8083,7 +8093,7 @@
       <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>248</v>
       </c>
@@ -8136,7 +8146,7 @@
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>68</v>
       </c>
@@ -8199,7 +8209,7 @@
       <c r="AR5" s="20"/>
       <c r="AS5" s="20"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>75</v>
       </c>
@@ -8278,7 +8288,7 @@
       <c r="AR6" s="20"/>
       <c r="AS6" s="20"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>81</v>
       </c>
@@ -8367,7 +8377,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>100</v>
       </c>
@@ -8450,7 +8460,7 @@
       <c r="AR8" s="20"/>
       <c r="AS8" s="20"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>95</v>
       </c>
@@ -8535,7 +8545,7 @@
       <c r="AR9" s="20"/>
       <c r="AS9" s="20"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -8586,7 +8596,7 @@
       <c r="AR10" s="20"/>
       <c r="AS10" s="20"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>103</v>
       </c>
@@ -8643,7 +8653,7 @@
       <c r="AR11" s="20"/>
       <c r="AS11" s="20"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>107</v>
       </c>
@@ -8718,7 +8728,7 @@
       <c r="AR12" s="20"/>
       <c r="AS12" s="20"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>112</v>
       </c>
@@ -8781,7 +8791,7 @@
       <c r="AR13" s="20"/>
       <c r="AS13" s="20"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>249</v>
       </c>
@@ -8836,7 +8846,7 @@
       <c r="AR14" s="20"/>
       <c r="AS14" s="20"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>119</v>
       </c>
@@ -8893,7 +8903,7 @@
       <c r="AR15" s="20"/>
       <c r="AS15" s="20"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>121</v>
       </c>
@@ -8948,7 +8958,7 @@
       <c r="AR16" s="20"/>
       <c r="AS16" s="20"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>219</v>
       </c>
@@ -9003,7 +9013,7 @@
       <c r="AR17" s="20"/>
       <c r="AS17" s="20"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>154</v>
       </c>
@@ -9095,13 +9105,13 @@
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9178,12 +9188,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="R2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="S2" t="s">
         <v>260</v>
@@ -9208,25 +9218,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.44140625" customWidth="1"/>
-    <col min="32" max="32" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.42578125" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9327,7 +9337,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -9413,7 +9423,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -9445,7 +9455,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -9471,26 +9481,26 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.44140625" customWidth="1"/>
-    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -9585,7 +9595,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -9646,7 +9656,7 @@
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>20</v>
       </c>
@@ -9687,7 +9697,7 @@
       <c r="AD3" s="20"/>
       <c r="AE3" s="20"/>
     </row>
-    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>25</v>
       </c>
@@ -9718,7 +9728,7 @@
         <v>1</v>
       </c>
       <c r="X4" s="12" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="Y4" s="21" t="s">
         <v>39</v>
@@ -9730,7 +9740,7 @@
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>178</v>
       </c>
@@ -9769,7 +9779,7 @@
       <c r="AD5" s="20"/>
       <c r="AE5" s="20"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>179</v>
       </c>
@@ -9808,7 +9818,7 @@
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>153</v>
       </c>
@@ -9847,7 +9857,7 @@
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>155</v>
       </c>
@@ -9884,7 +9894,7 @@
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>154</v>
       </c>
@@ -9921,7 +9931,7 @@
       <c r="AD9" s="20"/>
       <c r="AE9" s="20"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>168</v>
       </c>
@@ -9958,7 +9968,7 @@
       <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>172</v>
       </c>
@@ -10001,7 +10011,7 @@
       <c r="AD11" s="20"/>
       <c r="AE11" s="20"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>170</v>
       </c>
@@ -10040,7 +10050,7 @@
       <c r="AD12" s="20"/>
       <c r="AE12" s="20"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>77</v>
       </c>
@@ -10079,7 +10089,7 @@
       <c r="AD13" s="20"/>
       <c r="AE13" s="20"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>43</v>
       </c>
@@ -10118,7 +10128,7 @@
       <c r="AD14" s="20"/>
       <c r="AE14" s="20"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>118</v>
       </c>
@@ -10167,7 +10177,7 @@
       <c r="AD15" s="20"/>
       <c r="AE15" s="20"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
@@ -10187,7 +10197,7 @@
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="41" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="R16" s="7" t="s">
         <v>443</v>
@@ -10208,7 +10218,7 @@
       <c r="AD16" s="20"/>
       <c r="AE16" s="20"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>46</v>
       </c>
@@ -10249,7 +10259,7 @@
       <c r="AD17" s="20"/>
       <c r="AE17" s="20"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>201</v>
       </c>
@@ -10304,7 +10314,7 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="20"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>241</v>
       </c>
@@ -10341,7 +10351,7 @@
       <c r="AD19" s="20"/>
       <c r="AE19" s="20"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>187</v>
       </c>
@@ -10388,7 +10398,7 @@
       <c r="AD20" s="20"/>
       <c r="AE20" s="20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>166</v>
       </c>
@@ -10435,7 +10445,7 @@
       <c r="AD21" s="20"/>
       <c r="AE21" s="20"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>343</v>
       </c>
@@ -10472,7 +10482,7 @@
       <c r="AD22" s="20"/>
       <c r="AE22" s="20"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>346</v>
       </c>
@@ -10509,7 +10519,7 @@
       <c r="AD23" s="20"/>
       <c r="AE23" s="20"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>348</v>
       </c>
@@ -10554,7 +10564,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
@@ -10622,17 +10632,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -10667,7 +10677,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>243</v>
       </c>
@@ -10676,7 +10686,7 @@
       </c>
       <c r="C2" s="20"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>245</v>
       </c>
@@ -10685,7 +10695,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>247</v>
       </c>
@@ -10694,7 +10704,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>312</v>
       </c>
@@ -10716,20 +10726,20 @@
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10797,7 +10807,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10841,7 +10851,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10857,7 +10867,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -10875,7 +10885,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -10883,7 +10893,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -10891,7 +10901,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -10928,37 +10938,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -11041,7 +11051,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11082,7 +11092,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -11098,7 +11108,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -11110,7 +11120,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -11128,7 +11138,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -11137,7 +11147,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -11149,7 +11159,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -11175,7 +11185,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -11186,7 +11196,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -11200,7 +11210,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
HF_EMEA TEST_DGLD_HF_EMEA_EU_RT_009 Changes in stores updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4D124F-7BB7-4D4F-920C-5A0145C11EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0DBC1F-5DBB-4974-B74B-81D3AD39DB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="569">
   <si>
     <t>UserName</t>
   </si>
@@ -1737,16 +1737,46 @@
   <si>
     <t>Standard Mouth Flex Straw Cap</t>
   </si>
+  <si>
+    <t>Rauhankatu 55</t>
+  </si>
+  <si>
+    <t>Joensuu</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>80100</t>
+  </si>
+  <si>
+    <t>2 Rue De La Zinsel</t>
+  </si>
+  <si>
+    <t>Baerenthal</t>
+  </si>
+  <si>
+    <t>Moselle</t>
+  </si>
+  <si>
+    <t>57230</t>
+  </si>
+  <si>
+    <t>de_BillingDetails</t>
+  </si>
+  <si>
+    <t>eu_BillingDetails</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1886,6 +1916,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1926,12 +1962,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1957,7 +1993,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1993,6 +2029,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2280,30 +2318,30 @@
       <selection activeCell="AC58" sqref="AC58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="21" width="22.28515625" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="18" width="30.5546875" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="21" width="22.33203125" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.28515625" customWidth="1"/>
+    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2449,7 +2487,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2507,7 +2545,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -2565,7 +2603,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:48" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>514</v>
       </c>
@@ -2620,7 +2658,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -2662,7 +2700,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>438</v>
       </c>
@@ -2720,7 +2758,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>540</v>
       </c>
@@ -2775,7 +2813,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="7"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>545</v>
       </c>
@@ -2832,7 +2870,7 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>547</v>
       </c>
@@ -2889,7 +2927,7 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="1:48" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>551</v>
       </c>
@@ -2946,7 +2984,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2964,7 +3002,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>199</v>
       </c>
@@ -2976,7 +3014,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>297</v>
       </c>
@@ -2992,7 +3030,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>155</v>
       </c>
@@ -3004,7 +3042,7 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="7"/>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -3017,7 +3055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>538</v>
       </c>
@@ -3028,7 +3066,7 @@
       <c r="X16" s="4"/>
       <c r="AD16" s="32"/>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>172</v>
       </c>
@@ -3047,7 +3085,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>170</v>
       </c>
@@ -3060,7 +3098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -3088,7 +3126,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>444</v>
       </c>
@@ -3102,7 +3140,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>176</v>
       </c>
@@ -3121,7 +3159,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>175</v>
       </c>
@@ -3134,7 +3172,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>189</v>
       </c>
@@ -3145,7 +3183,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -3169,7 +3207,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3182,7 +3220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -3198,7 +3236,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -3212,7 +3250,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -3249,7 +3287,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -3263,7 +3301,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -3305,7 +3343,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -3319,7 +3357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -3348,7 +3386,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -3365,7 +3403,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -3382,7 +3420,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>118</v>
       </c>
@@ -3411,7 +3449,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>151</v>
       </c>
@@ -3419,7 +3457,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>164</v>
       </c>
@@ -3430,7 +3468,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>166</v>
       </c>
@@ -3469,7 +3507,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>184</v>
       </c>
@@ -3484,7 +3522,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>279</v>
       </c>
@@ -3492,7 +3530,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>284</v>
       </c>
@@ -3506,7 +3544,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>215</v>
       </c>
@@ -3523,7 +3561,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>209</v>
       </c>
@@ -3540,7 +3578,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>339</v>
       </c>
@@ -3563,7 +3601,7 @@
       </c>
       <c r="R44" s="5"/>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>343</v>
       </c>
@@ -3571,7 +3609,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>346</v>
       </c>
@@ -3585,7 +3623,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>348</v>
       </c>
@@ -3602,7 +3640,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>353</v>
       </c>
@@ -3610,7 +3648,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>201</v>
       </c>
@@ -3645,7 +3683,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>363</v>
       </c>
@@ -3653,7 +3691,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>432</v>
       </c>
@@ -3661,7 +3699,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="52" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>433</v>
       </c>
@@ -3669,7 +3707,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="53" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>232</v>
       </c>
@@ -3680,7 +3718,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="54" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A54" s="33" t="s">
         <v>153</v>
       </c>
@@ -3719,7 +3757,7 @@
       </c>
       <c r="AE54" s="33"/>
     </row>
-    <row r="55" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>448</v>
       </c>
@@ -3727,7 +3765,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="56" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>510</v>
       </c>
@@ -3735,7 +3773,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="57" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>521</v>
       </c>
@@ -3743,7 +3781,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="58" spans="1:47" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:47" ht="60" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>529</v>
       </c>
@@ -3751,7 +3789,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="59" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>533</v>
       </c>
@@ -3838,18 +3876,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3947,7 +3985,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3994,7 +4032,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4044,7 +4082,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -4091,7 +4129,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4107,7 +4145,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -4119,7 +4157,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -4130,7 +4168,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4152,7 +4190,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -4165,7 +4203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -4181,7 +4219,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4195,7 +4233,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -4211,7 +4249,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -4225,7 +4263,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -4267,7 +4305,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -4293,7 +4331,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -4304,7 +4342,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4319,7 +4357,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -4377,12 +4415,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4453,7 +4491,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4500,7 +4538,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4516,7 +4554,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -4547,7 +4585,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4555,7 +4593,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -4588,20 +4626,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.28515625" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4690,7 +4728,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4738,7 +4776,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4754,7 +4792,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -4774,7 +4812,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -4793,7 +4831,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -4812,7 +4850,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -4820,7 +4858,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -4828,7 +4866,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -4845,7 +4883,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -4862,7 +4900,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -4879,7 +4917,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -4896,7 +4934,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -4907,7 +4945,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -4918,7 +4956,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4935,7 +4973,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -4964,7 +5002,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4975,7 +5013,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4989,7 +5027,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -5003,7 +5041,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -5017,7 +5055,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -5025,7 +5063,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -5055,7 +5093,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -5125,19 +5163,19 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5163,7 +5201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5186,7 +5224,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -5217,16 +5255,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5240,7 +5278,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -5266,27 +5304,27 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5703125" customWidth="1"/>
-    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5546875" customWidth="1"/>
+    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.140625" customWidth="1"/>
+    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.109375" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -5345,7 +5383,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>228</v>
       </c>
@@ -5370,7 +5408,7 @@
       <c r="R2" s="20"/>
       <c r="S2" s="20"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>230</v>
       </c>
@@ -5399,7 +5437,7 @@
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>232</v>
       </c>
@@ -5424,7 +5462,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>233</v>
       </c>
@@ -5451,7 +5489,7 @@
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>236</v>
       </c>
@@ -5484,7 +5522,7 @@
       <c r="R6" s="20"/>
       <c r="S6" s="20"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>238</v>
       </c>
@@ -5509,7 +5547,7 @@
       <c r="R7" s="20"/>
       <c r="S7" s="20"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>262</v>
       </c>
@@ -5534,7 +5572,7 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>281</v>
       </c>
@@ -5559,7 +5597,7 @@
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>286</v>
       </c>
@@ -5586,7 +5624,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>318</v>
       </c>
@@ -5611,7 +5649,7 @@
       <c r="R11" s="20"/>
       <c r="S11" s="20"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>320</v>
       </c>
@@ -5638,7 +5676,7 @@
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>321</v>
       </c>
@@ -5663,7 +5701,7 @@
       <c r="R13" s="20"/>
       <c r="S13" s="20"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>323</v>
       </c>
@@ -5688,7 +5726,7 @@
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>334</v>
       </c>
@@ -5713,7 +5751,7 @@
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>337</v>
       </c>
@@ -5738,7 +5776,7 @@
       <c r="R16" s="20"/>
       <c r="S16" s="20"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>450</v>
       </c>
@@ -5746,7 +5784,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>451</v>
       </c>
@@ -5754,7 +5792,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>452</v>
       </c>
@@ -5762,7 +5800,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>528</v>
       </c>
@@ -5784,31 +5822,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.7109375" customWidth="1"/>
-    <col min="17" max="24" width="30.5703125" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" customWidth="1"/>
-    <col min="26" max="27" width="22.28515625" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.6640625" customWidth="1"/>
+    <col min="17" max="24" width="30.5546875" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" customWidth="1"/>
+    <col min="26" max="27" width="22.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.28515625" customWidth="1"/>
+    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5960,7 +5998,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6030,7 +6068,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>455</v>
       </c>
@@ -6100,7 +6138,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>457</v>
       </c>
@@ -6170,7 +6208,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>458</v>
       </c>
@@ -6240,7 +6278,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>461</v>
       </c>
@@ -6310,7 +6348,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -6380,7 +6418,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>468</v>
       </c>
@@ -6421,7 +6459,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>469</v>
       </c>
@@ -6462,7 +6500,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>463</v>
       </c>
@@ -6532,7 +6570,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>406</v>
       </c>
@@ -6593,7 +6631,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -6652,7 +6690,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>359</v>
       </c>
@@ -6698,7 +6736,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6721,7 +6759,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>297</v>
       </c>
@@ -6744,7 +6782,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -6763,7 +6801,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6774,7 +6812,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6796,7 +6834,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>366</v>
       </c>
@@ -6809,7 +6847,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>368</v>
       </c>
@@ -6822,7 +6860,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -6835,7 +6873,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>375</v>
       </c>
@@ -6848,7 +6886,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>397</v>
       </c>
@@ -6861,7 +6899,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>376</v>
       </c>
@@ -6874,7 +6912,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -6890,7 +6928,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -6906,7 +6944,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>401</v>
       </c>
@@ -6925,7 +6963,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>405</v>
       </c>
@@ -6944,7 +6982,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>382</v>
       </c>
@@ -6960,7 +6998,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>385</v>
       </c>
@@ -6976,7 +7014,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>411</v>
       </c>
@@ -6992,7 +7030,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>412</v>
       </c>
@@ -7008,7 +7046,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>386</v>
       </c>
@@ -7024,7 +7062,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>389</v>
       </c>
@@ -7037,7 +7075,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>403</v>
       </c>
@@ -7050,7 +7088,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -7063,7 +7101,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>424</v>
       </c>
@@ -7076,7 +7114,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>398</v>
       </c>
@@ -7089,7 +7127,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>394</v>
       </c>
@@ -7105,7 +7143,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>423</v>
       </c>
@@ -7121,7 +7159,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -7137,7 +7175,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>402</v>
       </c>
@@ -7150,7 +7188,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>415</v>
       </c>
@@ -7172,7 +7210,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -7190,7 +7228,7 @@
       <c r="AI44" s="25"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>414</v>
       </c>
@@ -7203,7 +7241,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -7223,7 +7261,7 @@
       <c r="AI46" s="25"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -7242,7 +7280,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -7255,7 +7293,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -7266,7 +7304,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -7279,7 +7317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -7302,7 +7340,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -7316,7 +7354,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -7353,7 +7391,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -7367,7 +7405,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -7409,7 +7447,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -7435,7 +7473,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -7459,7 +7497,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -7483,7 +7521,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -7509,7 +7547,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -7541,7 +7579,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -7555,7 +7593,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>373</v>
       </c>
@@ -7569,7 +7607,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -7586,7 +7624,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -7603,7 +7641,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>339</v>
       </c>
@@ -7625,7 +7663,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>343</v>
       </c>
@@ -7633,7 +7671,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>346</v>
       </c>
@@ -7644,7 +7682,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>348</v>
       </c>
@@ -7661,7 +7699,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>353</v>
       </c>
@@ -7669,7 +7707,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -7704,7 +7742,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>363</v>
       </c>
@@ -7795,36 +7833,36 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -7961,7 +7999,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -8036,7 +8074,7 @@
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
@@ -8093,7 +8131,7 @@
       <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>248</v>
       </c>
@@ -8146,7 +8184,7 @@
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>68</v>
       </c>
@@ -8209,7 +8247,7 @@
       <c r="AR5" s="20"/>
       <c r="AS5" s="20"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>75</v>
       </c>
@@ -8288,7 +8326,7 @@
       <c r="AR6" s="20"/>
       <c r="AS6" s="20"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>81</v>
       </c>
@@ -8377,7 +8415,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>100</v>
       </c>
@@ -8460,7 +8498,7 @@
       <c r="AR8" s="20"/>
       <c r="AS8" s="20"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>95</v>
       </c>
@@ -8545,7 +8583,7 @@
       <c r="AR9" s="20"/>
       <c r="AS9" s="20"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -8596,7 +8634,7 @@
       <c r="AR10" s="20"/>
       <c r="AS10" s="20"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>103</v>
       </c>
@@ -8653,7 +8691,7 @@
       <c r="AR11" s="20"/>
       <c r="AS11" s="20"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>107</v>
       </c>
@@ -8728,7 +8766,7 @@
       <c r="AR12" s="20"/>
       <c r="AS12" s="20"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>112</v>
       </c>
@@ -8791,7 +8829,7 @@
       <c r="AR13" s="20"/>
       <c r="AS13" s="20"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>249</v>
       </c>
@@ -8846,7 +8884,7 @@
       <c r="AR14" s="20"/>
       <c r="AS14" s="20"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>119</v>
       </c>
@@ -8903,7 +8941,7 @@
       <c r="AR15" s="20"/>
       <c r="AS15" s="20"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>121</v>
       </c>
@@ -8958,7 +8996,7 @@
       <c r="AR16" s="20"/>
       <c r="AS16" s="20"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>219</v>
       </c>
@@ -9013,7 +9051,7 @@
       <c r="AR17" s="20"/>
       <c r="AS17" s="20"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>154</v>
       </c>
@@ -9105,13 +9143,13 @@
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9188,7 +9226,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -9218,25 +9256,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9337,7 +9375,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -9423,7 +9461,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -9455,7 +9493,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -9475,33 +9513,33 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AE29"/>
+  <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -9596,7 +9634,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -9607,10 +9645,10 @@
         <v>329</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>330</v>
+        <v>29</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>330</v>
+        <v>29</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>14</v>
@@ -9657,7 +9695,7 @@
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>20</v>
       </c>
@@ -9698,7 +9736,7 @@
       <c r="AD3" s="20"/>
       <c r="AE3" s="20"/>
     </row>
-    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>25</v>
       </c>
@@ -9721,7 +9759,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
       <c r="T4" s="20" t="s">
-        <v>257</v>
+        <v>558</v>
       </c>
       <c r="U4" s="20"/>
       <c r="V4" s="20"/>
@@ -9732,7 +9770,7 @@
         <v>534</v>
       </c>
       <c r="Y4" s="21" t="s">
-        <v>39</v>
+        <v>557</v>
       </c>
       <c r="Z4" s="20"/>
       <c r="AA4" s="20"/>
@@ -9741,7 +9779,7 @@
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>178</v>
       </c>
@@ -9780,7 +9818,7 @@
       <c r="AD5" s="20"/>
       <c r="AE5" s="20"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>179</v>
       </c>
@@ -9819,7 +9857,7 @@
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>153</v>
       </c>
@@ -9858,7 +9896,7 @@
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>155</v>
       </c>
@@ -9895,7 +9933,7 @@
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>154</v>
       </c>
@@ -9932,7 +9970,7 @@
       <c r="AD9" s="20"/>
       <c r="AE9" s="20"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>168</v>
       </c>
@@ -9969,7 +10007,7 @@
       <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>172</v>
       </c>
@@ -10012,7 +10050,7 @@
       <c r="AD11" s="20"/>
       <c r="AE11" s="20"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>170</v>
       </c>
@@ -10051,7 +10089,7 @@
       <c r="AD12" s="20"/>
       <c r="AE12" s="20"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>77</v>
       </c>
@@ -10090,7 +10128,7 @@
       <c r="AD13" s="20"/>
       <c r="AE13" s="20"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>43</v>
       </c>
@@ -10129,7 +10167,7 @@
       <c r="AD14" s="20"/>
       <c r="AE14" s="20"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>118</v>
       </c>
@@ -10178,7 +10216,7 @@
       <c r="AD15" s="20"/>
       <c r="AE15" s="20"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
@@ -10219,7 +10257,7 @@
       <c r="AD16" s="20"/>
       <c r="AE16" s="20"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>46</v>
       </c>
@@ -10260,7 +10298,7 @@
       <c r="AD17" s="20"/>
       <c r="AE17" s="20"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>201</v>
       </c>
@@ -10315,7 +10353,7 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="20"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>241</v>
       </c>
@@ -10352,7 +10390,7 @@
       <c r="AD19" s="20"/>
       <c r="AE19" s="20"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>187</v>
       </c>
@@ -10399,7 +10437,7 @@
       <c r="AD20" s="20"/>
       <c r="AE20" s="20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>166</v>
       </c>
@@ -10446,7 +10484,7 @@
       <c r="AD21" s="20"/>
       <c r="AE21" s="20"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>343</v>
       </c>
@@ -10483,7 +10521,7 @@
       <c r="AD22" s="20"/>
       <c r="AE22" s="20"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>346</v>
       </c>
@@ -10520,7 +10558,7 @@
       <c r="AD23" s="20"/>
       <c r="AE23" s="20"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>348</v>
       </c>
@@ -10565,7 +10603,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
@@ -10600,7 +10638,7 @@
       <c r="AD25" s="20"/>
       <c r="AE25" s="20"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>540</v>
       </c>
@@ -10645,7 +10683,7 @@
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>545</v>
       </c>
@@ -10690,7 +10728,7 @@
       </c>
       <c r="P27" s="41"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>547</v>
       </c>
@@ -10735,7 +10773,7 @@
       </c>
       <c r="P28" s="41"/>
     </row>
-    <row r="29" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>551</v>
       </c>
@@ -10779,13 +10817,65 @@
         <v>9898989898</v>
       </c>
       <c r="P29" s="41"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>567</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="44" t="s">
+        <v>559</v>
+      </c>
+      <c r="L30" s="44" t="s">
+        <v>560</v>
+      </c>
+      <c r="M30" s="44" t="s">
+        <v>561</v>
+      </c>
+      <c r="N30" s="45" t="s">
+        <v>562</v>
+      </c>
+      <c r="O30">
+        <v>9898989898</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>568</v>
+      </c>
+      <c r="F31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" t="s">
+        <v>563</v>
+      </c>
+      <c r="L31" t="s">
+        <v>564</v>
+      </c>
+      <c r="M31" s="18" t="s">
+        <v>565</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="O31">
+        <v>9898989898</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="mailto:spanem@helenoftroy.com" xr:uid="{CC67BCBF-E076-4645-AAE7-B7E656BA65BA}"/>
     <hyperlink ref="C2" r:id="rId2" display="mailto:spanem@helenoftroy.com" xr:uid="{B9951B2A-1254-4C0B-9A14-C6A846810C91}"/>
-    <hyperlink ref="D2" r:id="rId3" display="mailto:Hydro@123" xr:uid="{74C7B7B6-D379-4E34-A081-A00A70371A86}"/>
-    <hyperlink ref="E2" r:id="rId4" display="mailto:Hydro@123" xr:uid="{1702FA67-6467-4E57-9DE2-FB4C9A48C932}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{74C7B7B6-D379-4E34-A081-A00A70371A86}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{1702FA67-6467-4E57-9DE2-FB4C9A48C932}"/>
     <hyperlink ref="H2" r:id="rId5" display="mailto:spanem@helenoftroy.com" xr:uid="{43710853-757A-4E86-AEEB-F5DD155D60F0}"/>
     <hyperlink ref="I2" r:id="rId6" display="mailto:spanem@helenoftroy.com" xr:uid="{B3D81E16-7F77-4EDD-A91C-F9F6093FDE1C}"/>
     <hyperlink ref="X4" r:id="rId7" display="https://www.hydroflask.com/12-oz-mug?color=Moonshadow" xr:uid="{2F702AF3-4F49-47B1-A82E-D55704330159}"/>
@@ -10834,17 +10924,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -10879,7 +10969,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>243</v>
       </c>
@@ -10888,7 +10978,7 @@
       </c>
       <c r="C2" s="20"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>245</v>
       </c>
@@ -10897,7 +10987,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>247</v>
       </c>
@@ -10906,7 +10996,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>312</v>
       </c>
@@ -10928,20 +11018,20 @@
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -11009,7 +11099,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11053,7 +11143,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -11069,7 +11159,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -11087,7 +11177,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -11095,7 +11185,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -11103,7 +11193,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -11140,37 +11230,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -11253,7 +11343,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11294,7 +11384,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -11310,7 +11400,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -11322,7 +11412,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -11340,7 +11430,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -11349,7 +11439,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -11361,7 +11451,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -11387,7 +11477,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -11398,7 +11488,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -11412,7 +11502,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
HF EMEA TEST_DGLD_HF_EMEA_FR_RT_009 changes in stores updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93F8BFE-D01B-47DF-8819-6C498187E8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0786B05C-D2E2-407F-9A65-CE6A68804F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="9960" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="579">
   <si>
     <t>UserName</t>
   </si>
@@ -1766,6 +1766,36 @@
   </si>
   <si>
     <t>Beachplum,Nectar,Oat,Sandpiper,Sunbeam</t>
+  </si>
+  <si>
+    <t>es_BillingDetails</t>
+  </si>
+  <si>
+    <t>CR-5212</t>
+  </si>
+  <si>
+    <t>Manzanares</t>
+  </si>
+  <si>
+    <t>Ciudad Real</t>
+  </si>
+  <si>
+    <t>13200</t>
+  </si>
+  <si>
+    <t>Saint-Malo</t>
+  </si>
+  <si>
+    <t>35400</t>
+  </si>
+  <si>
+    <t>Ille-et-Vilaine</t>
+  </si>
+  <si>
+    <t>12 Rue De La Hulotais</t>
+  </si>
+  <si>
+    <t>fr_BillingDetails</t>
   </si>
 </sst>
 </file>
@@ -2318,30 +2348,30 @@
       <selection activeCell="AC58" sqref="AC58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="21" width="22.28515625" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="18" width="30.5546875" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="21" width="22.33203125" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.28515625" customWidth="1"/>
+    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2487,7 +2517,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2545,7 +2575,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -2603,7 +2633,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:48" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>513</v>
       </c>
@@ -2658,7 +2688,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -2700,7 +2730,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>438</v>
       </c>
@@ -2758,7 +2788,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>538</v>
       </c>
@@ -2813,7 +2843,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="7"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>543</v>
       </c>
@@ -2870,7 +2900,7 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>545</v>
       </c>
@@ -2927,7 +2957,7 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="1:48" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>549</v>
       </c>
@@ -2984,7 +3014,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3002,7 +3032,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>199</v>
       </c>
@@ -3014,7 +3044,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>297</v>
       </c>
@@ -3030,7 +3060,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>155</v>
       </c>
@@ -3042,7 +3072,7 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="7"/>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -3055,7 +3085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>536</v>
       </c>
@@ -3066,7 +3096,7 @@
       <c r="X16" s="4"/>
       <c r="AD16" s="32"/>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>172</v>
       </c>
@@ -3085,7 +3115,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>170</v>
       </c>
@@ -3098,7 +3128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -3126,7 +3156,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>443</v>
       </c>
@@ -3140,7 +3170,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>176</v>
       </c>
@@ -3159,7 +3189,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>175</v>
       </c>
@@ -3172,7 +3202,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>189</v>
       </c>
@@ -3183,7 +3213,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -3207,7 +3237,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3220,7 +3250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -3236,7 +3266,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -3250,7 +3280,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -3287,7 +3317,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -3301,7 +3331,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -3343,7 +3373,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -3357,7 +3387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -3386,7 +3416,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -3403,7 +3433,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -3420,7 +3450,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>118</v>
       </c>
@@ -3449,7 +3479,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>151</v>
       </c>
@@ -3457,7 +3487,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>164</v>
       </c>
@@ -3468,7 +3498,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>166</v>
       </c>
@@ -3507,7 +3537,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>184</v>
       </c>
@@ -3522,7 +3552,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>279</v>
       </c>
@@ -3530,7 +3560,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>284</v>
       </c>
@@ -3544,7 +3574,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>215</v>
       </c>
@@ -3561,7 +3591,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>209</v>
       </c>
@@ -3578,7 +3608,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>339</v>
       </c>
@@ -3601,7 +3631,7 @@
       </c>
       <c r="R44" s="5"/>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>343</v>
       </c>
@@ -3609,7 +3639,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>346</v>
       </c>
@@ -3623,7 +3653,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>348</v>
       </c>
@@ -3640,7 +3670,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>353</v>
       </c>
@@ -3648,7 +3678,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>201</v>
       </c>
@@ -3683,7 +3713,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>363</v>
       </c>
@@ -3691,7 +3721,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>432</v>
       </c>
@@ -3699,7 +3729,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="52" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>433</v>
       </c>
@@ -3707,7 +3737,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="53" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>232</v>
       </c>
@@ -3718,7 +3748,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="54" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A54" s="33" t="s">
         <v>153</v>
       </c>
@@ -3757,7 +3787,7 @@
       </c>
       <c r="AE54" s="33"/>
     </row>
-    <row r="55" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>447</v>
       </c>
@@ -3765,7 +3795,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="56" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>509</v>
       </c>
@@ -3773,7 +3803,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="57" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>520</v>
       </c>
@@ -3781,7 +3811,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="58" spans="1:47" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:47" ht="60" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>527</v>
       </c>
@@ -3789,7 +3819,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="59" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>531</v>
       </c>
@@ -3876,18 +3906,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3985,7 +4015,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4032,7 +4062,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4082,7 +4112,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -4129,7 +4159,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4145,7 +4175,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -4157,7 +4187,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -4168,7 +4198,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4190,7 +4220,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -4203,7 +4233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -4219,7 +4249,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4233,7 +4263,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -4249,7 +4279,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -4263,7 +4293,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -4305,7 +4335,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -4331,7 +4361,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -4342,7 +4372,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4357,7 +4387,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -4415,12 +4445,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4491,7 +4521,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4538,7 +4568,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4554,7 +4584,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -4585,7 +4615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4593,7 +4623,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -4626,20 +4656,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.28515625" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4728,7 +4758,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4776,7 +4806,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4792,7 +4822,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -4812,7 +4842,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -4831,7 +4861,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -4850,7 +4880,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -4858,7 +4888,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -4866,7 +4896,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -4883,7 +4913,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -4900,7 +4930,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -4917,7 +4947,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -4934,7 +4964,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -4945,7 +4975,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -4956,7 +4986,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -4973,7 +5003,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -5002,7 +5032,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -5013,7 +5043,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -5027,7 +5057,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -5041,7 +5071,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -5055,7 +5085,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -5063,7 +5093,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -5093,7 +5123,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -5163,19 +5193,19 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5201,7 +5231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5224,7 +5254,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -5255,16 +5285,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5278,7 +5308,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -5300,31 +5330,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAA7450-0FE7-4C50-95DC-266117BAF81B}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5703125" customWidth="1"/>
-    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5546875" customWidth="1"/>
+    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.140625" customWidth="1"/>
+    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.109375" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -5383,7 +5413,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>228</v>
       </c>
@@ -5408,7 +5438,7 @@
       <c r="R2" s="20"/>
       <c r="S2" s="20"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>230</v>
       </c>
@@ -5437,7 +5467,7 @@
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>232</v>
       </c>
@@ -5462,7 +5492,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>233</v>
       </c>
@@ -5489,7 +5519,7 @@
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>236</v>
       </c>
@@ -5522,7 +5552,7 @@
       <c r="R6" s="20"/>
       <c r="S6" s="20"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>238</v>
       </c>
@@ -5547,7 +5577,7 @@
       <c r="R7" s="20"/>
       <c r="S7" s="20"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>262</v>
       </c>
@@ -5572,7 +5602,7 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>281</v>
       </c>
@@ -5597,7 +5627,7 @@
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>286</v>
       </c>
@@ -5624,7 +5654,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>318</v>
       </c>
@@ -5649,7 +5679,7 @@
       <c r="R11" s="20"/>
       <c r="S11" s="20"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>320</v>
       </c>
@@ -5676,7 +5706,7 @@
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>321</v>
       </c>
@@ -5701,7 +5731,7 @@
       <c r="R13" s="20"/>
       <c r="S13" s="20"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>323</v>
       </c>
@@ -5726,7 +5756,7 @@
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>334</v>
       </c>
@@ -5751,7 +5781,7 @@
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>337</v>
       </c>
@@ -5776,7 +5806,7 @@
       <c r="R16" s="20"/>
       <c r="S16" s="20"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>449</v>
       </c>
@@ -5784,7 +5814,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>450</v>
       </c>
@@ -5792,7 +5822,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>451</v>
       </c>
@@ -5800,7 +5830,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>526</v>
       </c>
@@ -5822,31 +5852,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.7109375" customWidth="1"/>
-    <col min="17" max="24" width="30.5703125" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" customWidth="1"/>
-    <col min="26" max="27" width="22.28515625" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.6640625" customWidth="1"/>
+    <col min="17" max="24" width="30.5546875" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" customWidth="1"/>
+    <col min="26" max="27" width="22.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.28515625" customWidth="1"/>
+    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5998,7 +6028,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6068,7 +6098,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>454</v>
       </c>
@@ -6138,7 +6168,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>456</v>
       </c>
@@ -6208,7 +6238,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>457</v>
       </c>
@@ -6278,7 +6308,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>460</v>
       </c>
@@ -6348,7 +6378,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>464</v>
       </c>
@@ -6418,7 +6448,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>467</v>
       </c>
@@ -6459,7 +6489,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>468</v>
       </c>
@@ -6500,7 +6530,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>462</v>
       </c>
@@ -6570,7 +6600,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>406</v>
       </c>
@@ -6631,7 +6661,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -6690,7 +6720,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>359</v>
       </c>
@@ -6736,7 +6766,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6759,7 +6789,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>297</v>
       </c>
@@ -6782,7 +6812,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -6801,7 +6831,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6812,7 +6842,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6834,7 +6864,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>366</v>
       </c>
@@ -6847,7 +6877,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>368</v>
       </c>
@@ -6860,7 +6890,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -6873,7 +6903,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>375</v>
       </c>
@@ -6886,7 +6916,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>397</v>
       </c>
@@ -6899,7 +6929,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>376</v>
       </c>
@@ -6912,7 +6942,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -6928,7 +6958,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -6944,7 +6974,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>401</v>
       </c>
@@ -6963,7 +6993,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>405</v>
       </c>
@@ -6982,7 +7012,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>382</v>
       </c>
@@ -6998,7 +7028,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>385</v>
       </c>
@@ -7014,7 +7044,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>411</v>
       </c>
@@ -7030,7 +7060,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>412</v>
       </c>
@@ -7046,7 +7076,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>386</v>
       </c>
@@ -7062,7 +7092,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>389</v>
       </c>
@@ -7075,7 +7105,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>403</v>
       </c>
@@ -7088,7 +7118,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -7101,7 +7131,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>424</v>
       </c>
@@ -7114,7 +7144,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>398</v>
       </c>
@@ -7127,7 +7157,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>394</v>
       </c>
@@ -7143,7 +7173,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>423</v>
       </c>
@@ -7159,7 +7189,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -7175,7 +7205,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>402</v>
       </c>
@@ -7188,7 +7218,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>415</v>
       </c>
@@ -7210,7 +7240,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -7228,7 +7258,7 @@
       <c r="AI44" s="25"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>414</v>
       </c>
@@ -7241,7 +7271,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -7261,7 +7291,7 @@
       <c r="AI46" s="25"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -7280,7 +7310,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -7293,7 +7323,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -7304,7 +7334,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -7317,7 +7347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -7340,7 +7370,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -7354,7 +7384,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -7391,7 +7421,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -7405,7 +7435,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -7447,7 +7477,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -7473,7 +7503,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -7497,7 +7527,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -7521,7 +7551,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -7547,7 +7577,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -7579,7 +7609,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -7593,7 +7623,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>373</v>
       </c>
@@ -7607,7 +7637,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -7624,7 +7654,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -7641,7 +7671,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>339</v>
       </c>
@@ -7663,7 +7693,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>343</v>
       </c>
@@ -7671,7 +7701,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>346</v>
       </c>
@@ -7682,7 +7712,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>348</v>
       </c>
@@ -7699,7 +7729,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>353</v>
       </c>
@@ -7707,7 +7737,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -7742,7 +7772,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>363</v>
       </c>
@@ -7833,36 +7863,36 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -7999,7 +8029,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -8074,7 +8104,7 @@
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
@@ -8131,7 +8161,7 @@
       <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>248</v>
       </c>
@@ -8184,7 +8214,7 @@
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>68</v>
       </c>
@@ -8247,7 +8277,7 @@
       <c r="AR5" s="20"/>
       <c r="AS5" s="20"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>75</v>
       </c>
@@ -8326,7 +8356,7 @@
       <c r="AR6" s="20"/>
       <c r="AS6" s="20"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>81</v>
       </c>
@@ -8415,7 +8445,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>100</v>
       </c>
@@ -8498,7 +8528,7 @@
       <c r="AR8" s="20"/>
       <c r="AS8" s="20"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>95</v>
       </c>
@@ -8583,7 +8613,7 @@
       <c r="AR9" s="20"/>
       <c r="AS9" s="20"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -8634,7 +8664,7 @@
       <c r="AR10" s="20"/>
       <c r="AS10" s="20"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>103</v>
       </c>
@@ -8691,7 +8721,7 @@
       <c r="AR11" s="20"/>
       <c r="AS11" s="20"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>107</v>
       </c>
@@ -8766,7 +8796,7 @@
       <c r="AR12" s="20"/>
       <c r="AS12" s="20"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>112</v>
       </c>
@@ -8829,7 +8859,7 @@
       <c r="AR13" s="20"/>
       <c r="AS13" s="20"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>249</v>
       </c>
@@ -8884,7 +8914,7 @@
       <c r="AR14" s="20"/>
       <c r="AS14" s="20"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>119</v>
       </c>
@@ -8941,7 +8971,7 @@
       <c r="AR15" s="20"/>
       <c r="AS15" s="20"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>121</v>
       </c>
@@ -8996,7 +9026,7 @@
       <c r="AR16" s="20"/>
       <c r="AS16" s="20"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>219</v>
       </c>
@@ -9051,7 +9081,7 @@
       <c r="AR17" s="20"/>
       <c r="AS17" s="20"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>154</v>
       </c>
@@ -9143,13 +9173,13 @@
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9226,7 +9256,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -9256,25 +9286,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9375,7 +9405,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -9461,7 +9491,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -9493,7 +9523,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -9513,33 +9543,33 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AE31"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -9634,7 +9664,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -9695,7 +9725,7 @@
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>20</v>
       </c>
@@ -9736,7 +9766,7 @@
       <c r="AD3" s="20"/>
       <c r="AE3" s="20"/>
     </row>
-    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>25</v>
       </c>
@@ -9779,7 +9809,7 @@
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>178</v>
       </c>
@@ -9818,7 +9848,7 @@
       <c r="AD5" s="20"/>
       <c r="AE5" s="20"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>179</v>
       </c>
@@ -9857,7 +9887,7 @@
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>153</v>
       </c>
@@ -9896,7 +9926,7 @@
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>155</v>
       </c>
@@ -9933,7 +9963,7 @@
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>154</v>
       </c>
@@ -9970,7 +10000,7 @@
       <c r="AD9" s="20"/>
       <c r="AE9" s="20"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>168</v>
       </c>
@@ -10007,7 +10037,7 @@
       <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>172</v>
       </c>
@@ -10050,7 +10080,7 @@
       <c r="AD11" s="20"/>
       <c r="AE11" s="20"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>170</v>
       </c>
@@ -10089,7 +10119,7 @@
       <c r="AD12" s="20"/>
       <c r="AE12" s="20"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>77</v>
       </c>
@@ -10128,7 +10158,7 @@
       <c r="AD13" s="20"/>
       <c r="AE13" s="20"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>43</v>
       </c>
@@ -10167,7 +10197,7 @@
       <c r="AD14" s="20"/>
       <c r="AE14" s="20"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>118</v>
       </c>
@@ -10216,7 +10246,7 @@
       <c r="AD15" s="20"/>
       <c r="AE15" s="20"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
@@ -10257,7 +10287,7 @@
       <c r="AD16" s="20"/>
       <c r="AE16" s="20"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>46</v>
       </c>
@@ -10298,7 +10328,7 @@
       <c r="AD17" s="20"/>
       <c r="AE17" s="20"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>201</v>
       </c>
@@ -10353,7 +10383,7 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="20"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>241</v>
       </c>
@@ -10390,7 +10420,7 @@
       <c r="AD19" s="20"/>
       <c r="AE19" s="20"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>187</v>
       </c>
@@ -10437,7 +10467,7 @@
       <c r="AD20" s="20"/>
       <c r="AE20" s="20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>166</v>
       </c>
@@ -10484,7 +10514,7 @@
       <c r="AD21" s="20"/>
       <c r="AE21" s="20"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>343</v>
       </c>
@@ -10521,7 +10551,7 @@
       <c r="AD22" s="20"/>
       <c r="AE22" s="20"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>346</v>
       </c>
@@ -10558,7 +10588,7 @@
       <c r="AD23" s="20"/>
       <c r="AE23" s="20"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>348</v>
       </c>
@@ -10603,7 +10633,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
@@ -10638,7 +10668,7 @@
       <c r="AD25" s="20"/>
       <c r="AE25" s="20"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>538</v>
       </c>
@@ -10683,7 +10713,7 @@
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>543</v>
       </c>
@@ -10728,7 +10758,7 @@
       </c>
       <c r="P27" s="41"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>545</v>
       </c>
@@ -10773,7 +10803,7 @@
       </c>
       <c r="P28" s="41"/>
     </row>
-    <row r="29" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>549</v>
       </c>
@@ -10818,7 +10848,7 @@
       </c>
       <c r="P29" s="41"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>565</v>
       </c>
@@ -10844,7 +10874,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>566</v>
       </c>
@@ -10867,6 +10897,58 @@
         <v>564</v>
       </c>
       <c r="O31">
+        <v>9898989898</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>569</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="K32" t="s">
+        <v>570</v>
+      </c>
+      <c r="L32" t="s">
+        <v>571</v>
+      </c>
+      <c r="M32" t="s">
+        <v>572</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="O32">
+        <v>9898989898</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>578</v>
+      </c>
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" t="s">
+        <v>577</v>
+      </c>
+      <c r="L33" t="s">
+        <v>574</v>
+      </c>
+      <c r="M33" t="s">
+        <v>576</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="O33">
         <v>9898989898</v>
       </c>
     </row>
@@ -10924,17 +11006,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -10969,7 +11051,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>243</v>
       </c>
@@ -10978,7 +11060,7 @@
       </c>
       <c r="C2" s="20"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>245</v>
       </c>
@@ -10987,7 +11069,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>247</v>
       </c>
@@ -10996,7 +11078,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>312</v>
       </c>
@@ -11018,20 +11100,20 @@
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -11099,7 +11181,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11143,7 +11225,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -11159,7 +11241,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -11177,7 +11259,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -11185,7 +11267,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -11193,7 +11275,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -11230,37 +11312,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -11343,7 +11425,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11384,7 +11466,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -11400,7 +11482,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -11412,7 +11494,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -11430,7 +11512,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -11439,7 +11521,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -11451,7 +11533,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -11477,7 +11559,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -11488,7 +11570,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -11502,7 +11584,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
HF EMEA Test_DGLD_HF_EMEA_RT_033_Validate_CountrySelector with testdata updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,26 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0786B05C-D2E2-407F-9A65-CE6A68804F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF47656-8E93-4397-8E96-C5D8A4E1DB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="9960" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DataSet" sheetId="1" r:id="rId1"/>
-    <sheet name="E2E" sheetId="15" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
-    <sheet name="PDP" sheetId="5" r:id="rId4"/>
-    <sheet name="Forms" sheetId="3" r:id="rId5"/>
-    <sheet name="Bundle" sheetId="4" r:id="rId6"/>
-    <sheet name="FooterLinks" sheetId="6" r:id="rId7"/>
-    <sheet name="Outofstock" sheetId="7" r:id="rId8"/>
-    <sheet name="Loqata" sheetId="8" r:id="rId9"/>
-    <sheet name="Address" sheetId="10" r:id="rId10"/>
-    <sheet name="MyHydro" sheetId="9" r:id="rId11"/>
-    <sheet name="Engraving" sheetId="13" r:id="rId12"/>
-    <sheet name="Account page" sheetId="11" r:id="rId13"/>
-    <sheet name="weblinks" sheetId="12" r:id="rId14"/>
-    <sheet name="HeaderLinks" sheetId="14" r:id="rId15"/>
+    <sheet name="Country" sheetId="16" r:id="rId1"/>
+    <sheet name="DataSet" sheetId="1" r:id="rId2"/>
+    <sheet name="E2E" sheetId="15" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
+    <sheet name="PDP" sheetId="5" r:id="rId5"/>
+    <sheet name="Forms" sheetId="3" r:id="rId6"/>
+    <sheet name="Bundle" sheetId="4" r:id="rId7"/>
+    <sheet name="FooterLinks" sheetId="6" r:id="rId8"/>
+    <sheet name="Outofstock" sheetId="7" r:id="rId9"/>
+    <sheet name="Loqata" sheetId="8" r:id="rId10"/>
+    <sheet name="Address" sheetId="10" r:id="rId11"/>
+    <sheet name="MyHydro" sheetId="9" r:id="rId12"/>
+    <sheet name="Engraving" sheetId="13" r:id="rId13"/>
+    <sheet name="Account page" sheetId="11" r:id="rId14"/>
+    <sheet name="weblinks" sheetId="12" r:id="rId15"/>
+    <sheet name="HeaderLinks" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="582">
   <si>
     <t>UserName</t>
   </si>
@@ -1797,14 +1798,23 @@
   <si>
     <t>fr_BillingDetails</t>
   </si>
+  <si>
+    <t>Countrynames</t>
+  </si>
+  <si>
+    <t>Countryselector</t>
+  </si>
+  <si>
+    <t>English (£), English (€), French (€), German (€), Spanish (€)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -1997,7 +2007,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -2023,7 +2033,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2341,6 +2351,2370 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66895830-5267-4F1F-BE18-CA2A151CA6D1}">
+  <dimension ref="A1:AF6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>580</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="7"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="B3" s="12"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="7"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="H4" s="9"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="7"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="H5" s="12"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="4"/>
+      <c r="V5" s="5"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="H6" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{424970FD-0802-41D9-95B0-A7EEAE48FFD7}">
+  <dimension ref="A1:AA11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="7"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="P3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="H4" t="s">
+        <v>203</v>
+      </c>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="7"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="S5" t="s">
+        <v>149</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="U5" t="s">
+        <v>27</v>
+      </c>
+      <c r="V5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="W6" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="2"/>
+      <c r="X7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L11" t="s">
+        <v>64</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{D6D44446-4E68-4240-BC3C-794C8762EF6C}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{F667B6EF-2843-441F-ADF3-A9F03FB2D127}"/>
+    <hyperlink ref="D9" r:id="rId3" xr:uid="{BA37854D-B94D-4462-95C3-1F9ADFCD61FB}"/>
+    <hyperlink ref="G10" r:id="rId4" xr:uid="{97AA2188-E825-4E95-BD32-7DE2E0872BDB}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{65D4744A-1A3C-492E-95BF-8C9052BD2013}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{15735CF8-DBB0-492B-A615-DCBD78A638E3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF1A3C9-3346-4B2E-B0CF-4F0FFA0F798B}">
+  <dimension ref="A1:AF18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" t="s">
+        <v>150</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" s="5"/>
+      <c r="S2" s="7"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" t="s">
+        <v>268</v>
+      </c>
+      <c r="L3" t="s">
+        <v>269</v>
+      </c>
+      <c r="M3" t="s">
+        <v>108</v>
+      </c>
+      <c r="N3" t="s">
+        <v>193</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" s="5"/>
+      <c r="S3" s="7"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" t="s">
+        <v>195</v>
+      </c>
+      <c r="L4" t="s">
+        <v>196</v>
+      </c>
+      <c r="N4" t="s">
+        <v>197</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="5"/>
+      <c r="S4" s="7"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="R5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="J6" t="s">
+        <v>203</v>
+      </c>
+      <c r="R6" s="5"/>
+      <c r="S6" s="7"/>
+    </row>
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>154</v>
+      </c>
+      <c r="J7" t="s">
+        <v>227</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="4"/>
+      <c r="V7" s="5"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="U8" t="s">
+        <v>257</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="W8" t="s">
+        <v>328</v>
+      </c>
+      <c r="X8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="V9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="AA10" t="s">
+        <v>258</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="R12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T14">
+        <v>123</v>
+      </c>
+      <c r="AC14" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" t="s">
+        <v>62</v>
+      </c>
+      <c r="L15" t="s">
+        <v>63</v>
+      </c>
+      <c r="N15" t="s">
+        <v>64</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" t="s">
+        <v>63</v>
+      </c>
+      <c r="N18" t="s">
+        <v>64</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{509FD8C7-2668-4F8A-8FCA-72E4C3F520AD}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{DBDB132B-EE23-4863-9A01-1CB94AE8210A}"/>
+    <hyperlink ref="H14" r:id="rId3" xr:uid="{7F08651C-07CE-4F9D-9DB6-E721F8008E52}"/>
+    <hyperlink ref="E16" r:id="rId4" xr:uid="{F74A2CD9-57F6-4D37-891F-1C14CEE7EE28}"/>
+    <hyperlink ref="H17" r:id="rId5" xr:uid="{5A441EDE-90F6-429A-B4F6-8AA0CB497374}"/>
+    <hyperlink ref="D2" r:id="rId6" xr:uid="{4D5420C0-4098-4F77-8C77-2D92FABA6A99}"/>
+    <hyperlink ref="B2" r:id="rId7" xr:uid="{0256F7FB-58C2-4BAB-BE67-4206DEC228E7}"/>
+    <hyperlink ref="H3" r:id="rId8" xr:uid="{07E85401-832F-48E6-A047-319CB6B7D5A8}"/>
+    <hyperlink ref="B3" r:id="rId9" xr:uid="{61228DC3-4729-4E9D-BA47-AEC733E6A768}"/>
+    <hyperlink ref="B4" r:id="rId10" xr:uid="{C98662A6-6882-485B-A267-73578CC7A81C}"/>
+    <hyperlink ref="H4" r:id="rId11" xr:uid="{0D8096A3-5F8F-472A-9A88-F4D314BA1D84}"/>
+    <hyperlink ref="C2" r:id="rId12" xr:uid="{C12DCAE2-5BE7-4CB7-B68A-8142A2C5BE18}"/>
+    <hyperlink ref="I2" r:id="rId13" xr:uid="{940F9767-2975-43CD-9672-73F2C1E9BB76}"/>
+    <hyperlink ref="C3" r:id="rId14" xr:uid="{6BDBED0E-D6CA-4A54-BB34-C338CC84BC2F}"/>
+    <hyperlink ref="I3" r:id="rId15" xr:uid="{0F906926-6594-4D15-A39D-8F9257E712CA}"/>
+    <hyperlink ref="I4" r:id="rId16" xr:uid="{644E9B73-D236-4CAF-AD8F-1A59764D2EA5}"/>
+    <hyperlink ref="C4" r:id="rId17" xr:uid="{89910DEA-1D5D-4633-BFBA-0D931A2E8862}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41F8855-2B61-4FEF-9344-24F4972CEB0C}">
+  <dimension ref="A1:W6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" t="s">
+        <v>271</v>
+      </c>
+      <c r="L2" t="s">
+        <v>272</v>
+      </c>
+      <c r="M2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="7"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="Q3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="T4" t="s">
+        <v>255</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="V4" t="s">
+        <v>83</v>
+      </c>
+      <c r="W4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="J5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>154</v>
+      </c>
+      <c r="J6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1AEC3987-D7C8-4A5C-8BED-E9899FF2BF82}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{D43D11A9-1C5A-4349-B704-6198442D85A5}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{C222A27C-0748-414C-B788-B3F7C73C9801}"/>
+    <hyperlink ref="I2" r:id="rId4" xr:uid="{CC1F9EDD-65C4-42D8-92CA-91B148215A49}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{38064991-06F0-4D2B-A8AB-8973A45D8A40}"/>
+    <hyperlink ref="B4" r:id="rId6" xr:uid="{CDF79D5A-0018-470A-BA9B-7B98F8046D3D}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{27C139E8-BC55-475F-9B0A-991734439882}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{BA43A1BD-CF68-467C-B68B-99104FF975B9}"/>
+    <hyperlink ref="E4" r:id="rId9" xr:uid="{864335AC-3375-4C8A-93C0-0A0C164FF3A5}"/>
+    <hyperlink ref="H2" r:id="rId10" xr:uid="{5D19C1A3-09F6-4B12-9D2C-F4C9A06AA4AD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29915A7A-9757-4FAB-8D6E-89B484B75E0F}">
+  <dimension ref="A1:AC23"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="7"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="R3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="U4" t="s">
+        <v>255</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="W4" s="5"/>
+      <c r="X4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="U5" t="s">
+        <v>308</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="W5" s="5"/>
+      <c r="X5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>222</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="U6" t="s">
+        <v>255</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="W6" s="5"/>
+      <c r="X6" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>155</v>
+      </c>
+      <c r="J7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="J8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>224</v>
+      </c>
+      <c r="X9" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>209</v>
+      </c>
+      <c r="X10" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>210</v>
+      </c>
+      <c r="X11" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>226</v>
+      </c>
+      <c r="X12" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>217</v>
+      </c>
+      <c r="W13" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="X13" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>153</v>
+      </c>
+      <c r="U14" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="V14" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="U15" t="s">
+        <v>257</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C16" t="s">
+        <v>274</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="U16" t="s">
+        <v>255</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="X16" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T18">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T19">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T20">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>168</v>
+      </c>
+      <c r="U21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" t="s">
+        <v>431</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="K22" t="s">
+        <v>62</v>
+      </c>
+      <c r="L22" t="s">
+        <v>63</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="N22" t="s">
+        <v>64</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" t="s">
+        <v>150</v>
+      </c>
+      <c r="L23" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="N23" t="s">
+        <v>19</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T23">
+        <v>123</v>
+      </c>
+      <c r="AC23" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{01674EEF-5B1B-4083-B112-261BF32E9151}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{34D31921-71E7-42CC-86C8-D746F2995905}"/>
+    <hyperlink ref="H17" r:id="rId3" xr:uid="{881DC81A-1D11-43B1-A649-219EE29DF576}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{34C5CAF3-2DCD-4229-BB46-CE0027675E35}"/>
+    <hyperlink ref="I2" r:id="rId5" xr:uid="{3D193472-9B38-41A4-AE75-7C5F6D3602BA}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{F5901482-C7A8-4FF2-B596-ABF445FEB63E}"/>
+    <hyperlink ref="H2" r:id="rId7" xr:uid="{9F7CAC9D-8E60-40FD-9B3E-4DF7D1F7B960}"/>
+    <hyperlink ref="D16" r:id="rId8" xr:uid="{F3D92567-3249-4D9A-BC44-71074C3A72B3}"/>
+    <hyperlink ref="H16" r:id="rId9" xr:uid="{C8A103B8-0E5D-4852-8D35-33CC8F223E0E}"/>
+    <hyperlink ref="H22" r:id="rId10" xr:uid="{0764A351-F269-48EF-8B6A-75A3942B351A}"/>
+    <hyperlink ref="H23" r:id="rId11" xr:uid="{9954984C-D6B1-4288-B72C-8B6336193DFF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EEBDD4E-15C0-4517-B53D-FC4E89764F23}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F3" t="s">
+        <v>530</v>
+      </c>
+      <c r="G3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{2E40CAD4-3DDF-4115-9EA5-6641F416A14E}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{937C9B4A-3558-49DC-A73A-68CFBEE42860}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{9F0FB54C-AED1-481D-93FA-90CC93BA9B59}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{50D8CCD7-0D9E-482F-B9EF-1FD77791185F}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{DC118BEB-F328-46D1-BAFE-2340D7A8407A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F808DC-2462-40F4-8FE6-41754E94FF50}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>503</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="F2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAA7450-0FE7-4C50-95DC-266117BAF81B}">
+  <dimension ref="A1:S20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" customWidth="1"/>
+    <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="78" customWidth="1"/>
+    <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5546875" customWidth="1"/>
+    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.109375" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>399</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="S1" s="37" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>522</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>480</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20" t="s">
+        <v>523</v>
+      </c>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="20" t="s">
+        <v>567</v>
+      </c>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="M6" s="20"/>
+      <c r="N6" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q6" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20" t="s">
+        <v>525</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="S10" s="20" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="35" t="s">
+        <v>481</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>466</v>
+      </c>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20" t="s">
+        <v>479</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20" t="s">
+        <v>365</v>
+      </c>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>449</v>
+      </c>
+      <c r="C17" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>450</v>
+      </c>
+      <c r="C18" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>526</v>
+      </c>
+      <c r="J20" t="s">
+        <v>535</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV59"/>
   <sheetViews>
@@ -3898,1953 +6272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF1A3C9-3346-4B2E-B0CF-4F0FFA0F798B}">
-  <dimension ref="A1:AF18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" t="s">
-        <v>150</v>
-      </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="R2" s="5"/>
-      <c r="S2" s="7"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" t="s">
-        <v>268</v>
-      </c>
-      <c r="L3" t="s">
-        <v>269</v>
-      </c>
-      <c r="M3" t="s">
-        <v>108</v>
-      </c>
-      <c r="N3" t="s">
-        <v>193</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="R3" s="5"/>
-      <c r="S3" s="7"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" t="s">
-        <v>195</v>
-      </c>
-      <c r="L4" t="s">
-        <v>196</v>
-      </c>
-      <c r="N4" t="s">
-        <v>197</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="R4" s="5"/>
-      <c r="S4" s="7"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="R5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T5">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="J6" t="s">
-        <v>203</v>
-      </c>
-      <c r="R6" s="5"/>
-      <c r="S6" s="7"/>
-    </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>154</v>
-      </c>
-      <c r="J7" t="s">
-        <v>227</v>
-      </c>
-      <c r="O7" s="3"/>
-      <c r="P7" s="4"/>
-      <c r="V7" s="5"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="U8" t="s">
-        <v>257</v>
-      </c>
-      <c r="V8" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="W8" t="s">
-        <v>328</v>
-      </c>
-      <c r="X8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="V9" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="AA10" t="s">
-        <v>258</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T11">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="R12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="S12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T12">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>48</v>
-      </c>
-      <c r="R13" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T13">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="K14" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q14" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="R14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T14">
-        <v>123</v>
-      </c>
-      <c r="AC14" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" t="s">
-        <v>62</v>
-      </c>
-      <c r="L15" t="s">
-        <v>63</v>
-      </c>
-      <c r="N15" t="s">
-        <v>64</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="P15" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" t="s">
-        <v>67</v>
-      </c>
-      <c r="K18" t="s">
-        <v>62</v>
-      </c>
-      <c r="L18" t="s">
-        <v>63</v>
-      </c>
-      <c r="N18" t="s">
-        <v>64</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{509FD8C7-2668-4F8A-8FCA-72E4C3F520AD}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{DBDB132B-EE23-4863-9A01-1CB94AE8210A}"/>
-    <hyperlink ref="H14" r:id="rId3" xr:uid="{7F08651C-07CE-4F9D-9DB6-E721F8008E52}"/>
-    <hyperlink ref="E16" r:id="rId4" xr:uid="{F74A2CD9-57F6-4D37-891F-1C14CEE7EE28}"/>
-    <hyperlink ref="H17" r:id="rId5" xr:uid="{5A441EDE-90F6-429A-B4F6-8AA0CB497374}"/>
-    <hyperlink ref="D2" r:id="rId6" xr:uid="{4D5420C0-4098-4F77-8C77-2D92FABA6A99}"/>
-    <hyperlink ref="B2" r:id="rId7" xr:uid="{0256F7FB-58C2-4BAB-BE67-4206DEC228E7}"/>
-    <hyperlink ref="H3" r:id="rId8" xr:uid="{07E85401-832F-48E6-A047-319CB6B7D5A8}"/>
-    <hyperlink ref="B3" r:id="rId9" xr:uid="{61228DC3-4729-4E9D-BA47-AEC733E6A768}"/>
-    <hyperlink ref="B4" r:id="rId10" xr:uid="{C98662A6-6882-485B-A267-73578CC7A81C}"/>
-    <hyperlink ref="H4" r:id="rId11" xr:uid="{0D8096A3-5F8F-472A-9A88-F4D314BA1D84}"/>
-    <hyperlink ref="C2" r:id="rId12" xr:uid="{C12DCAE2-5BE7-4CB7-B68A-8142A2C5BE18}"/>
-    <hyperlink ref="I2" r:id="rId13" xr:uid="{940F9767-2975-43CD-9672-73F2C1E9BB76}"/>
-    <hyperlink ref="C3" r:id="rId14" xr:uid="{6BDBED0E-D6CA-4A54-BB34-C338CC84BC2F}"/>
-    <hyperlink ref="I3" r:id="rId15" xr:uid="{0F906926-6594-4D15-A39D-8F9257E712CA}"/>
-    <hyperlink ref="I4" r:id="rId16" xr:uid="{644E9B73-D236-4CAF-AD8F-1A59764D2EA5}"/>
-    <hyperlink ref="C4" r:id="rId17" xr:uid="{89910DEA-1D5D-4633-BFBA-0D931A2E8862}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41F8855-2B61-4FEF-9344-24F4972CEB0C}">
-  <dimension ref="A1:W6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" t="s">
-        <v>271</v>
-      </c>
-      <c r="L2" t="s">
-        <v>272</v>
-      </c>
-      <c r="M2" t="s">
-        <v>64</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="7"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="Q3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="T4" t="s">
-        <v>255</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="V4" t="s">
-        <v>83</v>
-      </c>
-      <c r="W4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>155</v>
-      </c>
-      <c r="J5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>154</v>
-      </c>
-      <c r="J6" t="s">
-        <v>227</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{1AEC3987-D7C8-4A5C-8BED-E9899FF2BF82}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{D43D11A9-1C5A-4349-B704-6198442D85A5}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{C222A27C-0748-414C-B788-B3F7C73C9801}"/>
-    <hyperlink ref="I2" r:id="rId4" xr:uid="{CC1F9EDD-65C4-42D8-92CA-91B148215A49}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{38064991-06F0-4D2B-A8AB-8973A45D8A40}"/>
-    <hyperlink ref="B4" r:id="rId6" xr:uid="{CDF79D5A-0018-470A-BA9B-7B98F8046D3D}"/>
-    <hyperlink ref="C4" r:id="rId7" xr:uid="{27C139E8-BC55-475F-9B0A-991734439882}"/>
-    <hyperlink ref="D4" r:id="rId8" xr:uid="{BA43A1BD-CF68-467C-B68B-99104FF975B9}"/>
-    <hyperlink ref="E4" r:id="rId9" xr:uid="{864335AC-3375-4C8A-93C0-0A0C164FF3A5}"/>
-    <hyperlink ref="H2" r:id="rId10" xr:uid="{5D19C1A3-09F6-4B12-9D2C-F4C9A06AA4AD}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29915A7A-9757-4FAB-8D6E-89B484B75E0F}">
-  <dimension ref="A1:AC23"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.33203125" customWidth="1"/>
-    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" t="s">
-        <v>63</v>
-      </c>
-      <c r="N2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="7"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="R3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>215</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="U4" t="s">
-        <v>255</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="W4" s="5"/>
-      <c r="X4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>221</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="U5" t="s">
-        <v>308</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="W5" s="5"/>
-      <c r="X5" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>222</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="U6" t="s">
-        <v>255</v>
-      </c>
-      <c r="V6" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="W6" s="5"/>
-      <c r="X6" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>155</v>
-      </c>
-      <c r="J7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>154</v>
-      </c>
-      <c r="J8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>224</v>
-      </c>
-      <c r="X9" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>214</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>209</v>
-      </c>
-      <c r="X10" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>214</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>210</v>
-      </c>
-      <c r="X11" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>226</v>
-      </c>
-      <c r="X12" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>217</v>
-      </c>
-      <c r="W13" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="X13" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>153</v>
-      </c>
-      <c r="U14" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="V14" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="U15" t="s">
-        <v>257</v>
-      </c>
-      <c r="V15" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>187</v>
-      </c>
-      <c r="B16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C16" t="s">
-        <v>274</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="U16" t="s">
-        <v>255</v>
-      </c>
-      <c r="V16" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="X16" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>44</v>
-      </c>
-      <c r="R18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="S18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T18">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="R19" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="S19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T19">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="R20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T20">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>168</v>
-      </c>
-      <c r="U21" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>166</v>
-      </c>
-      <c r="F22" t="s">
-        <v>431</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="K22" t="s">
-        <v>62</v>
-      </c>
-      <c r="L22" t="s">
-        <v>63</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="N22" t="s">
-        <v>64</v>
-      </c>
-      <c r="O22" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q22" s="5"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" t="s">
-        <v>50</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K23" t="s">
-        <v>150</v>
-      </c>
-      <c r="L23" t="s">
-        <v>17</v>
-      </c>
-      <c r="M23" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="N23" t="s">
-        <v>19</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P23" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q23" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="R23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T23">
-        <v>123</v>
-      </c>
-      <c r="AC23" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{01674EEF-5B1B-4083-B112-261BF32E9151}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{34D31921-71E7-42CC-86C8-D746F2995905}"/>
-    <hyperlink ref="H17" r:id="rId3" xr:uid="{881DC81A-1D11-43B1-A649-219EE29DF576}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{34C5CAF3-2DCD-4229-BB46-CE0027675E35}"/>
-    <hyperlink ref="I2" r:id="rId5" xr:uid="{3D193472-9B38-41A4-AE75-7C5F6D3602BA}"/>
-    <hyperlink ref="C2" r:id="rId6" xr:uid="{F5901482-C7A8-4FF2-B596-ABF445FEB63E}"/>
-    <hyperlink ref="H2" r:id="rId7" xr:uid="{9F7CAC9D-8E60-40FD-9B3E-4DF7D1F7B960}"/>
-    <hyperlink ref="D16" r:id="rId8" xr:uid="{F3D92567-3249-4D9A-BC44-71074C3A72B3}"/>
-    <hyperlink ref="H16" r:id="rId9" xr:uid="{C8A103B8-0E5D-4852-8D35-33CC8F223E0E}"/>
-    <hyperlink ref="H22" r:id="rId10" xr:uid="{0764A351-F269-48EF-8B6A-75A3942B351A}"/>
-    <hyperlink ref="H23" r:id="rId11" xr:uid="{9954984C-D6B1-4288-B72C-8B6336193DFF}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EEBDD4E-15C0-4517-B53D-FC4E89764F23}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.6640625" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F3" t="s">
-        <v>530</v>
-      </c>
-      <c r="G3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{2E40CAD4-3DDF-4115-9EA5-6641F416A14E}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{937C9B4A-3558-49DC-A73A-68CFBEE42860}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{9F0FB54C-AED1-481D-93FA-90CC93BA9B59}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{50D8CCD7-0D9E-482F-B9EF-1FD77791185F}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{DC118BEB-F328-46D1-BAFE-2340D7A8407A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F808DC-2462-40F4-8FE6-41754E94FF50}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>503</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="F2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAA7450-0FE7-4C50-95DC-266117BAF81B}">
-  <dimension ref="A1:S20"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.88671875" customWidth="1"/>
-    <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="78" customWidth="1"/>
-    <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5546875" customWidth="1"/>
-    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.109375" customWidth="1"/>
-    <col min="17" max="17" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>267</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>400</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>234</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>317</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="O1" s="19" t="s">
-        <v>399</v>
-      </c>
-      <c r="P1" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>263</v>
-      </c>
-      <c r="R1" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="S1" s="37" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>522</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>480</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20" t="s">
-        <v>523</v>
-      </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="20" t="s">
-        <v>567</v>
-      </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="19" t="s">
-        <v>428</v>
-      </c>
-      <c r="M6" s="20"/>
-      <c r="N6" s="19" t="s">
-        <v>336</v>
-      </c>
-      <c r="O6" s="19" t="s">
-        <v>336</v>
-      </c>
-      <c r="P6" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q6" s="20" t="s">
-        <v>335</v>
-      </c>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="28" t="s">
-        <v>524</v>
-      </c>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>262</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="19" t="s">
-        <v>568</v>
-      </c>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20" t="s">
-        <v>525</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="S10" s="20" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
-        <v>318</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20" t="s">
-        <v>319</v>
-      </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-    </row>
-    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>320</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="35" t="s">
-        <v>481</v>
-      </c>
-      <c r="H12" s="28" t="s">
-        <v>466</v>
-      </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
-        <v>321</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20" t="s">
-        <v>322</v>
-      </c>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>323</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20" t="s">
-        <v>324</v>
-      </c>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20" t="s">
-        <v>479</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20" t="s">
-        <v>365</v>
-      </c>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
-        <v>449</v>
-      </c>
-      <c r="C17" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
-        <v>450</v>
-      </c>
-      <c r="C18" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
-        <v>451</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>526</v>
-      </c>
-      <c r="J20" t="s">
-        <v>535</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4579BB67-5E19-4DC2-AEAD-551C7DC854EB}">
   <dimension ref="A1:AX71"/>
   <sheetViews>
@@ -7855,7 +8283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AS18"/>
   <sheetViews>
@@ -9165,7 +9593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
@@ -9278,7 +9706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
@@ -9541,11 +9969,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -10998,7 +11426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF53EDC-31F8-48E9-83B2-56073048BB22}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -11092,7 +11520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ACADB97-3AA8-40BF-AE7E-787123A27C76}">
   <dimension ref="A1:V7"/>
   <sheetViews>
@@ -11302,323 +11730,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{424970FD-0802-41D9-95B0-A7EEAE48FFD7}">
-  <dimension ref="A1:AA11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" t="s">
-        <v>150</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="7"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="P3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="H4" t="s">
-        <v>203</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="7"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="S5" t="s">
-        <v>149</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="U5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="W6" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="2"/>
-      <c r="X7" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L8" t="s">
-        <v>64</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>118</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" t="s">
-        <v>62</v>
-      </c>
-      <c r="J11" t="s">
-        <v>63</v>
-      </c>
-      <c r="L11" t="s">
-        <v>64</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{D6D44446-4E68-4240-BC3C-794C8762EF6C}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{F667B6EF-2843-441F-ADF3-A9F03FB2D127}"/>
-    <hyperlink ref="D9" r:id="rId3" xr:uid="{BA37854D-B94D-4462-95C3-1F9ADFCD61FB}"/>
-    <hyperlink ref="G10" r:id="rId4" xr:uid="{97AA2188-E825-4E95-BD32-7DE2E0872BDB}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{65D4744A-1A3C-492E-95BF-8C9052BD2013}"/>
-    <hyperlink ref="C2" r:id="rId6" xr:uid="{15735CF8-DBB0-492B-A615-DCBD78A638E3}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
HF-EMEA: fot he below testcase added excel data TEST_DGLD_HF_EMEA_RT_047_Placeorder_Guest_user_Checkout_with_multiple_products_as_full_Redemption_using_gift_card_code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8112FBD2-EAFC-4E55-A0E5-2FB0E3A8E675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FE0F74-3D1D-49A2-BBC3-B170395D6F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="589">
   <si>
     <t>UserName</t>
   </si>
@@ -1574,9 +1574,6 @@
 https://mcloud-na-stage4.hydroflask.com/prodeal/application/index/</t>
   </si>
   <si>
-    <t>8DZ67T85R4856M74K23D</t>
-  </si>
-  <si>
     <t>Hfemeanewaccount@gmail.com</t>
   </si>
   <si>
@@ -1673,9 +1670,6 @@
     <t>Below5 Shipping method</t>
   </si>
   <si>
-    <t>9GT64Y68Y7425Z97J65X</t>
-  </si>
-  <si>
     <t>es_Address</t>
   </si>
   <si>
@@ -1815,6 +1809,24 @@
   </si>
   <si>
     <t>DESort</t>
+  </si>
+  <si>
+    <t>5JC75F26E6322M52J32G</t>
+  </si>
+  <si>
+    <t>4YE64C42T7689L86N48T</t>
+  </si>
+  <si>
+    <t>4US62A42G7963M72M42Z</t>
+  </si>
+  <si>
+    <t>7SR29P66H7963P96Z78R</t>
+  </si>
+  <si>
+    <t>Full_RedeemGiftcard_2</t>
+  </si>
+  <si>
+    <t>4HK26S23S4448J92R64X</t>
   </si>
 </sst>
 </file>
@@ -2375,10 +2387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW59"/>
+  <dimension ref="A1:AW60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AM19" sqref="AM19"/>
+    <sheetView tabSelected="1" topLeftCell="N15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2523,7 +2535,7 @@
         <v>165</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>313</v>
@@ -2544,7 +2556,7 @@
         <v>207</v>
       </c>
       <c r="AU1" s="40" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>436</v>
@@ -2591,16 +2603,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" t="s">
+        <v>516</v>
+      </c>
+      <c r="T2" t="s">
+        <v>514</v>
+      </c>
+      <c r="V2" t="s">
         <v>517</v>
       </c>
-      <c r="T2" t="s">
-        <v>515</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="W2" s="5" t="s">
         <v>518</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>519</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>59</v>
@@ -2616,10 +2628,10 @@
         <v>294</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2634,10 +2646,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -2671,7 +2683,7 @@
     </row>
     <row r="4" spans="1:49" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>498</v>
@@ -2707,16 +2719,16 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="15" t="s">
+        <v>513</v>
+      </c>
+      <c r="T4" t="s">
         <v>514</v>
-      </c>
-      <c r="T4" t="s">
-        <v>515</v>
       </c>
       <c r="V4" t="s">
         <v>486</v>
       </c>
       <c r="W4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>59</v>
@@ -2729,10 +2741,10 @@
         <v>359</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -2747,10 +2759,10 @@
         <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2826,7 +2838,7 @@
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>498</v>
@@ -2862,16 +2874,16 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" t="s">
+        <v>537</v>
+      </c>
+      <c r="T7" t="s">
+        <v>538</v>
+      </c>
+      <c r="V7" t="s">
         <v>539</v>
       </c>
-      <c r="T7" t="s">
+      <c r="W7" s="5" t="s">
         <v>540</v>
-      </c>
-      <c r="V7" t="s">
-        <v>541</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>542</v>
       </c>
       <c r="X7" s="5" t="s">
         <v>59</v>
@@ -2881,7 +2893,7 @@
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>498</v>
@@ -2917,17 +2929,17 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="20" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="T8" s="20" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="U8" s="20"/>
       <c r="V8" s="42" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="W8" s="41" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="X8" s="41" t="s">
         <v>59</v>
@@ -2938,7 +2950,7 @@
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>498</v>
@@ -2974,17 +2986,17 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="20" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="T9" s="41" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="U9" s="20"/>
       <c r="V9" s="42" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="W9" s="41" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="X9" s="41" t="s">
         <v>59</v>
@@ -2995,7 +3007,7 @@
     </row>
     <row r="10" spans="1:49" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>498</v>
@@ -3031,17 +3043,17 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="20" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="T10" s="41" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="U10" s="20"/>
       <c r="V10" s="42" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="W10" s="41" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="X10" s="41">
         <v>9898989898</v>
@@ -3123,7 +3135,7 @@
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J16" s="18" t="s">
         <v>483</v>
@@ -3171,16 +3183,16 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="AC19" s="12" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="AD19" s="32">
         <v>1</v>
       </c>
       <c r="AE19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AF19" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="AG19" t="s">
         <v>190</v>
@@ -3463,10 +3475,10 @@
         <v>69</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.25">
@@ -3581,7 +3593,7 @@
         <v>184</v>
       </c>
       <c r="H39" s="23" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I39" s="12"/>
       <c r="AC39" t="s">
@@ -3663,7 +3675,7 @@
         <v>341</v>
       </c>
       <c r="P44" s="26" t="s">
-        <v>504</v>
+        <v>584</v>
       </c>
       <c r="Q44" s="5" t="s">
         <v>355</v>
@@ -3686,10 +3698,10 @@
         <v>430</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="N46" s="24" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.25">
@@ -3703,7 +3715,7 @@
         <v>349</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AP47" t="s">
         <v>351</v>
@@ -3713,163 +3725,171 @@
       <c r="A48" t="s">
         <v>353</v>
       </c>
-      <c r="P48" t="s">
-        <v>537</v>
+      <c r="P48" s="26" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>201</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F49" t="s">
-        <v>14</v>
-      </c>
-      <c r="G49" t="s">
-        <v>349</v>
-      </c>
-      <c r="H49" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="S49" t="s">
-        <v>499</v>
-      </c>
-      <c r="T49" t="s">
-        <v>501</v>
-      </c>
-      <c r="U49" t="s">
-        <v>490</v>
-      </c>
-      <c r="V49" t="s">
-        <v>500</v>
-      </c>
-      <c r="W49" s="5" t="s">
-        <v>502</v>
-      </c>
-      <c r="X49" s="5" t="s">
-        <v>59</v>
+        <v>587</v>
+      </c>
+      <c r="P49" s="26" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>363</v>
-      </c>
-      <c r="P50" s="5" t="s">
-        <v>364</v>
+        <v>201</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" t="s">
+        <v>349</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="S50" t="s">
+        <v>499</v>
+      </c>
+      <c r="T50" t="s">
+        <v>501</v>
+      </c>
+      <c r="U50" t="s">
+        <v>490</v>
+      </c>
+      <c r="V50" t="s">
+        <v>500</v>
+      </c>
+      <c r="W50" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="X50" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>432</v>
-      </c>
-      <c r="P51" s="27" t="s">
-        <v>434</v>
+        <v>363</v>
+      </c>
+      <c r="P51" s="26" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>433</v>
-      </c>
-      <c r="P52" s="26" t="s">
-        <v>511</v>
+        <v>432</v>
+      </c>
+      <c r="P52" s="27" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>433</v>
+      </c>
+      <c r="P53" s="26" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>232</v>
       </c>
-      <c r="AU53" t="s">
-        <v>529</v>
-      </c>
-      <c r="AV53" s="31" t="s">
+      <c r="AU54" t="s">
+        <v>528</v>
+      </c>
+      <c r="AV54" s="31" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B54" s="33"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="33"/>
-      <c r="J54" s="33"/>
-      <c r="K54" s="33"/>
-      <c r="L54" s="33"/>
-      <c r="M54" s="33"/>
-      <c r="N54" s="33"/>
-      <c r="O54" s="33"/>
-      <c r="P54" s="33"/>
-      <c r="Q54" s="33"/>
-      <c r="R54" s="33"/>
-      <c r="S54" s="33"/>
-      <c r="T54" s="33"/>
-      <c r="U54" s="33"/>
-      <c r="V54" s="33"/>
-      <c r="W54" s="33"/>
-      <c r="X54" s="33"/>
-      <c r="Y54" s="33"/>
-      <c r="Z54" s="33"/>
-      <c r="AA54" s="33"/>
-      <c r="AB54" s="33"/>
-      <c r="AC54" s="33" t="s">
+      <c r="B55" s="33"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="33"/>
+      <c r="J55" s="33"/>
+      <c r="K55" s="33"/>
+      <c r="L55" s="33"/>
+      <c r="M55" s="33"/>
+      <c r="N55" s="33"/>
+      <c r="O55" s="33"/>
+      <c r="P55" s="33"/>
+      <c r="Q55" s="33"/>
+      <c r="R55" s="33"/>
+      <c r="S55" s="33"/>
+      <c r="T55" s="33"/>
+      <c r="U55" s="33"/>
+      <c r="V55" s="33"/>
+      <c r="W55" s="33"/>
+      <c r="X55" s="33"/>
+      <c r="Y55" s="33"/>
+      <c r="Z55" s="33"/>
+      <c r="AA55" s="33"/>
+      <c r="AB55" s="33"/>
+      <c r="AC55" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="AD54" s="33">
+      <c r="AD55" s="33">
         <v>1</v>
       </c>
-      <c r="AE54" s="33"/>
-    </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>447</v>
-      </c>
-      <c r="P55" s="26" t="s">
-        <v>510</v>
-      </c>
+      <c r="AE55" s="33"/>
     </row>
     <row r="56" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>447</v>
+      </c>
+      <c r="P56" s="26" t="s">
         <v>509</v>
-      </c>
-      <c r="P56" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>508</v>
+      </c>
+      <c r="P57" s="26" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="58" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>519</v>
+      </c>
+      <c r="S58" t="s">
         <v>520</v>
       </c>
-      <c r="S57" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="58" spans="1:48" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>527</v>
-      </c>
-      <c r="AC58" s="43" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:48" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>531</v>
-      </c>
-      <c r="P59" t="s">
-        <v>508</v>
+        <v>526</v>
+      </c>
+      <c r="AC59" s="43" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="60" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>530</v>
+      </c>
+      <c r="P60" t="s">
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -3890,7 +3910,7 @@
     <hyperlink ref="E3" r:id="rId14" xr:uid="{32229FD5-4AFA-45C3-BF60-2566B7569180}"/>
     <hyperlink ref="AC19" r:id="rId15" display="https://mcloud-na-preprod.hydroflask.com/wide-mouth-flex-cap?color=Black" xr:uid="{618667E2-3380-4A1C-B34F-ABDD50D4EE61}"/>
     <hyperlink ref="H47" r:id="rId16" xr:uid="{7BF19D0A-861B-44DA-ABCD-EB14EC4082CF}"/>
-    <hyperlink ref="H49" r:id="rId17" xr:uid="{7332F9F7-6E5B-4009-8325-28D766EC646E}"/>
+    <hyperlink ref="H50" r:id="rId17" xr:uid="{7332F9F7-6E5B-4009-8325-28D766EC646E}"/>
     <hyperlink ref="E6" r:id="rId18" xr:uid="{2C317B8E-AF32-4D4C-AE44-1F2FC9B108BE}"/>
     <hyperlink ref="D6" r:id="rId19" xr:uid="{E6081600-960B-4A22-B355-F1C4E40470AA}"/>
     <hyperlink ref="B6" r:id="rId20" xr:uid="{7D100C12-0453-4673-AC35-2EA4A2603564}"/>
@@ -3935,7 +3955,7 @@
     <hyperlink ref="B10" r:id="rId59" xr:uid="{17E9DB6C-30D3-4F48-81EA-C35AF660B980}"/>
     <hyperlink ref="I10" r:id="rId60" xr:uid="{797DAE89-D941-4743-B597-439A5C30AAF0}"/>
     <hyperlink ref="C10" r:id="rId61" xr:uid="{34EC3537-EEF4-4D6F-923E-4AE4713BD831}"/>
-    <hyperlink ref="D49" r:id="rId62" xr:uid="{D9B3D2C8-8647-42D9-A4A0-095F61674861}"/>
+    <hyperlink ref="D50" r:id="rId62" xr:uid="{D9B3D2C8-8647-42D9-A4A0-095F61674861}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId63"/>
@@ -5622,7 +5642,7 @@
         <v>199</v>
       </c>
       <c r="F3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G3" t="s">
         <v>327</v>
@@ -5781,7 +5801,7 @@
         <v>228</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -5842,7 +5862,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
@@ -5870,7 +5890,7 @@
       <c r="H5" s="20"/>
       <c r="I5" s="30"/>
       <c r="J5" s="20" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
@@ -5931,7 +5951,7 @@
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
       <c r="M7" s="28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
@@ -5960,7 +5980,7 @@
       <c r="O8" s="20"/>
       <c r="P8" s="20"/>
       <c r="Q8" s="19" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
@@ -5973,7 +5993,7 @@
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -6195,10 +6215,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J20" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -6226,7 +6246,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -6261,10 +6281,10 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -9172,10 +9192,10 @@
         <v>3000146837</v>
       </c>
       <c r="AL11" s="47" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="AM11" s="12" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AN11" s="20"/>
       <c r="AO11" s="20"/>
@@ -9722,7 +9742,7 @@
         <v>25</v>
       </c>
       <c r="R2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="S2" t="s">
         <v>260</v>
@@ -10250,7 +10270,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
       <c r="T4" s="20" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="U4" s="20"/>
       <c r="V4" s="20"/>
@@ -10258,10 +10278,10 @@
         <v>1</v>
       </c>
       <c r="X4" s="12" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Y4" s="21" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="Z4" s="20"/>
       <c r="AA4" s="20"/>
@@ -10727,7 +10747,7 @@
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="41" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="R16" s="7" t="s">
         <v>442</v>
@@ -11037,7 +11057,7 @@
       <c r="T23" s="20"/>
       <c r="U23" s="20"/>
       <c r="V23" s="20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="W23" s="20"/>
       <c r="X23" s="20"/>
@@ -11064,7 +11084,7 @@
         <v>349</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
@@ -11131,7 +11151,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>498</v>
@@ -11158,16 +11178,16 @@
         <v>498</v>
       </c>
       <c r="K26" t="s">
+        <v>537</v>
+      </c>
+      <c r="L26" t="s">
+        <v>538</v>
+      </c>
+      <c r="M26" t="s">
         <v>539</v>
       </c>
-      <c r="L26" t="s">
+      <c r="N26" s="5" t="s">
         <v>540</v>
-      </c>
-      <c r="M26" t="s">
-        <v>541</v>
-      </c>
-      <c r="N26" s="5" t="s">
-        <v>542</v>
       </c>
       <c r="O26" s="5" t="s">
         <v>59</v>
@@ -11176,7 +11196,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>498</v>
@@ -11203,16 +11223,16 @@
         <v>498</v>
       </c>
       <c r="K27" s="20" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="L27" s="20" t="s">
+        <v>538</v>
+      </c>
+      <c r="M27" s="42" t="s">
+        <v>542</v>
+      </c>
+      <c r="N27" s="41" t="s">
         <v>540</v>
-      </c>
-      <c r="M27" s="42" t="s">
-        <v>544</v>
-      </c>
-      <c r="N27" s="41" t="s">
-        <v>542</v>
       </c>
       <c r="O27" s="41" t="s">
         <v>59</v>
@@ -11221,7 +11241,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>498</v>
@@ -11248,16 +11268,16 @@
         <v>498</v>
       </c>
       <c r="K28" s="20" t="s">
+        <v>544</v>
+      </c>
+      <c r="L28" s="41" t="s">
+        <v>545</v>
+      </c>
+      <c r="M28" s="42" t="s">
+        <v>545</v>
+      </c>
+      <c r="N28" s="41" t="s">
         <v>546</v>
-      </c>
-      <c r="L28" s="41" t="s">
-        <v>547</v>
-      </c>
-      <c r="M28" s="42" t="s">
-        <v>547</v>
-      </c>
-      <c r="N28" s="41" t="s">
-        <v>548</v>
       </c>
       <c r="O28" s="41" t="s">
         <v>59</v>
@@ -11266,7 +11286,7 @@
     </row>
     <row r="29" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>498</v>
@@ -11293,16 +11313,16 @@
         <v>498</v>
       </c>
       <c r="K29" s="20" t="s">
+        <v>548</v>
+      </c>
+      <c r="L29" s="41" t="s">
+        <v>549</v>
+      </c>
+      <c r="M29" s="42" t="s">
         <v>550</v>
       </c>
-      <c r="L29" s="41" t="s">
+      <c r="N29" s="41" t="s">
         <v>551</v>
-      </c>
-      <c r="M29" s="42" t="s">
-        <v>552</v>
-      </c>
-      <c r="N29" s="41" t="s">
-        <v>553</v>
       </c>
       <c r="O29" s="41">
         <v>9898989898</v>
@@ -11311,7 +11331,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F30" t="s">
         <v>14</v>
@@ -11320,16 +11340,16 @@
         <v>15</v>
       </c>
       <c r="K30" s="44" t="s">
+        <v>555</v>
+      </c>
+      <c r="L30" s="44" t="s">
+        <v>556</v>
+      </c>
+      <c r="M30" s="44" t="s">
         <v>557</v>
       </c>
-      <c r="L30" s="44" t="s">
+      <c r="N30" s="45" t="s">
         <v>558</v>
-      </c>
-      <c r="M30" s="44" t="s">
-        <v>559</v>
-      </c>
-      <c r="N30" s="45" t="s">
-        <v>560</v>
       </c>
       <c r="O30">
         <v>9898989898</v>
@@ -11337,7 +11357,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F31" t="s">
         <v>14</v>
@@ -11346,16 +11366,16 @@
         <v>15</v>
       </c>
       <c r="K31" t="s">
+        <v>559</v>
+      </c>
+      <c r="L31" t="s">
+        <v>560</v>
+      </c>
+      <c r="M31" s="18" t="s">
         <v>561</v>
       </c>
-      <c r="L31" t="s">
+      <c r="N31" s="5" t="s">
         <v>562</v>
-      </c>
-      <c r="M31" s="18" t="s">
-        <v>563</v>
-      </c>
-      <c r="N31" s="5" t="s">
-        <v>564</v>
       </c>
       <c r="O31">
         <v>9898989898</v>
@@ -11363,7 +11383,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F32" t="s">
         <v>14</v>
@@ -11372,16 +11392,16 @@
         <v>15</v>
       </c>
       <c r="K32" t="s">
+        <v>568</v>
+      </c>
+      <c r="L32" t="s">
+        <v>569</v>
+      </c>
+      <c r="M32" t="s">
         <v>570</v>
       </c>
-      <c r="L32" t="s">
+      <c r="N32" s="5" t="s">
         <v>571</v>
-      </c>
-      <c r="M32" t="s">
-        <v>572</v>
-      </c>
-      <c r="N32" s="5" t="s">
-        <v>573</v>
       </c>
       <c r="O32">
         <v>9898989898</v>
@@ -11389,7 +11409,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F33" t="s">
         <v>14</v>
@@ -11398,16 +11418,16 @@
         <v>15</v>
       </c>
       <c r="K33" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="L33" t="s">
+        <v>572</v>
+      </c>
+      <c r="M33" t="s">
         <v>574</v>
       </c>
-      <c r="M33" t="s">
-        <v>576</v>
-      </c>
       <c r="N33" s="5" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="O33">
         <v>9898989898</v>

</xml_diff>

<commit_message>
HF-EMEA Testdata and helepr changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3272A5-F111-4EE5-B150-E9EA2971A864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDBB9EE-56F8-45F8-BE3A-A579FE9A9670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="596">
   <si>
     <t>UserName</t>
   </si>
@@ -1845,6 +1845,9 @@
   </si>
   <si>
     <t>Our Story,Privacy Policy,Cookie Policy</t>
+  </si>
+  <si>
+    <t>HFEMEATEST5</t>
   </si>
 </sst>
 </file>
@@ -2407,8 +2410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW60"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AJ26" sqref="AJ26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3329,7 +3332,7 @@
         <v>480</v>
       </c>
       <c r="AJ26" t="s">
-        <v>264</v>
+        <v>595</v>
       </c>
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.25">
@@ -10077,8 +10080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10201,7 +10204,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>329</v>
+        <v>438</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>329</v>
@@ -10219,7 +10222,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>329</v>
+        <v>438</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>329</v>
@@ -11486,44 +11489,44 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="mailto:spanem@helenoftroy.com" xr:uid="{CC67BCBF-E076-4645-AAE7-B7E656BA65BA}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{CC67BCBF-E076-4645-AAE7-B7E656BA65BA}"/>
     <hyperlink ref="C2" r:id="rId2" display="mailto:spanem@helenoftroy.com" xr:uid="{B9951B2A-1254-4C0B-9A14-C6A846810C91}"/>
     <hyperlink ref="D2" r:id="rId3" xr:uid="{74C7B7B6-D379-4E34-A081-A00A70371A86}"/>
     <hyperlink ref="E2" r:id="rId4" xr:uid="{1702FA67-6467-4E57-9DE2-FB4C9A48C932}"/>
-    <hyperlink ref="H2" r:id="rId5" display="mailto:spanem@helenoftroy.com" xr:uid="{43710853-757A-4E86-AEEB-F5DD155D60F0}"/>
-    <hyperlink ref="I2" r:id="rId6" display="mailto:spanem@helenoftroy.com" xr:uid="{B3D81E16-7F77-4EDD-A91C-F9F6093FDE1C}"/>
-    <hyperlink ref="X4" r:id="rId7" display="https://www.hydroflask.com/12-oz-mug?color=Moonshadow" xr:uid="{2F702AF3-4F49-47B1-A82E-D55704330159}"/>
-    <hyperlink ref="H13" r:id="rId8" display="mailto:oxobuyer@oxo.com" xr:uid="{F703F13B-8A00-4A75-B16B-BB47D9846FC3}"/>
-    <hyperlink ref="B18" r:id="rId9" display="mailto:hmaram+991@helenoftroy.com" xr:uid="{DFBAB818-5BA3-4627-82C1-2CAC5A38DA29}"/>
-    <hyperlink ref="D18" r:id="rId10" display="mailto:Lotus@123" xr:uid="{28DBD95D-7F24-4CA5-90B6-5D7EE9C211E0}"/>
-    <hyperlink ref="H18" r:id="rId11" display="mailto:hmaram+991@helenoftroy.com" xr:uid="{D33C6A77-1D8A-4989-B011-B3EC18D603BE}"/>
-    <hyperlink ref="B20" r:id="rId12" display="mailto:LotusQA.GLD.PP.HYF.AutoTest2@gmail.com" xr:uid="{5ED567C6-C7C9-409A-B37F-4B27F631F296}"/>
-    <hyperlink ref="C20" r:id="rId13" display="mailto:LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{ED6C3419-A80F-4A4A-9244-B1858B017A52}"/>
-    <hyperlink ref="D20" r:id="rId14" display="mailto:Lotuswave@123" xr:uid="{13894A42-11B2-43E5-A940-219C069B253B}"/>
-    <hyperlink ref="E20" r:id="rId15" display="mailto:Lotuswave@123" xr:uid="{A59ABD88-352A-4F2F-BE3F-3D7FE2ED8628}"/>
-    <hyperlink ref="H21" r:id="rId16" display="mailto:qatesting.lotuswave@gmail.com" xr:uid="{B7904D5A-78CF-4256-B487-367AA497945A}"/>
-    <hyperlink ref="H24" r:id="rId17" display="mailto:anbogi@helenoftroy.com" xr:uid="{E5E20641-574A-45A3-9813-A9FDD7348D38}"/>
-    <hyperlink ref="E27" r:id="rId18" xr:uid="{487914A8-4697-4DB6-854A-EF572783CAE5}"/>
-    <hyperlink ref="D27" r:id="rId19" xr:uid="{DCBFD706-9320-4558-9FB9-5215E74EF027}"/>
-    <hyperlink ref="B27" r:id="rId20" xr:uid="{958E0D5A-99DC-4229-A9B5-F858C288DF93}"/>
-    <hyperlink ref="C27" r:id="rId21" xr:uid="{03D0261B-19FB-4B07-94F7-B5E05B00A0AD}"/>
-    <hyperlink ref="B26" r:id="rId22" xr:uid="{9D7ED4E0-A81B-429D-A39C-920A83DA144B}"/>
-    <hyperlink ref="C26" r:id="rId23" xr:uid="{486135B8-12EF-4895-8C0A-C397D6F79836}"/>
-    <hyperlink ref="E28" r:id="rId24" xr:uid="{9368F616-FB0E-4629-B847-AB078159FF31}"/>
-    <hyperlink ref="D28" r:id="rId25" xr:uid="{D54C9969-1238-402C-8B4A-A5FDFD5D588D}"/>
-    <hyperlink ref="B28" r:id="rId26" xr:uid="{40619871-6630-4D8A-87B7-2E98ADD15F6B}"/>
-    <hyperlink ref="C28" r:id="rId27" xr:uid="{2C89D78D-381D-400E-BF64-3D5EC22DF26B}"/>
-    <hyperlink ref="E29" r:id="rId28" xr:uid="{BA694217-0C35-4D10-ABC2-378FCC42C23C}"/>
-    <hyperlink ref="D29" r:id="rId29" xr:uid="{3FC28D22-984F-4899-9C90-44074B8F6F21}"/>
-    <hyperlink ref="B29" r:id="rId30" xr:uid="{EF536980-2486-44C3-AECF-B11EF9433874}"/>
-    <hyperlink ref="C29" r:id="rId31" xr:uid="{46CF19F0-F4AC-41A8-ACA4-D8E37C528FB6}"/>
-    <hyperlink ref="H27" r:id="rId32" xr:uid="{9585710E-0B91-4B35-86E8-B635F5BBCCBD}"/>
-    <hyperlink ref="I27" r:id="rId33" xr:uid="{2AA152F2-4C75-43C9-8FB7-3DB11076239B}"/>
-    <hyperlink ref="I26" r:id="rId34" xr:uid="{F3690A94-65A4-4F9B-8AE6-E5656F40DC4B}"/>
-    <hyperlink ref="H28" r:id="rId35" xr:uid="{EDEAC841-23AB-4DCF-9E5C-275E7FFA36E4}"/>
-    <hyperlink ref="I28" r:id="rId36" xr:uid="{E337B82A-8EBA-45A9-933E-F5B946AE530C}"/>
-    <hyperlink ref="H29" r:id="rId37" xr:uid="{ED2441B7-6548-423C-8B21-2D2EAE63A151}"/>
-    <hyperlink ref="I29" r:id="rId38" xr:uid="{80D06A9D-A965-4DF1-8B42-D4A8BF6A4DEB}"/>
+    <hyperlink ref="I2" r:id="rId5" display="mailto:spanem@helenoftroy.com" xr:uid="{B3D81E16-7F77-4EDD-A91C-F9F6093FDE1C}"/>
+    <hyperlink ref="X4" r:id="rId6" display="https://www.hydroflask.com/12-oz-mug?color=Moonshadow" xr:uid="{2F702AF3-4F49-47B1-A82E-D55704330159}"/>
+    <hyperlink ref="H13" r:id="rId7" display="mailto:oxobuyer@oxo.com" xr:uid="{F703F13B-8A00-4A75-B16B-BB47D9846FC3}"/>
+    <hyperlink ref="B18" r:id="rId8" display="mailto:hmaram+991@helenoftroy.com" xr:uid="{DFBAB818-5BA3-4627-82C1-2CAC5A38DA29}"/>
+    <hyperlink ref="D18" r:id="rId9" display="mailto:Lotus@123" xr:uid="{28DBD95D-7F24-4CA5-90B6-5D7EE9C211E0}"/>
+    <hyperlink ref="H18" r:id="rId10" display="mailto:hmaram+991@helenoftroy.com" xr:uid="{D33C6A77-1D8A-4989-B011-B3EC18D603BE}"/>
+    <hyperlink ref="B20" r:id="rId11" display="mailto:LotusQA.GLD.PP.HYF.AutoTest2@gmail.com" xr:uid="{5ED567C6-C7C9-409A-B37F-4B27F631F296}"/>
+    <hyperlink ref="C20" r:id="rId12" display="mailto:LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{ED6C3419-A80F-4A4A-9244-B1858B017A52}"/>
+    <hyperlink ref="D20" r:id="rId13" display="mailto:Lotuswave@123" xr:uid="{13894A42-11B2-43E5-A940-219C069B253B}"/>
+    <hyperlink ref="E20" r:id="rId14" display="mailto:Lotuswave@123" xr:uid="{A59ABD88-352A-4F2F-BE3F-3D7FE2ED8628}"/>
+    <hyperlink ref="H21" r:id="rId15" display="mailto:qatesting.lotuswave@gmail.com" xr:uid="{B7904D5A-78CF-4256-B487-367AA497945A}"/>
+    <hyperlink ref="H24" r:id="rId16" display="mailto:anbogi@helenoftroy.com" xr:uid="{E5E20641-574A-45A3-9813-A9FDD7348D38}"/>
+    <hyperlink ref="E27" r:id="rId17" xr:uid="{487914A8-4697-4DB6-854A-EF572783CAE5}"/>
+    <hyperlink ref="D27" r:id="rId18" xr:uid="{DCBFD706-9320-4558-9FB9-5215E74EF027}"/>
+    <hyperlink ref="B27" r:id="rId19" xr:uid="{958E0D5A-99DC-4229-A9B5-F858C288DF93}"/>
+    <hyperlink ref="C27" r:id="rId20" xr:uid="{03D0261B-19FB-4B07-94F7-B5E05B00A0AD}"/>
+    <hyperlink ref="B26" r:id="rId21" xr:uid="{9D7ED4E0-A81B-429D-A39C-920A83DA144B}"/>
+    <hyperlink ref="C26" r:id="rId22" xr:uid="{486135B8-12EF-4895-8C0A-C397D6F79836}"/>
+    <hyperlink ref="E28" r:id="rId23" xr:uid="{9368F616-FB0E-4629-B847-AB078159FF31}"/>
+    <hyperlink ref="D28" r:id="rId24" xr:uid="{D54C9969-1238-402C-8B4A-A5FDFD5D588D}"/>
+    <hyperlink ref="B28" r:id="rId25" xr:uid="{40619871-6630-4D8A-87B7-2E98ADD15F6B}"/>
+    <hyperlink ref="C28" r:id="rId26" xr:uid="{2C89D78D-381D-400E-BF64-3D5EC22DF26B}"/>
+    <hyperlink ref="E29" r:id="rId27" xr:uid="{BA694217-0C35-4D10-ABC2-378FCC42C23C}"/>
+    <hyperlink ref="D29" r:id="rId28" xr:uid="{3FC28D22-984F-4899-9C90-44074B8F6F21}"/>
+    <hyperlink ref="B29" r:id="rId29" xr:uid="{EF536980-2486-44C3-AECF-B11EF9433874}"/>
+    <hyperlink ref="C29" r:id="rId30" xr:uid="{46CF19F0-F4AC-41A8-ACA4-D8E37C528FB6}"/>
+    <hyperlink ref="H27" r:id="rId31" xr:uid="{9585710E-0B91-4B35-86E8-B635F5BBCCBD}"/>
+    <hyperlink ref="I27" r:id="rId32" xr:uid="{2AA152F2-4C75-43C9-8FB7-3DB11076239B}"/>
+    <hyperlink ref="I26" r:id="rId33" xr:uid="{F3690A94-65A4-4F9B-8AE6-E5656F40DC4B}"/>
+    <hyperlink ref="H28" r:id="rId34" xr:uid="{EDEAC841-23AB-4DCF-9E5C-275E7FFA36E4}"/>
+    <hyperlink ref="I28" r:id="rId35" xr:uid="{E337B82A-8EBA-45A9-933E-F5B946AE530C}"/>
+    <hyperlink ref="H29" r:id="rId36" xr:uid="{ED2441B7-6548-423C-8B21-2D2EAE63A151}"/>
+    <hyperlink ref="I29" r:id="rId37" xr:uid="{80D06A9D-A965-4DF1-8B42-D4A8BF6A4DEB}"/>
+    <hyperlink ref="H2" r:id="rId38" xr:uid="{E7F5D2F0-ED8F-4AB5-B623-9122A2B6A26B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId39"/>
@@ -11534,7 +11537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF53EDC-31F8-48E9-83B2-56073048BB22}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
HF-EMEA : Added new testcases 003 and 004
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDBB9EE-56F8-45F8-BE3A-A579FE9A9670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5898C2AC-FA28-4124-8DCF-F77A8DB6ACCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="598">
   <si>
     <t>UserName</t>
   </si>
@@ -1848,6 +1848,12 @@
   </si>
   <si>
     <t>HFEMEATEST5</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>99999</t>
   </si>
 </sst>
 </file>
@@ -2408,10 +2414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW60"/>
+  <dimension ref="A1:AW61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AJ26" sqref="AJ26"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3115,10 +3121,42 @@
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>297</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="F13" t="s">
+        <v>331</v>
+      </c>
+      <c r="G13" t="s">
+        <v>332</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="N13" t="s">
+        <v>333</v>
+      </c>
+      <c r="O13" t="s">
+        <v>64</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="T13" t="s">
+        <v>333</v>
+      </c>
+      <c r="U13" t="s">
+        <v>64</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>597</v>
+      </c>
       <c r="Z13" s="5" t="s">
         <v>298</v>
       </c>
@@ -3131,22 +3169,21 @@
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>297</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="J14" t="s">
-        <v>203</v>
-      </c>
       <c r="Z14" s="5"/>
       <c r="AA14" s="7"/>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>154</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>481</v>
+        <v>155</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="J15" t="s">
+        <v>203</v>
       </c>
       <c r="W15" s="3"/>
       <c r="X15" s="4"/>
@@ -3156,7 +3193,7 @@
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>526</v>
+        <v>154</v>
       </c>
       <c r="J16" s="18" t="s">
         <v>481</v>
@@ -3167,7 +3204,10 @@
     </row>
     <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>526</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="W17" s="3"/>
       <c r="X17" s="4"/>
@@ -3186,7 +3226,7 @@
     </row>
     <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="W18" s="3"/>
       <c r="X18" s="4"/>
@@ -3199,10 +3239,8 @@
     </row>
     <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+        <v>170</v>
+      </c>
       <c r="AC19" s="12" t="s">
         <v>543</v>
       </c>
@@ -3227,7 +3265,7 @@
     </row>
     <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>442</v>
+        <v>25</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -3241,7 +3279,7 @@
     </row>
     <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>442</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -3260,7 +3298,7 @@
     </row>
     <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -3273,7 +3311,7 @@
     </row>
     <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -3284,23 +3322,9 @@
     </row>
     <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" t="s">
-        <v>35</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="AL24" s="12" t="s">
         <v>444</v>
@@ -3308,9 +3332,23 @@
     </row>
     <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="I25" s="2"/>
       <c r="AD25" s="5" t="s">
         <v>113</v>
@@ -3321,11 +3359,8 @@
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="G26" s="6"/>
+        <v>40</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="AI26" t="s">
@@ -3337,8 +3372,13 @@
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
       <c r="Z27" s="5" t="s">
         <v>45</v>
       </c>
@@ -3351,16 +3391,8 @@
     </row>
     <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+        <v>44</v>
+      </c>
       <c r="S28" t="s">
         <v>150</v>
       </c>
@@ -3388,8 +3420,16 @@
     </row>
     <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
       <c r="Z29" s="5" t="s">
         <v>49</v>
       </c>
@@ -3402,15 +3442,8 @@
     </row>
     <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" t="s">
-        <v>50</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="2"/>
+        <v>48</v>
+      </c>
       <c r="S30" t="s">
         <v>150</v>
       </c>
@@ -3444,8 +3477,15 @@
     </row>
     <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F31" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="2"/>
       <c r="Z31" s="5" t="s">
         <v>56</v>
       </c>
@@ -3458,13 +3498,7 @@
     </row>
     <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>61</v>
-      </c>
-      <c r="F32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="S32" t="s">
         <v>495</v>
@@ -3487,33 +3521,31 @@
     </row>
     <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>500</v>
+        <v>61</v>
+      </c>
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>491</v>
-      </c>
-      <c r="E34" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="H34" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="I34" s="2"/>
+        <v>500</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>500</v>
+      </c>
       <c r="W34" s="5"/>
       <c r="X34" s="5" t="s">
         <v>59</v>
@@ -3521,14 +3553,16 @@
     </row>
     <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>118</v>
-      </c>
-      <c r="F35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" t="s">
-        <v>15</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="H35" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="I35" s="2"/>
       <c r="S35" t="s">
         <v>495</v>
       </c>
@@ -3550,7 +3584,13 @@
     </row>
     <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>118</v>
+      </c>
+      <c r="F36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" t="s">
+        <v>15</v>
       </c>
       <c r="AL36" t="s">
         <v>436</v>
@@ -3558,7 +3598,7 @@
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="AM37" t="s">
         <v>296</v>
@@ -3572,23 +3612,8 @@
     </row>
     <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>166</v>
-      </c>
-      <c r="F38" t="s">
-        <v>167</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
-      <c r="P38" s="12"/>
-      <c r="Q38" s="12"/>
+        <v>164</v>
+      </c>
       <c r="R38" s="12"/>
       <c r="S38" t="s">
         <v>495</v>
@@ -3611,12 +3636,23 @@
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>184</v>
-      </c>
-      <c r="H39" s="23" t="s">
-        <v>500</v>
+        <v>166</v>
+      </c>
+      <c r="F39" t="s">
+        <v>167</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="12"/>
       <c r="AC39" t="s">
         <v>257</v>
       </c>
@@ -3626,21 +3662,19 @@
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>279</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="H40" s="23" t="s">
+        <v>500</v>
+      </c>
+      <c r="I40" s="12"/>
       <c r="AP40" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>284</v>
-      </c>
-      <c r="F41" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41" t="s">
-        <v>14</v>
+        <v>279</v>
       </c>
       <c r="AP41" t="s">
         <v>285</v>
@@ -3648,7 +3682,13 @@
     </row>
     <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>215</v>
+        <v>284</v>
+      </c>
+      <c r="F42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" t="s">
+        <v>14</v>
       </c>
       <c r="AC42" t="s">
         <v>255</v>
@@ -3665,7 +3705,7 @@
     </row>
     <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="AF43" t="s">
         <v>39</v>
@@ -3682,30 +3722,30 @@
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>339</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="O44" t="s">
-        <v>341</v>
-      </c>
-      <c r="P44" s="26" t="s">
-        <v>574</v>
-      </c>
-      <c r="Q44" s="5" t="s">
-        <v>355</v>
+        <v>209</v>
       </c>
       <c r="R44" s="5"/>
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>343</v>
+        <v>339</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="O45" t="s">
+        <v>341</v>
+      </c>
+      <c r="P45" s="26" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q45" s="5" t="s">
+        <v>355</v>
       </c>
       <c r="R45" t="s">
         <v>345</v>
@@ -3713,30 +3753,21 @@
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>346</v>
-      </c>
-      <c r="L46" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="M46" s="5" t="s">
-        <v>502</v>
-      </c>
-      <c r="N46" s="24" t="s">
-        <v>501</v>
+        <v>343</v>
       </c>
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>348</v>
-      </c>
-      <c r="F47" t="s">
-        <v>14</v>
-      </c>
-      <c r="G47" t="s">
-        <v>349</v>
-      </c>
-      <c r="H47" s="12" t="s">
-        <v>507</v>
+        <v>346</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="M47" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="N47" s="24" t="s">
+        <v>501</v>
       </c>
       <c r="AP47" t="s">
         <v>351</v>
@@ -3744,41 +3775,32 @@
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>353</v>
-      </c>
-      <c r="P48" s="26" t="s">
-        <v>575</v>
+        <v>348</v>
+      </c>
+      <c r="F48" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" t="s">
+        <v>349</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>577</v>
+        <v>353</v>
       </c>
       <c r="P49" s="26" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>201</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F50" t="s">
-        <v>14</v>
-      </c>
-      <c r="G50" t="s">
-        <v>349</v>
-      </c>
-      <c r="H50" s="12" t="s">
-        <v>305</v>
+        <v>577</v>
+      </c>
+      <c r="P50" s="26" t="s">
+        <v>578</v>
       </c>
       <c r="S50" t="s">
         <v>495</v>
@@ -3801,31 +3823,49 @@
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>363</v>
-      </c>
-      <c r="P51" s="26" t="s">
-        <v>573</v>
+        <v>201</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" t="s">
+        <v>349</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>431</v>
-      </c>
-      <c r="P52" s="27" t="s">
-        <v>433</v>
+        <v>363</v>
+      </c>
+      <c r="P52" s="26" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>432</v>
-      </c>
-      <c r="P53" s="26" t="s">
-        <v>506</v>
+        <v>431</v>
+      </c>
+      <c r="P53" s="27" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>232</v>
+        <v>432</v>
+      </c>
+      <c r="P54" s="26" t="s">
+        <v>506</v>
       </c>
       <c r="AU54" t="s">
         <v>520</v>
@@ -3835,25 +3875,9 @@
       </c>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A55" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="B55" s="33"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="33"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="33"/>
-      <c r="H55" s="33"/>
-      <c r="I55" s="33"/>
-      <c r="J55" s="33"/>
-      <c r="K55" s="33"/>
-      <c r="L55" s="33"/>
-      <c r="M55" s="33"/>
-      <c r="N55" s="33"/>
-      <c r="O55" s="33"/>
-      <c r="P55" s="33"/>
-      <c r="Q55" s="33"/>
+      <c r="A55" t="s">
+        <v>232</v>
+      </c>
       <c r="R55" s="33"/>
       <c r="S55" s="33"/>
       <c r="T55" s="33"/>
@@ -3874,24 +3898,40 @@
       <c r="AE55" s="33"/>
     </row>
     <row r="56" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>446</v>
-      </c>
-      <c r="P56" s="26" t="s">
-        <v>505</v>
-      </c>
+      <c r="A56" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" s="33"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="33"/>
+      <c r="N56" s="33"/>
+      <c r="O56" s="33"/>
+      <c r="P56" s="33"/>
+      <c r="Q56" s="33"/>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>504</v>
+        <v>446</v>
       </c>
       <c r="P57" s="26" t="s">
-        <v>576</v>
+        <v>505</v>
       </c>
     </row>
     <row r="58" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>515</v>
+        <v>504</v>
+      </c>
+      <c r="P58" s="26" t="s">
+        <v>576</v>
       </c>
       <c r="S58" t="s">
         <v>516</v>
@@ -3899,7 +3939,7 @@
     </row>
     <row r="59" spans="1:48" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="AC59" s="43" t="s">
         <v>545</v>
@@ -3907,38 +3947,43 @@
     </row>
     <row r="60" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="61" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>522</v>
       </c>
-      <c r="P60" t="s">
+      <c r="P61" t="s">
         <v>503</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{92F09EC2-FC6F-443B-965E-DCA7B56F1753}"/>
-    <hyperlink ref="D24" r:id="rId2" display="Lotuswave@123" xr:uid="{27A376CC-4E23-4441-B806-FE9FF359794E}"/>
+    <hyperlink ref="D25" r:id="rId2" display="Lotuswave@123" xr:uid="{27A376CC-4E23-4441-B806-FE9FF359794E}"/>
     <hyperlink ref="E2" r:id="rId3" xr:uid="{5B310480-7344-4661-AB0F-D7D61F727B40}"/>
-    <hyperlink ref="H30" r:id="rId4" xr:uid="{D3AC8605-ACE0-4742-A275-CC55BA0B713E}"/>
-    <hyperlink ref="H34" r:id="rId5" xr:uid="{EBF04138-1F63-4113-A63D-68EC86409EAF}"/>
+    <hyperlink ref="H31" r:id="rId4" xr:uid="{D3AC8605-ACE0-4742-A275-CC55BA0B713E}"/>
+    <hyperlink ref="H35" r:id="rId5" xr:uid="{EBF04138-1F63-4113-A63D-68EC86409EAF}"/>
     <hyperlink ref="AL24" r:id="rId6" xr:uid="{C3ED735C-0638-4013-B1A9-35D874D27CCD}"/>
-    <hyperlink ref="H38" r:id="rId7" xr:uid="{7B92FAF6-FC7B-4378-BAA5-F455D3557016}"/>
+    <hyperlink ref="H39" r:id="rId7" xr:uid="{7B92FAF6-FC7B-4378-BAA5-F455D3557016}"/>
     <hyperlink ref="D2" r:id="rId8" xr:uid="{6D9C84C2-080E-49A8-91A9-0C4040F17B99}"/>
-    <hyperlink ref="H39" r:id="rId9" xr:uid="{5EDA0D22-59C6-4E86-B1C8-F3DDADDA222C}"/>
+    <hyperlink ref="H40" r:id="rId9" xr:uid="{5EDA0D22-59C6-4E86-B1C8-F3DDADDA222C}"/>
     <hyperlink ref="B2" r:id="rId10" xr:uid="{49EA4C67-65EF-4ECE-B592-DD27DDBFE9D8}"/>
     <hyperlink ref="I2" r:id="rId11" xr:uid="{41758504-FDAA-49B8-A517-3CF2E58C91CC}"/>
     <hyperlink ref="C2" r:id="rId12" xr:uid="{12FE48FE-6D5F-46FF-BB71-C2756AE73EE8}"/>
     <hyperlink ref="D3" r:id="rId13" xr:uid="{62C3648F-7D52-4B9F-ADF3-7CB24D30FA17}"/>
     <hyperlink ref="E3" r:id="rId14" xr:uid="{32229FD5-4AFA-45C3-BF60-2566B7569180}"/>
     <hyperlink ref="AC19" r:id="rId15" display="https://mcloud-na-preprod.hydroflask.com/wide-mouth-flex-cap?color=Black" xr:uid="{618667E2-3380-4A1C-B34F-ABDD50D4EE61}"/>
-    <hyperlink ref="H47" r:id="rId16" xr:uid="{7BF19D0A-861B-44DA-ABCD-EB14EC4082CF}"/>
-    <hyperlink ref="H50" r:id="rId17" xr:uid="{7332F9F7-6E5B-4009-8325-28D766EC646E}"/>
+    <hyperlink ref="H48" r:id="rId16" xr:uid="{7BF19D0A-861B-44DA-ABCD-EB14EC4082CF}"/>
+    <hyperlink ref="H51" r:id="rId17" xr:uid="{7332F9F7-6E5B-4009-8325-28D766EC646E}"/>
     <hyperlink ref="E6" r:id="rId18" xr:uid="{2C317B8E-AF32-4D4C-AE44-1F2FC9B108BE}"/>
     <hyperlink ref="D6" r:id="rId19" xr:uid="{E6081600-960B-4A22-B355-F1C4E40470AA}"/>
     <hyperlink ref="B6" r:id="rId20" xr:uid="{7D100C12-0453-4673-AC35-2EA4A2603564}"/>
     <hyperlink ref="I6" r:id="rId21" display="LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{4380A0E0-76DF-485C-8BEA-6C28F9B24971}"/>
     <hyperlink ref="C6" r:id="rId22" display="LotusQA.GLD.PR.HYF.AutoTest7@gmail.com" xr:uid="{8F318BE4-05CB-41C2-8BFD-E5C42814E494}"/>
     <hyperlink ref="H6" r:id="rId23" xr:uid="{407C8F4E-9B49-4856-B5B1-AADA1B530463}"/>
-    <hyperlink ref="D33" r:id="rId24" xr:uid="{CFA846D7-1044-49EA-A0C9-5358EDB0782D}"/>
+    <hyperlink ref="D34" r:id="rId24" xr:uid="{CFA846D7-1044-49EA-A0C9-5358EDB0782D}"/>
     <hyperlink ref="B3" r:id="rId25" xr:uid="{A4EF70F2-1E9D-4209-9990-D57B7B04D033}"/>
     <hyperlink ref="C3" r:id="rId26" xr:uid="{A02552C8-A6E5-4D41-80F6-00B2ABF9087C}"/>
     <hyperlink ref="H3" r:id="rId27" xr:uid="{475B0B91-5BB6-4DC1-8A14-637459A21F69}"/>
@@ -3953,8 +3998,8 @@
     <hyperlink ref="C5" r:id="rId36" xr:uid="{817C7CDF-7723-4347-999A-B70D0C4C4C9F}"/>
     <hyperlink ref="H5" r:id="rId37" xr:uid="{46997A70-4DF6-42DF-98DE-3A15FE00FF24}"/>
     <hyperlink ref="I5" r:id="rId38" xr:uid="{323D0279-E435-4C6C-805F-A066B3FCDA92}"/>
-    <hyperlink ref="H33" r:id="rId39" xr:uid="{EDD9788C-AEBE-4F86-8A6C-8043A32B81A6}"/>
-    <hyperlink ref="I33" r:id="rId40" xr:uid="{68882096-6651-4D29-9355-6F1410B100AA}"/>
+    <hyperlink ref="H34" r:id="rId39" xr:uid="{EDD9788C-AEBE-4F86-8A6C-8043A32B81A6}"/>
+    <hyperlink ref="I34" r:id="rId40" xr:uid="{68882096-6651-4D29-9355-6F1410B100AA}"/>
     <hyperlink ref="H8" r:id="rId41" xr:uid="{867EC1A7-B881-422A-8354-C1C7FCE40AAE}"/>
     <hyperlink ref="E8" r:id="rId42" xr:uid="{5ACEF6FA-BF68-4BBD-BE65-3578FCD63C44}"/>
     <hyperlink ref="D8" r:id="rId43" xr:uid="{3607587D-2F3E-4312-8C6F-F1EF148F7A1A}"/>
@@ -3976,10 +4021,11 @@
     <hyperlink ref="B10" r:id="rId59" xr:uid="{17E9DB6C-30D3-4F48-81EA-C35AF660B980}"/>
     <hyperlink ref="I10" r:id="rId60" xr:uid="{797DAE89-D941-4743-B597-439A5C30AAF0}"/>
     <hyperlink ref="C10" r:id="rId61" xr:uid="{34EC3537-EEF4-4D6F-923E-4AE4713BD831}"/>
-    <hyperlink ref="D50" r:id="rId62" xr:uid="{D9B3D2C8-8647-42D9-A4A0-095F61674861}"/>
+    <hyperlink ref="D51" r:id="rId62" xr:uid="{D9B3D2C8-8647-42D9-A4A0-095F61674861}"/>
+    <hyperlink ref="H13" r:id="rId63" xr:uid="{E9756DE8-6826-41D1-9FFA-8650413C0FFA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId63"/>
+  <pageSetup orientation="portrait" r:id="rId64"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
HF-EMEA: Added testdata and method changes form 01 and 02 testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5898C2AC-FA28-4124-8DCF-F77A8DB6ACCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7AE99C-0F3C-4E8A-A15C-447B05C4A8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1892" uniqueCount="599">
   <si>
     <t>UserName</t>
   </si>
@@ -1854,6 +1854,9 @@
   </si>
   <si>
     <t>99999</t>
+  </si>
+  <si>
+    <t>instagram,tiktok</t>
   </si>
 </sst>
 </file>
@@ -2416,8 +2419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AL37" sqref="AL37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3518,6 +3521,15 @@
       <c r="X32" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="Z32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA32" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB32" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -3599,6 +3611,9 @@
     <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>151</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>598</v>
       </c>
       <c r="AM37" t="s">
         <v>296</v>

</xml_diff>

<commit_message>
TEST_DGLD_HF_EMEA_RT_016_Track_My_Order_For_Guest_User changes as per the prod emea
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA0493E-3B16-4612-B8EE-EFE2DF97F134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AF913B-E310-4B85-B3D3-4B4F324302EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="602">
   <si>
     <t>UserName</t>
   </si>
@@ -1772,9 +1772,6 @@
     <t>English (£), English (€), French (€), German (€), Spanish (€)</t>
   </si>
   <si>
-    <t>Bogi</t>
-  </si>
-  <si>
     <t>skatipelli@helenoftroy.com</t>
   </si>
   <si>
@@ -1866,6 +1863,9 @@
   </si>
   <si>
     <t>https://mcloud-na-preprod.hydroflask.com/gb/hydroflask</t>
+  </si>
+  <si>
+    <t>HFP44000000152</t>
   </si>
 </sst>
 </file>
@@ -2428,8 +2428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AL20" sqref="AL20"/>
+    <sheetView tabSelected="1" topLeftCell="AG23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AI36" activeCellId="1" sqref="AJ27 AI36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2574,7 +2574,7 @@
         <v>165</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>313</v>
@@ -3152,10 +3152,10 @@
         <v>64</v>
       </c>
       <c r="P13" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="Q13" s="5" t="s">
         <v>596</v>
-      </c>
-      <c r="Q13" s="5" t="s">
-        <v>597</v>
       </c>
       <c r="T13" t="s">
         <v>333</v>
@@ -3164,10 +3164,10 @@
         <v>64</v>
       </c>
       <c r="V13" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="W13" s="5" t="s">
         <v>596</v>
-      </c>
-      <c r="W13" s="5" t="s">
-        <v>597</v>
       </c>
       <c r="Z13" s="5" t="s">
         <v>298</v>
@@ -3365,11 +3365,8 @@
       <c r="AD25" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="AH25">
-        <v>3</v>
-      </c>
       <c r="AL25" s="12" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.3">
@@ -3378,11 +3375,8 @@
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="AI26" t="s">
-        <v>480</v>
-      </c>
-      <c r="AJ26" t="s">
-        <v>595</v>
+      <c r="AH26">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.3">
@@ -3403,6 +3397,12 @@
       <c r="AB27">
         <v>123</v>
       </c>
+      <c r="AI27" t="s">
+        <v>480</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="28" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -3553,6 +3553,24 @@
       <c r="G33" t="s">
         <v>15</v>
       </c>
+      <c r="S33" t="s">
+        <v>495</v>
+      </c>
+      <c r="T33" t="s">
+        <v>497</v>
+      </c>
+      <c r="U33" t="s">
+        <v>488</v>
+      </c>
+      <c r="V33" t="s">
+        <v>496</v>
+      </c>
+      <c r="W33" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="X33" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -3625,7 +3643,7 @@
         <v>151</v>
       </c>
       <c r="AL37" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="AM37" t="s">
         <v>296</v>
@@ -3769,7 +3787,7 @@
         <v>341</v>
       </c>
       <c r="P45" s="26" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="Q45" s="5" t="s">
         <v>355</v>
@@ -3819,15 +3837,15 @@
         <v>353</v>
       </c>
       <c r="P49" s="26" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>576</v>
+      </c>
+      <c r="P50" s="26" t="s">
         <v>577</v>
-      </c>
-      <c r="P50" s="26" t="s">
-        <v>578</v>
       </c>
       <c r="S50" t="s">
         <v>495</v>
@@ -3853,10 +3871,10 @@
         <v>201</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>29</v>
@@ -3876,7 +3894,7 @@
         <v>363</v>
       </c>
       <c r="P52" s="26" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.3">
@@ -3958,7 +3976,7 @@
         <v>504</v>
       </c>
       <c r="P58" s="26" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="S58" t="s">
         <v>516</v>
@@ -5717,7 +5735,7 @@
         <v>438</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -5740,7 +5758,7 @@
         <v>521</v>
       </c>
       <c r="G3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
   </sheetData>
@@ -5896,7 +5914,7 @@
         <v>228</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -5957,7 +5975,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
@@ -5985,7 +6003,7 @@
       <c r="H5" s="20"/>
       <c r="I5" s="30"/>
       <c r="J5" s="20" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
@@ -6012,7 +6030,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="M6" s="20"/>
       <c r="N6" s="19" t="s">
@@ -6032,7 +6050,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -6045,7 +6063,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="M7" s="20"/>
       <c r="N7" s="19"/>
@@ -6071,7 +6089,7 @@
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="28" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
@@ -6113,7 +6131,7 @@
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -6338,15 +6356,15 @@
         <v>517</v>
       </c>
       <c r="J21" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
+        <v>583</v>
+      </c>
+      <c r="J22" t="s">
         <v>584</v>
-      </c>
-      <c r="J22" t="s">
-        <v>585</v>
       </c>
     </row>
   </sheetData>
@@ -8469,8 +8487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AS18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AM12" sqref="AM12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9316,14 +9334,14 @@
       <c r="AJ11" s="46">
         <v>43001000060</v>
       </c>
-      <c r="AK11" s="20">
-        <v>3000146837</v>
+      <c r="AK11" s="20" t="s">
+        <v>601</v>
       </c>
       <c r="AL11" s="47" t="s">
-        <v>570</v>
+        <v>15</v>
       </c>
       <c r="AM11" s="12" t="s">
-        <v>507</v>
+        <v>494</v>
       </c>
       <c r="AN11" s="20"/>
       <c r="AO11" s="20"/>
@@ -9768,9 +9786,10 @@
     <hyperlink ref="D15" r:id="rId21" display="mailto:Hydro@123" xr:uid="{19B3239B-92D6-4161-A16C-C292047E6281}"/>
     <hyperlink ref="J17" r:id="rId22" display="mailto:hfemealotus@gmail.com" xr:uid="{E993336E-7B7C-4502-8DC0-8F014C95BA85}"/>
     <hyperlink ref="D2" r:id="rId23" xr:uid="{5E49D6E1-928A-4914-A1E4-323C3D303FB0}"/>
+    <hyperlink ref="AM11" r:id="rId24" xr:uid="{FF940DE7-2AC2-4E6F-8FBE-6E9806A3DD64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -10154,8 +10173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10799,8 +10818,8 @@
       <c r="AA14" s="20" t="s">
         <v>480</v>
       </c>
-      <c r="AB14" s="20" t="s">
-        <v>264</v>
+      <c r="AB14" t="s">
+        <v>594</v>
       </c>
       <c r="AC14" s="20"/>
       <c r="AD14" s="20"/>
@@ -11636,7 +11655,7 @@
         <v>246</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -11667,7 +11686,7 @@
         <v>243</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C2" s="20"/>
     </row>
@@ -11677,10 +11696,10 @@
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="20" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
@@ -11698,7 +11717,7 @@
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HF-EMEA : url_color_validation product added to testcada
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64F06ED-1C04-4E25-A3FA-073DA076CBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9881551E-8367-41C1-AFA5-2AAA9347F143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="603">
   <si>
     <t>UserName</t>
   </si>
@@ -1866,6 +1866,9 @@
   </si>
   <si>
     <t>HFP44000000152</t>
+  </si>
+  <si>
+    <t>Micro Hydro Mini Bottle</t>
   </si>
 </sst>
 </file>
@@ -2418,7 +2421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
@@ -3275,8 +3278,8 @@
         <v>545</v>
       </c>
       <c r="AD20" s="32"/>
-      <c r="AE20" s="42" t="s">
-        <v>545</v>
+      <c r="AE20" s="22" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="21" spans="1:49" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
PLP changes for Hydroflask EMEA
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA30C51-07C3-4A15-A70A-1182D29AEFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB9BE89-1078-4E87-99F2-546EAD818009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="607">
   <si>
     <t>UserName</t>
   </si>
@@ -2433,8 +2433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AF9" sqref="AF9"/>
+    <sheetView tabSelected="1" topLeftCell="AF25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AI36" sqref="AI36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3701,6 +3701,15 @@
       <c r="X39" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="AM39" t="s">
+        <v>296</v>
+      </c>
+      <c r="AN39" t="s">
+        <v>314</v>
+      </c>
+      <c r="AO39" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -3964,6 +3973,12 @@
         <v>1</v>
       </c>
       <c r="AE56" s="33"/>
+      <c r="AU56" t="s">
+        <v>520</v>
+      </c>
+      <c r="AV56" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A57" s="33" t="s">
@@ -4005,17 +4020,18 @@
         <v>516</v>
       </c>
     </row>
-    <row r="60" spans="1:48" ht="60" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:48" ht="30" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>515</v>
       </c>
-      <c r="AC60" s="42" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="61" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AC60" s="42"/>
+    </row>
+    <row r="61" spans="1:48" ht="60" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>518</v>
+      </c>
+      <c r="AC61" s="42" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="62" spans="1:48" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
HF-EMEA: Code correction for 066 and 040 testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB9BE89-1078-4E87-99F2-546EAD818009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9897B74A-1146-4BD9-A77D-EE2483A4506C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28800" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="608">
   <si>
     <t>UserName</t>
   </si>
@@ -1881,6 +1881,9 @@
   </si>
   <si>
     <t>Agave</t>
+  </si>
+  <si>
+    <t>Gift card for Hydroflask-EMEA</t>
   </si>
 </sst>
 </file>
@@ -2433,34 +2436,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AI36" sqref="AI36"/>
+    <sheetView tabSelected="1" topLeftCell="J20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R47" sqref="R47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="18" width="30.5546875" customWidth="1"/>
-    <col min="19" max="19" width="19.6640625" customWidth="1"/>
-    <col min="20" max="21" width="22.33203125" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" customWidth="1"/>
-    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="18" width="30.5703125" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1"/>
+    <col min="20" max="21" width="22.28515625" customWidth="1"/>
+    <col min="22" max="22" width="14.7109375" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.33203125" customWidth="1"/>
+    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2609,7 +2612,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2667,7 +2670,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -2725,7 +2728,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:49" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>508</v>
       </c>
@@ -2780,7 +2783,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -2822,7 +2825,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>437</v>
       </c>
@@ -2880,7 +2883,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>527</v>
       </c>
@@ -2935,7 +2938,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="7"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>532</v>
       </c>
@@ -2992,7 +2995,7 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>534</v>
       </c>
@@ -3049,7 +3052,7 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="1:49" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:49" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>538</v>
       </c>
@@ -3106,7 +3109,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3124,7 +3127,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>199</v>
       </c>
@@ -3136,7 +3139,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -3184,7 +3187,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>297</v>
       </c>
@@ -3193,7 +3196,7 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="7"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -3208,7 +3211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -3219,7 +3222,7 @@
       <c r="X16" s="4"/>
       <c r="AD16" s="32"/>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>526</v>
       </c>
@@ -3241,7 +3244,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -3254,7 +3257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>170</v>
       </c>
@@ -3280,7 +3283,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="20" spans="1:49" ht="60" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:49" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -3297,7 +3300,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="21" spans="1:49" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>604</v>
       </c>
@@ -3312,7 +3315,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>442</v>
       </c>
@@ -3331,7 +3334,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>176</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>175</v>
       </c>
@@ -3355,7 +3358,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>189</v>
       </c>
@@ -3365,7 +3368,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -3392,7 +3395,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -3402,7 +3405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -3427,7 +3430,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -3456,7 +3459,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -3478,7 +3481,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -3513,7 +3516,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -3534,7 +3537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -3566,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -3595,7 +3598,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -3616,7 +3619,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -3647,7 +3650,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -3661,7 +3664,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -3678,7 +3681,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>164</v>
       </c>
@@ -3711,7 +3714,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>166</v>
       </c>
@@ -3737,7 +3740,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>184</v>
       </c>
@@ -3749,7 +3752,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>279</v>
       </c>
@@ -3757,7 +3760,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>284</v>
       </c>
@@ -3780,7 +3783,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>215</v>
       </c>
@@ -3797,13 +3800,13 @@
         <v>214</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>209</v>
       </c>
       <c r="R45" s="5"/>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>339</v>
       </c>
@@ -3828,12 +3831,15 @@
         <v>345</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="R47" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>346</v>
       </c>
@@ -3850,7 +3856,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>348</v>
       </c>
@@ -3863,8 +3869,11 @@
       <c r="H49" s="12" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AP49" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="50" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>353</v>
       </c>
@@ -3872,7 +3881,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>576</v>
       </c>
@@ -3898,7 +3907,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>201</v>
       </c>
@@ -3921,7 +3930,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>363</v>
       </c>
@@ -3929,7 +3938,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>431</v>
       </c>
@@ -3937,7 +3946,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>432</v>
       </c>
@@ -3951,7 +3960,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>232</v>
       </c>
@@ -3980,7 +3989,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="57" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
         <v>153</v>
       </c>
@@ -4001,7 +4010,7 @@
       <c r="P57" s="33"/>
       <c r="Q57" s="33"/>
     </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>446</v>
       </c>
@@ -4009,7 +4018,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>504</v>
       </c>
@@ -4020,13 +4029,13 @@
         <v>516</v>
       </c>
     </row>
-    <row r="60" spans="1:48" ht="30" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>515</v>
       </c>
       <c r="AC60" s="42"/>
     </row>
-    <row r="61" spans="1:48" ht="60" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:48" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>518</v>
       </c>
@@ -4034,7 +4043,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="62" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>522</v>
       </c>
@@ -4122,37 +4131,37 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4235,7 +4244,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4276,7 +4285,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4292,7 +4301,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -4304,7 +4313,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4322,7 +4331,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4331,7 +4340,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -4343,7 +4352,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -4369,7 +4378,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -4380,7 +4389,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -4394,7 +4403,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -4441,18 +4450,18 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4550,7 +4559,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4597,7 +4606,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4647,7 +4656,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -4694,7 +4703,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4710,7 +4719,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -4722,7 +4731,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -4733,7 +4742,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4755,7 +4764,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -4768,7 +4777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -4784,7 +4793,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4798,7 +4807,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -4814,7 +4823,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -4828,7 +4837,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -4870,7 +4879,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -4896,7 +4905,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -4907,7 +4916,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4922,7 +4931,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -4980,12 +4989,12 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5056,7 +5065,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5103,7 +5112,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -5119,7 +5128,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -5150,7 +5159,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -5158,7 +5167,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -5191,20 +5200,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.33203125" customWidth="1"/>
-    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.28515625" customWidth="1"/>
+    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5293,7 +5302,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5341,7 +5350,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -5357,7 +5366,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -5377,7 +5386,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -5396,7 +5405,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -5415,7 +5424,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -5423,7 +5432,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -5431,7 +5440,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -5448,7 +5457,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -5465,7 +5474,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -5482,7 +5491,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -5499,7 +5508,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -5510,7 +5519,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -5521,7 +5530,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -5538,7 +5547,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -5567,7 +5576,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -5578,7 +5587,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -5592,7 +5601,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -5606,7 +5615,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -5620,7 +5629,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -5628,7 +5637,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -5658,7 +5667,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -5728,19 +5737,19 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.6640625" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5766,7 +5775,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5789,7 +5798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -5820,16 +5829,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5843,7 +5852,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -5869,27 +5878,27 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5546875" customWidth="1"/>
-    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5703125" customWidth="1"/>
+    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.109375" customWidth="1"/>
+    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.140625" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -5948,7 +5957,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>228</v>
       </c>
@@ -5973,7 +5982,7 @@
       <c r="R2" s="20"/>
       <c r="S2" s="20"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>230</v>
       </c>
@@ -6002,7 +6011,7 @@
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>232</v>
       </c>
@@ -6027,7 +6036,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>233</v>
       </c>
@@ -6054,7 +6063,7 @@
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>236</v>
       </c>
@@ -6087,7 +6096,7 @@
       <c r="R6" s="20"/>
       <c r="S6" s="20"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>587</v>
       </c>
@@ -6112,7 +6121,7 @@
       <c r="R7" s="20"/>
       <c r="S7" s="20"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>238</v>
       </c>
@@ -6137,7 +6146,7 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>262</v>
       </c>
@@ -6162,7 +6171,7 @@
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>281</v>
       </c>
@@ -6187,7 +6196,7 @@
       <c r="R10" s="20"/>
       <c r="S10" s="20"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>286</v>
       </c>
@@ -6214,7 +6223,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>318</v>
       </c>
@@ -6239,7 +6248,7 @@
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
     </row>
-    <row r="13" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>320</v>
       </c>
@@ -6266,7 +6275,7 @@
       <c r="R13" s="20"/>
       <c r="S13" s="20"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>321</v>
       </c>
@@ -6291,7 +6300,7 @@
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>323</v>
       </c>
@@ -6316,7 +6325,7 @@
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>334</v>
       </c>
@@ -6341,7 +6350,7 @@
       <c r="R16" s="20"/>
       <c r="S16" s="20"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>337</v>
       </c>
@@ -6366,7 +6375,7 @@
       <c r="R17" s="20"/>
       <c r="S17" s="20"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>448</v>
       </c>
@@ -6374,7 +6383,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>449</v>
       </c>
@@ -6382,7 +6391,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>450</v>
       </c>
@@ -6390,7 +6399,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>517</v>
       </c>
@@ -6398,7 +6407,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>583</v>
       </c>
@@ -6420,13 +6429,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -6464,7 +6473,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>568</v>
       </c>
@@ -6482,27 +6491,27 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="H4" s="9"/>
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H5" s="12"/>
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
       <c r="V5" s="5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H6" s="5"/>
     </row>
   </sheetData>
@@ -6519,31 +6528,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.6640625" customWidth="1"/>
-    <col min="17" max="24" width="30.5546875" customWidth="1"/>
-    <col min="25" max="25" width="19.6640625" customWidth="1"/>
-    <col min="26" max="27" width="22.33203125" customWidth="1"/>
-    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.7109375" customWidth="1"/>
+    <col min="17" max="24" width="30.5703125" customWidth="1"/>
+    <col min="25" max="25" width="19.7109375" customWidth="1"/>
+    <col min="26" max="27" width="22.28515625" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.33203125" customWidth="1"/>
+    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -6695,7 +6704,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6765,7 +6774,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>453</v>
       </c>
@@ -6835,7 +6844,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>455</v>
       </c>
@@ -6905,7 +6914,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>456</v>
       </c>
@@ -6975,7 +6984,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>459</v>
       </c>
@@ -7045,7 +7054,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>463</v>
       </c>
@@ -7115,7 +7124,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>466</v>
       </c>
@@ -7156,7 +7165,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>467</v>
       </c>
@@ -7197,7 +7206,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>461</v>
       </c>
@@ -7267,7 +7276,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>406</v>
       </c>
@@ -7328,7 +7337,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -7387,7 +7396,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>359</v>
       </c>
@@ -7433,7 +7442,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -7456,7 +7465,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>297</v>
       </c>
@@ -7479,7 +7488,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -7498,7 +7507,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -7509,7 +7518,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -7531,7 +7540,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>366</v>
       </c>
@@ -7544,7 +7553,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>368</v>
       </c>
@@ -7557,7 +7566,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -7570,7 +7579,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>375</v>
       </c>
@@ -7583,7 +7592,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>397</v>
       </c>
@@ -7596,7 +7605,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>376</v>
       </c>
@@ -7609,7 +7618,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -7625,7 +7634,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -7641,7 +7650,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>401</v>
       </c>
@@ -7660,7 +7669,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>405</v>
       </c>
@@ -7679,7 +7688,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>382</v>
       </c>
@@ -7695,7 +7704,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>385</v>
       </c>
@@ -7711,7 +7720,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>411</v>
       </c>
@@ -7727,7 +7736,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>412</v>
       </c>
@@ -7743,7 +7752,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>386</v>
       </c>
@@ -7759,7 +7768,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>389</v>
       </c>
@@ -7772,7 +7781,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>403</v>
       </c>
@@ -7785,7 +7794,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -7798,7 +7807,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>424</v>
       </c>
@@ -7811,7 +7820,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>398</v>
       </c>
@@ -7824,7 +7833,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>394</v>
       </c>
@@ -7840,7 +7849,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>423</v>
       </c>
@@ -7856,7 +7865,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -7872,7 +7881,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>402</v>
       </c>
@@ -7885,7 +7894,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>415</v>
       </c>
@@ -7907,7 +7916,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -7925,7 +7934,7 @@
       <c r="AI44" s="25"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>414</v>
       </c>
@@ -7938,7 +7947,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -7958,7 +7967,7 @@
       <c r="AI46" s="25"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -7977,7 +7986,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -7990,7 +7999,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -8001,7 +8010,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -8014,7 +8023,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -8037,7 +8046,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -8051,7 +8060,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -8088,7 +8097,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -8102,7 +8111,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -8144,7 +8153,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -8170,7 +8179,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -8194,7 +8203,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -8218,7 +8227,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -8244,7 +8253,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -8276,7 +8285,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -8290,7 +8299,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>373</v>
       </c>
@@ -8304,7 +8313,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -8321,7 +8330,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -8338,7 +8347,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>339</v>
       </c>
@@ -8360,7 +8369,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>343</v>
       </c>
@@ -8368,7 +8377,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>346</v>
       </c>
@@ -8379,7 +8388,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>348</v>
       </c>
@@ -8396,7 +8405,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>353</v>
       </c>
@@ -8404,7 +8413,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -8439,7 +8448,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>363</v>
       </c>
@@ -8530,37 +8539,37 @@
       <selection activeCell="AM12" sqref="AM12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -8697,7 +8706,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -8772,7 +8781,7 @@
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
@@ -8829,7 +8838,7 @@
       <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>248</v>
       </c>
@@ -8882,7 +8891,7 @@
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>68</v>
       </c>
@@ -8945,7 +8954,7 @@
       <c r="AR5" s="20"/>
       <c r="AS5" s="20"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>75</v>
       </c>
@@ -9024,7 +9033,7 @@
       <c r="AR6" s="20"/>
       <c r="AS6" s="20"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>81</v>
       </c>
@@ -9113,7 +9122,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>100</v>
       </c>
@@ -9196,7 +9205,7 @@
       <c r="AR8" s="20"/>
       <c r="AS8" s="20"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>95</v>
       </c>
@@ -9281,7 +9290,7 @@
       <c r="AR9" s="20"/>
       <c r="AS9" s="20"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -9332,7 +9341,7 @@
       <c r="AR10" s="20"/>
       <c r="AS10" s="20"/>
     </row>
-    <row r="11" spans="1:45" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>103</v>
       </c>
@@ -9389,7 +9398,7 @@
       <c r="AR11" s="20"/>
       <c r="AS11" s="20"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>107</v>
       </c>
@@ -9464,7 +9473,7 @@
       <c r="AR12" s="20"/>
       <c r="AS12" s="20"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>112</v>
       </c>
@@ -9527,7 +9536,7 @@
       <c r="AR13" s="20"/>
       <c r="AS13" s="20"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>249</v>
       </c>
@@ -9582,7 +9591,7 @@
       <c r="AR14" s="20"/>
       <c r="AS14" s="20"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>119</v>
       </c>
@@ -9639,7 +9648,7 @@
       <c r="AR15" s="20"/>
       <c r="AS15" s="20"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>121</v>
       </c>
@@ -9694,7 +9703,7 @@
       <c r="AR16" s="20"/>
       <c r="AS16" s="20"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>219</v>
       </c>
@@ -9749,7 +9758,7 @@
       <c r="AR17" s="20"/>
       <c r="AS17" s="20"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>154</v>
       </c>
@@ -9840,13 +9849,13 @@
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9923,7 +9932,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -9953,25 +9962,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.44140625" customWidth="1"/>
-    <col min="32" max="32" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.42578125" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10072,7 +10081,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -10158,7 +10167,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -10190,7 +10199,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -10216,27 +10225,27 @@
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.44140625" customWidth="1"/>
-    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -10331,7 +10340,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -10392,7 +10401,7 @@
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>20</v>
       </c>
@@ -10433,7 +10442,7 @@
       <c r="AD3" s="20"/>
       <c r="AE3" s="20"/>
     </row>
-    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>25</v>
       </c>
@@ -10476,7 +10485,7 @@
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>178</v>
       </c>
@@ -10515,7 +10524,7 @@
       <c r="AD5" s="20"/>
       <c r="AE5" s="20"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>179</v>
       </c>
@@ -10554,7 +10563,7 @@
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>153</v>
       </c>
@@ -10593,7 +10602,7 @@
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>155</v>
       </c>
@@ -10630,7 +10639,7 @@
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>154</v>
       </c>
@@ -10667,7 +10676,7 @@
       <c r="AD9" s="20"/>
       <c r="AE9" s="20"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>168</v>
       </c>
@@ -10704,7 +10713,7 @@
       <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>172</v>
       </c>
@@ -10747,7 +10756,7 @@
       <c r="AD11" s="20"/>
       <c r="AE11" s="20"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>170</v>
       </c>
@@ -10786,7 +10795,7 @@
       <c r="AD12" s="20"/>
       <c r="AE12" s="20"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>77</v>
       </c>
@@ -10825,7 +10834,7 @@
       <c r="AD13" s="20"/>
       <c r="AE13" s="20"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>43</v>
       </c>
@@ -10864,7 +10873,7 @@
       <c r="AD14" s="20"/>
       <c r="AE14" s="20"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>118</v>
       </c>
@@ -10913,7 +10922,7 @@
       <c r="AD15" s="20"/>
       <c r="AE15" s="20"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
@@ -10954,7 +10963,7 @@
       <c r="AD16" s="20"/>
       <c r="AE16" s="20"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>46</v>
       </c>
@@ -10995,7 +11004,7 @@
       <c r="AD17" s="20"/>
       <c r="AE17" s="20"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>201</v>
       </c>
@@ -11050,7 +11059,7 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="20"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>241</v>
       </c>
@@ -11087,7 +11096,7 @@
       <c r="AD19" s="20"/>
       <c r="AE19" s="20"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>187</v>
       </c>
@@ -11134,7 +11143,7 @@
       <c r="AD20" s="20"/>
       <c r="AE20" s="20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>166</v>
       </c>
@@ -11181,7 +11190,7 @@
       <c r="AD21" s="20"/>
       <c r="AE21" s="20"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>343</v>
       </c>
@@ -11218,7 +11227,7 @@
       <c r="AD22" s="20"/>
       <c r="AE22" s="20"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>346</v>
       </c>
@@ -11255,7 +11264,7 @@
       <c r="AD23" s="20"/>
       <c r="AE23" s="20"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>348</v>
       </c>
@@ -11300,7 +11309,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
@@ -11335,7 +11344,7 @@
       <c r="AD25" s="20"/>
       <c r="AE25" s="20"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>527</v>
       </c>
@@ -11380,7 +11389,7 @@
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>532</v>
       </c>
@@ -11425,7 +11434,7 @@
       </c>
       <c r="P27" s="40"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>534</v>
       </c>
@@ -11470,7 +11479,7 @@
       </c>
       <c r="P28" s="40"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>538</v>
       </c>
@@ -11515,7 +11524,7 @@
       </c>
       <c r="P29" s="40"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>554</v>
       </c>
@@ -11541,7 +11550,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>555</v>
       </c>
@@ -11567,7 +11576,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>557</v>
       </c>
@@ -11593,7 +11602,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>566</v>
       </c>
@@ -11673,17 +11682,17 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -11720,7 +11729,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>243</v>
       </c>
@@ -11729,7 +11738,7 @@
       </c>
       <c r="C2" s="20"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>245</v>
       </c>
@@ -11741,7 +11750,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>247</v>
       </c>
@@ -11750,7 +11759,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>312</v>
       </c>
@@ -11772,20 +11781,20 @@
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -11853,7 +11862,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11897,7 +11906,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -11913,7 +11922,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -11931,7 +11940,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -11939,7 +11948,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -11947,7 +11956,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
Changed the email format for the Hydroflask EMEA Stores
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9897B74A-1146-4BD9-A77D-EE2483A4506C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4270199-2FC2-47ED-B784-331BFD568E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28800" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1562,9 +1562,6 @@
 https://mcloud-na-stage4.hydroflask.com/prodeal/application/index/</t>
   </si>
   <si>
-    <t>Hfemeanewaccount@gmail.com</t>
-  </si>
-  <si>
     <t>£25.00</t>
   </si>
   <si>
@@ -1884,6 +1881,9 @@
   </si>
   <si>
     <t>Gift card for Hydroflask-EMEA</t>
+  </si>
+  <si>
+    <t>Hfemeanewaccount+@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2436,34 +2436,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="21" width="22.28515625" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="18" width="30.5546875" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="21" width="22.33203125" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.28515625" customWidth="1"/>
+    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>165</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>313</v>
@@ -2603,7 +2603,7 @@
         <v>207</v>
       </c>
       <c r="AU1" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>435</v>
@@ -2612,7 +2612,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2650,16 +2650,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" t="s">
+        <v>511</v>
+      </c>
+      <c r="T2" t="s">
+        <v>509</v>
+      </c>
+      <c r="V2" t="s">
         <v>512</v>
       </c>
-      <c r="T2" t="s">
-        <v>510</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="W2" s="5" t="s">
         <v>513</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>514</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>59</v>
@@ -2670,15 +2670,15 @@
         <v>493</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>294</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2693,10 +2693,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -2728,9 +2728,9 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:49" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>494</v>
@@ -2766,16 +2766,16 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="15" t="s">
+        <v>508</v>
+      </c>
+      <c r="T4" t="s">
         <v>509</v>
-      </c>
-      <c r="T4" t="s">
-        <v>510</v>
       </c>
       <c r="V4" t="s">
         <v>484</v>
       </c>
       <c r="W4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>59</v>
@@ -2783,15 +2783,15 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>359</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -2806,10 +2806,10 @@
         <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2825,7 +2825,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>437</v>
       </c>
@@ -2883,9 +2883,9 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>494</v>
@@ -2921,16 +2921,16 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" t="s">
+        <v>527</v>
+      </c>
+      <c r="T7" t="s">
         <v>528</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>529</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" s="5" t="s">
         <v>530</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>531</v>
       </c>
       <c r="X7" s="5" t="s">
         <v>59</v>
@@ -2938,9 +2938,9 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="7"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>494</v>
@@ -2976,17 +2976,17 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="20" t="s">
+        <v>527</v>
+      </c>
+      <c r="T8" s="20" t="s">
         <v>528</v>
-      </c>
-      <c r="T8" s="20" t="s">
-        <v>529</v>
       </c>
       <c r="U8" s="20"/>
       <c r="V8" s="41" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="W8" s="40" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="X8" s="40" t="s">
         <v>59</v>
@@ -2995,9 +2995,9 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>494</v>
@@ -3033,17 +3033,17 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="20" t="s">
+        <v>534</v>
+      </c>
+      <c r="T9" s="40" t="s">
         <v>535</v>
-      </c>
-      <c r="T9" s="40" t="s">
-        <v>536</v>
       </c>
       <c r="U9" s="20"/>
       <c r="V9" s="41" t="s">
+        <v>535</v>
+      </c>
+      <c r="W9" s="40" t="s">
         <v>536</v>
-      </c>
-      <c r="W9" s="40" t="s">
-        <v>537</v>
       </c>
       <c r="X9" s="40" t="s">
         <v>59</v>
@@ -3052,9 +3052,9 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="1:49" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>494</v>
@@ -3090,17 +3090,17 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="20" t="s">
+        <v>538</v>
+      </c>
+      <c r="T10" s="40" t="s">
         <v>539</v>
-      </c>
-      <c r="T10" s="40" t="s">
-        <v>540</v>
       </c>
       <c r="U10" s="20"/>
       <c r="V10" s="41" t="s">
+        <v>540</v>
+      </c>
+      <c r="W10" s="40" t="s">
         <v>541</v>
-      </c>
-      <c r="W10" s="40" t="s">
-        <v>542</v>
       </c>
       <c r="X10" s="40">
         <v>9898989898</v>
@@ -3109,7 +3109,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>199</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -3160,10 +3160,10 @@
         <v>64</v>
       </c>
       <c r="P13" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="Q13" s="5" t="s">
         <v>595</v>
-      </c>
-      <c r="Q13" s="5" t="s">
-        <v>596</v>
       </c>
       <c r="T13" t="s">
         <v>333</v>
@@ -3172,10 +3172,10 @@
         <v>64</v>
       </c>
       <c r="V13" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="W13" s="5" t="s">
         <v>595</v>
-      </c>
-      <c r="W13" s="5" t="s">
-        <v>596</v>
       </c>
       <c r="Z13" s="5" t="s">
         <v>298</v>
@@ -3187,7 +3187,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>297</v>
       </c>
@@ -3196,7 +3196,7 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="7"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -3222,9 +3222,9 @@
       <c r="X16" s="4"/>
       <c r="AD16" s="32"/>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J17" s="18" t="s">
         <v>481</v>
@@ -3244,7 +3244,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -3257,21 +3257,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>170</v>
       </c>
       <c r="AC19" s="12" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="AD19" s="32">
         <v>1</v>
       </c>
       <c r="AE19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="AF19" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="AG19" t="s">
         <v>190</v>
@@ -3283,39 +3283,39 @@
         <v>357</v>
       </c>
     </row>
-    <row r="20" spans="1:49" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" ht="60" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="AC20" s="42" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AD20" s="32"/>
       <c r="AE20" s="22" t="s">
+        <v>601</v>
+      </c>
+      <c r="AF20" t="s">
         <v>602</v>
       </c>
-      <c r="AF20" t="s">
+    </row>
+    <row r="21" spans="1:49" ht="30" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>603</v>
-      </c>
-    </row>
-    <row r="21" spans="1:49" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>604</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="AC21" s="42"/>
       <c r="AD21" s="32"/>
       <c r="AE21" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="AF21" t="s">
         <v>605</v>
       </c>
-      <c r="AF21" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>442</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>176</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>175</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>189</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -3392,10 +3392,10 @@
         <v>113</v>
       </c>
       <c r="AL26" s="12" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="27" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -3427,10 +3427,10 @@
         <v>480</v>
       </c>
       <c r="AJ28" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="29" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -3609,17 +3609,17 @@
         <v>69</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="W35" s="5"/>
       <c r="X35" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -3664,12 +3664,12 @@
         <v>436</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>151</v>
       </c>
       <c r="AL38" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="AM38" t="s">
         <v>296</v>
@@ -3681,7 +3681,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>164</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>166</v>
       </c>
@@ -3740,19 +3740,19 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>184</v>
       </c>
       <c r="H41" s="23" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="I41" s="12"/>
       <c r="AP41" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>279</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>284</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>215</v>
       </c>
@@ -3800,13 +3800,13 @@
         <v>214</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>209</v>
       </c>
       <c r="R45" s="5"/>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>339</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>341</v>
       </c>
       <c r="P46" s="26" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="Q46" s="5" t="s">
         <v>355</v>
@@ -3831,7 +3831,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>343</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>346</v>
       </c>
@@ -3847,16 +3847,16 @@
         <v>429</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="N48" s="24" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AP48" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>348</v>
       </c>
@@ -3867,26 +3867,26 @@
         <v>349</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="AP49" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.25">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="50" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>353</v>
       </c>
       <c r="P50" s="26" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="51" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>575</v>
+      </c>
+      <c r="P51" s="26" t="s">
         <v>576</v>
-      </c>
-      <c r="P51" s="26" t="s">
-        <v>577</v>
       </c>
       <c r="S51" t="s">
         <v>495</v>
@@ -3907,15 +3907,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>201</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>29</v>
@@ -3930,15 +3930,15 @@
         <v>305</v>
       </c>
     </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>363</v>
       </c>
       <c r="P53" s="26" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="54" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>431</v>
       </c>
@@ -3946,21 +3946,21 @@
         <v>433</v>
       </c>
     </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>432</v>
       </c>
       <c r="P55" s="26" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="AU55" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AV55" s="31" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>232</v>
       </c>
@@ -3983,13 +3983,13 @@
       </c>
       <c r="AE56" s="33"/>
       <c r="AU56" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AV56" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="57" spans="1:48" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="57" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A57" s="33" t="s">
         <v>153</v>
       </c>
@@ -4010,45 +4010,45 @@
       <c r="P57" s="33"/>
       <c r="Q57" s="33"/>
     </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>446</v>
       </c>
       <c r="P58" s="26" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.25">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="59" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="P59" s="26" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="S59" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="60" spans="1:48" ht="30" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="60" spans="1:48" ht="30" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AC60" s="42"/>
     </row>
-    <row r="61" spans="1:48" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:48" ht="60" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AC61" s="42" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="62" spans="1:48" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="62" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P62" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -4061,7 +4061,7 @@
     <hyperlink ref="AL25" r:id="rId6" xr:uid="{C3ED735C-0638-4013-B1A9-35D874D27CCD}"/>
     <hyperlink ref="H40" r:id="rId7" xr:uid="{7B92FAF6-FC7B-4378-BAA5-F455D3557016}"/>
     <hyperlink ref="D2" r:id="rId8" xr:uid="{6D9C84C2-080E-49A8-91A9-0C4040F17B99}"/>
-    <hyperlink ref="H41" r:id="rId9" xr:uid="{5EDA0D22-59C6-4E86-B1C8-F3DDADDA222C}"/>
+    <hyperlink ref="H41" r:id="rId9" display="Hfemeanewaccount@gmail.com" xr:uid="{5EDA0D22-59C6-4E86-B1C8-F3DDADDA222C}"/>
     <hyperlink ref="B2" r:id="rId10" xr:uid="{49EA4C67-65EF-4ECE-B592-DD27DDBFE9D8}"/>
     <hyperlink ref="I2" r:id="rId11" xr:uid="{41758504-FDAA-49B8-A517-3CF2E58C91CC}"/>
     <hyperlink ref="C2" r:id="rId12" xr:uid="{12FE48FE-6D5F-46FF-BB71-C2756AE73EE8}"/>
@@ -4078,21 +4078,21 @@
     <hyperlink ref="H6" r:id="rId23" xr:uid="{407C8F4E-9B49-4856-B5B1-AADA1B530463}"/>
     <hyperlink ref="D35" r:id="rId24" xr:uid="{CFA846D7-1044-49EA-A0C9-5358EDB0782D}"/>
     <hyperlink ref="B3" r:id="rId25" xr:uid="{A4EF70F2-1E9D-4209-9990-D57B7B04D033}"/>
-    <hyperlink ref="C3" r:id="rId26" xr:uid="{A02552C8-A6E5-4D41-80F6-00B2ABF9087C}"/>
-    <hyperlink ref="H3" r:id="rId27" xr:uid="{475B0B91-5BB6-4DC1-8A14-637459A21F69}"/>
-    <hyperlink ref="I3" r:id="rId28" xr:uid="{31D5282C-3A0B-47FC-A07B-CC23BA4F574E}"/>
+    <hyperlink ref="C3" r:id="rId26" display="Hfemeanewaccount@gmail.com" xr:uid="{A02552C8-A6E5-4D41-80F6-00B2ABF9087C}"/>
+    <hyperlink ref="H3" r:id="rId27" display="Hfemeanewaccount@gmail.com" xr:uid="{475B0B91-5BB6-4DC1-8A14-637459A21F69}"/>
+    <hyperlink ref="I3" r:id="rId28" display="Hfemeanewaccount@gmail.com" xr:uid="{31D5282C-3A0B-47FC-A07B-CC23BA4F574E}"/>
     <hyperlink ref="H4" r:id="rId29" xr:uid="{D910C898-EA43-409E-B04E-9B9BFB5A3D9D}"/>
     <hyperlink ref="E4" r:id="rId30" xr:uid="{B86A9B6C-A653-4B11-A92A-B12ECCF56B54}"/>
     <hyperlink ref="D4" r:id="rId31" xr:uid="{5357CB07-F4C9-42F8-8AA6-82DE7438DA1F}"/>
     <hyperlink ref="B4" r:id="rId32" xr:uid="{6B5AE7EC-0874-471E-8B2A-119BB6055DFF}"/>
     <hyperlink ref="I4" r:id="rId33" xr:uid="{C425EF67-01D4-42EC-8E86-0A6DFDCBD4BA}"/>
     <hyperlink ref="C4" r:id="rId34" xr:uid="{50F1E974-01BC-40BB-A015-3C5D601540DD}"/>
-    <hyperlink ref="B5" r:id="rId35" xr:uid="{0A429E56-7D42-4B18-B613-96996A8386C4}"/>
-    <hyperlink ref="C5" r:id="rId36" xr:uid="{817C7CDF-7723-4347-999A-B70D0C4C4C9F}"/>
-    <hyperlink ref="H5" r:id="rId37" xr:uid="{46997A70-4DF6-42DF-98DE-3A15FE00FF24}"/>
-    <hyperlink ref="I5" r:id="rId38" xr:uid="{323D0279-E435-4C6C-805F-A066B3FCDA92}"/>
-    <hyperlink ref="H35" r:id="rId39" xr:uid="{EDD9788C-AEBE-4F86-8A6C-8043A32B81A6}"/>
-    <hyperlink ref="I35" r:id="rId40" xr:uid="{68882096-6651-4D29-9355-6F1410B100AA}"/>
+    <hyperlink ref="B5" r:id="rId35" display="Hfemeanewaccount@gmail.com" xr:uid="{0A429E56-7D42-4B18-B613-96996A8386C4}"/>
+    <hyperlink ref="C5" r:id="rId36" display="Hfemeanewaccount@gmail.com" xr:uid="{817C7CDF-7723-4347-999A-B70D0C4C4C9F}"/>
+    <hyperlink ref="H5" r:id="rId37" display="Hfemeanewaccount@gmail.com" xr:uid="{46997A70-4DF6-42DF-98DE-3A15FE00FF24}"/>
+    <hyperlink ref="I5" r:id="rId38" display="Hfemeanewaccount@gmail.com" xr:uid="{323D0279-E435-4C6C-805F-A066B3FCDA92}"/>
+    <hyperlink ref="H35" r:id="rId39" display="Hfemeanewaccount@gmail.com" xr:uid="{EDD9788C-AEBE-4F86-8A6C-8043A32B81A6}"/>
+    <hyperlink ref="I35" r:id="rId40" display="Hfemeanewaccount@gmail.com" xr:uid="{68882096-6651-4D29-9355-6F1410B100AA}"/>
     <hyperlink ref="H8" r:id="rId41" xr:uid="{867EC1A7-B881-422A-8354-C1C7FCE40AAE}"/>
     <hyperlink ref="E8" r:id="rId42" xr:uid="{5ACEF6FA-BF68-4BBD-BE65-3578FCD63C44}"/>
     <hyperlink ref="D8" r:id="rId43" xr:uid="{3607587D-2F3E-4312-8C6F-F1EF148F7A1A}"/>
@@ -4128,40 +4128,40 @@
   <dimension ref="A1:AA11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4244,12 +4244,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>29</v>
@@ -4285,7 +4285,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -4313,7 +4313,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -4403,7 +4403,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -4435,8 +4435,7 @@
     <hyperlink ref="D2" r:id="rId2" xr:uid="{F667B6EF-2843-441F-ADF3-A9F03FB2D127}"/>
     <hyperlink ref="D9" r:id="rId3" xr:uid="{BA37854D-B94D-4462-95C3-1F9ADFCD61FB}"/>
     <hyperlink ref="G10" r:id="rId4" xr:uid="{97AA2188-E825-4E95-BD32-7DE2E0872BDB}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{65D4744A-1A3C-492E-95BF-8C9052BD2013}"/>
-    <hyperlink ref="C2" r:id="rId6" xr:uid="{15735CF8-DBB0-492B-A615-DCBD78A638E3}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{15735CF8-DBB0-492B-A615-DCBD78A638E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4447,21 +4446,21 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4559,15 +4558,15 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -4582,10 +4581,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
@@ -4606,15 +4605,15 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>29</v>
@@ -4629,10 +4628,10 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s">
@@ -4656,15 +4655,15 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>194</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -4679,10 +4678,10 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" t="s">
@@ -4703,7 +4702,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4719,7 +4718,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -4731,7 +4730,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -4742,7 +4741,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4764,7 +4763,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -4777,7 +4776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -4793,7 +4792,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4807,7 +4806,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -4823,7 +4822,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -4837,7 +4836,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -4845,7 +4844,7 @@
         <v>50</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="I14" s="2"/>
       <c r="K14" t="s">
@@ -4879,7 +4878,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -4905,7 +4904,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -4916,7 +4915,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4931,7 +4930,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -4959,23 +4958,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{509FD8C7-2668-4F8A-8FCA-72E4C3F520AD}"/>
+    <hyperlink ref="H2" r:id="rId1" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{509FD8C7-2668-4F8A-8FCA-72E4C3F520AD}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{DBDB132B-EE23-4863-9A01-1CB94AE8210A}"/>
-    <hyperlink ref="H14" r:id="rId3" xr:uid="{7F08651C-07CE-4F9D-9DB6-E721F8008E52}"/>
+    <hyperlink ref="H14" r:id="rId3" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{7F08651C-07CE-4F9D-9DB6-E721F8008E52}"/>
     <hyperlink ref="E16" r:id="rId4" xr:uid="{F74A2CD9-57F6-4D37-891F-1C14CEE7EE28}"/>
     <hyperlink ref="H17" r:id="rId5" xr:uid="{5A441EDE-90F6-429A-B4F6-8AA0CB497374}"/>
     <hyperlink ref="D2" r:id="rId6" xr:uid="{4D5420C0-4098-4F77-8C77-2D92FABA6A99}"/>
-    <hyperlink ref="B2" r:id="rId7" xr:uid="{0256F7FB-58C2-4BAB-BE67-4206DEC228E7}"/>
-    <hyperlink ref="H3" r:id="rId8" xr:uid="{07E85401-832F-48E6-A047-319CB6B7D5A8}"/>
-    <hyperlink ref="B3" r:id="rId9" xr:uid="{61228DC3-4729-4E9D-BA47-AEC733E6A768}"/>
-    <hyperlink ref="B4" r:id="rId10" xr:uid="{C98662A6-6882-485B-A267-73578CC7A81C}"/>
-    <hyperlink ref="H4" r:id="rId11" xr:uid="{0D8096A3-5F8F-472A-9A88-F4D314BA1D84}"/>
-    <hyperlink ref="C2" r:id="rId12" xr:uid="{C12DCAE2-5BE7-4CB7-B68A-8142A2C5BE18}"/>
-    <hyperlink ref="I2" r:id="rId13" xr:uid="{940F9767-2975-43CD-9672-73F2C1E9BB76}"/>
-    <hyperlink ref="C3" r:id="rId14" xr:uid="{6BDBED0E-D6CA-4A54-BB34-C338CC84BC2F}"/>
-    <hyperlink ref="I3" r:id="rId15" xr:uid="{0F906926-6594-4D15-A39D-8F9257E712CA}"/>
-    <hyperlink ref="I4" r:id="rId16" xr:uid="{644E9B73-D236-4CAF-AD8F-1A59764D2EA5}"/>
-    <hyperlink ref="C4" r:id="rId17" xr:uid="{89910DEA-1D5D-4633-BFBA-0D931A2E8862}"/>
+    <hyperlink ref="B2" r:id="rId7" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{0256F7FB-58C2-4BAB-BE67-4206DEC228E7}"/>
+    <hyperlink ref="H3" r:id="rId8" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{07E85401-832F-48E6-A047-319CB6B7D5A8}"/>
+    <hyperlink ref="B3" r:id="rId9" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{61228DC3-4729-4E9D-BA47-AEC733E6A768}"/>
+    <hyperlink ref="B4" r:id="rId10" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{C98662A6-6882-485B-A267-73578CC7A81C}"/>
+    <hyperlink ref="H4" r:id="rId11" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{0D8096A3-5F8F-472A-9A88-F4D314BA1D84}"/>
+    <hyperlink ref="C2" r:id="rId12" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{C12DCAE2-5BE7-4CB7-B68A-8142A2C5BE18}"/>
+    <hyperlink ref="I2" r:id="rId13" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{940F9767-2975-43CD-9672-73F2C1E9BB76}"/>
+    <hyperlink ref="C3" r:id="rId14" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{6BDBED0E-D6CA-4A54-BB34-C338CC84BC2F}"/>
+    <hyperlink ref="I3" r:id="rId15" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{0F906926-6594-4D15-A39D-8F9257E712CA}"/>
+    <hyperlink ref="I4" r:id="rId16" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{644E9B73-D236-4CAF-AD8F-1A59764D2EA5}"/>
+    <hyperlink ref="C4" r:id="rId17" display="gaddamramyasree0809+automation@gmail.com" xr:uid="{89910DEA-1D5D-4633-BFBA-0D931A2E8862}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4986,15 +4985,15 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5065,7 +5064,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5112,7 +5111,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -5128,7 +5127,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -5159,7 +5158,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -5167,7 +5166,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -5200,20 +5199,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.28515625" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5302,7 +5301,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5350,7 +5349,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -5366,7 +5365,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -5386,7 +5385,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -5405,7 +5404,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -5424,7 +5423,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -5432,7 +5431,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -5440,7 +5439,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -5457,7 +5456,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -5474,7 +5473,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -5491,7 +5490,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -5508,7 +5507,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -5519,7 +5518,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -5530,7 +5529,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -5547,7 +5546,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -5576,7 +5575,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -5587,7 +5586,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -5601,7 +5600,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -5615,7 +5614,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -5629,7 +5628,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -5637,7 +5636,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -5667,7 +5666,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -5737,19 +5736,19 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5775,7 +5774,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5783,7 +5782,7 @@
         <v>438</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -5798,15 +5797,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>199</v>
       </c>
       <c r="F3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
   </sheetData>
@@ -5829,16 +5828,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5852,7 +5851,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -5874,31 +5873,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAA7450-0FE7-4C50-95DC-266117BAF81B}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5703125" customWidth="1"/>
-    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5546875" customWidth="1"/>
+    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.140625" customWidth="1"/>
+    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.109375" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -5957,12 +5956,12 @@
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>228</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -5982,7 +5981,7 @@
       <c r="R2" s="20"/>
       <c r="S2" s="20"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>230</v>
       </c>
@@ -6011,7 +6010,7 @@
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>232</v>
       </c>
@@ -6023,7 +6022,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
@@ -6036,7 +6035,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>233</v>
       </c>
@@ -6051,7 +6050,7 @@
       <c r="H5" s="20"/>
       <c r="I5" s="30"/>
       <c r="J5" s="20" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
@@ -6063,7 +6062,7 @@
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>236</v>
       </c>
@@ -6078,7 +6077,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="M6" s="20"/>
       <c r="N6" s="19" t="s">
@@ -6096,9 +6095,9 @@
       <c r="R6" s="20"/>
       <c r="S6" s="20"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -6111,7 +6110,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="M7" s="20"/>
       <c r="N7" s="19"/>
@@ -6121,7 +6120,7 @@
       <c r="R7" s="20"/>
       <c r="S7" s="20"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>238</v>
       </c>
@@ -6137,7 +6136,7 @@
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="28" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
@@ -6146,7 +6145,7 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>262</v>
       </c>
@@ -6166,12 +6165,12 @@
       <c r="O9" s="20"/>
       <c r="P9" s="20"/>
       <c r="Q9" s="19" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>281</v>
       </c>
@@ -6179,7 +6178,7 @@
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -6196,7 +6195,7 @@
       <c r="R10" s="20"/>
       <c r="S10" s="20"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>286</v>
       </c>
@@ -6223,7 +6222,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>318</v>
       </c>
@@ -6248,7 +6247,7 @@
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
     </row>
-    <row r="13" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>320</v>
       </c>
@@ -6275,7 +6274,7 @@
       <c r="R13" s="20"/>
       <c r="S13" s="20"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>321</v>
       </c>
@@ -6300,7 +6299,7 @@
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>323</v>
       </c>
@@ -6325,7 +6324,7 @@
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>334</v>
       </c>
@@ -6350,7 +6349,7 @@
       <c r="R16" s="20"/>
       <c r="S16" s="20"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>337</v>
       </c>
@@ -6375,7 +6374,7 @@
       <c r="R17" s="20"/>
       <c r="S17" s="20"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>448</v>
       </c>
@@ -6383,7 +6382,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>449</v>
       </c>
@@ -6391,7 +6390,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>450</v>
       </c>
@@ -6399,20 +6398,20 @@
         <v>451</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J21" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+      <c r="J22" t="s">
         <v>583</v>
-      </c>
-      <c r="J22" t="s">
-        <v>584</v>
       </c>
     </row>
   </sheetData>
@@ -6429,18 +6428,18 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -6473,12 +6472,12 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>568</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>569</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -6491,27 +6490,27 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="H4" s="9"/>
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="H5" s="12"/>
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
       <c r="V5" s="5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="H6" s="5"/>
     </row>
   </sheetData>
@@ -6528,31 +6527,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.7109375" customWidth="1"/>
-    <col min="17" max="24" width="30.5703125" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" customWidth="1"/>
-    <col min="26" max="27" width="22.28515625" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.6640625" customWidth="1"/>
+    <col min="17" max="24" width="30.5546875" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" customWidth="1"/>
+    <col min="26" max="27" width="22.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.28515625" customWidth="1"/>
+    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -6704,7 +6703,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6774,7 +6773,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>453</v>
       </c>
@@ -6844,7 +6843,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>455</v>
       </c>
@@ -6914,7 +6913,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>456</v>
       </c>
@@ -6984,7 +6983,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>459</v>
       </c>
@@ -7054,7 +7053,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>463</v>
       </c>
@@ -7124,7 +7123,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>466</v>
       </c>
@@ -7165,7 +7164,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>467</v>
       </c>
@@ -7206,7 +7205,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>461</v>
       </c>
@@ -7276,7 +7275,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>406</v>
       </c>
@@ -7337,7 +7336,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -7396,7 +7395,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>359</v>
       </c>
@@ -7442,7 +7441,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -7465,7 +7464,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>297</v>
       </c>
@@ -7488,7 +7487,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -7507,7 +7506,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -7518,7 +7517,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -7540,7 +7539,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>366</v>
       </c>
@@ -7553,7 +7552,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>368</v>
       </c>
@@ -7566,7 +7565,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -7579,7 +7578,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>375</v>
       </c>
@@ -7592,7 +7591,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>397</v>
       </c>
@@ -7605,7 +7604,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>376</v>
       </c>
@@ -7618,7 +7617,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -7634,7 +7633,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -7650,7 +7649,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>401</v>
       </c>
@@ -7669,7 +7668,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>405</v>
       </c>
@@ -7688,7 +7687,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>382</v>
       </c>
@@ -7704,7 +7703,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>385</v>
       </c>
@@ -7720,7 +7719,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>411</v>
       </c>
@@ -7736,7 +7735,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>412</v>
       </c>
@@ -7752,7 +7751,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>386</v>
       </c>
@@ -7768,7 +7767,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>389</v>
       </c>
@@ -7781,7 +7780,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>403</v>
       </c>
@@ -7794,7 +7793,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -7807,7 +7806,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>424</v>
       </c>
@@ -7820,7 +7819,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>398</v>
       </c>
@@ -7833,7 +7832,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>394</v>
       </c>
@@ -7849,7 +7848,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>423</v>
       </c>
@@ -7865,7 +7864,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -7881,7 +7880,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>402</v>
       </c>
@@ -7894,7 +7893,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>415</v>
       </c>
@@ -7916,7 +7915,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -7934,7 +7933,7 @@
       <c r="AI44" s="25"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>414</v>
       </c>
@@ -7947,7 +7946,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -7967,7 +7966,7 @@
       <c r="AI46" s="25"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -7986,7 +7985,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -7999,7 +7998,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -8010,7 +8009,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -8023,7 +8022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -8046,7 +8045,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -8060,7 +8059,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -8097,7 +8096,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -8111,7 +8110,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -8153,7 +8152,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -8179,7 +8178,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -8203,7 +8202,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -8227,7 +8226,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -8253,7 +8252,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -8285,7 +8284,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -8299,7 +8298,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>373</v>
       </c>
@@ -8313,7 +8312,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -8330,7 +8329,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -8347,7 +8346,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>339</v>
       </c>
@@ -8369,7 +8368,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>343</v>
       </c>
@@ -8377,7 +8376,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>346</v>
       </c>
@@ -8388,7 +8387,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>348</v>
       </c>
@@ -8405,7 +8404,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>353</v>
       </c>
@@ -8413,7 +8412,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -8448,7 +8447,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>363</v>
       </c>
@@ -8539,37 +8538,37 @@
       <selection activeCell="AM12" sqref="AM12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -8706,7 +8705,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -8781,7 +8780,7 @@
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
@@ -8838,7 +8837,7 @@
       <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>248</v>
       </c>
@@ -8891,7 +8890,7 @@
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>68</v>
       </c>
@@ -8954,7 +8953,7 @@
       <c r="AR5" s="20"/>
       <c r="AS5" s="20"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>75</v>
       </c>
@@ -9033,7 +9032,7 @@
       <c r="AR6" s="20"/>
       <c r="AS6" s="20"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>81</v>
       </c>
@@ -9122,7 +9121,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>100</v>
       </c>
@@ -9205,7 +9204,7 @@
       <c r="AR8" s="20"/>
       <c r="AS8" s="20"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>95</v>
       </c>
@@ -9290,7 +9289,7 @@
       <c r="AR9" s="20"/>
       <c r="AS9" s="20"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -9341,7 +9340,7 @@
       <c r="AR10" s="20"/>
       <c r="AS10" s="20"/>
     </row>
-    <row r="11" spans="1:45" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>103</v>
       </c>
@@ -9383,7 +9382,7 @@
         <v>43001000060</v>
       </c>
       <c r="AK11" s="20" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="AL11" s="46" t="s">
         <v>15</v>
@@ -9398,7 +9397,7 @@
       <c r="AR11" s="20"/>
       <c r="AS11" s="20"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>107</v>
       </c>
@@ -9473,7 +9472,7 @@
       <c r="AR12" s="20"/>
       <c r="AS12" s="20"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>112</v>
       </c>
@@ -9536,7 +9535,7 @@
       <c r="AR13" s="20"/>
       <c r="AS13" s="20"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>249</v>
       </c>
@@ -9591,7 +9590,7 @@
       <c r="AR14" s="20"/>
       <c r="AS14" s="20"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>119</v>
       </c>
@@ -9648,7 +9647,7 @@
       <c r="AR15" s="20"/>
       <c r="AS15" s="20"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>121</v>
       </c>
@@ -9703,7 +9702,7 @@
       <c r="AR16" s="20"/>
       <c r="AS16" s="20"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>219</v>
       </c>
@@ -9758,7 +9757,7 @@
       <c r="AR17" s="20"/>
       <c r="AS17" s="20"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>154</v>
       </c>
@@ -9849,13 +9848,13 @@
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9932,12 +9931,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="R2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="S2" t="s">
         <v>260</v>
@@ -9962,25 +9961,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10081,7 +10080,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -10167,7 +10166,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -10199,7 +10198,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -10225,27 +10224,27 @@
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -10340,7 +10339,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -10401,7 +10400,7 @@
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>20</v>
       </c>
@@ -10442,7 +10441,7 @@
       <c r="AD3" s="20"/>
       <c r="AE3" s="20"/>
     </row>
-    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>25</v>
       </c>
@@ -10465,7 +10464,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
       <c r="T4" s="20" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="U4" s="20"/>
       <c r="V4" s="20"/>
@@ -10473,10 +10472,10 @@
         <v>1</v>
       </c>
       <c r="X4" s="12" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="Y4" s="21" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Z4" s="20"/>
       <c r="AA4" s="20"/>
@@ -10485,7 +10484,7 @@
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>178</v>
       </c>
@@ -10524,7 +10523,7 @@
       <c r="AD5" s="20"/>
       <c r="AE5" s="20"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>179</v>
       </c>
@@ -10563,7 +10562,7 @@
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>153</v>
       </c>
@@ -10602,7 +10601,7 @@
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>155</v>
       </c>
@@ -10639,7 +10638,7 @@
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>154</v>
       </c>
@@ -10676,7 +10675,7 @@
       <c r="AD9" s="20"/>
       <c r="AE9" s="20"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>168</v>
       </c>
@@ -10713,7 +10712,7 @@
       <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>172</v>
       </c>
@@ -10756,7 +10755,7 @@
       <c r="AD11" s="20"/>
       <c r="AE11" s="20"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>170</v>
       </c>
@@ -10795,7 +10794,7 @@
       <c r="AD12" s="20"/>
       <c r="AE12" s="20"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>77</v>
       </c>
@@ -10834,7 +10833,7 @@
       <c r="AD13" s="20"/>
       <c r="AE13" s="20"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>43</v>
       </c>
@@ -10867,13 +10866,13 @@
         <v>480</v>
       </c>
       <c r="AB14" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="AC14" s="20"/>
       <c r="AD14" s="20"/>
       <c r="AE14" s="20"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>118</v>
       </c>
@@ -10922,7 +10921,7 @@
       <c r="AD15" s="20"/>
       <c r="AE15" s="20"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
@@ -10942,7 +10941,7 @@
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="40" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="R16" s="7" t="s">
         <v>441</v>
@@ -10963,7 +10962,7 @@
       <c r="AD16" s="20"/>
       <c r="AE16" s="20"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>46</v>
       </c>
@@ -11004,7 +11003,7 @@
       <c r="AD17" s="20"/>
       <c r="AE17" s="20"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>201</v>
       </c>
@@ -11059,7 +11058,7 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="20"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>241</v>
       </c>
@@ -11096,7 +11095,7 @@
       <c r="AD19" s="20"/>
       <c r="AE19" s="20"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>187</v>
       </c>
@@ -11143,7 +11142,7 @@
       <c r="AD20" s="20"/>
       <c r="AE20" s="20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>166</v>
       </c>
@@ -11190,7 +11189,7 @@
       <c r="AD21" s="20"/>
       <c r="AE21" s="20"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>343</v>
       </c>
@@ -11227,7 +11226,7 @@
       <c r="AD22" s="20"/>
       <c r="AE22" s="20"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>346</v>
       </c>
@@ -11252,7 +11251,7 @@
       <c r="T23" s="20"/>
       <c r="U23" s="20"/>
       <c r="V23" s="20" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="W23" s="20"/>
       <c r="X23" s="20"/>
@@ -11264,7 +11263,7 @@
       <c r="AD23" s="20"/>
       <c r="AE23" s="20"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>348</v>
       </c>
@@ -11279,7 +11278,7 @@
         <v>349</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
@@ -11309,7 +11308,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
@@ -11344,9 +11343,9 @@
       <c r="AD25" s="20"/>
       <c r="AE25" s="20"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>494</v>
@@ -11373,25 +11372,25 @@
         <v>494</v>
       </c>
       <c r="K26" t="s">
+        <v>527</v>
+      </c>
+      <c r="L26" t="s">
         <v>528</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>529</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" s="5" t="s">
         <v>530</v>
-      </c>
-      <c r="N26" s="5" t="s">
-        <v>531</v>
       </c>
       <c r="O26" s="5" t="s">
         <v>59</v>
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>494</v>
@@ -11418,25 +11417,25 @@
         <v>494</v>
       </c>
       <c r="K27" s="20" t="s">
+        <v>527</v>
+      </c>
+      <c r="L27" s="20" t="s">
         <v>528</v>
       </c>
-      <c r="L27" s="20" t="s">
-        <v>529</v>
-      </c>
       <c r="M27" s="41" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="N27" s="40" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="O27" s="40" t="s">
         <v>59</v>
       </c>
       <c r="P27" s="40"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>494</v>
@@ -11463,25 +11462,25 @@
         <v>494</v>
       </c>
       <c r="K28" s="20" t="s">
+        <v>534</v>
+      </c>
+      <c r="L28" s="40" t="s">
         <v>535</v>
       </c>
-      <c r="L28" s="40" t="s">
+      <c r="M28" s="41" t="s">
+        <v>535</v>
+      </c>
+      <c r="N28" s="40" t="s">
         <v>536</v>
-      </c>
-      <c r="M28" s="41" t="s">
-        <v>536</v>
-      </c>
-      <c r="N28" s="40" t="s">
-        <v>537</v>
       </c>
       <c r="O28" s="40" t="s">
         <v>59</v>
       </c>
       <c r="P28" s="40"/>
     </row>
-    <row r="29" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>494</v>
@@ -11508,25 +11507,25 @@
         <v>494</v>
       </c>
       <c r="K29" s="20" t="s">
+        <v>538</v>
+      </c>
+      <c r="L29" s="40" t="s">
         <v>539</v>
       </c>
-      <c r="L29" s="40" t="s">
+      <c r="M29" s="41" t="s">
         <v>540</v>
       </c>
-      <c r="M29" s="41" t="s">
+      <c r="N29" s="40" t="s">
         <v>541</v>
-      </c>
-      <c r="N29" s="40" t="s">
-        <v>542</v>
       </c>
       <c r="O29" s="40">
         <v>9898989898</v>
       </c>
       <c r="P29" s="40"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F30" t="s">
         <v>14</v>
@@ -11535,24 +11534,24 @@
         <v>15</v>
       </c>
       <c r="K30" s="43" t="s">
+        <v>545</v>
+      </c>
+      <c r="L30" s="43" t="s">
         <v>546</v>
       </c>
-      <c r="L30" s="43" t="s">
+      <c r="M30" s="43" t="s">
         <v>547</v>
       </c>
-      <c r="M30" s="43" t="s">
+      <c r="N30" s="44" t="s">
         <v>548</v>
-      </c>
-      <c r="N30" s="44" t="s">
-        <v>549</v>
       </c>
       <c r="O30">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F31" t="s">
         <v>14</v>
@@ -11561,24 +11560,24 @@
         <v>15</v>
       </c>
       <c r="K31" t="s">
+        <v>549</v>
+      </c>
+      <c r="L31" t="s">
         <v>550</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" s="18" t="s">
         <v>551</v>
       </c>
-      <c r="M31" s="18" t="s">
+      <c r="N31" s="5" t="s">
         <v>552</v>
-      </c>
-      <c r="N31" s="5" t="s">
-        <v>553</v>
       </c>
       <c r="O31">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F32" t="s">
         <v>14</v>
@@ -11587,24 +11586,24 @@
         <v>15</v>
       </c>
       <c r="K32" t="s">
+        <v>557</v>
+      </c>
+      <c r="L32" t="s">
         <v>558</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>559</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" s="5" t="s">
         <v>560</v>
-      </c>
-      <c r="N32" s="5" t="s">
-        <v>561</v>
       </c>
       <c r="O32">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F33" t="s">
         <v>14</v>
@@ -11613,16 +11612,16 @@
         <v>15</v>
       </c>
       <c r="K33" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L33" t="s">
+        <v>561</v>
+      </c>
+      <c r="M33" t="s">
+        <v>563</v>
+      </c>
+      <c r="N33" s="5" t="s">
         <v>562</v>
-      </c>
-      <c r="M33" t="s">
-        <v>564</v>
-      </c>
-      <c r="N33" s="5" t="s">
-        <v>563</v>
       </c>
       <c r="O33">
         <v>9898989898</v>
@@ -11682,17 +11681,17 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -11703,7 +11702,7 @@
         <v>246</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -11729,28 +11728,28 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>243</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C2" s="20"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>245</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="20" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D3" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>247</v>
       </c>
@@ -11759,13 +11758,13 @@
         <v>492</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>312</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
   </sheetData>
@@ -11781,20 +11780,20 @@
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -11862,7 +11861,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11906,7 +11905,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -11922,7 +11921,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -11940,7 +11939,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -11948,7 +11947,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -11956,7 +11955,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
Test_DGLD_HF_EMEA_RT_044_Validate_Blog_page added new testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4270199-2FC2-47ED-B784-331BFD568E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A284EFD8-B8A8-4974-85D6-AB11A3EBF526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28800" windowHeight="14685" firstSheet="7" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Account page" sheetId="11" r:id="rId14"/>
     <sheet name="weblinks" sheetId="12" r:id="rId15"/>
     <sheet name="HeaderLinks" sheetId="14" r:id="rId16"/>
+    <sheet name="Blog" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="611">
   <si>
     <t>UserName</t>
   </si>
@@ -1884,6 +1885,15 @@
   </si>
   <si>
     <t>Hfemeanewaccount+@gmail.com</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>blog</t>
+  </si>
+  <si>
+    <t>Tips &amp; Tricks,Recipes,People &amp; Partners,Clean &amp; Care,Product Recommendations</t>
   </si>
 </sst>
 </file>
@@ -2440,30 +2450,30 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="18" width="30.5546875" customWidth="1"/>
-    <col min="19" max="19" width="19.6640625" customWidth="1"/>
-    <col min="20" max="21" width="22.33203125" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" customWidth="1"/>
-    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="18" width="30.5703125" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1"/>
+    <col min="20" max="21" width="22.28515625" customWidth="1"/>
+    <col min="22" max="22" width="14.7109375" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.33203125" customWidth="1"/>
+    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2612,7 +2622,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2670,7 +2680,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -2728,7 +2738,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:49" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>507</v>
       </c>
@@ -2783,7 +2793,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -2825,7 +2835,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>437</v>
       </c>
@@ -2883,7 +2893,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>526</v>
       </c>
@@ -2938,7 +2948,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="7"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>531</v>
       </c>
@@ -2995,7 +3005,7 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>533</v>
       </c>
@@ -3052,7 +3062,7 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="1:49" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:49" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>537</v>
       </c>
@@ -3109,7 +3119,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3127,7 +3137,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>199</v>
       </c>
@@ -3139,7 +3149,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -3187,7 +3197,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>297</v>
       </c>
@@ -3196,7 +3206,7 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="7"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -3211,7 +3221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -3222,7 +3232,7 @@
       <c r="X16" s="4"/>
       <c r="AD16" s="32"/>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>525</v>
       </c>
@@ -3244,7 +3254,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -3257,7 +3267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>170</v>
       </c>
@@ -3283,7 +3293,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="20" spans="1:49" ht="60" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:49" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -3300,7 +3310,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="21" spans="1:49" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>603</v>
       </c>
@@ -3315,7 +3325,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>442</v>
       </c>
@@ -3334,7 +3344,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>176</v>
       </c>
@@ -3347,7 +3357,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>175</v>
       </c>
@@ -3358,7 +3368,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>189</v>
       </c>
@@ -3368,7 +3378,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -3395,7 +3405,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -3405,7 +3415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -3430,7 +3440,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -3459,7 +3469,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -3481,7 +3491,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -3516,7 +3526,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -3537,7 +3547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -3569,7 +3579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -3598,7 +3608,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -3619,7 +3629,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -3650,7 +3660,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -3664,7 +3674,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -3681,7 +3691,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>164</v>
       </c>
@@ -3714,7 +3724,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>166</v>
       </c>
@@ -3740,7 +3750,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>184</v>
       </c>
@@ -3752,7 +3762,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>279</v>
       </c>
@@ -3760,7 +3770,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>284</v>
       </c>
@@ -3783,7 +3793,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>215</v>
       </c>
@@ -3800,13 +3810,13 @@
         <v>214</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>209</v>
       </c>
       <c r="R45" s="5"/>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>339</v>
       </c>
@@ -3831,7 +3841,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>343</v>
       </c>
@@ -3839,7 +3849,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>346</v>
       </c>
@@ -3856,7 +3866,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>348</v>
       </c>
@@ -3873,7 +3883,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>353</v>
       </c>
@@ -3881,7 +3891,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>575</v>
       </c>
@@ -3907,7 +3917,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>201</v>
       </c>
@@ -3930,7 +3940,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>363</v>
       </c>
@@ -3938,7 +3948,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>431</v>
       </c>
@@ -3946,7 +3956,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>432</v>
       </c>
@@ -3960,7 +3970,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>232</v>
       </c>
@@ -3989,7 +3999,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="57" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
         <v>153</v>
       </c>
@@ -4010,7 +4020,7 @@
       <c r="P57" s="33"/>
       <c r="Q57" s="33"/>
     </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>446</v>
       </c>
@@ -4018,7 +4028,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>503</v>
       </c>
@@ -4029,13 +4039,13 @@
         <v>515</v>
       </c>
     </row>
-    <row r="60" spans="1:48" ht="30" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>514</v>
       </c>
       <c r="AC60" s="42"/>
     </row>
-    <row r="61" spans="1:48" ht="60" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:48" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>517</v>
       </c>
@@ -4043,7 +4053,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="62" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>521</v>
       </c>
@@ -4131,37 +4141,37 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4244,7 +4254,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4285,7 +4295,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4301,7 +4311,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -4313,7 +4323,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4331,7 +4341,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4340,7 +4350,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -4352,7 +4362,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -4378,7 +4388,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -4389,7 +4399,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -4403,7 +4413,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -4449,18 +4459,18 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4558,7 +4568,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4605,7 +4615,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4655,7 +4665,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -4702,7 +4712,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4718,7 +4728,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -4730,7 +4740,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -4741,7 +4751,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4763,7 +4773,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -4776,7 +4786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -4792,7 +4802,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4806,7 +4816,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -4822,7 +4832,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -4836,7 +4846,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -4878,7 +4888,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -4904,7 +4914,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -4915,7 +4925,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -4930,7 +4940,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -4988,12 +4998,12 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5064,7 +5074,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5111,7 +5121,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -5127,7 +5137,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -5158,7 +5168,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -5166,7 +5176,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -5199,20 +5209,20 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="15.33203125" customWidth="1"/>
-    <col min="27" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="21" max="21" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.28515625" customWidth="1"/>
+    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5301,7 +5311,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5349,7 +5359,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -5365,7 +5375,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -5385,7 +5395,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -5404,7 +5414,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -5423,7 +5433,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -5431,7 +5441,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -5439,7 +5449,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -5456,7 +5466,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -5473,7 +5483,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -5490,7 +5500,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -5507,7 +5517,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -5518,7 +5528,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -5529,7 +5539,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -5546,7 +5556,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -5575,7 +5585,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -5586,7 +5596,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -5600,7 +5610,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -5614,7 +5624,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -5628,7 +5638,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -5636,7 +5646,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -5666,7 +5676,7 @@
       </c>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -5736,19 +5746,19 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="158.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="158.6640625" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="158.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5774,7 +5784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5797,7 +5807,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -5828,16 +5838,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5851,7 +5861,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -5873,31 +5883,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAA7450-0FE7-4C50-95DC-266117BAF81B}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" customWidth="1"/>
     <col min="4" max="4" width="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5546875" customWidth="1"/>
-    <col min="9" max="9" width="77.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5703125" customWidth="1"/>
+    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.109375" customWidth="1"/>
+    <col min="14" max="14" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="59.140625" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -5956,7 +5966,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>228</v>
       </c>
@@ -5981,7 +5991,7 @@
       <c r="R2" s="20"/>
       <c r="S2" s="20"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>230</v>
       </c>
@@ -6010,7 +6020,7 @@
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>232</v>
       </c>
@@ -6035,7 +6045,7 @@
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>233</v>
       </c>
@@ -6062,7 +6072,7 @@
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>236</v>
       </c>
@@ -6095,7 +6105,7 @@
       <c r="R6" s="20"/>
       <c r="S6" s="20"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>586</v>
       </c>
@@ -6120,7 +6130,7 @@
       <c r="R7" s="20"/>
       <c r="S7" s="20"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>238</v>
       </c>
@@ -6145,7 +6155,7 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>262</v>
       </c>
@@ -6170,7 +6180,7 @@
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>281</v>
       </c>
@@ -6195,7 +6205,7 @@
       <c r="R10" s="20"/>
       <c r="S10" s="20"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>286</v>
       </c>
@@ -6222,7 +6232,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>318</v>
       </c>
@@ -6247,7 +6257,7 @@
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
     </row>
-    <row r="13" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>320</v>
       </c>
@@ -6274,7 +6284,7 @@
       <c r="R13" s="20"/>
       <c r="S13" s="20"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>321</v>
       </c>
@@ -6299,7 +6309,7 @@
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>323</v>
       </c>
@@ -6324,7 +6334,7 @@
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>334</v>
       </c>
@@ -6349,7 +6359,7 @@
       <c r="R16" s="20"/>
       <c r="S16" s="20"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>337</v>
       </c>
@@ -6374,7 +6384,7 @@
       <c r="R17" s="20"/>
       <c r="S17" s="20"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>448</v>
       </c>
@@ -6382,7 +6392,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>449</v>
       </c>
@@ -6390,7 +6400,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>450</v>
       </c>
@@ -6398,7 +6408,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>516</v>
       </c>
@@ -6406,7 +6416,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>582</v>
       </c>
@@ -6417,6 +6427,37 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A11CD39-B43D-4ECF-B59A-D818AB33DAB7}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6428,13 +6469,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -6472,7 +6513,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>567</v>
       </c>
@@ -6490,27 +6531,27 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="H4" s="9"/>
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H5" s="12"/>
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
       <c r="V5" s="5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H6" s="5"/>
     </row>
   </sheetData>
@@ -6527,31 +6568,31 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.6640625" customWidth="1"/>
-    <col min="17" max="24" width="30.5546875" customWidth="1"/>
-    <col min="25" max="25" width="19.6640625" customWidth="1"/>
-    <col min="26" max="27" width="22.33203125" customWidth="1"/>
-    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.7109375" customWidth="1"/>
+    <col min="17" max="24" width="30.5703125" customWidth="1"/>
+    <col min="25" max="25" width="19.7109375" customWidth="1"/>
+    <col min="26" max="27" width="22.28515625" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.33203125" customWidth="1"/>
+    <col min="34" max="34" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -6703,7 +6744,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6773,7 +6814,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>453</v>
       </c>
@@ -6843,7 +6884,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>455</v>
       </c>
@@ -6913,7 +6954,7 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>456</v>
       </c>
@@ -6983,7 +7024,7 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>459</v>
       </c>
@@ -7053,7 +7094,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>463</v>
       </c>
@@ -7123,7 +7164,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>466</v>
       </c>
@@ -7164,7 +7205,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>467</v>
       </c>
@@ -7205,7 +7246,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="7"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>461</v>
       </c>
@@ -7275,7 +7316,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>406</v>
       </c>
@@ -7336,7 +7377,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -7395,7 +7436,7 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>359</v>
       </c>
@@ -7441,7 +7482,7 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -7464,7 +7505,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>297</v>
       </c>
@@ -7487,7 +7528,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -7506,7 +7547,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -7517,7 +7558,7 @@
       <c r="AD17" s="4"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -7539,7 +7580,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>366</v>
       </c>
@@ -7552,7 +7593,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>368</v>
       </c>
@@ -7565,7 +7606,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -7578,7 +7619,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>375</v>
       </c>
@@ -7591,7 +7632,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>397</v>
       </c>
@@ -7604,7 +7645,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>376</v>
       </c>
@@ -7617,7 +7658,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>378</v>
       </c>
@@ -7633,7 +7674,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -7649,7 +7690,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>401</v>
       </c>
@@ -7668,7 +7709,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>405</v>
       </c>
@@ -7687,7 +7728,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>382</v>
       </c>
@@ -7703,7 +7744,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>385</v>
       </c>
@@ -7719,7 +7760,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>411</v>
       </c>
@@ -7735,7 +7776,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>412</v>
       </c>
@@ -7751,7 +7792,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>386</v>
       </c>
@@ -7767,7 +7808,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>389</v>
       </c>
@@ -7780,7 +7821,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>403</v>
       </c>
@@ -7793,7 +7834,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -7806,7 +7847,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>424</v>
       </c>
@@ -7819,7 +7860,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>398</v>
       </c>
@@ -7832,7 +7873,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>394</v>
       </c>
@@ -7848,7 +7889,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>423</v>
       </c>
@@ -7864,7 +7905,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -7880,7 +7921,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>402</v>
       </c>
@@ -7893,7 +7934,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>415</v>
       </c>
@@ -7915,7 +7956,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -7933,7 +7974,7 @@
       <c r="AI44" s="25"/>
       <c r="AJ44" s="5"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>414</v>
       </c>
@@ -7946,7 +7987,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -7966,7 +8007,7 @@
       <c r="AI46" s="25"/>
       <c r="AJ46" s="5"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -7985,7 +8026,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -7998,7 +8039,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>189</v>
       </c>
@@ -8009,7 +8050,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -8022,7 +8063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -8045,7 +8086,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -8059,7 +8100,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -8096,7 +8137,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -8110,7 +8151,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -8152,7 +8193,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -8178,7 +8219,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -8202,7 +8243,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -8226,7 +8267,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -8252,7 +8293,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -8284,7 +8325,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -8298,7 +8339,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>373</v>
       </c>
@@ -8312,7 +8353,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -8329,7 +8370,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -8346,7 +8387,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>339</v>
       </c>
@@ -8368,7 +8409,7 @@
       </c>
       <c r="X65" s="5"/>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>343</v>
       </c>
@@ -8376,7 +8417,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>346</v>
       </c>
@@ -8387,7 +8428,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>348</v>
       </c>
@@ -8404,7 +8445,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>353</v>
       </c>
@@ -8412,7 +8453,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -8447,7 +8488,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>363</v>
       </c>
@@ -8538,37 +8579,37 @@
       <selection activeCell="AM12" sqref="AM12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -8705,7 +8746,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -8780,7 +8821,7 @@
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
@@ -8837,7 +8878,7 @@
       <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>248</v>
       </c>
@@ -8890,7 +8931,7 @@
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>68</v>
       </c>
@@ -8953,7 +8994,7 @@
       <c r="AR5" s="20"/>
       <c r="AS5" s="20"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>75</v>
       </c>
@@ -9032,7 +9073,7 @@
       <c r="AR6" s="20"/>
       <c r="AS6" s="20"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>81</v>
       </c>
@@ -9121,7 +9162,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>100</v>
       </c>
@@ -9204,7 +9245,7 @@
       <c r="AR8" s="20"/>
       <c r="AS8" s="20"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>95</v>
       </c>
@@ -9289,7 +9330,7 @@
       <c r="AR9" s="20"/>
       <c r="AS9" s="20"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -9340,7 +9381,7 @@
       <c r="AR10" s="20"/>
       <c r="AS10" s="20"/>
     </row>
-    <row r="11" spans="1:45" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>103</v>
       </c>
@@ -9397,7 +9438,7 @@
       <c r="AR11" s="20"/>
       <c r="AS11" s="20"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>107</v>
       </c>
@@ -9472,7 +9513,7 @@
       <c r="AR12" s="20"/>
       <c r="AS12" s="20"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>112</v>
       </c>
@@ -9535,7 +9576,7 @@
       <c r="AR13" s="20"/>
       <c r="AS13" s="20"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>249</v>
       </c>
@@ -9590,7 +9631,7 @@
       <c r="AR14" s="20"/>
       <c r="AS14" s="20"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>119</v>
       </c>
@@ -9647,7 +9688,7 @@
       <c r="AR15" s="20"/>
       <c r="AS15" s="20"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>121</v>
       </c>
@@ -9702,7 +9743,7 @@
       <c r="AR16" s="20"/>
       <c r="AS16" s="20"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>219</v>
       </c>
@@ -9757,7 +9798,7 @@
       <c r="AR17" s="20"/>
       <c r="AS17" s="20"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>154</v>
       </c>
@@ -9848,13 +9889,13 @@
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9931,7 +9972,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -9961,25 +10002,25 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.44140625" customWidth="1"/>
-    <col min="32" max="32" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.42578125" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10080,7 +10121,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -10166,7 +10207,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -10198,7 +10239,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -10224,27 +10265,27 @@
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.44140625" customWidth="1"/>
-    <col min="22" max="22" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -10339,7 +10380,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -10400,7 +10441,7 @@
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>20</v>
       </c>
@@ -10441,7 +10482,7 @@
       <c r="AD3" s="20"/>
       <c r="AE3" s="20"/>
     </row>
-    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>25</v>
       </c>
@@ -10484,7 +10525,7 @@
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>178</v>
       </c>
@@ -10523,7 +10564,7 @@
       <c r="AD5" s="20"/>
       <c r="AE5" s="20"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>179</v>
       </c>
@@ -10562,7 +10603,7 @@
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>153</v>
       </c>
@@ -10601,7 +10642,7 @@
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>155</v>
       </c>
@@ -10638,7 +10679,7 @@
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>154</v>
       </c>
@@ -10675,7 +10716,7 @@
       <c r="AD9" s="20"/>
       <c r="AE9" s="20"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>168</v>
       </c>
@@ -10712,7 +10753,7 @@
       <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>172</v>
       </c>
@@ -10755,7 +10796,7 @@
       <c r="AD11" s="20"/>
       <c r="AE11" s="20"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>170</v>
       </c>
@@ -10794,7 +10835,7 @@
       <c r="AD12" s="20"/>
       <c r="AE12" s="20"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>77</v>
       </c>
@@ -10833,7 +10874,7 @@
       <c r="AD13" s="20"/>
       <c r="AE13" s="20"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>43</v>
       </c>
@@ -10872,7 +10913,7 @@
       <c r="AD14" s="20"/>
       <c r="AE14" s="20"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>118</v>
       </c>
@@ -10921,7 +10962,7 @@
       <c r="AD15" s="20"/>
       <c r="AE15" s="20"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
@@ -10962,7 +11003,7 @@
       <c r="AD16" s="20"/>
       <c r="AE16" s="20"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>46</v>
       </c>
@@ -11003,7 +11044,7 @@
       <c r="AD17" s="20"/>
       <c r="AE17" s="20"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>201</v>
       </c>
@@ -11058,7 +11099,7 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="20"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>241</v>
       </c>
@@ -11095,7 +11136,7 @@
       <c r="AD19" s="20"/>
       <c r="AE19" s="20"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>187</v>
       </c>
@@ -11142,7 +11183,7 @@
       <c r="AD20" s="20"/>
       <c r="AE20" s="20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>166</v>
       </c>
@@ -11189,7 +11230,7 @@
       <c r="AD21" s="20"/>
       <c r="AE21" s="20"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>343</v>
       </c>
@@ -11226,7 +11267,7 @@
       <c r="AD22" s="20"/>
       <c r="AE22" s="20"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>346</v>
       </c>
@@ -11263,7 +11304,7 @@
       <c r="AD23" s="20"/>
       <c r="AE23" s="20"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>348</v>
       </c>
@@ -11308,7 +11349,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
@@ -11343,7 +11384,7 @@
       <c r="AD25" s="20"/>
       <c r="AE25" s="20"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>526</v>
       </c>
@@ -11388,7 +11429,7 @@
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>531</v>
       </c>
@@ -11433,7 +11474,7 @@
       </c>
       <c r="P27" s="40"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>533</v>
       </c>
@@ -11478,7 +11519,7 @@
       </c>
       <c r="P28" s="40"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>537</v>
       </c>
@@ -11523,7 +11564,7 @@
       </c>
       <c r="P29" s="40"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>553</v>
       </c>
@@ -11549,7 +11590,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>554</v>
       </c>
@@ -11575,7 +11616,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>556</v>
       </c>
@@ -11601,7 +11642,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>565</v>
       </c>
@@ -11681,17 +11722,17 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="154.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="154.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -11728,7 +11769,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>243</v>
       </c>
@@ -11737,7 +11778,7 @@
       </c>
       <c r="C2" s="20"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>245</v>
       </c>
@@ -11749,7 +11790,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>247</v>
       </c>
@@ -11758,7 +11799,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>312</v>
       </c>
@@ -11780,20 +11821,20 @@
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -11861,7 +11902,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11905,7 +11946,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -11921,7 +11962,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -11939,7 +11980,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -11947,7 +11988,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -11955,7 +11996,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
HFEMEA: 022 and 71 Testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask_EMEA/GoldHydroEMEA_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2286E12-FC15-4EF3-9460-1AB1EC06D3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE47CC57-76AA-4AAA-8447-C58A2BA08843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28800" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1925" uniqueCount="620">
   <si>
     <t>UserName</t>
   </si>
@@ -1912,6 +1912,15 @@
   </si>
   <si>
     <t>Bottle Brush</t>
+  </si>
+  <si>
+    <t>GiftCard_MyAccount</t>
+  </si>
+  <si>
+    <t>4GF55E64T6999A72C22A</t>
+  </si>
+  <si>
+    <t>Below30_Product</t>
   </si>
 </sst>
 </file>
@@ -2462,10 +2471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW65"/>
+  <dimension ref="A1:AW67"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3330,245 +3339,225 @@
     </row>
     <row r="21" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="AC21" s="42" t="s">
-        <v>616</v>
+        <v>542</v>
       </c>
       <c r="AD21" s="32"/>
       <c r="AE21" s="22"/>
     </row>
     <row r="22" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="AC22" s="42"/>
-      <c r="AD22" s="32" t="s">
-        <v>613</v>
-      </c>
+      <c r="AC22" s="42" t="s">
+        <v>616</v>
+      </c>
+      <c r="AD22" s="32"/>
       <c r="AE22" s="22"/>
     </row>
     <row r="23" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="AC23" s="42"/>
       <c r="AD23" s="32" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="AE23" s="22"/>
     </row>
     <row r="24" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>603</v>
+        <v>614</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="AC24" s="42"/>
-      <c r="AD24" s="32"/>
-      <c r="AE24" s="22" t="s">
-        <v>604</v>
-      </c>
-      <c r="AF24" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AD24" s="32" t="s">
+        <v>615</v>
+      </c>
+      <c r="AE24" s="22"/>
+    </row>
+    <row r="25" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>442</v>
+        <v>603</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="AC25" t="s">
-        <v>177</v>
-      </c>
-      <c r="AD25" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>177</v>
+      <c r="AC25" s="42"/>
+      <c r="AD25" s="32"/>
+      <c r="AE25" s="22" t="s">
+        <v>604</v>
       </c>
       <c r="AF25" t="s">
-        <v>39</v>
+        <v>605</v>
       </c>
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>442</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="AC26" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AD26" s="5" t="s">
         <v>120</v>
       </c>
+      <c r="AE26" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="AD27" s="5"/>
-      <c r="AF27" t="s">
-        <v>259</v>
+      <c r="AC27" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD27" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="AL28" s="12" t="s">
-        <v>444</v>
+      <c r="AD28" s="5"/>
+      <c r="AF28" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" t="s">
-        <v>35</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="AD29" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="AL29" s="12" t="s">
-        <v>599</v>
+        <v>444</v>
       </c>
     </row>
     <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="I30" s="2"/>
-      <c r="AH30">
-        <v>3</v>
+      <c r="AD30" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL30" s="12" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="G31" s="6"/>
+        <v>40</v>
+      </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="Z31" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA31" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="AB31">
-        <v>123</v>
-      </c>
-      <c r="AI31" t="s">
-        <v>480</v>
-      </c>
-      <c r="AJ31" t="s">
-        <v>593</v>
+      <c r="AH31">
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>44</v>
-      </c>
-      <c r="S32" t="s">
-        <v>150</v>
-      </c>
-      <c r="T32" t="s">
-        <v>17</v>
-      </c>
-      <c r="V32" t="s">
-        <v>19</v>
-      </c>
-      <c r="W32" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="X32" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
       <c r="Z32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AA32" s="7" t="s">
         <v>441</v>
       </c>
       <c r="AB32">
-        <v>1234</v>
+        <v>123</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>480</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="S33" t="s">
+        <v>150</v>
+      </c>
+      <c r="T33" t="s">
+        <v>17</v>
+      </c>
+      <c r="V33" t="s">
+        <v>19</v>
+      </c>
+      <c r="W33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="X33" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="Z33" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA33" s="7" t="s">
         <v>441</v>
       </c>
       <c r="AB33">
-        <v>123</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="S34" t="s">
-        <v>150</v>
-      </c>
-      <c r="T34" t="s">
-        <v>17</v>
-      </c>
-      <c r="V34" t="s">
-        <v>19</v>
-      </c>
-      <c r="W34" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="X34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y34" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
       <c r="Z34" s="5" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="AA34" s="7" t="s">
         <v>441</v>
@@ -3576,53 +3565,53 @@
       <c r="AB34">
         <v>123</v>
       </c>
-      <c r="AK34" s="5" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>60</v>
-      </c>
-      <c r="F35" t="s">
-        <v>50</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="S35" t="s">
+        <v>150</v>
+      </c>
+      <c r="T35" t="s">
+        <v>17</v>
+      </c>
+      <c r="V35" t="s">
+        <v>19</v>
+      </c>
+      <c r="W35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="X35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y35" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="Z35" s="5" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="AA35" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB35" s="5">
-        <v>1</v>
+        <v>441</v>
+      </c>
+      <c r="AB35">
+        <v>123</v>
+      </c>
+      <c r="AK35" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>55</v>
-      </c>
-      <c r="S36" t="s">
-        <v>495</v>
-      </c>
-      <c r="T36" t="s">
-        <v>497</v>
-      </c>
-      <c r="U36" t="s">
-        <v>488</v>
-      </c>
-      <c r="V36" t="s">
-        <v>496</v>
-      </c>
-      <c r="W36" s="5" t="s">
-        <v>498</v>
-      </c>
-      <c r="X36" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F36" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="2"/>
       <c r="Z36" s="5" t="s">
         <v>56</v>
       </c>
@@ -3635,13 +3624,7 @@
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
-      </c>
-      <c r="F37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="S37" t="s">
         <v>495</v>
@@ -3661,112 +3644,117 @@
       <c r="X37" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="Z37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA37" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB37" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="W38" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="F38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+      <c r="S38" t="s">
+        <v>495</v>
+      </c>
+      <c r="T38" t="s">
+        <v>497</v>
+      </c>
+      <c r="U38" t="s">
+        <v>488</v>
+      </c>
+      <c r="V38" t="s">
+        <v>496</v>
+      </c>
+      <c r="W38" s="5" t="s">
+        <v>498</v>
+      </c>
       <c r="X38" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>491</v>
-      </c>
-      <c r="E39" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="H39" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="I39" s="2"/>
-      <c r="S39" t="s">
-        <v>495</v>
-      </c>
-      <c r="T39" t="s">
-        <v>497</v>
-      </c>
-      <c r="U39" t="s">
-        <v>488</v>
-      </c>
-      <c r="V39" t="s">
-        <v>496</v>
-      </c>
-      <c r="W39" s="5" t="s">
-        <v>498</v>
-      </c>
+        <v>607</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="W39" s="5"/>
       <c r="X39" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>118</v>
-      </c>
-      <c r="F40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL40" t="s">
-        <v>436</v>
+        <v>77</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="I40" s="2"/>
+      <c r="S40" t="s">
+        <v>495</v>
+      </c>
+      <c r="T40" t="s">
+        <v>497</v>
+      </c>
+      <c r="U40" t="s">
+        <v>488</v>
+      </c>
+      <c r="V40" t="s">
+        <v>496</v>
+      </c>
+      <c r="W40" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="X40" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>118</v>
+      </c>
+      <c r="F41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" t="s">
+        <v>15</v>
       </c>
       <c r="AL41" t="s">
-        <v>596</v>
-      </c>
-      <c r="AM41" t="s">
-        <v>296</v>
-      </c>
-      <c r="AN41" t="s">
-        <v>314</v>
-      </c>
-      <c r="AO41" t="s">
-        <v>314</v>
+        <v>436</v>
       </c>
     </row>
     <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>164</v>
-      </c>
-      <c r="R42" s="12"/>
-      <c r="S42" t="s">
-        <v>495</v>
-      </c>
-      <c r="T42" t="s">
-        <v>497</v>
-      </c>
-      <c r="U42" t="s">
-        <v>488</v>
-      </c>
-      <c r="V42" t="s">
-        <v>496</v>
-      </c>
-      <c r="W42" s="5" t="s">
-        <v>498</v>
-      </c>
-      <c r="X42" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>596</v>
       </c>
       <c r="AM42" t="s">
         <v>296</v>
@@ -3780,76 +3768,98 @@
     </row>
     <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>166</v>
-      </c>
-      <c r="F43" t="s">
-        <v>167</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="12"/>
-      <c r="P43" s="12"/>
-      <c r="Q43" s="12"/>
-      <c r="AC43" t="s">
-        <v>257</v>
-      </c>
-      <c r="AP43" t="s">
-        <v>186</v>
+        <v>164</v>
+      </c>
+      <c r="R43" s="12"/>
+      <c r="S43" t="s">
+        <v>495</v>
+      </c>
+      <c r="T43" t="s">
+        <v>497</v>
+      </c>
+      <c r="U43" t="s">
+        <v>488</v>
+      </c>
+      <c r="V43" t="s">
+        <v>496</v>
+      </c>
+      <c r="W43" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="X43" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM43" t="s">
+        <v>296</v>
+      </c>
+      <c r="AN43" t="s">
+        <v>314</v>
+      </c>
+      <c r="AO43" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>184</v>
-      </c>
-      <c r="H44" s="23" t="s">
-        <v>607</v>
+        <v>166</v>
+      </c>
+      <c r="F44" t="s">
+        <v>167</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
+      <c r="AC44" t="s">
+        <v>257</v>
+      </c>
       <c r="AP44" t="s">
-        <v>280</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>279</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>607</v>
+      </c>
+      <c r="I45" s="12"/>
       <c r="AP45" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>284</v>
-      </c>
-      <c r="F46" t="s">
-        <v>15</v>
-      </c>
-      <c r="G46" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC46" t="s">
-        <v>255</v>
-      </c>
-      <c r="AD46" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ46" t="s">
-        <v>83</v>
+        <v>279</v>
+      </c>
+      <c r="AP46" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>215</v>
+        <v>284</v>
+      </c>
+      <c r="F47" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>255</v>
+      </c>
+      <c r="AD47" s="5" t="s">
+        <v>120</v>
